<commit_message>
Version updated to web/alpha page. updated input files and results, removed a lot of stuff that I'm not using now, reorganized some things, added license document and some FAST v8.0 documentation.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@298 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 47f4a0adb40b7228962ad0888b21081fe6b80f96
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -12,6 +12,9 @@
     <sheet name="ServoDyn" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ElastoDyn!$A$510:$J$519</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -5370,7 +5373,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="506">
+  <dxfs count="500">
     <dxf>
       <font>
         <u val="none"/>
@@ -9605,57 +9608,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -10602,8 +10554,8 @@
   <dimension ref="A1:K801"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A490" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E519" sqref="E519"/>
+      <pane ySplit="11" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34453,8 +34405,8 @@
   <dimension ref="A1:J210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J154" sqref="J154"/>
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40279,7 +40231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A50" sqref="A50:XFD54"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
+ I fixed some cosmetic issues with printing messages to the screen. + I added a check that the BladedDLL isn't called too many times at a given time step + modified to work with fixed SubDyn names (ModName routines)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@482 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 0be2bffc201979cababee2f7cc9304880be4a8a3
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="540" windowWidth="14880" windowHeight="7605" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="540" windowWidth="14880" windowHeight="7605" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12557" uniqueCount="2253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12567" uniqueCount="2255">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -6903,6 +6903,12 @@
   </si>
   <si>
     <t># used in VIND</t>
+  </si>
+  <si>
+    <t>LastTimeCalled</t>
+  </si>
+  <si>
+    <t>"last time the CalcOutput/Bladed DLL was called"</t>
   </si>
 </sst>
 </file>
@@ -7090,7 +7096,41 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="632">
+  <dxfs count="636">
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <u val="none"/>
@@ -13377,10 +13417,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="609" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="613" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="608" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="612" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36220,1394 +36260,1394 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A241:A297 A501:A509 A313 A304 A530:A531 A636:A669 A514 A1:A12 A51 A20:A39 A685:A700 A680:A683 A702:A708 A674:A678 A486 A488:A492 A237:A239 A496:A499 A525 A519:A523 A816:A1048576 A765:A766 A327:A336 A355:A358 A369:A371 A382:A385 A779:A783 A545:A616 A408:A432 A434:A441 A480:A484 A443:A476 A376:A379 A786:A788 A770:A771 A618:A634">
-    <cfRule type="containsText" dxfId="607" priority="819" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="611" priority="819" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="606" priority="820" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="610" priority="820" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A240">
-    <cfRule type="containsText" dxfId="605" priority="807" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="609" priority="807" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A240)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="604" priority="808" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="608" priority="808" operator="beginsWith" text="#">
       <formula>LEFT(A240,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A17">
-    <cfRule type="containsText" dxfId="603" priority="801" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="607" priority="801" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="602" priority="802" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="606" priority="802" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:A53">
-    <cfRule type="containsText" dxfId="601" priority="797" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="605" priority="797" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A52)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="600" priority="798" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="604" priority="798" operator="beginsWith" text="#">
       <formula>LEFT(A52,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A14">
-    <cfRule type="containsText" dxfId="599" priority="795" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="603" priority="795" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A13)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="598" priority="796" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="602" priority="796" operator="beginsWith" text="#">
       <formula>LEFT(A13,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A527">
-    <cfRule type="containsText" dxfId="597" priority="791" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="601" priority="791" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A527)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="596" priority="792" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="600" priority="792" operator="beginsWith" text="#">
       <formula>LEFT(A527,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A526">
-    <cfRule type="containsText" dxfId="595" priority="793" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="599" priority="793" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A526)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="594" priority="794" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="598" priority="794" operator="beginsWith" text="#">
       <formula>LEFT(A526,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A539">
-    <cfRule type="containsText" dxfId="593" priority="789" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="597" priority="789" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A539)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="592" priority="790" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="596" priority="790" operator="beginsWith" text="#">
       <formula>LEFT(A539,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A540">
-    <cfRule type="containsText" dxfId="591" priority="787" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="595" priority="787" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A540)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="590" priority="788" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="594" priority="788" operator="beginsWith" text="#">
       <formula>LEFT(A540,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A537">
-    <cfRule type="containsText" dxfId="589" priority="785" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="593" priority="785" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A537)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="588" priority="786" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="592" priority="786" operator="beginsWith" text="#">
       <formula>LEFT(A537,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A538">
-    <cfRule type="containsText" dxfId="587" priority="783" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="591" priority="783" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A538)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="586" priority="784" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="590" priority="784" operator="beginsWith" text="#">
       <formula>LEFT(A538,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A541">
-    <cfRule type="containsText" dxfId="585" priority="779" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="589" priority="779" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A541)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="584" priority="780" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="588" priority="780" operator="beginsWith" text="#">
       <formula>LEFT(A541,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A500">
-    <cfRule type="containsText" dxfId="583" priority="775" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="587" priority="775" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A500)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="582" priority="776" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="586" priority="776" operator="beginsWith" text="#">
       <formula>LEFT(A500,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A528">
-    <cfRule type="containsText" dxfId="581" priority="773" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="585" priority="773" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A528)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="580" priority="774" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="584" priority="774" operator="beginsWith" text="#">
       <formula>LEFT(A528,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A542">
-    <cfRule type="containsText" dxfId="579" priority="771" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="583" priority="771" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A542)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="578" priority="772" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="582" priority="772" operator="beginsWith" text="#">
       <formula>LEFT(A542,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A635">
-    <cfRule type="containsText" dxfId="577" priority="769" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="581" priority="769" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A635)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="576" priority="770" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="580" priority="770" operator="beginsWith" text="#">
       <formula>LEFT(A635,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A529">
-    <cfRule type="containsText" dxfId="575" priority="763" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="579" priority="763" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A529)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="574" priority="764" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="578" priority="764" operator="beginsWith" text="#">
       <formula>LEFT(A529,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A298:A300">
-    <cfRule type="containsText" dxfId="573" priority="761" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="577" priority="761" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A298)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="572" priority="762" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="576" priority="762" operator="beginsWith" text="#">
       <formula>LEFT(A298,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A301">
-    <cfRule type="containsText" dxfId="571" priority="757" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="575" priority="757" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A301)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="570" priority="758" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="574" priority="758" operator="beginsWith" text="#">
       <formula>LEFT(A301,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A302:A303 A305:A310">
-    <cfRule type="containsText" dxfId="569" priority="755" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="573" priority="755" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A302)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="568" priority="756" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="572" priority="756" operator="beginsWith" text="#">
       <formula>LEFT(A302,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A311:A312 A314:A320 A533">
-    <cfRule type="containsText" dxfId="567" priority="753" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="571" priority="753" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A311)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="566" priority="754" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="570" priority="754" operator="beginsWith" text="#">
       <formula>LEFT(A311,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A532">
-    <cfRule type="containsText" dxfId="565" priority="709" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="569" priority="709" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A532)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="564" priority="710" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="568" priority="710" operator="beginsWith" text="#">
       <formula>LEFT(A532,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A322">
-    <cfRule type="containsText" dxfId="563" priority="697" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="567" priority="697" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A322)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="562" priority="698" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="566" priority="698" operator="beginsWith" text="#">
       <formula>LEFT(A322,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A321">
-    <cfRule type="containsText" dxfId="561" priority="699" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="565" priority="699" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A321)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="560" priority="700" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="564" priority="700" operator="beginsWith" text="#">
       <formula>LEFT(A321,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A534">
-    <cfRule type="containsText" dxfId="559" priority="695" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="563" priority="695" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A534)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="558" priority="696" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="562" priority="696" operator="beginsWith" text="#">
       <formula>LEFT(A534,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A535">
-    <cfRule type="containsText" dxfId="557" priority="693" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="561" priority="693" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A535)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="556" priority="694" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="560" priority="694" operator="beginsWith" text="#">
       <formula>LEFT(A535,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A323:A324">
-    <cfRule type="containsText" dxfId="555" priority="691" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="559" priority="691" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A323)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="554" priority="692" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="558" priority="692" operator="beginsWith" text="#">
       <formula>LEFT(A323,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A544">
-    <cfRule type="containsText" dxfId="553" priority="683" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="557" priority="683" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A544)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="552" priority="684" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="556" priority="684" operator="beginsWith" text="#">
       <formula>LEFT(A544,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A543">
-    <cfRule type="containsText" dxfId="551" priority="685" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="555" priority="685" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A543)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="550" priority="686" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="554" priority="686" operator="beginsWith" text="#">
       <formula>LEFT(A543,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A671">
-    <cfRule type="containsText" dxfId="549" priority="653" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="553" priority="653" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A671)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="548" priority="654" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="552" priority="654" operator="beginsWith" text="#">
       <formula>LEFT(A671,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A325:A326 A360">
-    <cfRule type="containsText" dxfId="547" priority="649" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="551" priority="649" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A325)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="546" priority="650" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="550" priority="650" operator="beginsWith" text="#">
       <formula>LEFT(A325,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A381">
-    <cfRule type="containsText" dxfId="545" priority="647" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="549" priority="647" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A381)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="544" priority="648" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="548" priority="648" operator="beginsWith" text="#">
       <formula>LEFT(A381,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A510:A511">
-    <cfRule type="containsText" dxfId="543" priority="643" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="547" priority="643" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A510)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="542" priority="644" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="546" priority="644" operator="beginsWith" text="#">
       <formula>LEFT(A510,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A513">
-    <cfRule type="containsText" dxfId="541" priority="641" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="545" priority="641" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A513)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="540" priority="642" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="544" priority="642" operator="beginsWith" text="#">
       <formula>LEFT(A513,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="containsText" dxfId="539" priority="615" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="543" priority="615" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A18)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="538" priority="616" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="542" priority="616" operator="beginsWith" text="#">
       <formula>LEFT(A18,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="containsText" dxfId="537" priority="613" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="541" priority="613" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A19)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="536" priority="614" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="540" priority="614" operator="beginsWith" text="#">
       <formula>LEFT(A19,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="containsText" dxfId="535" priority="605" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="539" priority="605" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A40)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="534" priority="606" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="538" priority="606" operator="beginsWith" text="#">
       <formula>LEFT(A40,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="containsText" dxfId="533" priority="603" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="537" priority="603" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A41)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="532" priority="604" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="536" priority="604" operator="beginsWith" text="#">
       <formula>LEFT(A41,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="containsText" dxfId="531" priority="601" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="535" priority="601" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A42)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="530" priority="602" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="534" priority="602" operator="beginsWith" text="#">
       <formula>LEFT(A42,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="containsText" dxfId="529" priority="599" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="533" priority="599" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A43)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="528" priority="600" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="532" priority="600" operator="beginsWith" text="#">
       <formula>LEFT(A43,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A709">
-    <cfRule type="containsText" dxfId="527" priority="597" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="531" priority="597" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A709)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="526" priority="598" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="530" priority="598" operator="beginsWith" text="#">
       <formula>LEFT(A709,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A710">
-    <cfRule type="containsText" dxfId="525" priority="595" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="529" priority="595" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A710)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="524" priority="596" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="528" priority="596" operator="beginsWith" text="#">
       <formula>LEFT(A710,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A711">
-    <cfRule type="containsText" dxfId="523" priority="593" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="527" priority="593" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A711)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="522" priority="594" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="526" priority="594" operator="beginsWith" text="#">
       <formula>LEFT(A711,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A764">
-    <cfRule type="containsText" dxfId="521" priority="591" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="525" priority="591" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A764)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="520" priority="592" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="524" priority="592" operator="beginsWith" text="#">
       <formula>LEFT(A764,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A713:A716">
-    <cfRule type="containsText" dxfId="519" priority="587" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="523" priority="587" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A713)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="518" priority="588" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="522" priority="588" operator="beginsWith" text="#">
       <formula>LEFT(A713,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A712">
-    <cfRule type="containsText" dxfId="517" priority="583" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="521" priority="583" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A712)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="516" priority="584" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="520" priority="584" operator="beginsWith" text="#">
       <formula>LEFT(A712,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A717:A724">
-    <cfRule type="containsText" dxfId="515" priority="577" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="519" priority="577" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A717)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="514" priority="578" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="518" priority="578" operator="beginsWith" text="#">
       <formula>LEFT(A717,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A725:A735">
-    <cfRule type="containsText" dxfId="513" priority="571" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="517" priority="571" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A725)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="512" priority="572" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="516" priority="572" operator="beginsWith" text="#">
       <formula>LEFT(A725,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A736">
-    <cfRule type="containsText" dxfId="511" priority="573" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="515" priority="573" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A736)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="510" priority="574" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="514" priority="574" operator="beginsWith" text="#">
       <formula>LEFT(A736,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A737:A747">
-    <cfRule type="containsText" dxfId="509" priority="565" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="513" priority="565" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A737)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="508" priority="566" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="512" priority="566" operator="beginsWith" text="#">
       <formula>LEFT(A737,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A748">
-    <cfRule type="containsText" dxfId="507" priority="567" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="511" priority="567" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A748)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="506" priority="568" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="510" priority="568" operator="beginsWith" text="#">
       <formula>LEFT(A748,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A749">
-    <cfRule type="containsText" dxfId="505" priority="561" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="509" priority="561" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A749)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="504" priority="562" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="508" priority="562" operator="beginsWith" text="#">
       <formula>LEFT(A749,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A753:A754">
-    <cfRule type="containsText" dxfId="503" priority="551" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="507" priority="551" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A753)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="502" priority="552" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="506" priority="552" operator="beginsWith" text="#">
       <formula>LEFT(A753,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A750">
-    <cfRule type="containsText" dxfId="501" priority="557" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="505" priority="557" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A750)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="500" priority="558" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="504" priority="558" operator="beginsWith" text="#">
       <formula>LEFT(A750,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A751">
-    <cfRule type="containsText" dxfId="499" priority="555" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="503" priority="555" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A751)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="498" priority="556" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="502" priority="556" operator="beginsWith" text="#">
       <formula>LEFT(A751,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A752">
-    <cfRule type="containsText" dxfId="497" priority="553" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="501" priority="553" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A752)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="496" priority="554" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="500" priority="554" operator="beginsWith" text="#">
       <formula>LEFT(A752,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A755:A756">
-    <cfRule type="containsText" dxfId="495" priority="547" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="499" priority="547" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A755)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="494" priority="548" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="498" priority="548" operator="beginsWith" text="#">
       <formula>LEFT(A755,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A757">
-    <cfRule type="containsText" dxfId="493" priority="537" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="497" priority="537" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A757)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="492" priority="538" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="496" priority="538" operator="beginsWith" text="#">
       <formula>LEFT(A757,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A536">
-    <cfRule type="containsText" dxfId="491" priority="533" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="495" priority="533" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A536)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="490" priority="534" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="494" priority="534" operator="beginsWith" text="#">
       <formula>LEFT(A536,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A670">
-    <cfRule type="containsText" dxfId="489" priority="503" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="493" priority="503" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A670)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="488" priority="504" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="492" priority="504" operator="beginsWith" text="#">
       <formula>LEFT(A670,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="containsText" dxfId="487" priority="501" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="491" priority="501" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A45)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="486" priority="502" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="490" priority="502" operator="beginsWith" text="#">
       <formula>LEFT(A45,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="containsText" dxfId="485" priority="499" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="489" priority="499" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A46)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="484" priority="500" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="488" priority="500" operator="beginsWith" text="#">
       <formula>LEFT(A46,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:A49">
-    <cfRule type="containsText" dxfId="483" priority="497" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="487" priority="497" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A47)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="482" priority="498" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="486" priority="498" operator="beginsWith" text="#">
       <formula>LEFT(A47,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A701">
-    <cfRule type="containsText" dxfId="481" priority="477" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="485" priority="477" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A701)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="480" priority="478" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="484" priority="478" operator="beginsWith" text="#">
       <formula>LEFT(A701,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A673">
-    <cfRule type="containsText" dxfId="479" priority="483" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="483" priority="483" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A673)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="478" priority="484" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="482" priority="484" operator="beginsWith" text="#">
       <formula>LEFT(A673,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A679">
-    <cfRule type="containsText" dxfId="477" priority="479" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="481" priority="479" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A679)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="476" priority="480" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="480" priority="480" operator="beginsWith" text="#">
       <formula>LEFT(A679,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A684">
-    <cfRule type="containsText" dxfId="475" priority="475" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="479" priority="475" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A684)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="474" priority="476" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="478" priority="476" operator="beginsWith" text="#">
       <formula>LEFT(A684,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A485">
-    <cfRule type="containsText" dxfId="473" priority="473" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="477" priority="473" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A485)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="472" priority="474" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="476" priority="474" operator="beginsWith" text="#">
       <formula>LEFT(A485,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A487">
-    <cfRule type="containsText" dxfId="471" priority="463" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="475" priority="463" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A487)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="470" priority="464" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="474" priority="464" operator="beginsWith" text="#">
       <formula>LEFT(A487,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A758">
-    <cfRule type="containsText" dxfId="469" priority="461" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="473" priority="461" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A758)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="468" priority="462" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="472" priority="462" operator="beginsWith" text="#">
       <formula>LEFT(A758,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90 A100:A102">
-    <cfRule type="containsText" dxfId="467" priority="271" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="471" priority="271" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="466" priority="272" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="470" priority="272" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A112">
-    <cfRule type="containsText" dxfId="465" priority="275" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="469" priority="275" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="464" priority="276" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="468" priority="276" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A126 A113">
-    <cfRule type="containsText" dxfId="463" priority="277" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="467" priority="277" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="462" priority="278" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="466" priority="278" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A131:A132 A128">
-    <cfRule type="containsText" dxfId="461" priority="279" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="465" priority="279" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="460" priority="280" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="464" priority="280" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A127">
-    <cfRule type="containsText" dxfId="459" priority="281" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="463" priority="281" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="458" priority="282" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="462" priority="282" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130">
-    <cfRule type="containsText" dxfId="457" priority="283" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="461" priority="283" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="456" priority="284" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="460" priority="284" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A133">
-    <cfRule type="containsText" dxfId="455" priority="285" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="459" priority="285" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="454" priority="286" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="458" priority="286" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A129">
-    <cfRule type="containsText" dxfId="453" priority="287" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="457" priority="287" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="452" priority="288" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="456" priority="288" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137">
-    <cfRule type="containsText" dxfId="451" priority="289" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="455" priority="289" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="450" priority="290" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="454" priority="290" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136 A147">
-    <cfRule type="containsText" dxfId="449" priority="291" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="453" priority="291" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="448" priority="292" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="452" priority="292" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A149">
-    <cfRule type="containsText" dxfId="447" priority="293" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="451" priority="293" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="446" priority="294" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="450" priority="294" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A151">
-    <cfRule type="containsText" dxfId="445" priority="295" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="449" priority="295" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="444" priority="296" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="448" priority="296" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A493">
-    <cfRule type="containsText" dxfId="443" priority="217" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="447" priority="217" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A493)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="442" priority="218" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="446" priority="218" operator="beginsWith" text="#">
       <formula>LEFT(A493,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A494">
-    <cfRule type="containsText" dxfId="441" priority="215" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="445" priority="215" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A494)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="440" priority="216" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="444" priority="216" operator="beginsWith" text="#">
       <formula>LEFT(A494,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A524">
-    <cfRule type="containsText" dxfId="439" priority="213" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="443" priority="213" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A524)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="438" priority="214" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="442" priority="214" operator="beginsWith" text="#">
       <formula>LEFT(A524,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A773">
-    <cfRule type="containsText" dxfId="437" priority="211" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="441" priority="211" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A773)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="436" priority="212" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="440" priority="212" operator="beginsWith" text="#">
       <formula>LEFT(A773,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A86">
-    <cfRule type="containsText" dxfId="435" priority="1403" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="439" priority="1403" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="434" priority="1404" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="438" priority="1404" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A789">
-    <cfRule type="containsText" dxfId="433" priority="203" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="437" priority="203" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A789)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="432" priority="204" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="436" priority="204" operator="beginsWith" text="#">
       <formula>LEFT(A789,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A791">
-    <cfRule type="containsText" dxfId="431" priority="199" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="435" priority="199" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A791)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="430" priority="200" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="434" priority="200" operator="beginsWith" text="#">
       <formula>LEFT(A791,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A790">
-    <cfRule type="containsText" dxfId="429" priority="201" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="433" priority="201" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A790)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="428" priority="202" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="432" priority="202" operator="beginsWith" text="#">
       <formula>LEFT(A790,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A793">
-    <cfRule type="containsText" dxfId="427" priority="197" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="431" priority="197" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A793)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="426" priority="198" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="430" priority="198" operator="beginsWith" text="#">
       <formula>LEFT(A793,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A797:A800">
-    <cfRule type="containsText" dxfId="425" priority="189" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="429" priority="189" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A797)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="424" priority="190" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="428" priority="190" operator="beginsWith" text="#">
       <formula>LEFT(A797,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A798">
-    <cfRule type="containsText" dxfId="423" priority="187" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="427" priority="187" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A798)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="422" priority="188" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="426" priority="188" operator="beginsWith" text="#">
       <formula>LEFT(A798,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A799">
-    <cfRule type="containsText" dxfId="421" priority="185" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="425" priority="185" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A799)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="420" priority="186" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="424" priority="186" operator="beginsWith" text="#">
       <formula>LEFT(A799,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A800">
-    <cfRule type="containsText" dxfId="419" priority="183" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="423" priority="183" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A800)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="418" priority="184" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="422" priority="184" operator="beginsWith" text="#">
       <formula>LEFT(A800,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A794">
-    <cfRule type="containsText" dxfId="417" priority="181" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="421" priority="181" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A794)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="416" priority="182" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="420" priority="182" operator="beginsWith" text="#">
       <formula>LEFT(A794,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A672">
-    <cfRule type="containsText" dxfId="415" priority="177" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="419" priority="177" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A672)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="414" priority="178" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="418" priority="178" operator="beginsWith" text="#">
       <formula>LEFT(A672,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A339">
-    <cfRule type="containsText" dxfId="413" priority="167" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="417" priority="167" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A339)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="412" priority="168" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="416" priority="168" operator="beginsWith" text="#">
       <formula>LEFT(A339,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A337">
-    <cfRule type="containsText" dxfId="411" priority="171" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="415" priority="171" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A337)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="410" priority="172" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="414" priority="172" operator="beginsWith" text="#">
       <formula>LEFT(A337,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A338">
-    <cfRule type="containsText" dxfId="409" priority="169" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="413" priority="169" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A338)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="408" priority="170" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="412" priority="170" operator="beginsWith" text="#">
       <formula>LEFT(A338,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A340">
-    <cfRule type="containsText" dxfId="407" priority="165" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="411" priority="165" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A340)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="406" priority="166" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="410" priority="166" operator="beginsWith" text="#">
       <formula>LEFT(A340,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A341">
-    <cfRule type="containsText" dxfId="405" priority="163" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="409" priority="163" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A341)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="404" priority="164" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="408" priority="164" operator="beginsWith" text="#">
       <formula>LEFT(A341,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A342">
-    <cfRule type="containsText" dxfId="403" priority="161" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="407" priority="161" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A342)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="402" priority="162" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="406" priority="162" operator="beginsWith" text="#">
       <formula>LEFT(A342,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A343">
-    <cfRule type="containsText" dxfId="401" priority="159" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="405" priority="159" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A343)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="400" priority="160" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="404" priority="160" operator="beginsWith" text="#">
       <formula>LEFT(A343,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A344">
-    <cfRule type="containsText" dxfId="399" priority="157" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="403" priority="157" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A344)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="398" priority="158" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="402" priority="158" operator="beginsWith" text="#">
       <formula>LEFT(A344,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A345">
-    <cfRule type="containsText" dxfId="397" priority="155" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="401" priority="155" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A345)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="396" priority="156" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="400" priority="156" operator="beginsWith" text="#">
       <formula>LEFT(A345,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A347">
-    <cfRule type="containsText" dxfId="395" priority="151" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="399" priority="151" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A347)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="394" priority="152" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="398" priority="152" operator="beginsWith" text="#">
       <formula>LEFT(A347,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A348">
-    <cfRule type="containsText" dxfId="393" priority="149" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="397" priority="149" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A348)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="392" priority="150" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="396" priority="150" operator="beginsWith" text="#">
       <formula>LEFT(A348,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A349">
-    <cfRule type="containsText" dxfId="391" priority="147" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="395" priority="147" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A349)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="390" priority="148" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="394" priority="148" operator="beginsWith" text="#">
       <formula>LEFT(A349,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A350">
-    <cfRule type="containsText" dxfId="389" priority="145" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="393" priority="145" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A350)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="388" priority="146" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="392" priority="146" operator="beginsWith" text="#">
       <formula>LEFT(A350,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A351">
-    <cfRule type="containsText" dxfId="387" priority="143" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="391" priority="143" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A351)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="386" priority="144" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="390" priority="144" operator="beginsWith" text="#">
       <formula>LEFT(A351,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A352">
-    <cfRule type="containsText" dxfId="385" priority="141" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="389" priority="141" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A352)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="384" priority="142" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="388" priority="142" operator="beginsWith" text="#">
       <formula>LEFT(A352,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A353">
-    <cfRule type="containsText" dxfId="383" priority="139" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="387" priority="139" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A353)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="382" priority="140" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="386" priority="140" operator="beginsWith" text="#">
       <formula>LEFT(A353,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A361:A367">
-    <cfRule type="containsText" dxfId="381" priority="137" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="385" priority="137" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A361)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="380" priority="138" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="384" priority="138" operator="beginsWith" text="#">
       <formula>LEFT(A361,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A359">
-    <cfRule type="containsText" dxfId="379" priority="135" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="383" priority="135" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A359)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="378" priority="136" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="382" priority="136" operator="beginsWith" text="#">
       <formula>LEFT(A359,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A368 A372:A375">
-    <cfRule type="containsText" dxfId="377" priority="133" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="381" priority="133" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A368)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="376" priority="134" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="380" priority="134" operator="beginsWith" text="#">
       <formula>LEFT(A368,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A380">
-    <cfRule type="containsText" dxfId="375" priority="131" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="379" priority="131" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A380)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="374" priority="132" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="378" priority="132" operator="beginsWith" text="#">
       <formula>LEFT(A380,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A391">
-    <cfRule type="containsText" dxfId="373" priority="129" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="377" priority="129" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A391)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="372" priority="130" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="376" priority="130" operator="beginsWith" text="#">
       <formula>LEFT(A391,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A354">
-    <cfRule type="containsText" dxfId="371" priority="127" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="375" priority="127" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A354)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="370" priority="128" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="374" priority="128" operator="beginsWith" text="#">
       <formula>LEFT(A354,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A386">
-    <cfRule type="containsText" dxfId="369" priority="125" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="373" priority="125" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A386)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="368" priority="126" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="372" priority="126" operator="beginsWith" text="#">
       <formula>LEFT(A386,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A387">
-    <cfRule type="containsText" dxfId="367" priority="123" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="371" priority="123" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A387)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="366" priority="124" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="370" priority="124" operator="beginsWith" text="#">
       <formula>LEFT(A387,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A388">
-    <cfRule type="containsText" dxfId="365" priority="121" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="369" priority="121" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A388)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="364" priority="122" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="368" priority="122" operator="beginsWith" text="#">
       <formula>LEFT(A388,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A389">
-    <cfRule type="containsText" dxfId="363" priority="119" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="367" priority="119" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A389)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="362" priority="120" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="366" priority="120" operator="beginsWith" text="#">
       <formula>LEFT(A389,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A390">
-    <cfRule type="containsText" dxfId="361" priority="117" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="365" priority="117" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A390)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="360" priority="118" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="364" priority="118" operator="beginsWith" text="#">
       <formula>LEFT(A390,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A392">
-    <cfRule type="containsText" dxfId="359" priority="115" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="363" priority="115" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A392)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="358" priority="116" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="362" priority="116" operator="beginsWith" text="#">
       <formula>LEFT(A392,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A393">
-    <cfRule type="containsText" dxfId="357" priority="113" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="361" priority="113" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A393)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="356" priority="114" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="360" priority="114" operator="beginsWith" text="#">
       <formula>LEFT(A393,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A433">
-    <cfRule type="containsText" dxfId="355" priority="111" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="359" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A433)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="354" priority="112" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="358" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(A433,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A394">
-    <cfRule type="containsText" dxfId="353" priority="109" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="357" priority="109" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A394)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="352" priority="110" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="356" priority="110" operator="beginsWith" text="#">
       <formula>LEFT(A394,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A395:A402">
-    <cfRule type="containsText" dxfId="351" priority="107" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="355" priority="107" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A395)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="350" priority="108" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="354" priority="108" operator="beginsWith" text="#">
       <formula>LEFT(A395,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A406">
-    <cfRule type="containsText" dxfId="349" priority="97" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="353" priority="97" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A406)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="348" priority="98" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="352" priority="98" operator="beginsWith" text="#">
       <formula>LEFT(A406,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A404">
-    <cfRule type="containsText" dxfId="347" priority="103" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="351" priority="103" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A404)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="346" priority="104" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="350" priority="104" operator="beginsWith" text="#">
       <formula>LEFT(A404,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A403">
-    <cfRule type="containsText" dxfId="345" priority="101" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="349" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A403)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="344" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="348" priority="102" operator="beginsWith" text="#">
       <formula>LEFT(A403,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A405">
-    <cfRule type="containsText" dxfId="343" priority="99" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="347" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A405)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="342" priority="100" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="346" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(A405,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A407">
-    <cfRule type="containsText" dxfId="341" priority="95" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="345" priority="95" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A407)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="340" priority="96" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="344" priority="96" operator="beginsWith" text="#">
       <formula>LEFT(A407,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A759">
-    <cfRule type="containsText" dxfId="339" priority="89" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="343" priority="89" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A759)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="338" priority="90" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="342" priority="90" operator="beginsWith" text="#">
       <formula>LEFT(A759,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A760">
-    <cfRule type="containsText" dxfId="337" priority="87" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="341" priority="87" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A760)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="336" priority="88" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="340" priority="88" operator="beginsWith" text="#">
       <formula>LEFT(A760,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A346">
-    <cfRule type="containsText" dxfId="335" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="339" priority="85" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A346)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="334" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="338" priority="86" operator="beginsWith" text="#">
       <formula>LEFT(A346,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A477">
-    <cfRule type="containsText" dxfId="333" priority="83" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="337" priority="83" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A477)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="332" priority="84" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="336" priority="84" operator="beginsWith" text="#">
       <formula>LEFT(A477,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A478">
-    <cfRule type="containsText" dxfId="331" priority="81" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="335" priority="81" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A478)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="330" priority="82" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="334" priority="82" operator="beginsWith" text="#">
       <formula>LEFT(A478,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A479">
-    <cfRule type="containsText" dxfId="329" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="333" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A479)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="328" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="332" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A479,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A516">
-    <cfRule type="containsText" dxfId="327" priority="77" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="331" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A516)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="326" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="330" priority="78" operator="beginsWith" text="#">
       <formula>LEFT(A516,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A512">
-    <cfRule type="containsText" dxfId="325" priority="75" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="329" priority="75" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A512)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="324" priority="76" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="328" priority="76" operator="beginsWith" text="#">
       <formula>LEFT(A512,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A795">
-    <cfRule type="containsText" dxfId="323" priority="71" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="327" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A795)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="322" priority="72" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="326" priority="72" operator="beginsWith" text="#">
       <formula>LEFT(A795,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A761">
-    <cfRule type="containsText" dxfId="321" priority="67" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="325" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A761)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="320" priority="68" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="324" priority="68" operator="beginsWith" text="#">
       <formula>LEFT(A761,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A236">
-    <cfRule type="containsText" dxfId="319" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="323" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A236)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="318" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="322" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A236,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A796">
-    <cfRule type="containsText" dxfId="317" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="321" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A796)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="316" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="320" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(A796,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A154:A162 A164:A235">
-    <cfRule type="containsText" dxfId="315" priority="381" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="319" priority="381" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="314" priority="382" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="318" priority="382" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A148 A150 A140 A142:A146 A61 A63:A64 A67:A75 A77:A78 A82:A84 A54 A56:A59">
-    <cfRule type="containsText" dxfId="313" priority="269" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="317" priority="269" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="312" priority="270" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="316" priority="270" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="containsText" dxfId="311" priority="1417" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="315" priority="1417" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="310" priority="1418" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="314" priority="1418" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A134:A135 A138 A114:A125 A97:A98 A89 A87 A91:A95">
-    <cfRule type="containsText" dxfId="309" priority="1699" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="313" priority="1699" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="308" priority="1700" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="312" priority="1700" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109 A103:A104 A106:A107">
-    <cfRule type="containsText" dxfId="307" priority="1759" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="311" priority="1759" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="306" priority="1760" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="310" priority="1760" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="containsText" dxfId="305" priority="1821" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="309" priority="1821" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="304" priority="1822" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="308" priority="1822" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111">
-    <cfRule type="containsText" dxfId="303" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="307" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="302" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="306" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110">
-    <cfRule type="containsText" dxfId="301" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="305" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="300" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="304" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A762">
-    <cfRule type="containsText" dxfId="299" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="303" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="298" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="302" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A763">
-    <cfRule type="containsText" dxfId="297" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="301" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="296" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="300" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A801">
-    <cfRule type="containsText" dxfId="295" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="299" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A801)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="294" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="298" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A801,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A802">
-    <cfRule type="containsText" dxfId="293" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="297" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A796)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="292" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="296" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(A796,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B806:B814">
-    <cfRule type="containsText" dxfId="291" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="295" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",B800)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="290" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="294" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(B800,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B803">
-    <cfRule type="containsText" dxfId="289" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="293" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",B797)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="288" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="292" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(B797,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A803">
-    <cfRule type="containsText" dxfId="287" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="291" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A803)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="286" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="290" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A803,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A804">
-    <cfRule type="containsText" dxfId="285" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="289" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A804)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="284" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="288" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A804,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B804">
-    <cfRule type="containsText" dxfId="283" priority="35" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="287" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",B798)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="282" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="286" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(B798,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A805">
-    <cfRule type="containsText" dxfId="281" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="285" priority="33" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A805)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="280" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="284" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(A805,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B805">
-    <cfRule type="containsText" dxfId="279" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="283" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",B799)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="278" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="282" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(B799,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A806:A814">
-    <cfRule type="containsText" dxfId="277" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="281" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A806)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="276" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="280" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A806,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B815">
-    <cfRule type="containsText" dxfId="275" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="279" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",B779)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="274" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="278" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(B779,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A815">
-    <cfRule type="containsText" dxfId="273" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="277" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A786)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="272" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="276" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A786,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A784:A785">
-    <cfRule type="containsText" dxfId="271" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="275" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A784)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="270" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="274" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A784,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A768">
-    <cfRule type="containsText" dxfId="269" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="273" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A768)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="268" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="272" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A768,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A769">
-    <cfRule type="containsText" dxfId="267" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="271" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A769)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="266" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="270" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A769,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108">
-    <cfRule type="containsText" dxfId="265" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="269" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="264" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="268" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A617">
-    <cfRule type="containsText" dxfId="263" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="267" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="262" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="266" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A767">
-    <cfRule type="containsText" dxfId="245" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="249" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A767)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="244" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="248" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A767,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37834,9 +37874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J283"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A264" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A273" sqref="A273:XFD276"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41267,6 +41307,38 @@
         <v>26</v>
       </c>
     </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E139" s="5" t="s">
+        <v>2253</v>
+      </c>
+      <c r="F139" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G139" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H139" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I139" s="10" t="s">
+        <v>2254</v>
+      </c>
+      <c r="J139" s="5" t="s">
+        <v>1173</v>
+      </c>
+    </row>
     <row r="142" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>13</v>
@@ -45312,467 +45384,475 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A13 A18 A232:A236 A273:A278 A108:A112 A141:A167 A280:A282 A285 A287:A1048576 A170:A196 A131:A134 A101:A104 A114:A127">
-    <cfRule type="containsText" dxfId="243" priority="299" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="247" priority="301" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="242" priority="300" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="246" priority="302" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="241" priority="291" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="245" priority="293" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="240" priority="292" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="244" priority="294" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="containsText" dxfId="239" priority="289" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="243" priority="291" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A14)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="238" priority="290" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="242" priority="292" operator="beginsWith" text="#">
       <formula>LEFT(A14,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:A20">
-    <cfRule type="containsText" dxfId="237" priority="287" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="241" priority="289" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A19)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="236" priority="288" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="240" priority="290" operator="beginsWith" text="#">
       <formula>LEFT(A19,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A16">
-    <cfRule type="containsText" dxfId="235" priority="285" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="239" priority="287" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="234" priority="286" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="238" priority="288" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A204">
-    <cfRule type="containsText" dxfId="233" priority="213" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="237" priority="215" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A204)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="232" priority="214" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="236" priority="216" operator="beginsWith" text="#">
       <formula>LEFT(A204,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A169">
-    <cfRule type="containsText" dxfId="231" priority="203" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="235" priority="205" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A169)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="230" priority="204" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="234" priority="206" operator="beginsWith" text="#">
       <formula>LEFT(A169,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="containsText" dxfId="229" priority="193" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="233" priority="195" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A105)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="228" priority="194" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="232" priority="196" operator="beginsWith" text="#">
       <formula>LEFT(A105,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A205">
-    <cfRule type="containsText" dxfId="227" priority="171" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="231" priority="173" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A205)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="226" priority="172" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="230" priority="174" operator="beginsWith" text="#">
       <formula>LEFT(A205,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A231">
-    <cfRule type="containsText" dxfId="225" priority="155" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="229" priority="157" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A231)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="224" priority="156" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="228" priority="158" operator="beginsWith" text="#">
       <formula>LEFT(A231,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="containsText" dxfId="223" priority="191" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="227" priority="193" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="222" priority="192" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="226" priority="194" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:A58">
-    <cfRule type="containsText" dxfId="221" priority="1099" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="225" priority="1101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="220" priority="1100" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="224" priority="1102" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A43">
-    <cfRule type="containsText" dxfId="219" priority="1149" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="223" priority="1151" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="218" priority="1150" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="222" priority="1152" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44:A47">
-    <cfRule type="containsText" dxfId="217" priority="1319" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="221" priority="1321" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="216" priority="1320" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="220" priority="1322" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:A63">
-    <cfRule type="containsText" dxfId="215" priority="1489" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="219" priority="1491" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="214" priority="1490" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="218" priority="1492" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A197">
-    <cfRule type="containsText" dxfId="213" priority="157" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="217" priority="159" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="212" priority="158" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="216" priority="160" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A279">
-    <cfRule type="containsText" dxfId="211" priority="149" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="215" priority="151" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A279)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="210" priority="150" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="214" priority="152" operator="beginsWith" text="#">
       <formula>LEFT(A279,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A238">
-    <cfRule type="containsText" dxfId="209" priority="139" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="213" priority="141" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A238)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="208" priority="140" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="212" priority="142" operator="beginsWith" text="#">
       <formula>LEFT(A238,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A267">
-    <cfRule type="containsText" dxfId="207" priority="141" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="211" priority="143" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A267)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="206" priority="142" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="210" priority="144" operator="beginsWith" text="#">
       <formula>LEFT(A267,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128">
-    <cfRule type="containsText" dxfId="205" priority="137" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="209" priority="139" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A128)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="204" priority="138" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="208" priority="140" operator="beginsWith" text="#">
       <formula>LEFT(A128,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A129">
-    <cfRule type="containsText" dxfId="203" priority="135" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="207" priority="137" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A129)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="202" priority="136" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="206" priority="138" operator="beginsWith" text="#">
       <formula>LEFT(A129,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130">
-    <cfRule type="containsText" dxfId="201" priority="133" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="205" priority="135" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A130)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="200" priority="134" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="204" priority="136" operator="beginsWith" text="#">
       <formula>LEFT(A130,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A242:A243">
-    <cfRule type="containsText" dxfId="199" priority="131" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="203" priority="133" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A242)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="198" priority="132" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="202" priority="134" operator="beginsWith" text="#">
       <formula>LEFT(A242,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A198">
-    <cfRule type="containsText" dxfId="197" priority="129" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="201" priority="131" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="196" priority="130" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="200" priority="132" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135">
-    <cfRule type="containsText" dxfId="195" priority="123" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="199" priority="125" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="194" priority="124" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="198" priority="126" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A244">
-    <cfRule type="containsText" dxfId="193" priority="121" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="197" priority="123" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A244)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="192" priority="122" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="196" priority="124" operator="beginsWith" text="#">
       <formula>LEFT(A244,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A240">
-    <cfRule type="containsText" dxfId="191" priority="117" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="195" priority="119" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A240)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="190" priority="118" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="194" priority="120" operator="beginsWith" text="#">
       <formula>LEFT(A240,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A247">
-    <cfRule type="containsText" dxfId="189" priority="115" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="193" priority="117" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A247)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="188" priority="116" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="192" priority="118" operator="beginsWith" text="#">
       <formula>LEFT(A247,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245">
-    <cfRule type="containsText" dxfId="187" priority="111" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="191" priority="113" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A245)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="186" priority="112" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="190" priority="114" operator="beginsWith" text="#">
       <formula>LEFT(A245,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A246">
-    <cfRule type="containsText" dxfId="185" priority="109" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="189" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A246)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="184" priority="110" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="188" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(A246,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A241">
-    <cfRule type="containsText" dxfId="183" priority="107" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="187" priority="109" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A241)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="182" priority="108" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="186" priority="110" operator="beginsWith" text="#">
       <formula>LEFT(A241,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A283">
-    <cfRule type="containsText" dxfId="181" priority="105" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="185" priority="107" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A283)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="180" priority="106" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="184" priority="108" operator="beginsWith" text="#">
       <formula>LEFT(A283,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A202">
-    <cfRule type="containsText" dxfId="179" priority="103" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="183" priority="105" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A202)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="178" priority="104" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="182" priority="106" operator="beginsWith" text="#">
       <formula>LEFT(A202,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A203">
-    <cfRule type="containsText" dxfId="177" priority="101" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="181" priority="103" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A203)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="176" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="180" priority="104" operator="beginsWith" text="#">
       <formula>LEFT(A203,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136">
-    <cfRule type="containsText" dxfId="175" priority="99" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="179" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="174" priority="100" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="178" priority="102" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137">
-    <cfRule type="containsText" dxfId="173" priority="97" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="177" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="172" priority="98" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="176" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A239">
-    <cfRule type="containsText" dxfId="171" priority="93" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="175" priority="95" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A239)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="170" priority="94" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="174" priority="96" operator="beginsWith" text="#">
       <formula>LEFT(A239,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A248">
-    <cfRule type="containsText" dxfId="169" priority="91" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="173" priority="93" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A248)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="168" priority="92" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="172" priority="94" operator="beginsWith" text="#">
       <formula>LEFT(A248,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A249">
-    <cfRule type="containsText" dxfId="167" priority="89" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="171" priority="91" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A249)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="166" priority="90" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="170" priority="92" operator="beginsWith" text="#">
       <formula>LEFT(A249,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A250">
-    <cfRule type="containsText" dxfId="165" priority="87" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="169" priority="89" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A250)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="164" priority="88" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="168" priority="90" operator="beginsWith" text="#">
       <formula>LEFT(A250,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A199:A201 A66:A67 A69">
-    <cfRule type="containsText" dxfId="163" priority="185" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="167" priority="187" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="162" priority="186" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="166" priority="188" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:A60">
-    <cfRule type="containsText" dxfId="161" priority="2113" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="165" priority="2115" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="160" priority="2114" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="164" priority="2116" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="159" priority="2225" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="163" priority="2227" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="158" priority="2226" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="162" priority="2228" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="containsText" dxfId="157" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="161" priority="87" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A68)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="156" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="160" priority="88" operator="beginsWith" text="#">
       <formula>LEFT(A68,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="containsText" dxfId="155" priority="75" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="159" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="154" priority="76" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="158" priority="78" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="containsText" dxfId="153" priority="71" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="157" priority="73" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A93)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="152" priority="72" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="156" priority="74" operator="beginsWith" text="#">
       <formula>LEFT(A93,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138">
-    <cfRule type="containsText" dxfId="151" priority="69" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="155" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="150" priority="70" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="154" priority="72" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A210">
-    <cfRule type="containsText" dxfId="149" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="153" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A210)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="148" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="152" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A210,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="containsText" dxfId="147" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="151" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A95)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="146" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="150" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A95,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A237">
-    <cfRule type="containsText" dxfId="145" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="149" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A237)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="144" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="148" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A237,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="containsText" dxfId="143" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="147" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A96)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="142" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="146" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A96,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="containsText" dxfId="141" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="145" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A97)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="140" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="144" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A97,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="containsText" dxfId="139" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="143" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A98)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="138" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="142" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A98,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="containsText" dxfId="137" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="141" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A99)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="136" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="140" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A99,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="containsText" dxfId="135" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="139" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A100)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="134" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="138" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A100,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A268">
-    <cfRule type="containsText" dxfId="133" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="137" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A268)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="132" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="136" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A268,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A269:A272">
-    <cfRule type="containsText" dxfId="131" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="135" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A269)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="130" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="134" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A269,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A113">
-    <cfRule type="containsText" dxfId="129" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="133" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A113)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="128" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="132" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A113,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A139">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45781,7 +45861,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="557" operator="containsText" text="......" id="{2740CB74-BF81-4E7E-8816-79D33A17FB72}">
+          <x14:cfRule type="containsText" priority="559" operator="containsText" text="......" id="{2740CB74-BF81-4E7E-8816-79D33A17FB72}">
             <xm:f>NOT(ISERROR(SEARCH("......",ElastoDyn!#REF!)))</xm:f>
             <x14:dxf>
               <font>
@@ -45790,7 +45870,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="558" operator="beginsWith" text="#" id="{3C7446DC-621E-41C0-8BDA-9CEAF8FB8B99}">
+          <x14:cfRule type="beginsWith" priority="560" operator="beginsWith" text="#" id="{3C7446DC-621E-41C0-8BDA-9CEAF8FB8B99}">
             <xm:f>LEFT(ElastoDyn!#REF!,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -45807,7 +45887,7 @@
           <xm:sqref>A168</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="179" operator="containsText" text="......" id="{45986398-BDBB-476E-B707-6E1702F9F4C3}">
+          <x14:cfRule type="containsText" priority="181" operator="containsText" text="......" id="{45986398-BDBB-476E-B707-6E1702F9F4C3}">
             <xm:f>NOT(ISERROR(SEARCH("......",ElastoDyn!#REF!)))</xm:f>
             <x14:dxf>
               <font>
@@ -45816,7 +45896,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="180" operator="beginsWith" text="#" id="{17FE44F8-569E-4B0A-84CB-2C9B419F47BC}">
+          <x14:cfRule type="beginsWith" priority="182" operator="beginsWith" text="#" id="{17FE44F8-569E-4B0A-84CB-2C9B419F47BC}">
             <xm:f>LEFT(ElastoDyn!#REF!,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -45833,7 +45913,7 @@
           <xm:sqref>A70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="177" operator="containsText" text="......" id="{FAD408D6-5A15-41F2-AF74-CCCC70BAEABE}">
+          <x14:cfRule type="containsText" priority="179" operator="containsText" text="......" id="{FAD408D6-5A15-41F2-AF74-CCCC70BAEABE}">
             <xm:f>NOT(ISERROR(SEARCH("......",ElastoDyn!#REF!)))</xm:f>
             <x14:dxf>
               <font>
@@ -45842,7 +45922,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="178" operator="beginsWith" text="#" id="{4E32124F-2922-4C24-9834-412E8E65D5FE}">
+          <x14:cfRule type="beginsWith" priority="180" operator="beginsWith" text="#" id="{4E32124F-2922-4C24-9834-412E8E65D5FE}">
             <xm:f>LEFT(ElastoDyn!#REF!,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -45859,7 +45939,7 @@
           <xm:sqref>A206</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="175" operator="containsText" text="......" id="{8F043A1C-8E80-49F6-BC48-5D97B0A79BA8}">
+          <x14:cfRule type="containsText" priority="177" operator="containsText" text="......" id="{8F043A1C-8E80-49F6-BC48-5D97B0A79BA8}">
             <xm:f>NOT(ISERROR(SEARCH("......",ElastoDyn!A180)))</xm:f>
             <x14:dxf>
               <font>
@@ -45868,7 +45948,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="176" operator="beginsWith" text="#" id="{AA404B8F-E7B1-4F0B-87EB-73313E57DE1F}">
+          <x14:cfRule type="beginsWith" priority="178" operator="beginsWith" text="#" id="{AA404B8F-E7B1-4F0B-87EB-73313E57DE1F}">
             <xm:f>LEFT(ElastoDyn!A180,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -45885,7 +45965,7 @@
           <xm:sqref>A208:A209</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="173" operator="containsText" text="......" id="{3AEF5FEB-1B08-4D05-A169-DF747818D30D}">
+          <x14:cfRule type="containsText" priority="175" operator="containsText" text="......" id="{3AEF5FEB-1B08-4D05-A169-DF747818D30D}">
             <xm:f>NOT(ISERROR(SEARCH("......",ElastoDyn!A178)))</xm:f>
             <x14:dxf>
               <font>
@@ -45894,7 +45974,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="174" operator="beginsWith" text="#" id="{8A127C95-F11B-4718-87B6-AFEBE091E974}">
+          <x14:cfRule type="beginsWith" priority="176" operator="beginsWith" text="#" id="{8A127C95-F11B-4718-87B6-AFEBE091E974}">
             <xm:f>LEFT(ElastoDyn!A178,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -45911,7 +45991,7 @@
           <xm:sqref>A211:A213 A207</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2411" operator="containsText" text="......" id="{3AEF5FEB-1B08-4D05-A169-DF747818D30D}">
+          <x14:cfRule type="containsText" priority="2413" operator="containsText" text="......" id="{3AEF5FEB-1B08-4D05-A169-DF747818D30D}">
             <xm:f>NOT(ISERROR(SEARCH("......",ElastoDyn!A207)))</xm:f>
             <x14:dxf>
               <font>
@@ -45920,7 +46000,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2412" operator="beginsWith" text="#" id="{8A127C95-F11B-4718-87B6-AFEBE091E974}">
+          <x14:cfRule type="beginsWith" priority="2414" operator="beginsWith" text="#" id="{8A127C95-F11B-4718-87B6-AFEBE091E974}">
             <xm:f>LEFT(ElastoDyn!A207,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -45937,7 +46017,7 @@
           <xm:sqref>A251:A253</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="41" operator="containsText" text="......" id="{1DD295AF-2F2B-4BC3-91EB-4FE7E936BCCB}">
+          <x14:cfRule type="containsText" priority="43" operator="containsText" text="......" id="{1DD295AF-2F2B-4BC3-91EB-4FE7E936BCCB}">
             <xm:f>NOT(ISERROR(SEARCH("......",ElastoDyn!B213)))</xm:f>
             <x14:dxf>
               <font>
@@ -45946,7 +46026,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="42" operator="beginsWith" text="#" id="{FF82794E-64B3-4F5D-9FD7-5316A3A54FC4}">
+          <x14:cfRule type="beginsWith" priority="44" operator="beginsWith" text="#" id="{FF82794E-64B3-4F5D-9FD7-5316A3A54FC4}">
             <xm:f>LEFT(ElastoDyn!B213,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -45963,7 +46043,7 @@
           <xm:sqref>B254:B266</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="51" operator="containsText" text="......" id="{3FA700AC-2A60-422E-8C8F-0D102D778139}">
+          <x14:cfRule type="containsText" priority="53" operator="containsText" text="......" id="{3FA700AC-2A60-422E-8C8F-0D102D778139}">
             <xm:f>NOT(ISERROR(SEARCH("......",ElastoDyn!A219)))</xm:f>
             <x14:dxf>
               <font>
@@ -45972,7 +46052,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="52" operator="beginsWith" text="#" id="{319FB54B-F448-4F54-B194-26089DA786F3}">
+          <x14:cfRule type="beginsWith" priority="54" operator="beginsWith" text="#" id="{319FB54B-F448-4F54-B194-26089DA786F3}">
             <xm:f>LEFT(ElastoDyn!A219,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -45989,7 +46069,7 @@
           <xm:sqref>A254:A266</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2455" operator="containsText" text="......" id="{3FA700AC-2A60-422E-8C8F-0D102D778139}">
+          <x14:cfRule type="containsText" priority="2457" operator="containsText" text="......" id="{3FA700AC-2A60-422E-8C8F-0D102D778139}">
             <xm:f>NOT(ISERROR(SEARCH("......",ElastoDyn!A75)))</xm:f>
             <x14:dxf>
               <font>
@@ -45998,7 +46078,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2456" operator="beginsWith" text="#" id="{319FB54B-F448-4F54-B194-26089DA786F3}">
+          <x14:cfRule type="beginsWith" priority="2458" operator="beginsWith" text="#" id="{319FB54B-F448-4F54-B194-26089DA786F3}">
             <xm:f>LEFT(ElastoDyn!A75,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -47266,266 +47346,266 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="109" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="113" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="108" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="112" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="containsText" dxfId="107" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="111" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A14)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="106" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="110" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(A14,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="105" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="109" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="104" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="108" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:A22">
-    <cfRule type="containsText" dxfId="103" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="107" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A19)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="102" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="106" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(A19,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="101" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="105" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="100" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="104" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="99" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="103" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="98" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="102" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="containsText" dxfId="97" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="101" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A23)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="100" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A23,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="containsText" dxfId="95" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="99" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A26)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="94" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="98" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(A26,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="containsText" dxfId="93" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="97" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A27)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="92" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="96" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(A27,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="containsText" dxfId="91" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="95" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A29)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="90" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="94" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A29,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="containsText" dxfId="89" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="93" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A28)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="92" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A28,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="containsText" dxfId="87" priority="43" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="91" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A30)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="86" priority="44" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="90" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A30,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="containsText" dxfId="85" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="89" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A31)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="84" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="88" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(A31,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="containsText" dxfId="83" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="87" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A32)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="82" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="86" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A32,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="containsText" dxfId="81" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="85" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A33)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="80" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="84" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A33,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="containsText" dxfId="79" priority="35" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="83" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A34)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="78" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="82" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A34,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="containsText" dxfId="77" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="81" priority="33" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A35)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="76" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="80" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(A35,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="containsText" dxfId="75" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="79" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A36)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="74" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="78" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(A36,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="containsText" dxfId="73" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="77" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A37)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="72" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="76" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A37,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="containsText" dxfId="71" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="75" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A38)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="70" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="74" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A38,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="containsText" dxfId="69" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="73" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A39)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="68" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="72" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A39,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="containsText" dxfId="67" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="71" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A40)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="66" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="70" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A40,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="containsText" dxfId="65" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="69" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A41)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="64" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="68" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A41,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="containsText" dxfId="63" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="67" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A42)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="62" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="66" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A42,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="containsText" dxfId="61" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="65" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A43)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="60" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="64" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A43,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44">
-    <cfRule type="containsText" dxfId="59" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="63" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A44)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="62" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A44,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="containsText" dxfId="57" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="61" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A45)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="60" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A45,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="containsText" dxfId="55" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="59" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A46)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="58" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A46,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="containsText" dxfId="53" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A47)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="52" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="56" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A47,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48">
-    <cfRule type="containsText" dxfId="51" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="55" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A48)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="50" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="54" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A48,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50 A52:A53">
-    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="53" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A50)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="52" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A50,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">
-    <cfRule type="containsText" dxfId="47" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A54)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="50" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A54,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="containsText" dxfId="45" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="49" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A51)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="44" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="48" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A51,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47569,9 +47649,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56914,42 +56994,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A339:A341">
-    <cfRule type="containsText" dxfId="31" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="35" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A339)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="34" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A339,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A287">
-    <cfRule type="containsText" dxfId="25" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="29" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A287)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="28" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A287,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A294">
-    <cfRule type="containsText" dxfId="21" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="25" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A294)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="24" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A294,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A297">
-    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A297)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="22" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A297,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A301">
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="21" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A301)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="20" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A301,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
changed wording from "File last changed" to "File last committed" to clarify what the date was.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@509 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 18e2223588ab62605098403b3fac38cf46a03090
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="14880" windowHeight="7545" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="600" windowWidth="14880" windowHeight="7545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="2" r:id="rId1"/>
@@ -5686,13 +5686,13 @@
     <t>"For AeroDyn: motions of the tower"</t>
   </si>
   <si>
-    <t># File last changed: $Date$</t>
-  </si>
-  <si>
     <t># (File) Revision #: $Rev$</t>
   </si>
   <si>
     <t># URL: $HeadURL$</t>
+  </si>
+  <si>
+    <t># File last committed $Date$</t>
   </si>
 </sst>
 </file>
@@ -5880,7 +5880,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="582">
+  <dxfs count="580">
     <dxf>
       <font>
         <u val="none"/>
@@ -10761,19 +10761,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <u val="none"/>
       </font>
@@ -10808,10 +10795,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -11742,10 +11725,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="575" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="579" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="574" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="578" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11757,9 +11740,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K820"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD15"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11870,19 +11853,19 @@
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>1847</v>
+        <v>1849</v>
       </c>
       <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="I14" s="12"/>
     </row>
@@ -34595,1428 +34578,1436 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A244:A300 A506:A514 A316 A307 A536:A537 A642:A675 A519 A54 A23:A42 A691:A706 A686:A689 A708:A714 A680:A684 A490 A492:A496 A240:A242 A501:A504 A531 A821:A1048576 A771:A772 A330:A339 A358:A361 A372:A374 A385:A388 A551:A622 A411:A435 A437:A444 A483 A446:A479 A379:A382 A776:A777 A624:A640 A783:A785 A796:A797 A524:A529 A485:A488 A1:A14">
-    <cfRule type="containsText" dxfId="573" priority="841" operator="containsText" text="......">
+  <conditionalFormatting sqref="A244:A300 A506:A514 A316 A307 A536:A537 A642:A675 A519 A54 A23:A42 A691:A706 A686:A689 A708:A714 A680:A684 A490 A492:A496 A240:A242 A501:A504 A531 A821:A1048576 A771:A772 A330:A339 A358:A361 A372:A374 A385:A388 A551:A622 A411:A435 A437:A444 A483 A446:A479 A379:A382 A776:A777 A624:A640 A783:A785 A796:A797 A524:A529 A485:A488 A1:A11 A13:A14">
+    <cfRule type="containsText" dxfId="577" priority="843" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="572" priority="842" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="576" priority="844" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A243">
-    <cfRule type="containsText" dxfId="571" priority="829" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="575" priority="831" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A243)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="570" priority="830" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="574" priority="832" operator="beginsWith" text="#">
       <formula>LEFT(A243,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:A20">
-    <cfRule type="containsText" dxfId="569" priority="823" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="573" priority="825" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A18)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="568" priority="824" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="572" priority="826" operator="beginsWith" text="#">
       <formula>LEFT(A18,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:A56">
-    <cfRule type="containsText" dxfId="567" priority="819" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="571" priority="821" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A55)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="566" priority="820" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="570" priority="822" operator="beginsWith" text="#">
       <formula>LEFT(A55,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A17">
-    <cfRule type="containsText" dxfId="565" priority="817" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="569" priority="819" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="564" priority="818" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="568" priority="820" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A533">
-    <cfRule type="containsText" dxfId="563" priority="813" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="567" priority="815" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A533)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="562" priority="814" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="566" priority="816" operator="beginsWith" text="#">
       <formula>LEFT(A533,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A532">
-    <cfRule type="containsText" dxfId="561" priority="815" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="565" priority="817" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A532)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="560" priority="816" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="564" priority="818" operator="beginsWith" text="#">
       <formula>LEFT(A532,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A545">
-    <cfRule type="containsText" dxfId="559" priority="811" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="563" priority="813" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A545)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="558" priority="812" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="562" priority="814" operator="beginsWith" text="#">
       <formula>LEFT(A545,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A546">
-    <cfRule type="containsText" dxfId="557" priority="809" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="561" priority="811" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A546)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="556" priority="810" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="560" priority="812" operator="beginsWith" text="#">
       <formula>LEFT(A546,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A543">
-    <cfRule type="containsText" dxfId="555" priority="807" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="559" priority="809" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A543)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="554" priority="808" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="558" priority="810" operator="beginsWith" text="#">
       <formula>LEFT(A543,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A544">
-    <cfRule type="containsText" dxfId="553" priority="805" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="557" priority="807" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A544)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="552" priority="806" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="556" priority="808" operator="beginsWith" text="#">
       <formula>LEFT(A544,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A547">
-    <cfRule type="containsText" dxfId="551" priority="801" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="555" priority="803" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A547)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="550" priority="802" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="554" priority="804" operator="beginsWith" text="#">
       <formula>LEFT(A547,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A505">
-    <cfRule type="containsText" dxfId="549" priority="797" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="553" priority="799" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A505)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="548" priority="798" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="552" priority="800" operator="beginsWith" text="#">
       <formula>LEFT(A505,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A534">
-    <cfRule type="containsText" dxfId="547" priority="795" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="551" priority="797" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A534)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="546" priority="796" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="550" priority="798" operator="beginsWith" text="#">
       <formula>LEFT(A534,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A548">
-    <cfRule type="containsText" dxfId="545" priority="793" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="549" priority="795" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A548)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="544" priority="794" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="548" priority="796" operator="beginsWith" text="#">
       <formula>LEFT(A548,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A641">
-    <cfRule type="containsText" dxfId="543" priority="791" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="547" priority="793" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A641)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="542" priority="792" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="546" priority="794" operator="beginsWith" text="#">
       <formula>LEFT(A641,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A535">
-    <cfRule type="containsText" dxfId="541" priority="785" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="545" priority="787" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A535)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="540" priority="786" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="544" priority="788" operator="beginsWith" text="#">
       <formula>LEFT(A535,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A301:A303">
-    <cfRule type="containsText" dxfId="539" priority="783" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="543" priority="785" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A301)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="538" priority="784" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="542" priority="786" operator="beginsWith" text="#">
       <formula>LEFT(A301,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A304">
-    <cfRule type="containsText" dxfId="537" priority="779" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="541" priority="781" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A304)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="536" priority="780" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="540" priority="782" operator="beginsWith" text="#">
       <formula>LEFT(A304,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A305:A306 A308:A313">
-    <cfRule type="containsText" dxfId="535" priority="777" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="539" priority="779" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A305)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="534" priority="778" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="538" priority="780" operator="beginsWith" text="#">
       <formula>LEFT(A305,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A314:A315 A317:A323 A539">
-    <cfRule type="containsText" dxfId="533" priority="775" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="537" priority="777" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A314)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="532" priority="776" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="536" priority="778" operator="beginsWith" text="#">
       <formula>LEFT(A314,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A538">
-    <cfRule type="containsText" dxfId="531" priority="731" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="535" priority="733" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A538)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="530" priority="732" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="534" priority="734" operator="beginsWith" text="#">
       <formula>LEFT(A538,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A325">
-    <cfRule type="containsText" dxfId="529" priority="719" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="533" priority="721" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A325)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="528" priority="720" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="532" priority="722" operator="beginsWith" text="#">
       <formula>LEFT(A325,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A324">
-    <cfRule type="containsText" dxfId="527" priority="721" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="531" priority="723" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A324)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="526" priority="722" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="530" priority="724" operator="beginsWith" text="#">
       <formula>LEFT(A324,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A540">
-    <cfRule type="containsText" dxfId="525" priority="717" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="529" priority="719" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A540)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="524" priority="718" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="528" priority="720" operator="beginsWith" text="#">
       <formula>LEFT(A540,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A541">
-    <cfRule type="containsText" dxfId="523" priority="715" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="527" priority="717" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A541)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="522" priority="716" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="526" priority="718" operator="beginsWith" text="#">
       <formula>LEFT(A541,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A326:A327">
-    <cfRule type="containsText" dxfId="521" priority="713" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="525" priority="715" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A326)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="520" priority="714" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="524" priority="716" operator="beginsWith" text="#">
       <formula>LEFT(A326,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A550">
-    <cfRule type="containsText" dxfId="519" priority="705" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="523" priority="707" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A550)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="518" priority="706" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="522" priority="708" operator="beginsWith" text="#">
       <formula>LEFT(A550,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A549">
-    <cfRule type="containsText" dxfId="517" priority="707" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="521" priority="709" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A549)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="516" priority="708" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="520" priority="710" operator="beginsWith" text="#">
       <formula>LEFT(A549,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A677">
-    <cfRule type="containsText" dxfId="515" priority="675" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="519" priority="677" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A677)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="514" priority="676" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="518" priority="678" operator="beginsWith" text="#">
       <formula>LEFT(A677,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A328:A329 A363">
-    <cfRule type="containsText" dxfId="513" priority="671" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="517" priority="673" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A328)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="512" priority="672" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="516" priority="674" operator="beginsWith" text="#">
       <formula>LEFT(A328,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A384">
-    <cfRule type="containsText" dxfId="511" priority="669" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="515" priority="671" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A384)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="510" priority="670" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="514" priority="672" operator="beginsWith" text="#">
       <formula>LEFT(A384,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A515:A516">
-    <cfRule type="containsText" dxfId="509" priority="665" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="513" priority="667" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A515)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="508" priority="666" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="512" priority="668" operator="beginsWith" text="#">
       <formula>LEFT(A515,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A518">
-    <cfRule type="containsText" dxfId="507" priority="663" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="511" priority="665" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A518)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="506" priority="664" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="510" priority="666" operator="beginsWith" text="#">
       <formula>LEFT(A518,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="containsText" dxfId="505" priority="637" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="509" priority="639" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A21)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="504" priority="638" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="508" priority="640" operator="beginsWith" text="#">
       <formula>LEFT(A21,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="containsText" dxfId="503" priority="635" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="507" priority="637" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A22)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="502" priority="636" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="506" priority="638" operator="beginsWith" text="#">
       <formula>LEFT(A22,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="containsText" dxfId="501" priority="627" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="505" priority="629" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A43)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="500" priority="628" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="504" priority="630" operator="beginsWith" text="#">
       <formula>LEFT(A43,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44">
-    <cfRule type="containsText" dxfId="499" priority="625" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="503" priority="627" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A44)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="498" priority="626" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="502" priority="628" operator="beginsWith" text="#">
       <formula>LEFT(A44,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="containsText" dxfId="497" priority="623" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="501" priority="625" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A45)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="496" priority="624" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="500" priority="626" operator="beginsWith" text="#">
       <formula>LEFT(A45,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="containsText" dxfId="495" priority="621" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="499" priority="623" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A46)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="494" priority="622" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="498" priority="624" operator="beginsWith" text="#">
       <formula>LEFT(A46,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A715">
-    <cfRule type="containsText" dxfId="493" priority="619" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="497" priority="621" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A715)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="492" priority="620" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="496" priority="622" operator="beginsWith" text="#">
       <formula>LEFT(A715,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A716">
-    <cfRule type="containsText" dxfId="491" priority="617" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="495" priority="619" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A716)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="490" priority="618" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="494" priority="620" operator="beginsWith" text="#">
       <formula>LEFT(A716,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A717">
-    <cfRule type="containsText" dxfId="489" priority="615" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="493" priority="617" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A717)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="488" priority="616" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="492" priority="618" operator="beginsWith" text="#">
       <formula>LEFT(A717,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A770">
-    <cfRule type="containsText" dxfId="487" priority="613" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="491" priority="615" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A770)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="486" priority="614" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="490" priority="616" operator="beginsWith" text="#">
       <formula>LEFT(A770,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A719:A722">
-    <cfRule type="containsText" dxfId="485" priority="609" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="489" priority="611" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A719)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="484" priority="610" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="488" priority="612" operator="beginsWith" text="#">
       <formula>LEFT(A719,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A718">
-    <cfRule type="containsText" dxfId="483" priority="605" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="487" priority="607" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A718)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="482" priority="606" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="486" priority="608" operator="beginsWith" text="#">
       <formula>LEFT(A718,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A723:A730">
-    <cfRule type="containsText" dxfId="481" priority="599" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="485" priority="601" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A723)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="480" priority="600" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="484" priority="602" operator="beginsWith" text="#">
       <formula>LEFT(A723,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A731:A741">
-    <cfRule type="containsText" dxfId="479" priority="593" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="483" priority="595" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A731)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="478" priority="594" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="482" priority="596" operator="beginsWith" text="#">
       <formula>LEFT(A731,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A742">
-    <cfRule type="containsText" dxfId="477" priority="595" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="481" priority="597" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A742)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="476" priority="596" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="480" priority="598" operator="beginsWith" text="#">
       <formula>LEFT(A742,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A743:A753">
-    <cfRule type="containsText" dxfId="475" priority="587" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="479" priority="589" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A743)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="474" priority="588" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="478" priority="590" operator="beginsWith" text="#">
       <formula>LEFT(A743,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A754">
-    <cfRule type="containsText" dxfId="473" priority="589" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="477" priority="591" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A754)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="472" priority="590" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="476" priority="592" operator="beginsWith" text="#">
       <formula>LEFT(A754,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A755">
-    <cfRule type="containsText" dxfId="471" priority="583" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="475" priority="585" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A755)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="470" priority="584" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="474" priority="586" operator="beginsWith" text="#">
       <formula>LEFT(A755,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A759:A760">
-    <cfRule type="containsText" dxfId="469" priority="573" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="473" priority="575" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A759)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="468" priority="574" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="472" priority="576" operator="beginsWith" text="#">
       <formula>LEFT(A759,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A756">
-    <cfRule type="containsText" dxfId="467" priority="579" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="471" priority="581" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A756)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="466" priority="580" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="470" priority="582" operator="beginsWith" text="#">
       <formula>LEFT(A756,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A757">
-    <cfRule type="containsText" dxfId="465" priority="577" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="469" priority="579" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A757)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="464" priority="578" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="468" priority="580" operator="beginsWith" text="#">
       <formula>LEFT(A757,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A758">
-    <cfRule type="containsText" dxfId="463" priority="575" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="467" priority="577" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A758)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="462" priority="576" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="466" priority="578" operator="beginsWith" text="#">
       <formula>LEFT(A758,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A761:A762">
-    <cfRule type="containsText" dxfId="461" priority="569" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="465" priority="571" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A761)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="460" priority="570" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="464" priority="572" operator="beginsWith" text="#">
       <formula>LEFT(A761,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A763">
-    <cfRule type="containsText" dxfId="459" priority="559" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="463" priority="561" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A763)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="458" priority="560" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="462" priority="562" operator="beginsWith" text="#">
       <formula>LEFT(A763,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A542">
-    <cfRule type="containsText" dxfId="457" priority="555" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="461" priority="557" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A542)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="456" priority="556" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="460" priority="558" operator="beginsWith" text="#">
       <formula>LEFT(A542,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A676">
-    <cfRule type="containsText" dxfId="455" priority="525" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="459" priority="527" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A676)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="454" priority="526" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="458" priority="528" operator="beginsWith" text="#">
       <formula>LEFT(A676,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48">
-    <cfRule type="containsText" dxfId="453" priority="523" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="457" priority="525" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A48)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="452" priority="524" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="456" priority="526" operator="beginsWith" text="#">
       <formula>LEFT(A48,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="containsText" dxfId="451" priority="521" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="455" priority="523" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A49)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="450" priority="522" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="454" priority="524" operator="beginsWith" text="#">
       <formula>LEFT(A49,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:A52">
-    <cfRule type="containsText" dxfId="449" priority="519" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="453" priority="521" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A50)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="448" priority="520" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="452" priority="522" operator="beginsWith" text="#">
       <formula>LEFT(A50,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A707">
-    <cfRule type="containsText" dxfId="447" priority="499" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="451" priority="501" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A707)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="446" priority="500" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="450" priority="502" operator="beginsWith" text="#">
       <formula>LEFT(A707,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A679">
-    <cfRule type="containsText" dxfId="445" priority="505" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="449" priority="507" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A679)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="444" priority="506" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="448" priority="508" operator="beginsWith" text="#">
       <formula>LEFT(A679,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A685">
-    <cfRule type="containsText" dxfId="443" priority="501" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="447" priority="503" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A685)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="442" priority="502" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="446" priority="504" operator="beginsWith" text="#">
       <formula>LEFT(A685,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A690">
-    <cfRule type="containsText" dxfId="441" priority="497" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="445" priority="499" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A690)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="440" priority="498" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="444" priority="500" operator="beginsWith" text="#">
       <formula>LEFT(A690,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A489">
-    <cfRule type="containsText" dxfId="439" priority="495" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="443" priority="497" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A489)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="438" priority="496" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="442" priority="498" operator="beginsWith" text="#">
       <formula>LEFT(A489,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A491">
-    <cfRule type="containsText" dxfId="437" priority="485" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="441" priority="487" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A491)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="436" priority="486" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="440" priority="488" operator="beginsWith" text="#">
       <formula>LEFT(A491,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A764">
-    <cfRule type="containsText" dxfId="435" priority="483" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="439" priority="485" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A764)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="434" priority="484" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="438" priority="486" operator="beginsWith" text="#">
       <formula>LEFT(A764,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93 A103:A105">
-    <cfRule type="containsText" dxfId="433" priority="293" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="437" priority="295" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="432" priority="294" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="436" priority="296" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A115">
-    <cfRule type="containsText" dxfId="431" priority="297" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="435" priority="299" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="430" priority="298" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="434" priority="300" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A129 A116">
-    <cfRule type="containsText" dxfId="429" priority="299" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="433" priority="301" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="428" priority="300" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="432" priority="302" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A134:A135 A131">
-    <cfRule type="containsText" dxfId="427" priority="301" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="431" priority="303" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="426" priority="302" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="430" priority="304" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130">
-    <cfRule type="containsText" dxfId="425" priority="303" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="429" priority="305" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="424" priority="304" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="428" priority="306" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A133">
-    <cfRule type="containsText" dxfId="423" priority="305" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="427" priority="307" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="422" priority="306" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="426" priority="308" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136">
-    <cfRule type="containsText" dxfId="421" priority="307" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="425" priority="309" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="420" priority="308" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="424" priority="310" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132">
-    <cfRule type="containsText" dxfId="419" priority="309" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="423" priority="311" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="418" priority="310" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="422" priority="312" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A140">
-    <cfRule type="containsText" dxfId="417" priority="311" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="421" priority="313" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="416" priority="312" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="420" priority="314" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A139 A150">
-    <cfRule type="containsText" dxfId="415" priority="313" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="419" priority="315" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="414" priority="314" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="418" priority="316" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152">
-    <cfRule type="containsText" dxfId="413" priority="315" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="417" priority="317" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="412" priority="316" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="416" priority="318" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A154">
-    <cfRule type="containsText" dxfId="411" priority="317" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="415" priority="319" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="410" priority="318" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="414" priority="320" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A497">
-    <cfRule type="containsText" dxfId="409" priority="239" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="413" priority="241" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A497)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="408" priority="240" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="412" priority="242" operator="beginsWith" text="#">
       <formula>LEFT(A497,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A498">
-    <cfRule type="containsText" dxfId="407" priority="237" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="411" priority="239" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A498)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="406" priority="238" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="410" priority="240" operator="beginsWith" text="#">
       <formula>LEFT(A498,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A530">
-    <cfRule type="containsText" dxfId="405" priority="235" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="409" priority="237" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A530)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="404" priority="236" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="408" priority="238" operator="beginsWith" text="#">
       <formula>LEFT(A530,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A779">
-    <cfRule type="containsText" dxfId="403" priority="233" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="407" priority="235" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A779)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="402" priority="234" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="406" priority="236" operator="beginsWith" text="#">
       <formula>LEFT(A779,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88:A89">
-    <cfRule type="containsText" dxfId="401" priority="1425" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="405" priority="1427" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="400" priority="1426" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="404" priority="1428" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A798">
-    <cfRule type="containsText" dxfId="399" priority="225" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="403" priority="227" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A798)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="398" priority="226" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="402" priority="228" operator="beginsWith" text="#">
       <formula>LEFT(A798,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A800">
-    <cfRule type="containsText" dxfId="397" priority="221" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="401" priority="223" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A800)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="396" priority="222" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="400" priority="224" operator="beginsWith" text="#">
       <formula>LEFT(A800,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A799">
-    <cfRule type="containsText" dxfId="395" priority="223" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="399" priority="225" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A799)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="394" priority="224" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="398" priority="226" operator="beginsWith" text="#">
       <formula>LEFT(A799,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A802">
-    <cfRule type="containsText" dxfId="393" priority="219" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="397" priority="221" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A802)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="392" priority="220" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="396" priority="222" operator="beginsWith" text="#">
       <formula>LEFT(A802,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A803">
-    <cfRule type="containsText" dxfId="391" priority="203" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="395" priority="205" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A803)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="390" priority="204" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="394" priority="206" operator="beginsWith" text="#">
       <formula>LEFT(A803,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A678">
-    <cfRule type="containsText" dxfId="389" priority="199" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="393" priority="201" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A678)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="388" priority="200" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="392" priority="202" operator="beginsWith" text="#">
       <formula>LEFT(A678,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A342">
-    <cfRule type="containsText" dxfId="387" priority="189" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="391" priority="191" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A342)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="386" priority="190" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="390" priority="192" operator="beginsWith" text="#">
       <formula>LEFT(A342,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A340">
-    <cfRule type="containsText" dxfId="385" priority="193" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="389" priority="195" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A340)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="384" priority="194" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="388" priority="196" operator="beginsWith" text="#">
       <formula>LEFT(A340,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A341">
-    <cfRule type="containsText" dxfId="383" priority="191" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="387" priority="193" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A341)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="382" priority="192" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="386" priority="194" operator="beginsWith" text="#">
       <formula>LEFT(A341,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A343">
-    <cfRule type="containsText" dxfId="381" priority="187" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="385" priority="189" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A343)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="380" priority="188" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="384" priority="190" operator="beginsWith" text="#">
       <formula>LEFT(A343,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A344">
-    <cfRule type="containsText" dxfId="379" priority="185" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="383" priority="187" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A344)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="378" priority="186" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="382" priority="188" operator="beginsWith" text="#">
       <formula>LEFT(A344,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A345">
-    <cfRule type="containsText" dxfId="377" priority="183" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="381" priority="185" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A345)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="376" priority="184" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="380" priority="186" operator="beginsWith" text="#">
       <formula>LEFT(A345,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A346">
-    <cfRule type="containsText" dxfId="375" priority="181" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="379" priority="183" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A346)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="374" priority="182" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="378" priority="184" operator="beginsWith" text="#">
       <formula>LEFT(A346,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A347">
-    <cfRule type="containsText" dxfId="373" priority="179" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="377" priority="181" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A347)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="372" priority="180" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="376" priority="182" operator="beginsWith" text="#">
       <formula>LEFT(A347,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A348">
-    <cfRule type="containsText" dxfId="371" priority="177" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="375" priority="179" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A348)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="370" priority="178" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="374" priority="180" operator="beginsWith" text="#">
       <formula>LEFT(A348,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A350">
-    <cfRule type="containsText" dxfId="369" priority="173" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="373" priority="175" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A350)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="368" priority="174" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="372" priority="176" operator="beginsWith" text="#">
       <formula>LEFT(A350,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A351">
-    <cfRule type="containsText" dxfId="367" priority="171" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="371" priority="173" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A351)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="366" priority="172" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="370" priority="174" operator="beginsWith" text="#">
       <formula>LEFT(A351,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A352">
-    <cfRule type="containsText" dxfId="365" priority="169" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="369" priority="171" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A352)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="364" priority="170" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="368" priority="172" operator="beginsWith" text="#">
       <formula>LEFT(A352,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A353">
-    <cfRule type="containsText" dxfId="363" priority="167" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="367" priority="169" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A353)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="362" priority="168" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="366" priority="170" operator="beginsWith" text="#">
       <formula>LEFT(A353,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A354">
-    <cfRule type="containsText" dxfId="361" priority="165" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="365" priority="167" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A354)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="360" priority="166" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="364" priority="168" operator="beginsWith" text="#">
       <formula>LEFT(A354,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A355">
-    <cfRule type="containsText" dxfId="359" priority="163" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="363" priority="165" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A355)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="358" priority="164" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="362" priority="166" operator="beginsWith" text="#">
       <formula>LEFT(A355,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A356">
-    <cfRule type="containsText" dxfId="357" priority="161" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="361" priority="163" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A356)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="356" priority="162" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="360" priority="164" operator="beginsWith" text="#">
       <formula>LEFT(A356,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A364:A370">
-    <cfRule type="containsText" dxfId="355" priority="159" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="359" priority="161" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A364)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="354" priority="160" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="358" priority="162" operator="beginsWith" text="#">
       <formula>LEFT(A364,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A362">
-    <cfRule type="containsText" dxfId="353" priority="157" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="357" priority="159" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A362)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="352" priority="158" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="356" priority="160" operator="beginsWith" text="#">
       <formula>LEFT(A362,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A371 A375:A378">
-    <cfRule type="containsText" dxfId="351" priority="155" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="355" priority="157" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A371)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="350" priority="156" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="354" priority="158" operator="beginsWith" text="#">
       <formula>LEFT(A371,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A383">
-    <cfRule type="containsText" dxfId="349" priority="153" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="353" priority="155" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A383)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="348" priority="154" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="352" priority="156" operator="beginsWith" text="#">
       <formula>LEFT(A383,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A394">
-    <cfRule type="containsText" dxfId="347" priority="151" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="351" priority="153" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A394)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="346" priority="152" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="350" priority="154" operator="beginsWith" text="#">
       <formula>LEFT(A394,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A357">
-    <cfRule type="containsText" dxfId="345" priority="149" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="349" priority="151" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A357)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="344" priority="150" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="348" priority="152" operator="beginsWith" text="#">
       <formula>LEFT(A357,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A389">
-    <cfRule type="containsText" dxfId="343" priority="147" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="347" priority="149" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A389)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="342" priority="148" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="346" priority="150" operator="beginsWith" text="#">
       <formula>LEFT(A389,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A390">
-    <cfRule type="containsText" dxfId="341" priority="145" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="345" priority="147" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A390)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="340" priority="146" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="344" priority="148" operator="beginsWith" text="#">
       <formula>LEFT(A390,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A391">
-    <cfRule type="containsText" dxfId="339" priority="143" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="343" priority="145" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A391)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="338" priority="144" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="342" priority="146" operator="beginsWith" text="#">
       <formula>LEFT(A391,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A392">
-    <cfRule type="containsText" dxfId="337" priority="141" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="341" priority="143" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A392)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="336" priority="142" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="340" priority="144" operator="beginsWith" text="#">
       <formula>LEFT(A392,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A393">
-    <cfRule type="containsText" dxfId="335" priority="139" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="339" priority="141" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A393)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="334" priority="140" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="338" priority="142" operator="beginsWith" text="#">
       <formula>LEFT(A393,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A395">
-    <cfRule type="containsText" dxfId="333" priority="137" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="337" priority="139" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A395)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="332" priority="138" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="336" priority="140" operator="beginsWith" text="#">
       <formula>LEFT(A395,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A396">
-    <cfRule type="containsText" dxfId="331" priority="135" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="335" priority="137" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A396)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="330" priority="136" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="334" priority="138" operator="beginsWith" text="#">
       <formula>LEFT(A396,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A436">
-    <cfRule type="containsText" dxfId="329" priority="133" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="333" priority="135" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A436)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="328" priority="134" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="332" priority="136" operator="beginsWith" text="#">
       <formula>LEFT(A436,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A397">
-    <cfRule type="containsText" dxfId="327" priority="131" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="331" priority="133" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A397)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="326" priority="132" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="330" priority="134" operator="beginsWith" text="#">
       <formula>LEFT(A397,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A398:A405">
-    <cfRule type="containsText" dxfId="325" priority="129" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="329" priority="131" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A398)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="324" priority="130" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="328" priority="132" operator="beginsWith" text="#">
       <formula>LEFT(A398,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A409">
-    <cfRule type="containsText" dxfId="323" priority="119" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="327" priority="121" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A409)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="322" priority="120" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="326" priority="122" operator="beginsWith" text="#">
       <formula>LEFT(A409,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A407">
-    <cfRule type="containsText" dxfId="321" priority="125" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="325" priority="127" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A407)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="320" priority="126" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="324" priority="128" operator="beginsWith" text="#">
       <formula>LEFT(A407,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A406">
-    <cfRule type="containsText" dxfId="319" priority="123" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="323" priority="125" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A406)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="318" priority="124" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="322" priority="126" operator="beginsWith" text="#">
       <formula>LEFT(A406,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A408">
-    <cfRule type="containsText" dxfId="317" priority="121" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="321" priority="123" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A408)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="316" priority="122" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="320" priority="124" operator="beginsWith" text="#">
       <formula>LEFT(A408,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A410">
-    <cfRule type="containsText" dxfId="315" priority="117" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="319" priority="119" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A410)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="314" priority="118" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="318" priority="120" operator="beginsWith" text="#">
       <formula>LEFT(A410,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A765">
-    <cfRule type="containsText" dxfId="313" priority="111" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="317" priority="113" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A765)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="312" priority="112" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="316" priority="114" operator="beginsWith" text="#">
       <formula>LEFT(A765,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A766">
-    <cfRule type="containsText" dxfId="311" priority="109" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="315" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A766)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="310" priority="110" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="314" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(A766,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A349">
-    <cfRule type="containsText" dxfId="309" priority="107" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="313" priority="109" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A349)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="308" priority="108" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="312" priority="110" operator="beginsWith" text="#">
       <formula>LEFT(A349,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A480">
-    <cfRule type="containsText" dxfId="307" priority="105" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="311" priority="107" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A480)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="306" priority="106" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="310" priority="108" operator="beginsWith" text="#">
       <formula>LEFT(A480,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A481">
-    <cfRule type="containsText" dxfId="305" priority="103" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="309" priority="105" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A481)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="304" priority="104" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="308" priority="106" operator="beginsWith" text="#">
       <formula>LEFT(A481,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A482">
-    <cfRule type="containsText" dxfId="303" priority="101" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="307" priority="103" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A482)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="302" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="306" priority="104" operator="beginsWith" text="#">
       <formula>LEFT(A482,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A521">
-    <cfRule type="containsText" dxfId="301" priority="99" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="305" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A521)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="300" priority="100" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="304" priority="102" operator="beginsWith" text="#">
       <formula>LEFT(A521,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A517">
-    <cfRule type="containsText" dxfId="299" priority="97" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="303" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A517)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="298" priority="98" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="302" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(A517,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A804">
-    <cfRule type="containsText" dxfId="297" priority="93" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="301" priority="95" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A804)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="296" priority="94" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="300" priority="96" operator="beginsWith" text="#">
       <formula>LEFT(A804,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A767">
-    <cfRule type="containsText" dxfId="295" priority="89" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="299" priority="91" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A767)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="294" priority="90" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="298" priority="92" operator="beginsWith" text="#">
       <formula>LEFT(A767,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A239">
-    <cfRule type="containsText" dxfId="293" priority="87" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="297" priority="89" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A239)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="292" priority="88" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="296" priority="90" operator="beginsWith" text="#">
       <formula>LEFT(A239,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A805">
-    <cfRule type="containsText" dxfId="291" priority="77" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="295" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A805)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="290" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="294" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A805,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A157:A165 A167:A238">
-    <cfRule type="containsText" dxfId="289" priority="403" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="293" priority="405" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="288" priority="404" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="292" priority="406" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A151 A153 A143 A145:A149 A64 A66:A67 A70:A78 A80:A81 A85:A87 A57 A59:A62">
-    <cfRule type="containsText" dxfId="287" priority="291" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="291" priority="293" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="286" priority="292" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="290" priority="294" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="containsText" dxfId="285" priority="1439" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="289" priority="1441" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="284" priority="1440" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="288" priority="1442" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137:A138 A141 A117:A128 A100:A101 A92 A90 A94:A98">
-    <cfRule type="containsText" dxfId="283" priority="1721" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="287" priority="1723" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="282" priority="1722" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="286" priority="1724" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A112 A106:A107 A109:A110">
-    <cfRule type="containsText" dxfId="281" priority="1781" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="285" priority="1783" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="280" priority="1782" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="284" priority="1784" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="containsText" dxfId="279" priority="1843" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="283" priority="1845" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="278" priority="1844" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="282" priority="1846" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114">
-    <cfRule type="containsText" dxfId="277" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="281" priority="87" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="276" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="280" priority="88" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A113">
-    <cfRule type="containsText" dxfId="275" priority="83" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="279" priority="85" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="274" priority="84" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="278" priority="86" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A768">
-    <cfRule type="containsText" dxfId="273" priority="81" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="277" priority="83" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="272" priority="82" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="276" priority="84" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A769">
-    <cfRule type="containsText" dxfId="271" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="275" priority="81" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="270" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="274" priority="82" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A806">
-    <cfRule type="containsText" dxfId="269" priority="75" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="273" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A806)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="268" priority="76" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="272" priority="78" operator="beginsWith" text="#">
       <formula>LEFT(A806,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A807">
-    <cfRule type="containsText" dxfId="267" priority="73" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="271" priority="75" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A805)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="266" priority="74" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="270" priority="76" operator="beginsWith" text="#">
       <formula>LEFT(A805,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B812:B819">
-    <cfRule type="containsText" dxfId="265" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="269" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",B806)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="264" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="268" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(B806,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B808 B811">
-    <cfRule type="containsText" dxfId="263" priority="67" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="267" priority="69" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="262" priority="68" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="266" priority="70" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A808">
-    <cfRule type="containsText" dxfId="261" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="265" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A808)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="260" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="264" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(A808,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A809">
-    <cfRule type="containsText" dxfId="259" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="263" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A809)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="258" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="262" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A809,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B809">
-    <cfRule type="containsText" dxfId="257" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="261" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="256" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="260" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A810">
-    <cfRule type="containsText" dxfId="255" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="259" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A810)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="254" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="258" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(A810,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B810">
-    <cfRule type="containsText" dxfId="253" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="257" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="252" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="256" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A811:A819">
-    <cfRule type="containsText" dxfId="251" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="255" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A811)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="250" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="254" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A811,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B820">
-    <cfRule type="containsText" dxfId="249" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="253" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="248" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="252" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A820">
-    <cfRule type="containsText" dxfId="247" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="251" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A796)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="246" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="250" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(A796,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A787:A789 A795">
-    <cfRule type="containsText" dxfId="245" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="249" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A787)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="244" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="248" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A787,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A774">
-    <cfRule type="containsText" dxfId="243" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="247" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A774)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="242" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="246" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(A774,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A775">
-    <cfRule type="containsText" dxfId="241" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="245" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A775)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="240" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="244" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A775,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111">
-    <cfRule type="containsText" dxfId="239" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="243" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="238" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="242" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A623">
-    <cfRule type="containsText" dxfId="237" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="241" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="236" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="240" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A773">
-    <cfRule type="containsText" dxfId="235" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="239" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A773)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="234" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="238" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A773,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A786">
-    <cfRule type="containsText" dxfId="233" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="237" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A786)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="232" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="236" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A786,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A484">
-    <cfRule type="containsText" dxfId="231" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="235" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A484)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="230" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="234" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A484,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A790">
-    <cfRule type="containsText" dxfId="229" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="233" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A790)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="228" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="232" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A790,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A791">
-    <cfRule type="containsText" dxfId="227" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="231" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A791)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="226" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="230" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A791,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A792">
-    <cfRule type="containsText" dxfId="225" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="229" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A792)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="224" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="228" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A792,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A793">
-    <cfRule type="containsText" dxfId="223" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="227" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A793)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="222" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="226" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A793,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A794">
-    <cfRule type="containsText" dxfId="221" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="225" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A794)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="220" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="224" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A794,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="209" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="223" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="208" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="222" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="#">
+      <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36025,7 +36016,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="553" operator="containsText" text="......" id="{465F9812-1C00-47A7-97E2-89B77398E1B1}">
+          <x14:cfRule type="containsText" priority="555" operator="containsText" text="......" id="{465F9812-1C00-47A7-97E2-89B77398E1B1}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A811)))</xm:f>
             <x14:dxf>
               <font>
@@ -36034,7 +36025,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="554" operator="beginsWith" text="#" id="{900241AA-A787-44C0-BE12-6FDEB9E0011A}">
+          <x14:cfRule type="beginsWith" priority="556" operator="beginsWith" text="#" id="{900241AA-A787-44C0-BE12-6FDEB9E0011A}">
             <xm:f>LEFT(ServoDyn!A811,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36051,7 +36042,7 @@
           <xm:sqref>A781:A782</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="277" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
+          <x14:cfRule type="containsText" priority="279" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A182)))</xm:f>
             <x14:dxf>
               <font>
@@ -36060,7 +36051,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="278" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
+          <x14:cfRule type="beginsWith" priority="280" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
             <xm:f>LEFT(ServoDyn!A182,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36077,7 +36068,7 @@
           <xm:sqref>A520 A79</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="201" operator="containsText" text="......" id="{5A5F5B76-44F7-40B2-B037-173F2905189B}">
+          <x14:cfRule type="containsText" priority="203" operator="containsText" text="......" id="{5A5F5B76-44F7-40B2-B037-173F2905189B}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A817)))</xm:f>
             <x14:dxf>
               <font>
@@ -36086,7 +36077,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="202" operator="beginsWith" text="#" id="{804DB11F-C4AE-4232-8FBE-AF82706C5D95}">
+          <x14:cfRule type="beginsWith" priority="204" operator="beginsWith" text="#" id="{804DB11F-C4AE-4232-8FBE-AF82706C5D95}">
             <xm:f>LEFT(ServoDyn!A817,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36103,7 +36094,7 @@
           <xm:sqref>A801</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2325" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
+          <x14:cfRule type="containsText" priority="2327" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A601)))</xm:f>
             <x14:dxf>
               <font>
@@ -36112,7 +36103,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2326" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
+          <x14:cfRule type="beginsWith" priority="2328" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
             <xm:f>LEFT(ServoDyn!A601,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36129,7 +36120,7 @@
           <xm:sqref>A522:A523 A499:A500</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2359" operator="containsText" text="......" id="{5FD4013B-8363-458B-8AA3-B485798DA1C8}">
+          <x14:cfRule type="containsText" priority="2361" operator="containsText" text="......" id="{5FD4013B-8363-458B-8AA3-B485798DA1C8}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A807)))</xm:f>
             <x14:dxf>
               <font>
@@ -36138,7 +36129,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2360" operator="beginsWith" text="#" id="{5826827B-E3D9-4440-94B4-857DA3C7325E}">
+          <x14:cfRule type="beginsWith" priority="2362" operator="beginsWith" text="#" id="{5826827B-E3D9-4440-94B4-857DA3C7325E}">
             <xm:f>LEFT(ServoDyn!A807,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36164,9 +36155,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36277,19 +36268,19 @@
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>1847</v>
+        <v>1849</v>
       </c>
       <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="I14" s="12"/>
     </row>
@@ -43692,482 +43683,482 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A11 A21 A234:A238 A275:A280 A111:A115 A144:A170 A282:A284 A287 A289:A1048576 A173:A199 A134:A137 A104:A107 A117:A130 A16">
-    <cfRule type="containsText" dxfId="207" priority="307" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="211" priority="307" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="206" priority="308" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="210" priority="308" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="containsText" dxfId="205" priority="299" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="209" priority="299" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A20)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="204" priority="300" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="208" priority="300" operator="beginsWith" text="#">
       <formula>LEFT(A20,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="203" priority="297" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="207" priority="297" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="202" priority="298" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="206" priority="298" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A23">
-    <cfRule type="containsText" dxfId="201" priority="295" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="205" priority="295" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A22)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="200" priority="296" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="204" priority="296" operator="beginsWith" text="#">
       <formula>LEFT(A22,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:A19">
-    <cfRule type="containsText" dxfId="199" priority="293" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="203" priority="293" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A18)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="198" priority="294" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="202" priority="294" operator="beginsWith" text="#">
       <formula>LEFT(A18,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A207">
-    <cfRule type="containsText" dxfId="197" priority="221" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="201" priority="221" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A207)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="196" priority="222" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="200" priority="222" operator="beginsWith" text="#">
       <formula>LEFT(A207,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A172">
-    <cfRule type="containsText" dxfId="195" priority="211" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="199" priority="211" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A172)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="194" priority="212" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="198" priority="212" operator="beginsWith" text="#">
       <formula>LEFT(A172,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108">
-    <cfRule type="containsText" dxfId="193" priority="201" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="197" priority="201" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A108)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="192" priority="202" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="196" priority="202" operator="beginsWith" text="#">
       <formula>LEFT(A108,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A208">
-    <cfRule type="containsText" dxfId="191" priority="179" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="195" priority="179" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A208)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="190" priority="180" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="194" priority="180" operator="beginsWith" text="#">
       <formula>LEFT(A208,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A233">
-    <cfRule type="containsText" dxfId="189" priority="163" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="193" priority="163" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A233)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="188" priority="164" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="192" priority="164" operator="beginsWith" text="#">
       <formula>LEFT(A233,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="containsText" dxfId="187" priority="199" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="191" priority="199" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="186" priority="200" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="190" priority="200" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:A61">
-    <cfRule type="containsText" dxfId="185" priority="1107" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="189" priority="1107" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="184" priority="1108" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="188" priority="1108" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:A46">
-    <cfRule type="containsText" dxfId="183" priority="1157" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="187" priority="1157" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="182" priority="1158" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="186" priority="1158" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:A50">
-    <cfRule type="containsText" dxfId="181" priority="1327" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="185" priority="1327" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="180" priority="1328" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="184" priority="1328" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64:A66">
-    <cfRule type="containsText" dxfId="179" priority="1497" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="183" priority="1497" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="178" priority="1498" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="182" priority="1498" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A200">
-    <cfRule type="containsText" dxfId="177" priority="165" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="181" priority="165" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="176" priority="166" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="180" priority="166" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A281">
-    <cfRule type="containsText" dxfId="175" priority="157" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="179" priority="157" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A281)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="174" priority="158" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="178" priority="158" operator="beginsWith" text="#">
       <formula>LEFT(A281,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A240">
-    <cfRule type="containsText" dxfId="173" priority="147" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="177" priority="147" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A240)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="172" priority="148" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="176" priority="148" operator="beginsWith" text="#">
       <formula>LEFT(A240,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A269">
-    <cfRule type="containsText" dxfId="171" priority="149" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="175" priority="149" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A269)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="170" priority="150" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="174" priority="150" operator="beginsWith" text="#">
       <formula>LEFT(A269,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A131">
-    <cfRule type="containsText" dxfId="169" priority="145" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="173" priority="145" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A131)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="168" priority="146" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="172" priority="146" operator="beginsWith" text="#">
       <formula>LEFT(A131,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132">
-    <cfRule type="containsText" dxfId="167" priority="143" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="171" priority="143" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A132)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="166" priority="144" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="170" priority="144" operator="beginsWith" text="#">
       <formula>LEFT(A132,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A133">
-    <cfRule type="containsText" dxfId="165" priority="141" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="169" priority="141" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A133)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="164" priority="142" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="168" priority="142" operator="beginsWith" text="#">
       <formula>LEFT(A133,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A244:A245">
-    <cfRule type="containsText" dxfId="163" priority="139" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="167" priority="139" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A244)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="162" priority="140" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="166" priority="140" operator="beginsWith" text="#">
       <formula>LEFT(A244,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A201">
-    <cfRule type="containsText" dxfId="161" priority="137" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="165" priority="137" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="160" priority="138" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="164" priority="138" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138">
-    <cfRule type="containsText" dxfId="159" priority="131" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="163" priority="131" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="158" priority="132" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="162" priority="132" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A246">
-    <cfRule type="containsText" dxfId="157" priority="129" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="161" priority="129" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A246)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="156" priority="130" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="160" priority="130" operator="beginsWith" text="#">
       <formula>LEFT(A246,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A242">
-    <cfRule type="containsText" dxfId="155" priority="125" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="159" priority="125" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A242)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="154" priority="126" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="158" priority="126" operator="beginsWith" text="#">
       <formula>LEFT(A242,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A249">
-    <cfRule type="containsText" dxfId="153" priority="123" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="157" priority="123" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A249)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="152" priority="124" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="156" priority="124" operator="beginsWith" text="#">
       <formula>LEFT(A249,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A247">
-    <cfRule type="containsText" dxfId="151" priority="119" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="155" priority="119" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A247)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="150" priority="120" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="154" priority="120" operator="beginsWith" text="#">
       <formula>LEFT(A247,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A248">
-    <cfRule type="containsText" dxfId="149" priority="117" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="153" priority="117" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A248)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="148" priority="118" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="152" priority="118" operator="beginsWith" text="#">
       <formula>LEFT(A248,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A243">
-    <cfRule type="containsText" dxfId="147" priority="115" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="151" priority="115" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A243)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="146" priority="116" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="150" priority="116" operator="beginsWith" text="#">
       <formula>LEFT(A243,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A285">
-    <cfRule type="containsText" dxfId="145" priority="113" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="149" priority="113" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A285)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="144" priority="114" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="148" priority="114" operator="beginsWith" text="#">
       <formula>LEFT(A285,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A205">
-    <cfRule type="containsText" dxfId="143" priority="111" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="147" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A205)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="142" priority="112" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="146" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(A205,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A206">
-    <cfRule type="containsText" dxfId="141" priority="109" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="145" priority="109" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A206)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="140" priority="110" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="144" priority="110" operator="beginsWith" text="#">
       <formula>LEFT(A206,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A139">
-    <cfRule type="containsText" dxfId="139" priority="107" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="143" priority="107" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="138" priority="108" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="142" priority="108" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A140">
-    <cfRule type="containsText" dxfId="137" priority="105" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="141" priority="105" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="136" priority="106" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="140" priority="106" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A241">
-    <cfRule type="containsText" dxfId="135" priority="101" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="139" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A241)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="134" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="138" priority="102" operator="beginsWith" text="#">
       <formula>LEFT(A241,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A250">
-    <cfRule type="containsText" dxfId="133" priority="99" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="137" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A250)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="132" priority="100" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="136" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(A250,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A251">
-    <cfRule type="containsText" dxfId="131" priority="97" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="135" priority="97" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A251)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="130" priority="98" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="134" priority="98" operator="beginsWith" text="#">
       <formula>LEFT(A251,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A252">
-    <cfRule type="containsText" dxfId="129" priority="95" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="133" priority="95" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A252)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="128" priority="96" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="132" priority="96" operator="beginsWith" text="#">
       <formula>LEFT(A252,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A202:A204 A69:A70 A72">
-    <cfRule type="containsText" dxfId="127" priority="193" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="131" priority="193" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="126" priority="194" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="130" priority="194" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:A63">
-    <cfRule type="containsText" dxfId="125" priority="2121" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="129" priority="2121" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="124" priority="2122" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="128" priority="2122" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="containsText" dxfId="123" priority="2233" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="127" priority="2233" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="122" priority="2234" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="126" priority="2234" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71">
-    <cfRule type="containsText" dxfId="121" priority="93" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="125" priority="93" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A71)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="120" priority="94" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="124" priority="94" operator="beginsWith" text="#">
       <formula>LEFT(A71,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="containsText" dxfId="119" priority="83" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="123" priority="83" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="118" priority="84" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="122" priority="84" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="containsText" dxfId="117" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="121" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A96)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="116" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="120" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A96,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A141">
-    <cfRule type="containsText" dxfId="115" priority="77" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="119" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="114" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="118" priority="78" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A213">
-    <cfRule type="containsText" dxfId="113" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="117" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A213)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="112" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="116" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A213,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="containsText" dxfId="111" priority="35" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="115" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A98)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="110" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="114" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A98,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A239">
-    <cfRule type="containsText" dxfId="109" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="113" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A239)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="108" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="112" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A239,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="containsText" dxfId="107" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="111" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A99)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="106" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="110" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A99,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="containsText" dxfId="105" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="109" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A100)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="104" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="108" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A100,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="containsText" dxfId="103" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="107" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A101)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="102" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="106" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A101,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="containsText" dxfId="101" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="105" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A102)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="100" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="104" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A102,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="containsText" dxfId="99" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="103" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A103)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="98" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="102" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A103,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A270">
-    <cfRule type="containsText" dxfId="97" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="101" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A270)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="100" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A270,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A271:A274">
-    <cfRule type="containsText" dxfId="95" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="99" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A271)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="94" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="98" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A271,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116">
-    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="97" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A116)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="92" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="96" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A116,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142">
-    <cfRule type="containsText" dxfId="91" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="90" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="94" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A143">
-    <cfRule type="containsText" dxfId="89" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="93" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="92" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45686,266 +45677,266 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="71" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="66" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="70" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="containsText" dxfId="65" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="69" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A14)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="64" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="68" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(A14,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="63" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="67" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="62" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="66" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:A22">
-    <cfRule type="containsText" dxfId="61" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="65" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A19)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="60" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="64" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(A19,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="59" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="63" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="62" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="61" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="60" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A23)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="58" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A23,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="containsText" dxfId="53" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="57" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A26)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="52" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="56" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(A26,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="containsText" dxfId="51" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="55" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A27)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="50" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="54" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(A27,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="53" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A29)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="52" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A29,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="51" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A28)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="50" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A28,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="containsText" dxfId="45" priority="43" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="49" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A30)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="44" priority="44" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="48" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A30,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="47" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A31)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="46" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(A31,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="containsText" dxfId="41" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="45" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A32)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="44" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A32,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="43" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A33)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="42" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A33,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="41" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A34)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="40" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A34,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="39" priority="33" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A35)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="38" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(A35,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="37" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A36)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="32" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="36" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(A36,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="35" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A37)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="34" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A37,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A38)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="32" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A38,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A39)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="30" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A39,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="29" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A40)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="28" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A40,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A41)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="26" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A41,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A42)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="24" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A42,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A43)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="22" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A43,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44">
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A44)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="20" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A44,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A45)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="18" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A45,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A46)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="16" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A46,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A47)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="14" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A47,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A48)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="12" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A48,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50 A52:A53">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A50)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="10" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A50,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A54)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="8" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A54,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A51)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="6" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A51,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
+ updated source code: -- fixed some minor bugs in coupling & cleaned it up a little -- added options for doing option 1 before option 2 (may be a better option later, when ServoDyn and/or AeroDyn deal with output and states properly)
+ I changed CertTest input files 
-- use "default" time steps
-- added line in SubDyn input files to correspond to changes in the code
-- removed additional HD preload and ED platform mass in monopile (committed accidentally last time)


git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@662 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: a9507e289ba8eedcb6890116abcdcdd3a43e8d87
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="14880" windowHeight="7545" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="600" windowWidth="14880" windowHeight="7545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="2" r:id="rId1"/>
@@ -11150,8 +11150,8 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <pane ySplit="8" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11783,9 +11783,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K821"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B155" sqref="B155"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36261,7 +36261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="11" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
     </sheetView>

</xml_diff>

<commit_message>
+ added "ElastoDyn PtfmRefzt must not be negative for floating offshore systems" check in FAST + modified linear teeter-damper moment in ED, based on bug reported here: https://wind.nrel.gov/forum/wind/viewtopic.php?f=4&t=1073 + added limit to pitch angles coming out of DISCON*.DLLs (previously could have gone outside range if pitch rate was max or min rate for extended period of time) + Created 64-bit version executable & 64-bit versions of MAP dll and DISCON.dll + added getPSD.m functionality to PlotFASToutput.m + updated HD, SD, NWTC_Library dependencies
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@707 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 58c31082df36b5c3c17b3affb8c4a9c72c401f9e
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -5895,7 +5895,41 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="586">
+  <dxfs count="590">
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <u val="none"/>
@@ -11791,10 +11825,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="585" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="589" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="584" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="588" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11807,8 +11841,8 @@
   <dimension ref="A1:K822"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="A1:XFD1048576"/>
+      <pane ySplit="11" topLeftCell="A511" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A525" sqref="A525:XFD525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26255,35 +26289,35 @@
         <v>26</v>
       </c>
     </row>
-    <row r="525" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A525" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B525" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C525" s="5" t="s">
+    <row r="525" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A525" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B525" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C525" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D525" s="5" t="s">
+      <c r="D525" s="3" t="s">
         <v>1623</v>
       </c>
-      <c r="E525" s="5" t="s">
+      <c r="E525" s="3" t="s">
         <v>1770</v>
       </c>
-      <c r="F525" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G525" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H525" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I525" s="5" t="s">
+      <c r="F525" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G525" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H525" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I525" s="12" t="s">
         <v>1771</v>
       </c>
-      <c r="J525" s="5" t="s">
+      <c r="J525" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -34706,1443 +34740,1451 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A261:A317 A508:A516 A333 A324 A538:A539 A644:A677 A521 A71 A40:A59 A693:A708 A688:A691 A710:A716 A682:A686 A25:A26 A28:A32 A257:A259 A533 A823:A1048576 A773:A774 A347:A356 A375:A378 A389:A391 A402:A405 A553:A624 A428:A452 A455:A462 A501 A464:A497 A396:A399 A778:A779 A626:A642 A785:A787 A798:A799 A526:A531 A1:A11 A13:A14 A503:A506 A20:A23">
-    <cfRule type="containsText" dxfId="583" priority="845" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="587" priority="847" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="582" priority="846" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="586" priority="848" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A260">
-    <cfRule type="containsText" dxfId="581" priority="833" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="585" priority="835" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A260)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="580" priority="834" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="584" priority="836" operator="beginsWith" text="#">
       <formula>LEFT(A260,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:A19 A37">
-    <cfRule type="containsText" dxfId="579" priority="827" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="583" priority="829" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A18)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="578" priority="828" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="582" priority="830" operator="beginsWith" text="#">
       <formula>LEFT(A18,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:A73">
-    <cfRule type="containsText" dxfId="577" priority="823" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="581" priority="825" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A72)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="576" priority="824" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="580" priority="826" operator="beginsWith" text="#">
       <formula>LEFT(A72,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A17">
-    <cfRule type="containsText" dxfId="575" priority="821" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="579" priority="823" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="574" priority="822" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="578" priority="824" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A535">
-    <cfRule type="containsText" dxfId="573" priority="817" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="577" priority="819" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A535)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="572" priority="818" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="576" priority="820" operator="beginsWith" text="#">
       <formula>LEFT(A535,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A534">
-    <cfRule type="containsText" dxfId="571" priority="819" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="575" priority="821" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A534)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="570" priority="820" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="574" priority="822" operator="beginsWith" text="#">
       <formula>LEFT(A534,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A547">
-    <cfRule type="containsText" dxfId="569" priority="815" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="573" priority="817" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A547)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="568" priority="816" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="572" priority="818" operator="beginsWith" text="#">
       <formula>LEFT(A547,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A548">
-    <cfRule type="containsText" dxfId="567" priority="813" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="571" priority="815" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A548)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="566" priority="814" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="570" priority="816" operator="beginsWith" text="#">
       <formula>LEFT(A548,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A545">
-    <cfRule type="containsText" dxfId="565" priority="811" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="569" priority="813" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A545)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="564" priority="812" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="568" priority="814" operator="beginsWith" text="#">
       <formula>LEFT(A545,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A546">
-    <cfRule type="containsText" dxfId="563" priority="809" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="567" priority="811" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A546)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="562" priority="810" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="566" priority="812" operator="beginsWith" text="#">
       <formula>LEFT(A546,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A549">
-    <cfRule type="containsText" dxfId="561" priority="805" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="565" priority="807" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A549)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="560" priority="806" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="564" priority="808" operator="beginsWith" text="#">
       <formula>LEFT(A549,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A507">
-    <cfRule type="containsText" dxfId="559" priority="801" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="563" priority="803" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A507)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="558" priority="802" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="562" priority="804" operator="beginsWith" text="#">
       <formula>LEFT(A507,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A536">
-    <cfRule type="containsText" dxfId="557" priority="799" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="561" priority="801" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A536)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="556" priority="800" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="560" priority="802" operator="beginsWith" text="#">
       <formula>LEFT(A536,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A550">
-    <cfRule type="containsText" dxfId="555" priority="797" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="559" priority="799" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A550)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="554" priority="798" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="558" priority="800" operator="beginsWith" text="#">
       <formula>LEFT(A550,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A643">
-    <cfRule type="containsText" dxfId="553" priority="795" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="557" priority="797" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A643)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="552" priority="796" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="556" priority="798" operator="beginsWith" text="#">
       <formula>LEFT(A643,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A537">
-    <cfRule type="containsText" dxfId="551" priority="789" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="555" priority="791" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A537)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="550" priority="790" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="554" priority="792" operator="beginsWith" text="#">
       <formula>LEFT(A537,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A318:A320">
-    <cfRule type="containsText" dxfId="549" priority="787" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="553" priority="789" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A318)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="548" priority="788" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="552" priority="790" operator="beginsWith" text="#">
       <formula>LEFT(A318,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A321">
-    <cfRule type="containsText" dxfId="547" priority="783" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="551" priority="785" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A321)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="546" priority="784" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="550" priority="786" operator="beginsWith" text="#">
       <formula>LEFT(A321,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A322:A323 A325:A330">
-    <cfRule type="containsText" dxfId="545" priority="781" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="549" priority="783" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A322)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="544" priority="782" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="548" priority="784" operator="beginsWith" text="#">
       <formula>LEFT(A322,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A331:A332 A334:A340 A541">
-    <cfRule type="containsText" dxfId="543" priority="779" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="547" priority="781" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A331)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="542" priority="780" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="546" priority="782" operator="beginsWith" text="#">
       <formula>LEFT(A331,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A540">
-    <cfRule type="containsText" dxfId="541" priority="735" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="545" priority="737" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A540)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="540" priority="736" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="544" priority="738" operator="beginsWith" text="#">
       <formula>LEFT(A540,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A342">
-    <cfRule type="containsText" dxfId="539" priority="723" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="543" priority="725" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A342)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="538" priority="724" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="542" priority="726" operator="beginsWith" text="#">
       <formula>LEFT(A342,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A341">
-    <cfRule type="containsText" dxfId="537" priority="725" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="541" priority="727" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A341)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="536" priority="726" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="540" priority="728" operator="beginsWith" text="#">
       <formula>LEFT(A341,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A542">
-    <cfRule type="containsText" dxfId="535" priority="721" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="539" priority="723" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A542)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="534" priority="722" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="538" priority="724" operator="beginsWith" text="#">
       <formula>LEFT(A542,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A543">
-    <cfRule type="containsText" dxfId="533" priority="719" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="537" priority="721" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A543)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="532" priority="720" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="536" priority="722" operator="beginsWith" text="#">
       <formula>LEFT(A543,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A343:A344">
-    <cfRule type="containsText" dxfId="531" priority="717" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="535" priority="719" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A343)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="530" priority="718" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="534" priority="720" operator="beginsWith" text="#">
       <formula>LEFT(A343,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A552">
-    <cfRule type="containsText" dxfId="529" priority="709" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="533" priority="711" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A552)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="528" priority="710" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="532" priority="712" operator="beginsWith" text="#">
       <formula>LEFT(A552,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A551">
-    <cfRule type="containsText" dxfId="527" priority="711" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="531" priority="713" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A551)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="526" priority="712" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="530" priority="714" operator="beginsWith" text="#">
       <formula>LEFT(A551,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A679">
-    <cfRule type="containsText" dxfId="525" priority="679" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="529" priority="681" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A679)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="524" priority="680" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="528" priority="682" operator="beginsWith" text="#">
       <formula>LEFT(A679,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A345:A346 A380">
-    <cfRule type="containsText" dxfId="523" priority="675" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="527" priority="677" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A345)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="522" priority="676" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="526" priority="678" operator="beginsWith" text="#">
       <formula>LEFT(A345,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A401">
-    <cfRule type="containsText" dxfId="521" priority="673" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="525" priority="675" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A401)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="520" priority="674" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="524" priority="676" operator="beginsWith" text="#">
       <formula>LEFT(A401,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A517:A518">
-    <cfRule type="containsText" dxfId="519" priority="669" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="523" priority="671" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A517)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="518" priority="670" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="522" priority="672" operator="beginsWith" text="#">
       <formula>LEFT(A517,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A520">
-    <cfRule type="containsText" dxfId="517" priority="667" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="521" priority="669" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A520)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="516" priority="668" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="520" priority="670" operator="beginsWith" text="#">
       <formula>LEFT(A520,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="containsText" dxfId="515" priority="641" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="519" priority="643" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A38)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="514" priority="642" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="518" priority="644" operator="beginsWith" text="#">
       <formula>LEFT(A38,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="containsText" dxfId="513" priority="639" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="517" priority="641" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A39)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="512" priority="640" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="516" priority="642" operator="beginsWith" text="#">
       <formula>LEFT(A39,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="containsText" dxfId="511" priority="631" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="515" priority="633" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A60)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="510" priority="632" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="514" priority="634" operator="beginsWith" text="#">
       <formula>LEFT(A60,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="containsText" dxfId="509" priority="629" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="513" priority="631" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A61)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="508" priority="630" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="512" priority="632" operator="beginsWith" text="#">
       <formula>LEFT(A61,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="containsText" dxfId="507" priority="627" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="511" priority="629" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A62)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="506" priority="628" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="510" priority="630" operator="beginsWith" text="#">
       <formula>LEFT(A62,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63">
-    <cfRule type="containsText" dxfId="505" priority="625" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="509" priority="627" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A63)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="504" priority="626" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="508" priority="628" operator="beginsWith" text="#">
       <formula>LEFT(A63,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A717">
-    <cfRule type="containsText" dxfId="503" priority="623" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="507" priority="625" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A717)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="502" priority="624" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="506" priority="626" operator="beginsWith" text="#">
       <formula>LEFT(A717,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A718">
-    <cfRule type="containsText" dxfId="501" priority="621" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="505" priority="623" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A718)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="500" priority="622" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="504" priority="624" operator="beginsWith" text="#">
       <formula>LEFT(A718,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A719">
-    <cfRule type="containsText" dxfId="499" priority="619" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="503" priority="621" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A719)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="498" priority="620" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="502" priority="622" operator="beginsWith" text="#">
       <formula>LEFT(A719,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A772">
-    <cfRule type="containsText" dxfId="497" priority="617" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="501" priority="619" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A772)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="496" priority="618" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="500" priority="620" operator="beginsWith" text="#">
       <formula>LEFT(A772,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A721:A724">
-    <cfRule type="containsText" dxfId="495" priority="613" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="499" priority="615" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A721)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="494" priority="614" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="498" priority="616" operator="beginsWith" text="#">
       <formula>LEFT(A721,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A720">
-    <cfRule type="containsText" dxfId="493" priority="609" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="497" priority="611" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A720)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="492" priority="610" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="496" priority="612" operator="beginsWith" text="#">
       <formula>LEFT(A720,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A725:A732">
-    <cfRule type="containsText" dxfId="491" priority="603" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="495" priority="605" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A725)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="490" priority="604" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="494" priority="606" operator="beginsWith" text="#">
       <formula>LEFT(A725,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A733:A743">
-    <cfRule type="containsText" dxfId="489" priority="597" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="493" priority="599" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A733)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="488" priority="598" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="492" priority="600" operator="beginsWith" text="#">
       <formula>LEFT(A733,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A744">
-    <cfRule type="containsText" dxfId="487" priority="599" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="491" priority="601" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A744)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="486" priority="600" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="490" priority="602" operator="beginsWith" text="#">
       <formula>LEFT(A744,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A745:A755">
-    <cfRule type="containsText" dxfId="485" priority="591" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="489" priority="593" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A745)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="484" priority="592" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="488" priority="594" operator="beginsWith" text="#">
       <formula>LEFT(A745,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A756">
-    <cfRule type="containsText" dxfId="483" priority="593" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="487" priority="595" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A756)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="482" priority="594" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="486" priority="596" operator="beginsWith" text="#">
       <formula>LEFT(A756,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A757">
-    <cfRule type="containsText" dxfId="481" priority="587" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="485" priority="589" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A757)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="480" priority="588" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="484" priority="590" operator="beginsWith" text="#">
       <formula>LEFT(A757,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A761:A762">
-    <cfRule type="containsText" dxfId="479" priority="577" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="483" priority="579" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A761)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="478" priority="578" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="482" priority="580" operator="beginsWith" text="#">
       <formula>LEFT(A761,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A758">
-    <cfRule type="containsText" dxfId="477" priority="583" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="481" priority="585" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A758)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="476" priority="584" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="480" priority="586" operator="beginsWith" text="#">
       <formula>LEFT(A758,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A759">
-    <cfRule type="containsText" dxfId="475" priority="581" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="479" priority="583" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A759)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="474" priority="582" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="478" priority="584" operator="beginsWith" text="#">
       <formula>LEFT(A759,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A760">
-    <cfRule type="containsText" dxfId="473" priority="579" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="477" priority="581" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A760)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="472" priority="580" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="476" priority="582" operator="beginsWith" text="#">
       <formula>LEFT(A760,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A763:A764">
-    <cfRule type="containsText" dxfId="471" priority="573" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="475" priority="575" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A763)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="470" priority="574" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="474" priority="576" operator="beginsWith" text="#">
       <formula>LEFT(A763,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A765">
-    <cfRule type="containsText" dxfId="469" priority="563" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="473" priority="565" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A765)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="468" priority="564" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="472" priority="566" operator="beginsWith" text="#">
       <formula>LEFT(A765,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A544">
-    <cfRule type="containsText" dxfId="467" priority="559" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="471" priority="561" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A544)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="466" priority="560" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="470" priority="562" operator="beginsWith" text="#">
       <formula>LEFT(A544,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A678">
-    <cfRule type="containsText" dxfId="465" priority="529" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="469" priority="531" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A678)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="464" priority="530" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="468" priority="532" operator="beginsWith" text="#">
       <formula>LEFT(A678,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="containsText" dxfId="463" priority="527" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="467" priority="529" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A65)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="462" priority="528" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="466" priority="530" operator="beginsWith" text="#">
       <formula>LEFT(A65,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="containsText" dxfId="461" priority="525" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="465" priority="527" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A66)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="460" priority="526" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="464" priority="528" operator="beginsWith" text="#">
       <formula>LEFT(A66,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67:A69">
-    <cfRule type="containsText" dxfId="459" priority="523" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="463" priority="525" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A67)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="458" priority="524" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="462" priority="526" operator="beginsWith" text="#">
       <formula>LEFT(A67,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A709">
-    <cfRule type="containsText" dxfId="457" priority="503" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="461" priority="505" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A709)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="456" priority="504" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="460" priority="506" operator="beginsWith" text="#">
       <formula>LEFT(A709,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A681">
-    <cfRule type="containsText" dxfId="455" priority="509" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="459" priority="511" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A681)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="454" priority="510" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="458" priority="512" operator="beginsWith" text="#">
       <formula>LEFT(A681,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A687">
-    <cfRule type="containsText" dxfId="453" priority="505" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="457" priority="507" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A687)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="452" priority="506" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="456" priority="508" operator="beginsWith" text="#">
       <formula>LEFT(A687,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A692">
-    <cfRule type="containsText" dxfId="451" priority="501" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="455" priority="503" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A692)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="450" priority="502" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="454" priority="504" operator="beginsWith" text="#">
       <formula>LEFT(A692,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="containsText" dxfId="449" priority="499" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="453" priority="501" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A24)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="448" priority="500" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="452" priority="502" operator="beginsWith" text="#">
       <formula>LEFT(A24,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="containsText" dxfId="447" priority="489" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="451" priority="491" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A27)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="446" priority="490" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="450" priority="492" operator="beginsWith" text="#">
       <formula>LEFT(A27,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A766">
-    <cfRule type="containsText" dxfId="445" priority="487" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="449" priority="489" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A766)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="444" priority="488" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="448" priority="490" operator="beginsWith" text="#">
       <formula>LEFT(A766,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110 A120:A122">
-    <cfRule type="containsText" dxfId="443" priority="297" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="447" priority="299" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="442" priority="298" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="446" priority="300" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132">
-    <cfRule type="containsText" dxfId="441" priority="301" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="445" priority="303" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="440" priority="302" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="444" priority="304" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A146 A133">
-    <cfRule type="containsText" dxfId="439" priority="303" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="443" priority="305" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="438" priority="304" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="442" priority="306" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A151:A152 A148">
-    <cfRule type="containsText" dxfId="437" priority="305" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="441" priority="307" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="436" priority="306" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="440" priority="308" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A147">
-    <cfRule type="containsText" dxfId="435" priority="307" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="439" priority="309" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="434" priority="308" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="438" priority="310" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A150">
-    <cfRule type="containsText" dxfId="433" priority="309" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="437" priority="311" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="432" priority="310" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="436" priority="312" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
-    <cfRule type="containsText" dxfId="431" priority="311" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="435" priority="313" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="430" priority="312" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="434" priority="314" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A149">
-    <cfRule type="containsText" dxfId="429" priority="313" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="433" priority="315" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="428" priority="314" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="432" priority="316" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A157">
-    <cfRule type="containsText" dxfId="427" priority="315" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="431" priority="317" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="426" priority="316" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="430" priority="318" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A156 A167">
-    <cfRule type="containsText" dxfId="425" priority="317" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="429" priority="319" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="424" priority="318" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="428" priority="320" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A169">
-    <cfRule type="containsText" dxfId="423" priority="319" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="427" priority="321" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="422" priority="320" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="426" priority="322" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A171">
-    <cfRule type="containsText" dxfId="421" priority="321" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="425" priority="323" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="420" priority="322" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="424" priority="324" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="containsText" dxfId="419" priority="243" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="423" priority="245" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A33)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="418" priority="244" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="422" priority="246" operator="beginsWith" text="#">
       <formula>LEFT(A33,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="containsText" dxfId="417" priority="241" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="421" priority="243" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A34)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="416" priority="242" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="420" priority="244" operator="beginsWith" text="#">
       <formula>LEFT(A34,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A532">
-    <cfRule type="containsText" dxfId="415" priority="239" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="419" priority="241" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A532)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="414" priority="240" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="418" priority="242" operator="beginsWith" text="#">
       <formula>LEFT(A532,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A781">
-    <cfRule type="containsText" dxfId="413" priority="237" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="417" priority="239" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A781)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="412" priority="238" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="416" priority="240" operator="beginsWith" text="#">
       <formula>LEFT(A781,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:A106">
-    <cfRule type="containsText" dxfId="411" priority="1429" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="415" priority="1431" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="410" priority="1430" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="414" priority="1432" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A800">
-    <cfRule type="containsText" dxfId="409" priority="229" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="413" priority="231" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A800)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="408" priority="230" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="412" priority="232" operator="beginsWith" text="#">
       <formula>LEFT(A800,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A802">
-    <cfRule type="containsText" dxfId="407" priority="225" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="411" priority="227" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A802)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="406" priority="226" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="410" priority="228" operator="beginsWith" text="#">
       <formula>LEFT(A802,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A801">
-    <cfRule type="containsText" dxfId="405" priority="227" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="409" priority="229" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A801)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="404" priority="228" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="408" priority="230" operator="beginsWith" text="#">
       <formula>LEFT(A801,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A804">
-    <cfRule type="containsText" dxfId="403" priority="223" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="407" priority="225" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A804)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="402" priority="224" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="406" priority="226" operator="beginsWith" text="#">
       <formula>LEFT(A804,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A805">
-    <cfRule type="containsText" dxfId="401" priority="207" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="405" priority="209" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A805)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="400" priority="208" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="404" priority="210" operator="beginsWith" text="#">
       <formula>LEFT(A805,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A680">
-    <cfRule type="containsText" dxfId="399" priority="203" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="403" priority="205" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A680)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="398" priority="204" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="402" priority="206" operator="beginsWith" text="#">
       <formula>LEFT(A680,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A359">
-    <cfRule type="containsText" dxfId="397" priority="193" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="401" priority="195" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A359)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="396" priority="194" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="400" priority="196" operator="beginsWith" text="#">
       <formula>LEFT(A359,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A357">
-    <cfRule type="containsText" dxfId="395" priority="197" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="399" priority="199" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A357)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="394" priority="198" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="398" priority="200" operator="beginsWith" text="#">
       <formula>LEFT(A357,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A358">
-    <cfRule type="containsText" dxfId="393" priority="195" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="397" priority="197" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A358)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="392" priority="196" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="396" priority="198" operator="beginsWith" text="#">
       <formula>LEFT(A358,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A360">
-    <cfRule type="containsText" dxfId="391" priority="191" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="395" priority="193" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A360)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="390" priority="192" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="394" priority="194" operator="beginsWith" text="#">
       <formula>LEFT(A360,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A361">
-    <cfRule type="containsText" dxfId="389" priority="189" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="393" priority="191" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A361)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="388" priority="190" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="392" priority="192" operator="beginsWith" text="#">
       <formula>LEFT(A361,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A362">
-    <cfRule type="containsText" dxfId="387" priority="187" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="391" priority="189" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A362)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="386" priority="188" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="390" priority="190" operator="beginsWith" text="#">
       <formula>LEFT(A362,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A363">
-    <cfRule type="containsText" dxfId="385" priority="185" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="389" priority="187" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A363)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="384" priority="186" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="388" priority="188" operator="beginsWith" text="#">
       <formula>LEFT(A363,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A364">
-    <cfRule type="containsText" dxfId="383" priority="183" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="387" priority="185" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A364)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="382" priority="184" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="386" priority="186" operator="beginsWith" text="#">
       <formula>LEFT(A364,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A365">
-    <cfRule type="containsText" dxfId="381" priority="181" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="385" priority="183" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A365)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="380" priority="182" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="384" priority="184" operator="beginsWith" text="#">
       <formula>LEFT(A365,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A367">
-    <cfRule type="containsText" dxfId="379" priority="177" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="383" priority="179" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A367)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="378" priority="178" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="382" priority="180" operator="beginsWith" text="#">
       <formula>LEFT(A367,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A368">
-    <cfRule type="containsText" dxfId="377" priority="175" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="381" priority="177" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A368)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="376" priority="176" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="380" priority="178" operator="beginsWith" text="#">
       <formula>LEFT(A368,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A369">
-    <cfRule type="containsText" dxfId="375" priority="173" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="379" priority="175" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A369)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="374" priority="174" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="378" priority="176" operator="beginsWith" text="#">
       <formula>LEFT(A369,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A370">
-    <cfRule type="containsText" dxfId="373" priority="171" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="377" priority="173" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A370)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="372" priority="172" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="376" priority="174" operator="beginsWith" text="#">
       <formula>LEFT(A370,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A371">
-    <cfRule type="containsText" dxfId="371" priority="169" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="375" priority="171" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A371)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="370" priority="170" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="374" priority="172" operator="beginsWith" text="#">
       <formula>LEFT(A371,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A372">
-    <cfRule type="containsText" dxfId="369" priority="167" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="373" priority="169" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A372)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="368" priority="168" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="372" priority="170" operator="beginsWith" text="#">
       <formula>LEFT(A372,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A373">
-    <cfRule type="containsText" dxfId="367" priority="165" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="371" priority="167" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A373)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="366" priority="166" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="370" priority="168" operator="beginsWith" text="#">
       <formula>LEFT(A373,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A381:A387">
-    <cfRule type="containsText" dxfId="365" priority="163" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="369" priority="165" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A381)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="364" priority="164" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="368" priority="166" operator="beginsWith" text="#">
       <formula>LEFT(A381,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A379">
-    <cfRule type="containsText" dxfId="363" priority="161" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="367" priority="163" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A379)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="362" priority="162" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="366" priority="164" operator="beginsWith" text="#">
       <formula>LEFT(A379,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A388 A392:A395">
-    <cfRule type="containsText" dxfId="361" priority="159" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="365" priority="161" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A388)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="360" priority="160" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="364" priority="162" operator="beginsWith" text="#">
       <formula>LEFT(A388,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A400">
-    <cfRule type="containsText" dxfId="359" priority="157" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="363" priority="159" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A400)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="358" priority="158" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="362" priority="160" operator="beginsWith" text="#">
       <formula>LEFT(A400,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A411">
-    <cfRule type="containsText" dxfId="357" priority="155" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="361" priority="157" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A411)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="356" priority="156" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="360" priority="158" operator="beginsWith" text="#">
       <formula>LEFT(A411,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A374">
-    <cfRule type="containsText" dxfId="355" priority="153" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="359" priority="155" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A374)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="354" priority="154" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="358" priority="156" operator="beginsWith" text="#">
       <formula>LEFT(A374,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A406">
-    <cfRule type="containsText" dxfId="353" priority="151" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="357" priority="153" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A406)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="352" priority="152" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="356" priority="154" operator="beginsWith" text="#">
       <formula>LEFT(A406,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A407">
-    <cfRule type="containsText" dxfId="351" priority="149" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="355" priority="151" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A407)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="350" priority="150" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="354" priority="152" operator="beginsWith" text="#">
       <formula>LEFT(A407,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A408">
-    <cfRule type="containsText" dxfId="349" priority="147" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="353" priority="149" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A408)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="348" priority="148" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="352" priority="150" operator="beginsWith" text="#">
       <formula>LEFT(A408,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A409">
-    <cfRule type="containsText" dxfId="347" priority="145" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="351" priority="147" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A409)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="346" priority="146" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="350" priority="148" operator="beginsWith" text="#">
       <formula>LEFT(A409,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A410">
-    <cfRule type="containsText" dxfId="345" priority="143" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="349" priority="145" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A410)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="344" priority="144" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="348" priority="146" operator="beginsWith" text="#">
       <formula>LEFT(A410,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A412">
-    <cfRule type="containsText" dxfId="343" priority="141" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="347" priority="143" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A412)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="342" priority="142" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="346" priority="144" operator="beginsWith" text="#">
       <formula>LEFT(A412,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A413">
-    <cfRule type="containsText" dxfId="341" priority="139" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="345" priority="141" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A413)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="340" priority="140" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="344" priority="142" operator="beginsWith" text="#">
       <formula>LEFT(A413,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A454">
-    <cfRule type="containsText" dxfId="339" priority="137" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="343" priority="139" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A454)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="338" priority="138" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="342" priority="140" operator="beginsWith" text="#">
       <formula>LEFT(A454,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A414">
-    <cfRule type="containsText" dxfId="337" priority="135" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="341" priority="137" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A414)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="336" priority="136" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="340" priority="138" operator="beginsWith" text="#">
       <formula>LEFT(A414,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A415:A422">
-    <cfRule type="containsText" dxfId="335" priority="133" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="339" priority="135" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A415)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="334" priority="134" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="338" priority="136" operator="beginsWith" text="#">
       <formula>LEFT(A415,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A426">
-    <cfRule type="containsText" dxfId="333" priority="123" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="337" priority="125" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A426)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="332" priority="124" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="336" priority="126" operator="beginsWith" text="#">
       <formula>LEFT(A426,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A424">
-    <cfRule type="containsText" dxfId="331" priority="129" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="335" priority="131" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A424)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="330" priority="130" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="334" priority="132" operator="beginsWith" text="#">
       <formula>LEFT(A424,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A423">
-    <cfRule type="containsText" dxfId="329" priority="127" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="333" priority="129" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A423)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="328" priority="128" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="332" priority="130" operator="beginsWith" text="#">
       <formula>LEFT(A423,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A425">
-    <cfRule type="containsText" dxfId="327" priority="125" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="331" priority="127" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A425)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="326" priority="126" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="330" priority="128" operator="beginsWith" text="#">
       <formula>LEFT(A425,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A427">
-    <cfRule type="containsText" dxfId="325" priority="121" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="329" priority="123" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A427)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="324" priority="122" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="328" priority="124" operator="beginsWith" text="#">
       <formula>LEFT(A427,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A767">
-    <cfRule type="containsText" dxfId="323" priority="115" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="327" priority="117" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A767)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="322" priority="116" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="326" priority="118" operator="beginsWith" text="#">
       <formula>LEFT(A767,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A768">
-    <cfRule type="containsText" dxfId="321" priority="113" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="325" priority="115" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A768)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="320" priority="114" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="324" priority="116" operator="beginsWith" text="#">
       <formula>LEFT(A768,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A366">
-    <cfRule type="containsText" dxfId="319" priority="111" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="323" priority="113" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A366)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="318" priority="112" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="322" priority="114" operator="beginsWith" text="#">
       <formula>LEFT(A366,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A498">
-    <cfRule type="containsText" dxfId="317" priority="109" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="321" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A498)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="316" priority="110" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="320" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(A498,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A499">
-    <cfRule type="containsText" dxfId="315" priority="107" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="319" priority="109" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A499)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="314" priority="108" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="318" priority="110" operator="beginsWith" text="#">
       <formula>LEFT(A499,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A500">
-    <cfRule type="containsText" dxfId="313" priority="105" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="317" priority="107" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A500)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="312" priority="106" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="316" priority="108" operator="beginsWith" text="#">
       <formula>LEFT(A500,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A523">
-    <cfRule type="containsText" dxfId="311" priority="103" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="315" priority="105" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A523)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="310" priority="104" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="314" priority="106" operator="beginsWith" text="#">
       <formula>LEFT(A523,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519">
-    <cfRule type="containsText" dxfId="309" priority="101" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="313" priority="103" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A519)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="308" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="312" priority="104" operator="beginsWith" text="#">
       <formula>LEFT(A519,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A806">
-    <cfRule type="containsText" dxfId="307" priority="97" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="311" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A806)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="306" priority="98" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="310" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(A806,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A769">
-    <cfRule type="containsText" dxfId="305" priority="93" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="309" priority="95" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A769)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="304" priority="94" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="308" priority="96" operator="beginsWith" text="#">
       <formula>LEFT(A769,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A256">
-    <cfRule type="containsText" dxfId="303" priority="91" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="307" priority="93" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A256)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="302" priority="92" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="306" priority="94" operator="beginsWith" text="#">
       <formula>LEFT(A256,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A807">
-    <cfRule type="containsText" dxfId="301" priority="81" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="305" priority="83" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A807)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="300" priority="82" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="304" priority="84" operator="beginsWith" text="#">
       <formula>LEFT(A807,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A174:A182 A184:A255">
-    <cfRule type="containsText" dxfId="299" priority="407" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="303" priority="409" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="298" priority="408" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="302" priority="410" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A168 A170 A160 A162:A166 A81 A83:A84 A87:A95 A97:A98 A102:A104 A74 A76:A79">
-    <cfRule type="containsText" dxfId="297" priority="295" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="301" priority="297" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="296" priority="296" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="300" priority="298" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116">
-    <cfRule type="containsText" dxfId="295" priority="1443" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="299" priority="1445" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="294" priority="1444" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="298" priority="1446" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A154:A155 A158 A134:A145 A117:A118 A109 A107 A111:A115">
-    <cfRule type="containsText" dxfId="293" priority="1725" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="297" priority="1727" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="292" priority="1726" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="296" priority="1728" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A129 A123:A124 A126:A127">
-    <cfRule type="containsText" dxfId="291" priority="1785" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="295" priority="1787" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="290" priority="1786" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="294" priority="1788" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A119">
-    <cfRule type="containsText" dxfId="289" priority="1847" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="293" priority="1849" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="288" priority="1848" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="292" priority="1850" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A131">
-    <cfRule type="containsText" dxfId="287" priority="89" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="291" priority="91" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="286" priority="90" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="290" priority="92" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130">
-    <cfRule type="containsText" dxfId="285" priority="87" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="289" priority="89" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="284" priority="88" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="288" priority="90" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A770">
-    <cfRule type="containsText" dxfId="283" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="287" priority="87" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="282" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="286" priority="88" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A771">
-    <cfRule type="containsText" dxfId="281" priority="83" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="285" priority="85" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="280" priority="84" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="284" priority="86" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A808">
-    <cfRule type="containsText" dxfId="279" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="283" priority="81" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A808)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="278" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="282" priority="82" operator="beginsWith" text="#">
       <formula>LEFT(A808,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A809">
-    <cfRule type="containsText" dxfId="277" priority="77" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="281" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A807)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="276" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="280" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A807,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B814:B821">
-    <cfRule type="containsText" dxfId="275" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="279" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",B808)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="274" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="278" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(B808,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B810 B813">
-    <cfRule type="containsText" dxfId="273" priority="71" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="277" priority="73" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="272" priority="72" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="276" priority="74" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A810">
-    <cfRule type="containsText" dxfId="271" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="275" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A810)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="270" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="274" priority="68" operator="beginsWith" text="#">
       <formula>LEFT(A810,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A811">
-    <cfRule type="containsText" dxfId="269" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="273" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A811)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="268" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="272" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A811,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B811">
-    <cfRule type="containsText" dxfId="267" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="271" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="266" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="270" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A812">
-    <cfRule type="containsText" dxfId="265" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="269" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A812)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="264" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="268" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A812,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B812">
-    <cfRule type="containsText" dxfId="263" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="267" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="262" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="266" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A813:A821">
-    <cfRule type="containsText" dxfId="261" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="265" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A813)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="260" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="264" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(A813,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B822">
-    <cfRule type="containsText" dxfId="259" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="263" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="258" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="262" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A822">
-    <cfRule type="containsText" dxfId="257" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="261" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A798)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="256" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="260" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A798,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A789:A791 A797">
-    <cfRule type="containsText" dxfId="255" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="259" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A789)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="254" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="258" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A789,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A776">
-    <cfRule type="containsText" dxfId="253" priority="43" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="257" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A776)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="252" priority="44" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="256" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A776,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A777">
-    <cfRule type="containsText" dxfId="251" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="255" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A777)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="250" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="254" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A777,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128">
-    <cfRule type="containsText" dxfId="249" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="253" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="248" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="252" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A625">
-    <cfRule type="containsText" dxfId="247" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="251" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="246" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="250" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A775">
-    <cfRule type="containsText" dxfId="245" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="249" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A775)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="244" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="248" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A775,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A788">
-    <cfRule type="containsText" dxfId="243" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="247" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A788)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="242" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="246" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A788,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A502">
-    <cfRule type="containsText" dxfId="241" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="245" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A502)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="240" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="244" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A502,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A792">
-    <cfRule type="containsText" dxfId="239" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="243" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A792)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="238" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="242" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A792,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A793">
-    <cfRule type="containsText" dxfId="237" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="241" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A793)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="236" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="240" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A793,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A794">
-    <cfRule type="containsText" dxfId="235" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="239" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A794)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="234" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="238" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A794,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A795">
-    <cfRule type="containsText" dxfId="233" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="237" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A795)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="232" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="236" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A795,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A796">
-    <cfRule type="containsText" dxfId="231" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="235" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A796)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="230" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="234" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A796,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="229" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="233" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="228" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="232" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="227" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="231" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="226" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="230" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A453">
-    <cfRule type="containsText" dxfId="225" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="229" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A453)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="224" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="228" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A453,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A525">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A525)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="#">
+      <formula>LEFT(A525,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36151,7 +36193,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="557" operator="containsText" text="......" id="{465F9812-1C00-47A7-97E2-89B77398E1B1}">
+          <x14:cfRule type="containsText" priority="559" operator="containsText" text="......" id="{465F9812-1C00-47A7-97E2-89B77398E1B1}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A812)))</xm:f>
             <x14:dxf>
               <font>
@@ -36160,7 +36202,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="558" operator="beginsWith" text="#" id="{900241AA-A787-44C0-BE12-6FDEB9E0011A}">
+          <x14:cfRule type="beginsWith" priority="560" operator="beginsWith" text="#" id="{900241AA-A787-44C0-BE12-6FDEB9E0011A}">
             <xm:f>LEFT(ServoDyn!A812,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36177,7 +36219,7 @@
           <xm:sqref>A783:A784</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="281" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
+          <x14:cfRule type="containsText" priority="283" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A624)))</xm:f>
             <x14:dxf>
               <font>
@@ -36186,7 +36228,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="282" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
+          <x14:cfRule type="beginsWith" priority="284" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
             <xm:f>LEFT(ServoDyn!A624,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36203,7 +36245,7 @@
           <xm:sqref>A522</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="205" operator="containsText" text="......" id="{5A5F5B76-44F7-40B2-B037-173F2905189B}">
+          <x14:cfRule type="containsText" priority="207" operator="containsText" text="......" id="{5A5F5B76-44F7-40B2-B037-173F2905189B}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A818)))</xm:f>
             <x14:dxf>
               <font>
@@ -36212,7 +36254,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="206" operator="beginsWith" text="#" id="{804DB11F-C4AE-4232-8FBE-AF82706C5D95}">
+          <x14:cfRule type="beginsWith" priority="208" operator="beginsWith" text="#" id="{804DB11F-C4AE-4232-8FBE-AF82706C5D95}">
             <xm:f>LEFT(ServoDyn!A818,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36229,7 +36271,7 @@
           <xm:sqref>A803</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2329" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
+          <x14:cfRule type="containsText" priority="2331" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A602)))</xm:f>
             <x14:dxf>
               <font>
@@ -36238,7 +36280,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2330" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
+          <x14:cfRule type="beginsWith" priority="2332" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
             <xm:f>LEFT(ServoDyn!A602,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36255,7 +36297,7 @@
           <xm:sqref>A35:A36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2363" operator="containsText" text="......" id="{5FD4013B-8363-458B-8AA3-B485798DA1C8}">
+          <x14:cfRule type="containsText" priority="2365" operator="containsText" text="......" id="{5FD4013B-8363-458B-8AA3-B485798DA1C8}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A808)))</xm:f>
             <x14:dxf>
               <font>
@@ -36264,7 +36306,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2364" operator="beginsWith" text="#" id="{5826827B-E3D9-4440-94B4-857DA3C7325E}">
+          <x14:cfRule type="beginsWith" priority="2366" operator="beginsWith" text="#" id="{5826827B-E3D9-4440-94B4-857DA3C7325E}">
             <xm:f>LEFT(ServoDyn!A808,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36281,7 +36323,7 @@
           <xm:sqref>A782 A780</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2469" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
+          <x14:cfRule type="containsText" priority="2471" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A183)))</xm:f>
             <x14:dxf>
               <font>
@@ -36290,7 +36332,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2470" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
+          <x14:cfRule type="beginsWith" priority="2472" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
             <xm:f>LEFT(ServoDyn!A183,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36307,7 +36349,7 @@
           <xm:sqref>A96</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2485" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
+          <x14:cfRule type="containsText" priority="2487" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A625)))</xm:f>
             <x14:dxf>
               <font>
@@ -36316,7 +36358,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2486" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
+          <x14:cfRule type="beginsWith" priority="2488" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
             <xm:f>LEFT(ServoDyn!A625,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -36330,7 +36372,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A524:A525</xm:sqref>
+          <xm:sqref>A524</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -43902,490 +43944,490 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A11 A21 A235:A239 A276:A281 A111:A115 A145:A171 A283:A285 A288 A290:A1048576 A174:A200 A134:A137 A104:A107 A117:A130 A16">
-    <cfRule type="containsText" dxfId="209" priority="309" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="213" priority="309" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="208" priority="310" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="212" priority="310" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="containsText" dxfId="207" priority="301" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="211" priority="301" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A20)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="206" priority="302" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="210" priority="302" operator="beginsWith" text="#">
       <formula>LEFT(A20,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="205" priority="299" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="209" priority="299" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="204" priority="300" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="208" priority="300" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A23">
-    <cfRule type="containsText" dxfId="203" priority="297" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="207" priority="297" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A22)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="202" priority="298" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="206" priority="298" operator="beginsWith" text="#">
       <formula>LEFT(A22,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:A19">
-    <cfRule type="containsText" dxfId="201" priority="295" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="205" priority="295" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A18)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="200" priority="296" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="204" priority="296" operator="beginsWith" text="#">
       <formula>LEFT(A18,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A208">
-    <cfRule type="containsText" dxfId="199" priority="223" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="203" priority="223" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A208)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="198" priority="224" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="202" priority="224" operator="beginsWith" text="#">
       <formula>LEFT(A208,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A173">
-    <cfRule type="containsText" dxfId="197" priority="213" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="201" priority="213" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A173)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="196" priority="214" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="200" priority="214" operator="beginsWith" text="#">
       <formula>LEFT(A173,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108">
-    <cfRule type="containsText" dxfId="195" priority="203" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="199" priority="203" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A108)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="194" priority="204" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="198" priority="204" operator="beginsWith" text="#">
       <formula>LEFT(A108,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A209">
-    <cfRule type="containsText" dxfId="193" priority="181" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="197" priority="181" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A209)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="192" priority="182" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="196" priority="182" operator="beginsWith" text="#">
       <formula>LEFT(A209,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A234">
-    <cfRule type="containsText" dxfId="191" priority="165" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="195" priority="165" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A234)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="190" priority="166" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="194" priority="166" operator="beginsWith" text="#">
       <formula>LEFT(A234,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="containsText" dxfId="189" priority="201" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="193" priority="201" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="188" priority="202" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="192" priority="202" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:A61">
-    <cfRule type="containsText" dxfId="187" priority="1109" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="191" priority="1109" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="186" priority="1110" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="190" priority="1110" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:A46">
-    <cfRule type="containsText" dxfId="185" priority="1159" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="189" priority="1159" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="184" priority="1160" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="188" priority="1160" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:A50">
-    <cfRule type="containsText" dxfId="183" priority="1329" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="187" priority="1329" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="182" priority="1330" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="186" priority="1330" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64:A66">
-    <cfRule type="containsText" dxfId="181" priority="1499" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="185" priority="1499" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="180" priority="1500" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="184" priority="1500" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A201">
-    <cfRule type="containsText" dxfId="179" priority="167" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="183" priority="167" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="178" priority="168" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="182" priority="168" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A282">
-    <cfRule type="containsText" dxfId="177" priority="159" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="181" priority="159" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A282)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="176" priority="160" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="180" priority="160" operator="beginsWith" text="#">
       <formula>LEFT(A282,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A241">
-    <cfRule type="containsText" dxfId="175" priority="149" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="179" priority="149" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A241)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="174" priority="150" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="178" priority="150" operator="beginsWith" text="#">
       <formula>LEFT(A241,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A270">
-    <cfRule type="containsText" dxfId="173" priority="151" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="177" priority="151" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A270)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="172" priority="152" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="176" priority="152" operator="beginsWith" text="#">
       <formula>LEFT(A270,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A131">
-    <cfRule type="containsText" dxfId="171" priority="147" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="175" priority="147" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A131)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="170" priority="148" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="174" priority="148" operator="beginsWith" text="#">
       <formula>LEFT(A131,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132">
-    <cfRule type="containsText" dxfId="169" priority="145" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="173" priority="145" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A132)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="168" priority="146" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="172" priority="146" operator="beginsWith" text="#">
       <formula>LEFT(A132,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A133">
-    <cfRule type="containsText" dxfId="167" priority="143" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="171" priority="143" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A133)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="166" priority="144" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="170" priority="144" operator="beginsWith" text="#">
       <formula>LEFT(A133,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245:A246">
-    <cfRule type="containsText" dxfId="165" priority="141" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="169" priority="141" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A245)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="164" priority="142" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="168" priority="142" operator="beginsWith" text="#">
       <formula>LEFT(A245,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A202">
-    <cfRule type="containsText" dxfId="163" priority="139" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="167" priority="139" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="162" priority="140" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="166" priority="140" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138">
-    <cfRule type="containsText" dxfId="161" priority="133" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="165" priority="133" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="160" priority="134" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="164" priority="134" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A247">
-    <cfRule type="containsText" dxfId="159" priority="131" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="163" priority="131" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A247)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="158" priority="132" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="162" priority="132" operator="beginsWith" text="#">
       <formula>LEFT(A247,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A243">
-    <cfRule type="containsText" dxfId="157" priority="127" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="161" priority="127" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A243)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="156" priority="128" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="160" priority="128" operator="beginsWith" text="#">
       <formula>LEFT(A243,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A250">
-    <cfRule type="containsText" dxfId="155" priority="125" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="159" priority="125" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A250)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="154" priority="126" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="158" priority="126" operator="beginsWith" text="#">
       <formula>LEFT(A250,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A248">
-    <cfRule type="containsText" dxfId="153" priority="121" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="157" priority="121" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A248)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="152" priority="122" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="156" priority="122" operator="beginsWith" text="#">
       <formula>LEFT(A248,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A249">
-    <cfRule type="containsText" dxfId="151" priority="119" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="155" priority="119" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A249)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="150" priority="120" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="154" priority="120" operator="beginsWith" text="#">
       <formula>LEFT(A249,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A244">
-    <cfRule type="containsText" dxfId="149" priority="117" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="153" priority="117" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A244)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="148" priority="118" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="152" priority="118" operator="beginsWith" text="#">
       <formula>LEFT(A244,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A286">
-    <cfRule type="containsText" dxfId="147" priority="115" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="151" priority="115" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A286)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="146" priority="116" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="150" priority="116" operator="beginsWith" text="#">
       <formula>LEFT(A286,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A206">
-    <cfRule type="containsText" dxfId="145" priority="113" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="149" priority="113" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A206)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="144" priority="114" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="148" priority="114" operator="beginsWith" text="#">
       <formula>LEFT(A206,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A207">
-    <cfRule type="containsText" dxfId="143" priority="111" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="147" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A207)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="142" priority="112" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="146" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(A207,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A139">
-    <cfRule type="containsText" dxfId="141" priority="109" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="145" priority="109" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="140" priority="110" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="144" priority="110" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A140">
-    <cfRule type="containsText" dxfId="139" priority="107" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="143" priority="107" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="138" priority="108" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="142" priority="108" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A242">
-    <cfRule type="containsText" dxfId="137" priority="103" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="141" priority="103" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A242)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="136" priority="104" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="140" priority="104" operator="beginsWith" text="#">
       <formula>LEFT(A242,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A251">
-    <cfRule type="containsText" dxfId="135" priority="101" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="139" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A251)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="134" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="138" priority="102" operator="beginsWith" text="#">
       <formula>LEFT(A251,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A252">
-    <cfRule type="containsText" dxfId="133" priority="99" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="137" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A252)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="132" priority="100" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="136" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(A252,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A253">
-    <cfRule type="containsText" dxfId="131" priority="97" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="135" priority="97" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A253)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="130" priority="98" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="134" priority="98" operator="beginsWith" text="#">
       <formula>LEFT(A253,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A203:A205 A69:A70 A72">
-    <cfRule type="containsText" dxfId="129" priority="195" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="133" priority="195" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="128" priority="196" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="132" priority="196" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:A63">
-    <cfRule type="containsText" dxfId="127" priority="2123" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="131" priority="2123" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="126" priority="2124" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="130" priority="2124" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="containsText" dxfId="125" priority="2235" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="129" priority="2235" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="124" priority="2236" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="128" priority="2236" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71">
-    <cfRule type="containsText" dxfId="123" priority="95" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="127" priority="95" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A71)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="122" priority="96" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="126" priority="96" operator="beginsWith" text="#">
       <formula>LEFT(A71,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="containsText" dxfId="121" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="125" priority="85" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="120" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="124" priority="86" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="containsText" dxfId="119" priority="81" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="123" priority="81" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A96)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="118" priority="82" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="122" priority="82" operator="beginsWith" text="#">
       <formula>LEFT(A96,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A141">
-    <cfRule type="containsText" dxfId="117" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="121" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="116" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="120" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A214">
-    <cfRule type="containsText" dxfId="115" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="119" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A214)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="114" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="118" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A214,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="containsText" dxfId="113" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="117" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A98)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="112" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="116" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A98,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A240">
-    <cfRule type="containsText" dxfId="111" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="115" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A240)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="110" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="114" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(A240,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="containsText" dxfId="109" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="113" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A99)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="108" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="112" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A99,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="containsText" dxfId="107" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="111" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A100)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="106" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="110" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A100,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="containsText" dxfId="105" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="109" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A101)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="104" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="108" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A101,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="containsText" dxfId="103" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="107" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A102)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="102" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="106" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A102,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="containsText" dxfId="101" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="105" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A103)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="100" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="104" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A103,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A271">
-    <cfRule type="containsText" dxfId="99" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="103" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A271)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="98" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="102" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A271,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272:A275">
-    <cfRule type="containsText" dxfId="97" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="101" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A272)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="100" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A272,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116">
-    <cfRule type="containsText" dxfId="95" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="99" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A116)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="94" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="98" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A116,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142">
-    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="97" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="92" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="96" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="containsText" dxfId="91" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="90" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="94" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A143">
-    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="93" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="92" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45904,266 +45946,266 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="71" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="66" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="70" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="containsText" dxfId="65" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="69" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A14)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="64" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="68" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(A14,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="63" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="67" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="62" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="66" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:A22">
-    <cfRule type="containsText" dxfId="61" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="65" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A19)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="60" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="64" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(A19,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="59" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="63" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="62" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="61" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="60" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A23)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="58" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A23,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="containsText" dxfId="53" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="57" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A26)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="52" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="56" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(A26,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="containsText" dxfId="51" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="55" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A27)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="50" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="54" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(A27,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="53" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A29)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="52" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A29,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="51" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A28)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="50" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A28,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="containsText" dxfId="45" priority="43" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="49" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A30)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="44" priority="44" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="48" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A30,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="47" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A31)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="46" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(A31,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="containsText" dxfId="41" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="45" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A32)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="44" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A32,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="43" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A33)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="42" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A33,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="41" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A34)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="40" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A34,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="39" priority="33" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A35)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="38" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(A35,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="37" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A36)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="32" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="36" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(A36,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="35" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A37)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="34" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A37,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A38)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="32" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A38,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A39)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="30" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A39,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="29" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A40)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="28" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A40,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A41)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="26" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A41,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A42)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="24" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A42,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A43)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="22" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A43,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44">
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A44)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="20" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A44,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A45)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="18" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A45,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A46)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="16" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A46,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A47)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="14" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A47,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A48)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="12" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A48,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50 A52:A53">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A50)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="10" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A50,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A54)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="8" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A54,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A51)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="6" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A51,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated FAST_SFunc.c to compile with Visual C++ 2010 Express
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@910 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 57f088ce086ccfb611034e7926af9222b943de64
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12251" uniqueCount="2241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12252" uniqueCount="2241">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -7142,7 +7142,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="656">
+  <dxfs count="654">
     <dxf>
       <font>
         <u val="none"/>
@@ -12635,23 +12635,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -13649,8 +13632,8 @@
   <dimension ref="A1:J322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <pane ySplit="11" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F182" sqref="F182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17802,8 +17785,8 @@
       <c r="E181" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="F181" s="27">
-        <v>3</v>
+      <c r="F181" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="G181" s="27" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
+ added libraries called in FAST mex function + updated dependencies + moved external inputs to FASt misc var type + added an input solve routine for InflowWind in the glue code
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@917 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: cc6bfadd8e895355f860c0c9e0b165375888019d
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12363" uniqueCount="2261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12428" uniqueCount="2273">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -6981,6 +6981,42 @@
   </si>
   <si>
     <t>"Map ServoDyn nacelle point mesh to ElastoDyn point mesh on the nacelle"</t>
+  </si>
+  <si>
+    <t>FAST_ExternInputType</t>
+  </si>
+  <si>
+    <t># ..... FAST External Initialization Input data .......................................................................................................</t>
+  </si>
+  <si>
+    <t>LidarFocus</t>
+  </si>
+  <si>
+    <t>"lidar focus (relative to lidar location)"</t>
+  </si>
+  <si>
+    <t>"generator torque input from Simulink/Labview"</t>
+  </si>
+  <si>
+    <t>"electric poser input from Simulink/Labview"</t>
+  </si>
+  <si>
+    <t>"yaw rate command from Simulink/Labview"</t>
+  </si>
+  <si>
+    <t>"yaw position command from Simulink/Labview"</t>
+  </si>
+  <si>
+    <t>"blade pitch commands from Simulink/Labview"</t>
+  </si>
+  <si>
+    <t>ExternInput</t>
+  </si>
+  <si>
+    <t>"external input values"</t>
+  </si>
+  <si>
+    <t>"rad/s"</t>
   </si>
 </sst>
 </file>
@@ -7202,7 +7238,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="686">
+  <dxfs count="670">
     <dxf>
       <font>
         <u val="none"/>
@@ -12848,19 +12884,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <u val="none"/>
       </font>
@@ -12878,129 +12901,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -13948,10 +13848,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="665" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="667" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="664" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="666" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13961,18 +13861,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J325"/>
+  <dimension ref="A1:J335"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J316" sqref="J316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" style="27" customWidth="1"/>
     <col min="2" max="2" width="32.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.85546875" style="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.140625" style="27" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" style="27" bestFit="1" customWidth="1"/>
@@ -21196,59 +21096,27 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="309" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A309" s="3" t="s">
-        <v>2004</v>
-      </c>
-      <c r="I309" s="12"/>
-    </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A310" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B310" s="27" t="s">
-        <v>1771</v>
-      </c>
-      <c r="C310" s="27" t="s">
-        <v>2005</v>
-      </c>
-      <c r="D310" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E310" s="27" t="s">
-        <v>1978</v>
-      </c>
-      <c r="F310" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G310" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H310" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I310" s="28" t="s">
-        <v>1979</v>
-      </c>
-      <c r="J310" s="27" t="s">
-        <v>1980</v>
-      </c>
+    <row r="310" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="3" t="s">
+        <v>2237</v>
+      </c>
+      <c r="I310" s="12"/>
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B311" s="27" t="s">
-        <v>27</v>
+        <v>1771</v>
       </c>
       <c r="C311" s="27" t="s">
-        <v>2005</v>
+        <v>2261</v>
       </c>
       <c r="D311" s="27" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E311" s="27" t="s">
-        <v>1981</v>
+        <v>960</v>
       </c>
       <c r="F311" s="27" t="s">
         <v>26</v>
@@ -21260,13 +21128,10 @@
         <v>26</v>
       </c>
       <c r="I311" s="28" t="s">
-        <v>1982</v>
-      </c>
-      <c r="J311" s="27" t="s">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="312" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>2265</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" s="27" t="s">
         <v>22</v>
       </c>
@@ -21274,13 +21139,13 @@
         <v>27</v>
       </c>
       <c r="C312" s="27" t="s">
-        <v>2005</v>
+        <v>2261</v>
       </c>
       <c r="D312" s="27" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E312" s="27" t="s">
-        <v>1983</v>
+        <v>956</v>
       </c>
       <c r="F312" s="27" t="s">
         <v>26</v>
@@ -21292,10 +21157,7 @@
         <v>26</v>
       </c>
       <c r="I312" s="28" t="s">
-        <v>1984</v>
-      </c>
-      <c r="J312" s="27" t="s">
-        <v>1980</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.25">
@@ -21306,13 +21168,13 @@
         <v>27</v>
       </c>
       <c r="C313" s="27" t="s">
-        <v>2005</v>
+        <v>2261</v>
       </c>
       <c r="D313" s="27" t="s">
         <v>34</v>
       </c>
       <c r="E313" s="27" t="s">
-        <v>1985</v>
+        <v>1068</v>
       </c>
       <c r="F313" s="27" t="s">
         <v>26</v>
@@ -21324,10 +21186,7 @@
         <v>26</v>
       </c>
       <c r="I313" s="28" t="s">
-        <v>1994</v>
-      </c>
-      <c r="J313" s="27" t="s">
-        <v>1980</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.25">
@@ -21338,13 +21197,13 @@
         <v>27</v>
       </c>
       <c r="C314" s="27" t="s">
-        <v>2005</v>
+        <v>2261</v>
       </c>
       <c r="D314" s="27" t="s">
-        <v>1991</v>
+        <v>34</v>
       </c>
       <c r="E314" s="27" t="s">
-        <v>1986</v>
+        <v>1069</v>
       </c>
       <c r="F314" s="27" t="s">
         <v>26</v>
@@ -21356,10 +21215,7 @@
         <v>26</v>
       </c>
       <c r="I314" s="28" t="s">
-        <v>1992</v>
-      </c>
-      <c r="J314" s="27" t="s">
-        <v>1980</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.25">
@@ -21370,16 +21226,16 @@
         <v>27</v>
       </c>
       <c r="C315" s="27" t="s">
-        <v>2005</v>
+        <v>2261</v>
       </c>
       <c r="D315" s="27" t="s">
-        <v>1991</v>
+        <v>34</v>
       </c>
       <c r="E315" s="27" t="s">
-        <v>1987</v>
-      </c>
-      <c r="F315" s="27" t="s">
-        <v>26</v>
+        <v>1042</v>
+      </c>
+      <c r="F315" s="27">
+        <v>3</v>
       </c>
       <c r="G315" s="27" t="s">
         <v>26</v>
@@ -21388,10 +21244,10 @@
         <v>26</v>
       </c>
       <c r="I315" s="28" t="s">
-        <v>1993</v>
+        <v>2269</v>
       </c>
       <c r="J315" s="27" t="s">
-        <v>1980</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.25">
@@ -21402,16 +21258,16 @@
         <v>27</v>
       </c>
       <c r="C316" s="27" t="s">
-        <v>2005</v>
+        <v>2261</v>
       </c>
       <c r="D316" s="27" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E316" s="27" t="s">
-        <v>1988</v>
-      </c>
-      <c r="F316" s="27" t="s">
-        <v>1990</v>
+        <v>2263</v>
+      </c>
+      <c r="F316" s="27">
+        <v>3</v>
       </c>
       <c r="G316" s="27" t="s">
         <v>26</v>
@@ -21420,85 +21276,33 @@
         <v>26</v>
       </c>
       <c r="I316" s="28" t="s">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A317" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B317" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C317" s="27" t="s">
-        <v>2005</v>
-      </c>
-      <c r="D317" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E317" s="27" t="s">
-        <v>1989</v>
-      </c>
-      <c r="F317" s="27" t="s">
-        <v>1990</v>
-      </c>
-      <c r="G317" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H317" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I317" s="28" t="s">
-        <v>1996</v>
-      </c>
-    </row>
-    <row r="318" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A318" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B318" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C318" s="27" t="s">
-        <v>2005</v>
-      </c>
-      <c r="D318" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="E318" s="27" t="s">
-        <v>2006</v>
-      </c>
-      <c r="F318" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G318" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H318" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I318" s="28" t="s">
-        <v>2007</v>
-      </c>
-      <c r="J318" s="27" t="s">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="319" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>2264</v>
+      </c>
+      <c r="J316" s="27" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A318" s="3" t="s">
+        <v>2004</v>
+      </c>
+      <c r="I318" s="12"/>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B319" s="27" t="s">
-        <v>27</v>
+        <v>1771</v>
       </c>
       <c r="C319" s="27" t="s">
         <v>2005</v>
       </c>
       <c r="D319" s="27" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E319" s="27" t="s">
-        <v>1997</v>
+        <v>1978</v>
       </c>
       <c r="F319" s="27" t="s">
         <v>26</v>
@@ -21510,10 +21314,10 @@
         <v>26</v>
       </c>
       <c r="I319" s="28" t="s">
-        <v>2002</v>
+        <v>1979</v>
       </c>
       <c r="J319" s="27" t="s">
-        <v>2003</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.25">
@@ -21527,10 +21331,10 @@
         <v>2005</v>
       </c>
       <c r="D320" s="27" t="s">
-        <v>1999</v>
+        <v>44</v>
       </c>
       <c r="E320" s="27" t="s">
-        <v>1998</v>
+        <v>1981</v>
       </c>
       <c r="F320" s="27" t="s">
         <v>26</v>
@@ -21542,17 +21346,75 @@
         <v>26</v>
       </c>
       <c r="I320" s="28" t="s">
-        <v>2000</v>
+        <v>1982</v>
       </c>
       <c r="J320" s="27" t="s">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="322" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A322" s="3" t="s">
-        <v>2237</v>
-      </c>
-      <c r="I322" s="12"/>
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A321" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B321" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C321" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D321" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E321" s="27" t="s">
+        <v>1983</v>
+      </c>
+      <c r="F321" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G321" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H321" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I321" s="28" t="s">
+        <v>1984</v>
+      </c>
+      <c r="J321" s="27" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A322" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B322" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C322" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D322" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E322" s="27" t="s">
+        <v>1985</v>
+      </c>
+      <c r="F322" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G322" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H322" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I322" s="28" t="s">
+        <v>1994</v>
+      </c>
+      <c r="J322" s="27" t="s">
+        <v>1980</v>
+      </c>
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323" s="27" t="s">
@@ -21562,402 +21424,666 @@
         <v>27</v>
       </c>
       <c r="C323" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D323" s="27" t="s">
+        <v>1991</v>
+      </c>
+      <c r="E323" s="27" t="s">
+        <v>1986</v>
+      </c>
+      <c r="F323" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G323" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H323" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I323" s="28" t="s">
+        <v>1992</v>
+      </c>
+      <c r="J323" s="27" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A324" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B324" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C324" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D324" s="27" t="s">
+        <v>1991</v>
+      </c>
+      <c r="E324" s="27" t="s">
+        <v>1987</v>
+      </c>
+      <c r="F324" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G324" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H324" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I324" s="28" t="s">
+        <v>1993</v>
+      </c>
+      <c r="J324" s="27" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A325" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B325" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C325" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D325" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E325" s="27" t="s">
+        <v>1988</v>
+      </c>
+      <c r="F325" s="27" t="s">
+        <v>1990</v>
+      </c>
+      <c r="G325" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H325" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I325" s="28" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A326" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B326" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C326" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D326" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E326" s="27" t="s">
+        <v>1989</v>
+      </c>
+      <c r="F326" s="27" t="s">
+        <v>1990</v>
+      </c>
+      <c r="G326" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H326" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I326" s="28" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="327" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A327" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B327" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C327" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D327" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E327" s="27" t="s">
+        <v>2006</v>
+      </c>
+      <c r="F327" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G327" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H327" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I327" s="28" t="s">
+        <v>2007</v>
+      </c>
+      <c r="J327" s="27" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="328" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A328" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B328" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C328" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D328" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E328" s="27" t="s">
+        <v>1997</v>
+      </c>
+      <c r="F328" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G328" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H328" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I328" s="28" t="s">
+        <v>2002</v>
+      </c>
+      <c r="J328" s="27" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A329" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B329" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C329" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D329" s="27" t="s">
+        <v>1999</v>
+      </c>
+      <c r="E329" s="27" t="s">
+        <v>1998</v>
+      </c>
+      <c r="F329" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G329" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H329" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I329" s="28" t="s">
+        <v>2000</v>
+      </c>
+      <c r="J329" s="27" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A330" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B330" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C330" s="27" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D330" s="27" t="s">
+        <v>2261</v>
+      </c>
+      <c r="E330" s="27" t="s">
+        <v>2270</v>
+      </c>
+      <c r="F330" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G330" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H330" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I330" s="28" t="s">
+        <v>2271</v>
+      </c>
+      <c r="J330" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="332" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A332" s="3" t="s">
+        <v>2262</v>
+      </c>
+      <c r="I332" s="12"/>
+    </row>
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A333" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B333" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C333" s="27" t="s">
         <v>2238</v>
       </c>
-      <c r="D323" s="27" t="s">
+      <c r="D333" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E323" s="27" t="s">
+      <c r="E333" s="27" t="s">
         <v>2182</v>
       </c>
-      <c r="F323" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G323" s="27">
+      <c r="F333" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G333" s="27">
         <v>-1</v>
       </c>
-      <c r="H323" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I323" s="28" t="s">
+      <c r="H333" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I333" s="28" t="s">
         <v>2239</v>
       </c>
-      <c r="J323" s="27" t="s">
+      <c r="J333" s="27" t="s">
         <v>1113</v>
       </c>
     </row>
-    <row r="324" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A324" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B324" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C324" s="27" t="s">
+    <row r="334" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A334" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B334" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C334" s="27" t="s">
         <v>2238</v>
       </c>
-      <c r="D324" s="27" t="s">
+      <c r="D334" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="E324" s="27" t="s">
+      <c r="E334" s="27" t="s">
         <v>2219</v>
       </c>
-      <c r="F324" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G324" s="27" t="s">
+      <c r="F334" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G334" s="27" t="s">
         <v>2211</v>
       </c>
-      <c r="H324" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I324" s="28" t="s">
+      <c r="H334" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I334" s="28" t="s">
         <v>2240</v>
       </c>
-      <c r="J324" s="27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="325" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A325" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B325" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C325" s="27" t="s">
+      <c r="J334" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A335" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B335" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C335" s="27" t="s">
         <v>2238</v>
       </c>
-      <c r="D325" s="27" t="s">
+      <c r="D335" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="E325" s="27" t="s">
+      <c r="E335" s="27" t="s">
         <v>2179</v>
       </c>
-      <c r="F325" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G325" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H325" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I325" s="28" t="s">
+      <c r="F335" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G335" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H335" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I335" s="28" t="s">
         <v>2204</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A11">
-    <cfRule type="containsText" dxfId="663" priority="77" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="665" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="662" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="664" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A14">
-    <cfRule type="containsText" dxfId="661" priority="75" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="663" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A13)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="660" priority="76" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="662" priority="78" operator="beginsWith" text="#">
       <formula>LEFT(A13,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="659" priority="73" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="661" priority="75" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="658" priority="74" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="660" priority="76" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="657" priority="71" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="659" priority="73" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="656" priority="72" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="658" priority="74" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="655" priority="69" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="657" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="654" priority="70" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="656" priority="72" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="653" priority="67" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="655" priority="69" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="652" priority="68" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="654" priority="70" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A115">
-    <cfRule type="containsText" dxfId="651" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="653" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A115)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="650" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="652" priority="68" operator="beginsWith" text="#">
       <formula>LEFT(A115,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132">
-    <cfRule type="containsText" dxfId="649" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="651" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A132)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="648" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="650" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A132,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A149">
-    <cfRule type="containsText" dxfId="647" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="649" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A149)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="646" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="648" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(A149,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A183">
-    <cfRule type="containsText" dxfId="645" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="647" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A183)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="644" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="646" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A183,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116">
-    <cfRule type="containsText" dxfId="643" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="645" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A116)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="642" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="644" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(A116,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A117">
-    <cfRule type="containsText" dxfId="641" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="643" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A117)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="640" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="642" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(A117,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A165">
-    <cfRule type="containsText" dxfId="639" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="641" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A165)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="638" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="640" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(A165,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A198">
-    <cfRule type="containsText" dxfId="637" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="639" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A198)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="636" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="638" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A198,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A213">
-    <cfRule type="containsText" dxfId="635" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="637" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A213)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="634" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="636" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(A213,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A228">
-    <cfRule type="containsText" dxfId="633" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="635" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A228)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="632" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="634" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(A228,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A243">
-    <cfRule type="containsText" dxfId="631" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="633" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A243)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="630" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="632" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A243,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A180">
-    <cfRule type="containsText" dxfId="629" priority="43" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="631" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A180)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="628" priority="44" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="630" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A180,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A258:A260">
-    <cfRule type="containsText" dxfId="627" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="629" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A258)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="626" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="628" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A258,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A267">
-    <cfRule type="containsText" dxfId="625" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="627" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A267)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="624" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="626" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(A267,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A270">
-    <cfRule type="containsText" dxfId="623" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="625" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A270)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="622" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="624" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A270,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A273">
-    <cfRule type="containsText" dxfId="621" priority="35" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="623" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A273)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="620" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="622" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A273,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A276">
-    <cfRule type="containsText" dxfId="619" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="621" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A276)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="618" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="620" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A276,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A284">
-    <cfRule type="containsText" dxfId="617" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="619" priority="33" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A284)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="616" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="618" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(A284,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A289">
-    <cfRule type="containsText" dxfId="615" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="617" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A289)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="614" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="616" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(A289,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A292">
-    <cfRule type="containsText" dxfId="613" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="615" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A292)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="612" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="614" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A292,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A295">
-    <cfRule type="containsText" dxfId="611" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="613" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A295)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="610" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="612" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A295,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A299">
+    <cfRule type="containsText" dxfId="611" priority="25" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A299)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="610" priority="26" operator="beginsWith" text="#">
+      <formula>LEFT(A299,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A318">
     <cfRule type="containsText" dxfId="609" priority="23" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A299)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A318)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="608" priority="24" operator="beginsWith" text="#">
-      <formula>LEFT(A299,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A309">
-    <cfRule type="containsText" dxfId="607" priority="21" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A309)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="606" priority="22" operator="beginsWith" text="#">
-      <formula>LEFT(A309,LEN("#"))="#"</formula>
+      <formula>LEFT(A318,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:A52">
-    <cfRule type="containsText" dxfId="605" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="607" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A51)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="604" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="606" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A51,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A32">
-    <cfRule type="containsText" dxfId="603" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="605" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A28)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="602" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="604" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A28,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="containsText" dxfId="601" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="603" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A47)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="600" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="602" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A47,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="containsText" dxfId="599" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="601" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A101)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="598" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="600" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A101,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="containsText" dxfId="597" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="599" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A62)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="596" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="598" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A62,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="containsText" dxfId="595" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="597" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A66)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="594" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="596" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A66,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="containsText" dxfId="593" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="595" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A77)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="592" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="594" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A77,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
+    <cfRule type="containsText" dxfId="593" priority="7" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A86)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="592" priority="8" operator="beginsWith" text="#">
+      <formula>LEFT(A86,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A332">
     <cfRule type="containsText" dxfId="591" priority="5" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A86)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A332)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="590" priority="6" operator="beginsWith" text="#">
-      <formula>LEFT(A86,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A322">
-    <cfRule type="containsText" dxfId="589" priority="3" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A322)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="588" priority="4" operator="beginsWith" text="#">
-      <formula>LEFT(A322,LEN("#"))="#"</formula>
+      <formula>LEFT(A332,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A281">
+    <cfRule type="containsText" dxfId="589" priority="3" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A281)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="588" priority="4" operator="beginsWith" text="#">
+      <formula>LEFT(A281,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A310">
     <cfRule type="containsText" dxfId="587" priority="1" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A281)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A310)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="586" priority="2" operator="beginsWith" text="#">
-      <formula>LEFT(A281,LEN("#"))="#"</formula>
+      <formula>LEFT(A310,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22809,7 +22935,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>22</v>
       </c>
@@ -22838,7 +22964,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>22</v>
       </c>
@@ -22867,7 +22993,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>22</v>
       </c>
@@ -22896,7 +23022,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>22</v>
       </c>
@@ -22925,7 +23051,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>22</v>
       </c>
@@ -22954,7 +23080,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>22</v>
       </c>
@@ -22983,7 +23109,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>22</v>
       </c>
@@ -23012,7 +23138,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>22</v>
       </c>
@@ -23041,7 +23167,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>22</v>
       </c>
@@ -23070,7 +23196,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>22</v>
       </c>
@@ -23099,7 +23225,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>22</v>
       </c>
@@ -23128,7 +23254,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>22</v>
       </c>
@@ -23157,7 +23283,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>22</v>
       </c>
@@ -23186,7 +23312,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>22</v>
       </c>
@@ -23215,7 +23341,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>22</v>
       </c>
@@ -23244,7 +23370,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>22</v>
       </c>
@@ -23273,7 +23399,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>22</v>
       </c>
@@ -23302,13 +23428,13 @@
         <v>888</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>1144</v>
       </c>
       <c r="I67" s="12"/>
     </row>
-    <row r="68" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>22</v>
       </c>
@@ -23340,7 +23466,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>22</v>
       </c>
@@ -23369,7 +23495,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="15" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
         <v>22</v>
       </c>
@@ -23401,7 +23527,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="15" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>22</v>
       </c>
@@ -23430,25 +23556,25 @@
         <v>844</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>206</v>
       </c>
       <c r="I74" s="12"/>
     </row>
-    <row r="75" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>240</v>
       </c>
       <c r="I75" s="12"/>
     </row>
-    <row r="76" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>1301</v>
       </c>
       <c r="I76" s="12"/>
     </row>
-    <row r="77" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>22</v>
       </c>
@@ -23480,7 +23606,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>22</v>
       </c>
@@ -23512,7 +23638,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>22</v>
       </c>
@@ -23544,7 +23670,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>22</v>
       </c>
@@ -23576,7 +23702,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>22</v>
       </c>
@@ -23608,7 +23734,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>22</v>
       </c>
@@ -23640,7 +23766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>22</v>
       </c>
@@ -23672,7 +23798,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>22</v>
       </c>
@@ -23704,7 +23830,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>22</v>
       </c>
@@ -23736,7 +23862,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>22</v>
       </c>
@@ -23768,7 +23894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>22</v>
       </c>
@@ -23800,7 +23926,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>22</v>
       </c>
@@ -23832,7 +23958,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>22</v>
       </c>
@@ -23864,7 +23990,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>22</v>
       </c>
@@ -23896,7 +24022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>22</v>
       </c>
@@ -23928,7 +24054,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>22</v>
       </c>
@@ -23960,7 +24086,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>22</v>
       </c>
@@ -23992,7 +24118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>22</v>
       </c>
@@ -24024,7 +24150,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>22</v>
       </c>
@@ -24056,7 +24182,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>22</v>
       </c>
@@ -24088,7 +24214,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>22</v>
       </c>
@@ -24120,7 +24246,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>22</v>
       </c>
@@ -24152,7 +24278,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>22</v>
       </c>
@@ -24184,7 +24310,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>22</v>
       </c>
@@ -24216,7 +24342,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="101" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>22</v>
       </c>
@@ -24248,7 +24374,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>22</v>
       </c>
@@ -24280,7 +24406,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>22</v>
       </c>
@@ -24312,7 +24438,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>22</v>
       </c>
@@ -24344,7 +24470,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>22</v>
       </c>
@@ -24376,7 +24502,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>22</v>
       </c>
@@ -24408,7 +24534,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>22</v>
       </c>
@@ -24440,7 +24566,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>22</v>
       </c>
@@ -24472,7 +24598,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>22</v>
       </c>
@@ -24504,7 +24630,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="110" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>22</v>
       </c>
@@ -24536,7 +24662,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>22</v>
       </c>
@@ -24568,7 +24694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>22</v>
       </c>
@@ -24600,7 +24726,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>22</v>
       </c>
@@ -24632,7 +24758,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>22</v>
       </c>
@@ -24664,7 +24790,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>22</v>
       </c>
@@ -24696,7 +24822,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>22</v>
       </c>
@@ -24728,7 +24854,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>22</v>
       </c>
@@ -24760,7 +24886,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>22</v>
       </c>
@@ -24792,7 +24918,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>22</v>
       </c>
@@ -24824,7 +24950,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>22</v>
       </c>
@@ -24856,7 +24982,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>22</v>
       </c>
@@ -24888,7 +25014,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>22</v>
       </c>
@@ -24920,7 +25046,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>22</v>
       </c>
@@ -24952,7 +25078,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>22</v>
       </c>
@@ -24984,7 +25110,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>22</v>
       </c>
@@ -25016,7 +25142,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>22</v>
       </c>
@@ -25048,7 +25174,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="127" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>22</v>
       </c>
@@ -25080,7 +25206,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>22</v>
       </c>
@@ -25112,7 +25238,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>22</v>
       </c>
@@ -25144,7 +25270,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>22</v>
       </c>
@@ -25176,7 +25302,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>22</v>
       </c>
@@ -25208,7 +25334,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>22</v>
       </c>
@@ -25240,7 +25366,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>22</v>
       </c>
@@ -25272,7 +25398,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>22</v>
       </c>
@@ -25304,7 +25430,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>22</v>
       </c>
@@ -25336,7 +25462,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>22</v>
       </c>
@@ -25368,7 +25494,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>22</v>
       </c>
@@ -25400,7 +25526,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>22</v>
       </c>
@@ -25432,7 +25558,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>22</v>
       </c>
@@ -25464,7 +25590,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>22</v>
       </c>
@@ -25496,7 +25622,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>22</v>
       </c>
@@ -25528,7 +25654,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>22</v>
       </c>
@@ -25560,7 +25686,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>22</v>
       </c>
@@ -25592,7 +25718,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>22</v>
       </c>
@@ -25624,7 +25750,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>22</v>
       </c>
@@ -25656,7 +25782,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>22</v>
       </c>
@@ -25688,7 +25814,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>22</v>
       </c>
@@ -25720,7 +25846,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>22</v>
       </c>
@@ -25752,7 +25878,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>22</v>
       </c>
@@ -25784,7 +25910,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>22</v>
       </c>
@@ -25816,7 +25942,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>22</v>
       </c>
@@ -25848,7 +25974,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>22</v>
       </c>
@@ -25880,7 +26006,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>22</v>
       </c>
@@ -25912,7 +26038,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>22</v>
       </c>
@@ -25944,7 +26070,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>22</v>
       </c>
@@ -25976,7 +26102,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>22</v>
       </c>
@@ -26008,7 +26134,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>22</v>
       </c>
@@ -26040,7 +26166,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>22</v>
       </c>
@@ -26072,7 +26198,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>22</v>
       </c>
@@ -26104,7 +26230,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>22</v>
       </c>
@@ -26136,7 +26262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>22</v>
       </c>
@@ -26168,7 +26294,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>22</v>
       </c>
@@ -26200,7 +26326,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>22</v>
       </c>
@@ -26232,7 +26358,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:10" s="1" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>47</v>
       </c>
@@ -26264,7 +26390,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="165" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>22</v>
       </c>
@@ -26296,7 +26422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:10" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>22</v>
       </c>
@@ -26328,7 +26454,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>22</v>
       </c>
@@ -26360,7 +26486,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>22</v>
       </c>
@@ -26392,7 +26518,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>22</v>
       </c>
@@ -26424,7 +26550,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>22</v>
       </c>
@@ -26456,7 +26582,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>22</v>
       </c>
@@ -26488,7 +26614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>22</v>
       </c>
@@ -26520,7 +26646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>22</v>
       </c>
@@ -46631,18 +46757,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A369">
-    <cfRule type="containsText" dxfId="197" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="213" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A369)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="196" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="212" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A369,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A799">
-    <cfRule type="containsText" dxfId="195" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="211" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A799)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="194" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="210" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A799,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48648,7 +48774,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>22</v>
       </c>
@@ -48680,7 +48806,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -48692,7 +48818,7 @@
       <c r="I76" s="10"/>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>22</v>
       </c>
@@ -48724,7 +48850,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>22</v>
       </c>
@@ -48756,7 +48882,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>22</v>
       </c>
@@ -48788,7 +48914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>22</v>
       </c>
@@ -48820,7 +48946,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>22</v>
       </c>
@@ -48852,7 +48978,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>22</v>
       </c>
@@ -48884,7 +49010,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>22</v>
       </c>
@@ -48916,7 +49042,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>22</v>
       </c>
@@ -48948,7 +49074,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>22</v>
       </c>
@@ -48980,7 +49106,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>22</v>
       </c>
@@ -49012,7 +49138,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>22</v>
       </c>
@@ -49044,7 +49170,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>22</v>
       </c>
@@ -49076,7 +49202,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>22</v>
       </c>
@@ -49108,7 +49234,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>22</v>
       </c>
@@ -49140,7 +49266,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>22</v>
       </c>
@@ -49172,7 +49298,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>22</v>
       </c>
@@ -49204,7 +49330,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>22</v>
       </c>
@@ -49236,7 +49362,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>22</v>
       </c>
@@ -49268,7 +49394,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>22</v>
       </c>
@@ -49364,7 +49490,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -49376,13 +49502,13 @@
       <c r="I98" s="6"/>
       <c r="J98" s="5"/>
     </row>
-    <row r="99" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>1601</v>
       </c>
       <c r="I99" s="12"/>
     </row>
-    <row r="100" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>22</v>
       </c>
@@ -49414,7 +49540,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>22</v>
       </c>
@@ -49446,7 +49572,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>22</v>
       </c>
@@ -49478,7 +49604,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>22</v>
       </c>
@@ -49510,7 +49636,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>22</v>
       </c>
@@ -49542,7 +49668,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>47</v>
       </c>
@@ -49574,7 +49700,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>22</v>
       </c>
@@ -49606,19 +49732,19 @@
         <v>249</v>
       </c>
     </row>
-    <row r="108" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I108" s="12"/>
     </row>
-    <row r="109" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I109" s="12"/>
     </row>
-    <row r="110" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>22</v>
       </c>
@@ -49650,7 +49776,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>22</v>
       </c>
@@ -49679,7 +49805,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>22</v>
       </c>
@@ -49711,7 +49837,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>22</v>
       </c>
@@ -49807,13 +49933,13 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="117" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I117" s="12"/>
     </row>
-    <row r="118" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>22</v>
       </c>
@@ -49845,7 +49971,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>22</v>
       </c>
@@ -49877,7 +50003,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>22</v>
       </c>
@@ -49909,7 +50035,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>22</v>
       </c>
@@ -49941,19 +50067,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I123" s="12"/>
     </row>
-    <row r="124" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I124" s="12"/>
     </row>
-    <row r="125" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>22</v>
       </c>
@@ -50017,13 +50143,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I128" s="12"/>
     </row>
-    <row r="129" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>22</v>
       </c>
@@ -50087,13 +50213,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I132" s="12"/>
     </row>
-    <row r="133" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>22</v>
       </c>
@@ -50157,13 +50283,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="136" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>219</v>
       </c>
       <c r="I136" s="12"/>
     </row>
-    <row r="137" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>22</v>
       </c>
@@ -50195,7 +50321,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>22</v>
       </c>
@@ -50227,7 +50353,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>22</v>
       </c>
@@ -50259,7 +50385,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>22</v>
       </c>
@@ -50291,7 +50417,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>22</v>
       </c>
@@ -50323,7 +50449,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>22</v>
       </c>
@@ -50355,7 +50481,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>22</v>
       </c>
@@ -50387,7 +50513,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>22</v>
       </c>
@@ -50419,7 +50545,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>22</v>
       </c>
@@ -50451,7 +50577,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>22</v>
       </c>
@@ -50483,7 +50609,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>22</v>
       </c>
@@ -50515,7 +50641,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>22</v>
       </c>
@@ -50547,7 +50673,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>22</v>
       </c>
@@ -50579,7 +50705,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>22</v>
       </c>
@@ -50611,7 +50737,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>22</v>
       </c>
@@ -50643,7 +50769,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>22</v>
       </c>
@@ -50707,25 +50833,25 @@
         <v>26</v>
       </c>
     </row>
-    <row r="155" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I155" s="12"/>
     </row>
-    <row r="156" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I156" s="12"/>
     </row>
-    <row r="157" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I157" s="12"/>
     </row>
-    <row r="158" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>22</v>
       </c>
@@ -50757,7 +50883,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>22</v>
       </c>
@@ -50789,7 +50915,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>22</v>
       </c>
@@ -55339,58 +55465,58 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A126">
-    <cfRule type="containsText" dxfId="51" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="69" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A126)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="50" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="68" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A126,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130">
-    <cfRule type="containsText" dxfId="47" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="67" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A130)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="66" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A130,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A134">
-    <cfRule type="containsText" dxfId="45" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="65" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A134)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="44" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="64" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A134,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
-    <cfRule type="containsText" dxfId="43" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="63" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A153)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="62" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A153,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A244">
-    <cfRule type="containsText" dxfId="41" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="61" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A244)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="60" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A244,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A298">
-    <cfRule type="containsText" dxfId="39" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="59" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A298)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="58" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A298,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A284">
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="57" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A284)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="56" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A284,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
+ hss brake now available with AB4 integrator as well as ABM4 + gBoxEff can be non-zero for AB4 and ABM4 integrators (rk4 should work if there are no corrections) + changed HSSBrMode to 0 instead of 1 when it is not used
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@947 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 7a40e968d00b526d13aa1b6e2bfcf75638e3cb18
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -22606,8 +22606,8 @@
   <dimension ref="A1:K837"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A537" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F539" sqref="F539"/>
+      <pane ySplit="11" topLeftCell="A529" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D538" sqref="D538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
made turbine-level data type and wrapper routines that use them to call routines in FAST_Subs.f90 to eventually allow for multi-turbine instances of FAST. (and so I don't have to modify the details of the glue code when I add modules in the future)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@970 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 4f548b47cab49ffa7b4057f725fe553df8942092
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="840" windowWidth="14880" windowHeight="7308" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="900" windowWidth="14880" windowHeight="7248" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12606" uniqueCount="2291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12766" uniqueCount="2325">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -7071,6 +7071,108 @@
   </si>
   <si>
     <t>{ED_NMX}</t>
+  </si>
+  <si>
+    <t># ..... FAST Turbine Data (one realization) .......................................................................................................</t>
+  </si>
+  <si>
+    <t>p_FAST</t>
+  </si>
+  <si>
+    <t>FAST_TurbineType</t>
+  </si>
+  <si>
+    <t>y_FAST</t>
+  </si>
+  <si>
+    <t>m_FAST</t>
+  </si>
+  <si>
+    <t>MeshMapData</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>SrvD</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>HD</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>MAP</t>
+  </si>
+  <si>
+    <t>FEAM</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>IceF</t>
+  </si>
+  <si>
+    <t>IceD</t>
+  </si>
+  <si>
+    <t>"Parameters for the glue code"</t>
+  </si>
+  <si>
+    <t>"Output variables for the glue code"</t>
+  </si>
+  <si>
+    <t>"Miscellaneous variables"</t>
+  </si>
+  <si>
+    <t>"Data for mapping between modules"</t>
+  </si>
+  <si>
+    <t>"Data for the ElastoDyn module"</t>
+  </si>
+  <si>
+    <t>"Data for the ServoDyn module"</t>
+  </si>
+  <si>
+    <t>"Data for the AeroDyn module"</t>
+  </si>
+  <si>
+    <t>"Data for InflowWind module"</t>
+  </si>
+  <si>
+    <t>"Data for the HydroDyn module"</t>
+  </si>
+  <si>
+    <t>"Data for the SubDyn module"</t>
+  </si>
+  <si>
+    <t>"Data for the MAP (Mooring Analysis Program) module"</t>
+  </si>
+  <si>
+    <t>"Data for the FEAMooring module"</t>
+  </si>
+  <si>
+    <t>"Data for the MoorDyn module"</t>
+  </si>
+  <si>
+    <t>"Data for the IceFloe module"</t>
+  </si>
+  <si>
+    <t>"Data for the IceDyn module"</t>
+  </si>
+  <si>
+    <t>IfW</t>
+  </si>
+  <si>
+    <t>TurbID</t>
+  </si>
+  <si>
+    <t>"Turbine ID Number"</t>
   </si>
 </sst>
 </file>
@@ -13023,6 +13125,10 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -13036,10 +13142,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -13970,10 +14072,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="675" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="677" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="674" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="676" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13983,11 +14085,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J350"/>
+  <dimension ref="A1:J368"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A330" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G341" sqref="G341"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A346" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G354" sqref="G354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22275,325 +22377,851 @@
         <v>2187</v>
       </c>
     </row>
+    <row r="352" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A352" s="3" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I352" s="12"/>
+    </row>
+    <row r="353" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A353" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B353" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C353" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D353" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E353" s="27" t="s">
+        <v>2323</v>
+      </c>
+      <c r="F353" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G353" s="27">
+        <v>1</v>
+      </c>
+      <c r="H353" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I353" s="28" t="s">
+        <v>2324</v>
+      </c>
+      <c r="J353" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="354" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A354" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B354" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C354" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D354" s="27" t="s">
+        <v>1991</v>
+      </c>
+      <c r="E354" s="27" t="s">
+        <v>2292</v>
+      </c>
+      <c r="F354" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G354" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H354" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I354" s="28" t="s">
+        <v>2307</v>
+      </c>
+      <c r="J354" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="355" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A355" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B355" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C355" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D355" s="27" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E355" s="27" t="s">
+        <v>2294</v>
+      </c>
+      <c r="F355" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G355" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H355" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I355" s="28" t="s">
+        <v>2308</v>
+      </c>
+      <c r="J355" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="356" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A356" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B356" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C356" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D356" s="27" t="s">
+        <v>1988</v>
+      </c>
+      <c r="E356" s="27" t="s">
+        <v>2295</v>
+      </c>
+      <c r="F356" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G356" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H356" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I356" s="28" t="s">
+        <v>2309</v>
+      </c>
+      <c r="J356" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="357" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A357" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B357" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C357" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D357" s="27" t="s">
+        <v>1892</v>
+      </c>
+      <c r="E357" s="27" t="s">
+        <v>2296</v>
+      </c>
+      <c r="F357" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G357" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H357" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I357" s="28" t="s">
+        <v>2310</v>
+      </c>
+      <c r="J357" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="358" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A358" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B358" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C358" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D358" s="27" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E358" s="27" t="s">
+        <v>2297</v>
+      </c>
+      <c r="F358" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G358" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H358" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I358" s="28" t="s">
+        <v>2311</v>
+      </c>
+      <c r="J358" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="359" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A359" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B359" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C359" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D359" s="27" t="s">
+        <v>1807</v>
+      </c>
+      <c r="E359" s="27" t="s">
+        <v>2298</v>
+      </c>
+      <c r="F359" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G359" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H359" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I359" s="28" t="s">
+        <v>2312</v>
+      </c>
+      <c r="J359" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="360" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A360" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B360" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C360" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D360" s="27" t="s">
+        <v>1834</v>
+      </c>
+      <c r="E360" s="27" t="s">
+        <v>2299</v>
+      </c>
+      <c r="F360" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G360" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H360" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I360" s="28" t="s">
+        <v>2313</v>
+      </c>
+      <c r="J360" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="361" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A361" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B361" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C361" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D361" s="27" t="s">
+        <v>1884</v>
+      </c>
+      <c r="E361" s="27" t="s">
+        <v>2322</v>
+      </c>
+      <c r="F361" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G361" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H361" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I361" s="28" t="s">
+        <v>2314</v>
+      </c>
+      <c r="J361" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="362" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A362" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B362" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C362" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D362" s="27" t="s">
+        <v>1843</v>
+      </c>
+      <c r="E362" s="27" t="s">
+        <v>2300</v>
+      </c>
+      <c r="F362" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G362" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H362" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I362" s="28" t="s">
+        <v>2315</v>
+      </c>
+      <c r="J362" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="363" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A363" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B363" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C363" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D363" s="27" t="s">
+        <v>1820</v>
+      </c>
+      <c r="E363" s="27" t="s">
+        <v>2301</v>
+      </c>
+      <c r="F363" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G363" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H363" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I363" s="28" t="s">
+        <v>2316</v>
+      </c>
+      <c r="J363" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="364" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A364" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B364" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C364" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D364" s="27" t="s">
+        <v>1881</v>
+      </c>
+      <c r="E364" s="27" t="s">
+        <v>2302</v>
+      </c>
+      <c r="F364" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G364" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H364" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I364" s="28" t="s">
+        <v>2317</v>
+      </c>
+      <c r="J364" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="365" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A365" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B365" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C365" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D365" s="27" t="s">
+        <v>1862</v>
+      </c>
+      <c r="E365" s="27" t="s">
+        <v>2303</v>
+      </c>
+      <c r="F365" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G365" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H365" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I365" s="28" t="s">
+        <v>2318</v>
+      </c>
+      <c r="J365" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="366" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A366" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B366" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C366" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D366" s="27" t="s">
+        <v>2257</v>
+      </c>
+      <c r="E366" s="27" t="s">
+        <v>2304</v>
+      </c>
+      <c r="F366" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G366" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H366" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I366" s="28" t="s">
+        <v>2319</v>
+      </c>
+      <c r="J366" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="367" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A367" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B367" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C367" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D367" s="27" t="s">
+        <v>1852</v>
+      </c>
+      <c r="E367" s="27" t="s">
+        <v>2305</v>
+      </c>
+      <c r="F367" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G367" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H367" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I367" s="28" t="s">
+        <v>2320</v>
+      </c>
+      <c r="J367" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="368" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A368" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B368" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C368" s="27" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D368" s="27" t="s">
+        <v>1765</v>
+      </c>
+      <c r="E368" s="27" t="s">
+        <v>2306</v>
+      </c>
+      <c r="F368" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G368" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H368" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I368" s="28" t="s">
+        <v>2321</v>
+      </c>
+      <c r="J368" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A11">
-    <cfRule type="containsText" dxfId="673" priority="81" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="675" priority="83" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="672" priority="82" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="674" priority="84" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A14">
-    <cfRule type="containsText" dxfId="671" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="673" priority="81" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A13)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="670" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="672" priority="82" operator="beginsWith" text="#">
       <formula>LEFT(A13,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="669" priority="77" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="671" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="668" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="670" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="667" priority="75" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="669" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="666" priority="76" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="668" priority="78" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="665" priority="73" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="667" priority="75" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="664" priority="74" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="666" priority="76" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="663" priority="71" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="665" priority="73" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="662" priority="72" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="664" priority="74" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A117">
-    <cfRule type="containsText" dxfId="661" priority="69" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="663" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A117)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="660" priority="70" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="662" priority="72" operator="beginsWith" text="#">
       <formula>LEFT(A117,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A134">
-    <cfRule type="containsText" dxfId="659" priority="67" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="661" priority="69" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A134)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="658" priority="68" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="660" priority="70" operator="beginsWith" text="#">
       <formula>LEFT(A134,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A151">
-    <cfRule type="containsText" dxfId="657" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="659" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A151)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="656" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="658" priority="68" operator="beginsWith" text="#">
       <formula>LEFT(A151,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A185">
-    <cfRule type="containsText" dxfId="655" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="657" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A185)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="654" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="656" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A185,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A118">
-    <cfRule type="containsText" dxfId="653" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="655" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A118)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="652" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="654" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(A118,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A119">
-    <cfRule type="containsText" dxfId="651" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="653" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A119)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="650" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="652" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A119,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A167">
-    <cfRule type="containsText" dxfId="649" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="651" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A167)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="648" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="650" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(A167,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A200">
-    <cfRule type="containsText" dxfId="647" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="649" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A200)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="646" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="648" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(A200,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A215">
-    <cfRule type="containsText" dxfId="645" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="647" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A215)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="644" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="646" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(A215,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A230">
-    <cfRule type="containsText" dxfId="643" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="645" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A230)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="642" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="644" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A230,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245">
-    <cfRule type="containsText" dxfId="641" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="643" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A245)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="640" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="642" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(A245,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A182">
-    <cfRule type="containsText" dxfId="639" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="641" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A182)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="638" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="640" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(A182,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A275:A277">
-    <cfRule type="containsText" dxfId="637" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="639" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A275)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="636" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="638" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A275,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A284">
-    <cfRule type="containsText" dxfId="635" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="637" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A284)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="634" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="636" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A284,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A287">
-    <cfRule type="containsText" dxfId="633" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="635" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A287)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="632" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="634" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(A287,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A290">
-    <cfRule type="containsText" dxfId="631" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="633" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A290)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="630" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="632" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A290,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A298">
-    <cfRule type="containsText" dxfId="629" priority="35" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="631" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A298)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="628" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="630" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A298,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A303">
-    <cfRule type="containsText" dxfId="627" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="629" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A303)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="626" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="628" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A303,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A306">
-    <cfRule type="containsText" dxfId="625" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="627" priority="33" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A306)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="624" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="626" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(A306,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A309">
-    <cfRule type="containsText" dxfId="623" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="625" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A309)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="622" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="624" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(A309,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A313">
-    <cfRule type="containsText" dxfId="621" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="623" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A313)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="620" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="622" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A313,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A333">
-    <cfRule type="containsText" dxfId="619" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="621" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A333)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="618" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="620" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A333,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A54">
-    <cfRule type="containsText" dxfId="617" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="619" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A53)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="616" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="618" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A53,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:A33">
-    <cfRule type="containsText" dxfId="615" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="617" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A29)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="614" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="616" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A29,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="containsText" dxfId="613" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="615" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A49)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="612" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="614" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A49,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="containsText" dxfId="611" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="613" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A103)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="610" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="612" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A103,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="609" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="611" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A64)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="608" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="610" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A64,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="containsText" dxfId="607" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="609" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A68)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="606" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="608" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A68,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79">
-    <cfRule type="containsText" dxfId="605" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="607" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A79)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="604" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="606" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A79,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="containsText" dxfId="603" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="605" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A88)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="602" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="604" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A88,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A347">
-    <cfRule type="containsText" dxfId="601" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="603" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A347)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="600" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="602" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A347,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A295">
-    <cfRule type="containsText" dxfId="599" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="601" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A295)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="598" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="600" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A295,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A324">
-    <cfRule type="containsText" dxfId="597" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="599" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A324)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="596" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="598" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A324,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A260">
+    <cfRule type="containsText" dxfId="597" priority="3" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A260)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="596" priority="4" operator="beginsWith" text="#">
+      <formula>LEFT(A260,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A352">
     <cfRule type="containsText" dxfId="595" priority="1" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A260)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A352)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="594" priority="2" operator="beginsWith" text="#">
-      <formula>LEFT(A260,LEN("#"))="#"</formula>
+      <formula>LEFT(A352,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22605,9 +23233,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K837"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A529" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D538" sqref="D538"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A820" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K837" sqref="K837"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added routine to create checkpoint file and to restore from checkpoint file; updated Types file with 14-Apr-2015 version of registry; removed some unused variables;
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@977 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: c2b1d096b295f887a924c6fa7a55270ca4825657
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12766" uniqueCount="2325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12766" uniqueCount="2326">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -7173,6 +7173,9 @@
   </si>
   <si>
     <t>"Turbine ID Number"</t>
+  </si>
+  <si>
+    <t>{MaxNBlades}</t>
   </si>
 </sst>
 </file>
@@ -14088,8 +14091,8 @@
   <dimension ref="A1:J368"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A346" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G354" sqref="G354"/>
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15675,7 +15678,7 @@
         <v>2090</v>
       </c>
       <c r="F81" s="27" t="s">
-        <v>2046</v>
+        <v>2325</v>
       </c>
       <c r="G81" s="27" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
+ added Twr base height to tower meshes in AD15 input files + added some initialization of outputs in ED_Init for BeamDyn init input.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1051 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 21c4f74e115c6c1548c0454bb356ad80cedef86a
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1140" windowWidth="11568" windowHeight="4584" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="1140" windowWidth="11568" windowHeight="4584" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="2" r:id="rId1"/>
@@ -8109,7 +8109,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="840">
+  <dxfs count="834">
     <dxf>
       <font>
         <u val="none"/>
@@ -14996,19 +14996,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <u val="none"/>
       </font>
@@ -15026,44 +15013,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -16164,10 +16113,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="811" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="813" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="810" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="812" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25441,370 +25390,370 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A11">
-    <cfRule type="containsText" dxfId="809" priority="93" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="811" priority="93" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="808" priority="94" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="810" priority="94" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A14">
-    <cfRule type="containsText" dxfId="807" priority="91" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="809" priority="91" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A13)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="806" priority="92" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="808" priority="92" operator="beginsWith" text="#">
       <formula>LEFT(A13,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="805" priority="89" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="807" priority="89" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="804" priority="90" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="806" priority="90" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="803" priority="87" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="805" priority="87" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="802" priority="88" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="804" priority="88" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="801" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="803" priority="85" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="800" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="802" priority="86" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="799" priority="83" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="801" priority="83" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="798" priority="84" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="800" priority="84" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A126">
-    <cfRule type="containsText" dxfId="797" priority="81" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="799" priority="81" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A126)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="796" priority="82" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="798" priority="82" operator="beginsWith" text="#">
       <formula>LEFT(A126,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A154">
-    <cfRule type="containsText" dxfId="795" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="797" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A154)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="794" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="796" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A154,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A168">
-    <cfRule type="containsText" dxfId="793" priority="77" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="795" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A168)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="792" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="794" priority="78" operator="beginsWith" text="#">
       <formula>LEFT(A168,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A217">
-    <cfRule type="containsText" dxfId="791" priority="75" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="793" priority="75" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A217)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="790" priority="76" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="792" priority="76" operator="beginsWith" text="#">
       <formula>LEFT(A217,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A127">
-    <cfRule type="containsText" dxfId="789" priority="73" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="791" priority="73" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A127)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="788" priority="74" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="790" priority="74" operator="beginsWith" text="#">
       <formula>LEFT(A127,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128">
-    <cfRule type="containsText" dxfId="787" priority="71" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="789" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A128)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="786" priority="72" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="788" priority="72" operator="beginsWith" text="#">
       <formula>LEFT(A128,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A193">
-    <cfRule type="containsText" dxfId="785" priority="69" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="787" priority="69" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A193)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="784" priority="70" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="786" priority="70" operator="beginsWith" text="#">
       <formula>LEFT(A193,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A229">
-    <cfRule type="containsText" dxfId="783" priority="67" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="785" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A229)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="782" priority="68" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="784" priority="68" operator="beginsWith" text="#">
       <formula>LEFT(A229,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A241">
-    <cfRule type="containsText" dxfId="781" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="783" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A241)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="780" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="782" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A241,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A253">
-    <cfRule type="containsText" dxfId="779" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="781" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A253)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="778" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="780" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(A253,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A265">
-    <cfRule type="containsText" dxfId="777" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="779" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A265)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="776" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="778" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A265,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A205">
-    <cfRule type="containsText" dxfId="775" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="777" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A205)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="774" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="776" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(A205,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A289:A290 A294">
-    <cfRule type="containsText" dxfId="773" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="775" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A289)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="772" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="774" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(A289,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A301">
-    <cfRule type="containsText" dxfId="771" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="773" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A301)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="770" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="772" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A301,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A304">
-    <cfRule type="containsText" dxfId="769" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="771" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A304)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="768" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="770" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(A304,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A307">
-    <cfRule type="containsText" dxfId="767" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="769" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A307)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="766" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="768" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(A307,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A315">
-    <cfRule type="containsText" dxfId="765" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="767" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A315)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="764" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="766" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A315,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A322">
-    <cfRule type="containsText" dxfId="763" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="765" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A322)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="762" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="764" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A322,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A325">
-    <cfRule type="containsText" dxfId="761" priority="43" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="763" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A325)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="760" priority="44" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="762" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A325,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A328">
-    <cfRule type="containsText" dxfId="759" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="761" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A328)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="758" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="760" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(A328,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A332">
-    <cfRule type="containsText" dxfId="757" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="759" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A332)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="756" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="758" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A332,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A354">
-    <cfRule type="containsText" dxfId="755" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="757" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A354)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="754" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="756" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A354,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:A58">
-    <cfRule type="containsText" dxfId="753" priority="35" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="755" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A57)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="752" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="754" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A57,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:A36">
-    <cfRule type="containsText" dxfId="751" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="753" priority="33" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A32)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="750" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="752" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(A32,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="containsText" dxfId="749" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="751" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A53)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="748" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="750" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(A53,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A112">
-    <cfRule type="containsText" dxfId="747" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="749" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A112)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="746" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="748" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A112,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="containsText" dxfId="745" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="747" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A70)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="744" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="746" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A70,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74">
-    <cfRule type="containsText" dxfId="743" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="745" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A74)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="742" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="744" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A74,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="containsText" dxfId="741" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="743" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A86)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="740" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="742" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A86,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="containsText" dxfId="739" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="741" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A96)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="738" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="740" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A96,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A367">
-    <cfRule type="containsText" dxfId="737" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="739" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A367)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="736" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="738" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A367,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A312">
-    <cfRule type="containsText" dxfId="735" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="737" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A312)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="734" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="736" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A312,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A345">
-    <cfRule type="containsText" dxfId="733" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="735" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A345)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="732" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="734" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A345,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A277">
-    <cfRule type="containsText" dxfId="731" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="733" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A277)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="730" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="732" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A277,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A372">
-    <cfRule type="containsText" dxfId="729" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="731" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A372)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="728" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="730" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A372,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A181">
-    <cfRule type="containsText" dxfId="727" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="729" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A181)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="726" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="728" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A181,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A140">
-    <cfRule type="containsText" dxfId="725" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="727" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A140)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="724" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="726" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A140,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A141">
-    <cfRule type="containsText" dxfId="723" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="725" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A141)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="722" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="724" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A141,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142">
-    <cfRule type="containsText" dxfId="721" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="723" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A142)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="720" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="722" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A142,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A291">
-    <cfRule type="containsText" dxfId="719" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="721" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A291)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="718" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="720" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A291,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25817,9 +25766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K841"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I535" sqref="I535"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A799" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E808" sqref="E808"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49296,1294 +49245,1302 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A266:A322 A515:A523 A338 A329 A552:A553 A658:A691 A528 A75 A44:A63 A707:A722 A702:A705 A724:A730 A696:A700 A28 A30:A34 A262:A264 A547 A842:A1048576 A789:A790 A352:A361 A381:A384 A395:A397 A408:A411 A567:A638 A435:A459 A462:A469 A508 A471:A497 A402:A405 A796:A797 A640:A656 A803:A805 A817:A818 A535 A1:A11 A13:A14 A510:A513 A22:A25 A500:A504 A542:A545">
-    <cfRule type="containsText" dxfId="717" priority="909" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="719" priority="913" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="716" priority="910" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="718" priority="914" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A265">
-    <cfRule type="containsText" dxfId="715" priority="897" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="717" priority="901" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A265)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="714" priority="898" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="716" priority="902" operator="beginsWith" text="#">
       <formula>LEFT(A265,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:A18 A41 A21">
-    <cfRule type="containsText" dxfId="713" priority="891" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="715" priority="895" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="712" priority="892" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="714" priority="896" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A76:A77">
-    <cfRule type="containsText" dxfId="711" priority="887" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="713" priority="891" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A76)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="710" priority="888" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="712" priority="892" operator="beginsWith" text="#">
       <formula>LEFT(A76,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="709" priority="885" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="711" priority="889" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="708" priority="886" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="710" priority="890" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A549">
-    <cfRule type="containsText" dxfId="707" priority="881" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="709" priority="885" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A549)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="706" priority="882" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="708" priority="886" operator="beginsWith" text="#">
       <formula>LEFT(A549,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A548">
-    <cfRule type="containsText" dxfId="705" priority="883" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="707" priority="887" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A548)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="704" priority="884" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="706" priority="888" operator="beginsWith" text="#">
       <formula>LEFT(A548,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A561">
-    <cfRule type="containsText" dxfId="703" priority="879" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="705" priority="883" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A561)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="702" priority="880" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="704" priority="884" operator="beginsWith" text="#">
       <formula>LEFT(A561,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A562">
-    <cfRule type="containsText" dxfId="701" priority="877" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="703" priority="881" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A562)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="700" priority="878" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="702" priority="882" operator="beginsWith" text="#">
       <formula>LEFT(A562,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A559">
-    <cfRule type="containsText" dxfId="699" priority="875" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="701" priority="879" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A559)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="698" priority="876" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="700" priority="880" operator="beginsWith" text="#">
       <formula>LEFT(A559,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A560">
-    <cfRule type="containsText" dxfId="697" priority="873" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="699" priority="877" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A560)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="696" priority="874" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="698" priority="878" operator="beginsWith" text="#">
       <formula>LEFT(A560,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A563">
-    <cfRule type="containsText" dxfId="695" priority="869" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="697" priority="873" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A563)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="694" priority="870" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="696" priority="874" operator="beginsWith" text="#">
       <formula>LEFT(A563,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A514">
-    <cfRule type="containsText" dxfId="693" priority="865" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="695" priority="869" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A514)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="692" priority="866" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="694" priority="870" operator="beginsWith" text="#">
       <formula>LEFT(A514,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A550">
-    <cfRule type="containsText" dxfId="691" priority="863" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="693" priority="867" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A550)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="690" priority="864" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="692" priority="868" operator="beginsWith" text="#">
       <formula>LEFT(A550,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A564">
-    <cfRule type="containsText" dxfId="689" priority="861" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="691" priority="865" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A564)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="688" priority="862" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="690" priority="866" operator="beginsWith" text="#">
       <formula>LEFT(A564,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A657">
-    <cfRule type="containsText" dxfId="687" priority="859" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="689" priority="863" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A657)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="686" priority="860" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="688" priority="864" operator="beginsWith" text="#">
       <formula>LEFT(A657,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A551">
-    <cfRule type="containsText" dxfId="685" priority="853" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="687" priority="857" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A551)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="684" priority="854" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="686" priority="858" operator="beginsWith" text="#">
       <formula>LEFT(A551,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A323:A325">
-    <cfRule type="containsText" dxfId="683" priority="851" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="685" priority="855" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A323)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="682" priority="852" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="684" priority="856" operator="beginsWith" text="#">
       <formula>LEFT(A323,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A326">
-    <cfRule type="containsText" dxfId="681" priority="847" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="683" priority="851" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A326)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="680" priority="848" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="682" priority="852" operator="beginsWith" text="#">
       <formula>LEFT(A326,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A327:A328 A330:A335">
-    <cfRule type="containsText" dxfId="679" priority="845" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="681" priority="849" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A327)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="678" priority="846" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="680" priority="850" operator="beginsWith" text="#">
       <formula>LEFT(A327,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A336:A337 A339:A345 A555">
-    <cfRule type="containsText" dxfId="677" priority="843" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="679" priority="847" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A336)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="676" priority="844" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="678" priority="848" operator="beginsWith" text="#">
       <formula>LEFT(A336,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A554">
-    <cfRule type="containsText" dxfId="675" priority="799" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="677" priority="803" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A554)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="674" priority="800" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="676" priority="804" operator="beginsWith" text="#">
       <formula>LEFT(A554,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A347">
-    <cfRule type="containsText" dxfId="673" priority="787" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="675" priority="791" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A347)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="672" priority="788" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="674" priority="792" operator="beginsWith" text="#">
       <formula>LEFT(A347,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A346">
-    <cfRule type="containsText" dxfId="671" priority="789" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="673" priority="793" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A346)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="670" priority="790" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="672" priority="794" operator="beginsWith" text="#">
       <formula>LEFT(A346,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A556">
-    <cfRule type="containsText" dxfId="669" priority="785" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="671" priority="789" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A556)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="668" priority="786" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="670" priority="790" operator="beginsWith" text="#">
       <formula>LEFT(A556,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A557">
-    <cfRule type="containsText" dxfId="667" priority="783" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="669" priority="787" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A557)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="666" priority="784" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="668" priority="788" operator="beginsWith" text="#">
       <formula>LEFT(A557,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A348:A349">
-    <cfRule type="containsText" dxfId="665" priority="781" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="667" priority="785" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A348)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="664" priority="782" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="666" priority="786" operator="beginsWith" text="#">
       <formula>LEFT(A348,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A566">
-    <cfRule type="containsText" dxfId="663" priority="773" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="665" priority="777" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A566)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="662" priority="774" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="664" priority="778" operator="beginsWith" text="#">
       <formula>LEFT(A566,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A565">
-    <cfRule type="containsText" dxfId="661" priority="775" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="663" priority="779" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A565)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="660" priority="776" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="662" priority="780" operator="beginsWith" text="#">
       <formula>LEFT(A565,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A693">
-    <cfRule type="containsText" dxfId="659" priority="743" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="661" priority="747" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A693)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="658" priority="744" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="660" priority="748" operator="beginsWith" text="#">
       <formula>LEFT(A693,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A350:A351 A386">
-    <cfRule type="containsText" dxfId="657" priority="739" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="659" priority="743" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A350)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="656" priority="740" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="658" priority="744" operator="beginsWith" text="#">
       <formula>LEFT(A350,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A407">
-    <cfRule type="containsText" dxfId="655" priority="737" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="657" priority="741" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A407)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="654" priority="738" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="656" priority="742" operator="beginsWith" text="#">
       <formula>LEFT(A407,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A524:A525">
-    <cfRule type="containsText" dxfId="653" priority="733" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="655" priority="737" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A524)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="652" priority="734" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="654" priority="738" operator="beginsWith" text="#">
       <formula>LEFT(A524,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A527">
-    <cfRule type="containsText" dxfId="651" priority="731" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="653" priority="735" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A527)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="650" priority="732" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="652" priority="736" operator="beginsWith" text="#">
       <formula>LEFT(A527,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="containsText" dxfId="649" priority="705" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="651" priority="709" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A42)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="648" priority="706" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="650" priority="710" operator="beginsWith" text="#">
       <formula>LEFT(A42,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="containsText" dxfId="647" priority="703" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="649" priority="707" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A43)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="646" priority="704" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="648" priority="708" operator="beginsWith" text="#">
       <formula>LEFT(A43,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="645" priority="695" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="647" priority="699" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A64)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="644" priority="696" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="646" priority="700" operator="beginsWith" text="#">
       <formula>LEFT(A64,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="containsText" dxfId="643" priority="693" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="645" priority="697" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A65)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="642" priority="694" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="644" priority="698" operator="beginsWith" text="#">
       <formula>LEFT(A65,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="containsText" dxfId="641" priority="691" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="643" priority="695" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A66)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="640" priority="692" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="642" priority="696" operator="beginsWith" text="#">
       <formula>LEFT(A66,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="containsText" dxfId="639" priority="689" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="641" priority="693" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A67)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="638" priority="690" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="640" priority="694" operator="beginsWith" text="#">
       <formula>LEFT(A67,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A731">
-    <cfRule type="containsText" dxfId="637" priority="687" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="639" priority="691" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A731)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="636" priority="688" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="638" priority="692" operator="beginsWith" text="#">
       <formula>LEFT(A731,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A732">
-    <cfRule type="containsText" dxfId="635" priority="685" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="637" priority="689" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A732)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="634" priority="686" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="636" priority="690" operator="beginsWith" text="#">
       <formula>LEFT(A732,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A733">
-    <cfRule type="containsText" dxfId="633" priority="683" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="635" priority="687" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A733)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="632" priority="684" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="634" priority="688" operator="beginsWith" text="#">
       <formula>LEFT(A733,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A735:A738">
-    <cfRule type="containsText" dxfId="631" priority="677" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="633" priority="681" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A735)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="630" priority="678" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="632" priority="682" operator="beginsWith" text="#">
       <formula>LEFT(A735,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A734">
-    <cfRule type="containsText" dxfId="629" priority="673" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="631" priority="677" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A734)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="628" priority="674" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="630" priority="678" operator="beginsWith" text="#">
       <formula>LEFT(A734,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A739:A746">
-    <cfRule type="containsText" dxfId="627" priority="667" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="629" priority="671" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A739)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="626" priority="668" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="628" priority="672" operator="beginsWith" text="#">
       <formula>LEFT(A739,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A747:A757">
-    <cfRule type="containsText" dxfId="625" priority="661" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="627" priority="665" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A747)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="624" priority="662" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="626" priority="666" operator="beginsWith" text="#">
       <formula>LEFT(A747,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A758">
-    <cfRule type="containsText" dxfId="623" priority="663" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="625" priority="667" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A758)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="622" priority="664" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="624" priority="668" operator="beginsWith" text="#">
       <formula>LEFT(A758,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A759:A769">
-    <cfRule type="containsText" dxfId="621" priority="655" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="623" priority="659" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A759)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="620" priority="656" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="622" priority="660" operator="beginsWith" text="#">
       <formula>LEFT(A759,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A770">
-    <cfRule type="containsText" dxfId="619" priority="657" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="621" priority="661" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A770)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="618" priority="658" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="620" priority="662" operator="beginsWith" text="#">
       <formula>LEFT(A770,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A771">
-    <cfRule type="containsText" dxfId="617" priority="651" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="619" priority="655" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A771)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="616" priority="652" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="618" priority="656" operator="beginsWith" text="#">
       <formula>LEFT(A771,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A775:A776">
-    <cfRule type="containsText" dxfId="615" priority="641" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="617" priority="645" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A775)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="614" priority="642" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="616" priority="646" operator="beginsWith" text="#">
       <formula>LEFT(A775,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A772">
-    <cfRule type="containsText" dxfId="613" priority="647" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="615" priority="651" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A772)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="612" priority="648" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="614" priority="652" operator="beginsWith" text="#">
       <formula>LEFT(A772,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A773">
-    <cfRule type="containsText" dxfId="611" priority="645" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="613" priority="649" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A773)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="610" priority="646" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="612" priority="650" operator="beginsWith" text="#">
       <formula>LEFT(A773,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A774">
-    <cfRule type="containsText" dxfId="609" priority="643" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="611" priority="647" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A774)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="608" priority="644" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="610" priority="648" operator="beginsWith" text="#">
       <formula>LEFT(A774,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A777:A778">
-    <cfRule type="containsText" dxfId="607" priority="637" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="609" priority="641" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A777)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="606" priority="638" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="608" priority="642" operator="beginsWith" text="#">
       <formula>LEFT(A777,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A779">
-    <cfRule type="containsText" dxfId="605" priority="627" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="607" priority="631" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A779)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="604" priority="628" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="606" priority="632" operator="beginsWith" text="#">
       <formula>LEFT(A779,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A558">
-    <cfRule type="containsText" dxfId="603" priority="623" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="605" priority="627" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A558)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="602" priority="624" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="604" priority="628" operator="beginsWith" text="#">
       <formula>LEFT(A558,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A692">
-    <cfRule type="containsText" dxfId="601" priority="593" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="603" priority="597" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A692)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="600" priority="594" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="602" priority="598" operator="beginsWith" text="#">
       <formula>LEFT(A692,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="containsText" dxfId="599" priority="591" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="601" priority="595" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A69)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="598" priority="592" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="600" priority="596" operator="beginsWith" text="#">
       <formula>LEFT(A69,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="containsText" dxfId="597" priority="589" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="599" priority="593" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A70)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="596" priority="590" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="598" priority="594" operator="beginsWith" text="#">
       <formula>LEFT(A70,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:A73">
-    <cfRule type="containsText" dxfId="595" priority="587" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="597" priority="591" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A71)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="594" priority="588" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="596" priority="592" operator="beginsWith" text="#">
       <formula>LEFT(A71,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A723">
-    <cfRule type="containsText" dxfId="593" priority="567" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="595" priority="571" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A723)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="592" priority="568" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="594" priority="572" operator="beginsWith" text="#">
       <formula>LEFT(A723,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A695">
-    <cfRule type="containsText" dxfId="591" priority="573" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="593" priority="577" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A695)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="590" priority="574" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="592" priority="578" operator="beginsWith" text="#">
       <formula>LEFT(A695,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A701">
-    <cfRule type="containsText" dxfId="589" priority="569" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="591" priority="573" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A701)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="588" priority="570" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="590" priority="574" operator="beginsWith" text="#">
       <formula>LEFT(A701,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A706">
-    <cfRule type="containsText" dxfId="587" priority="565" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="589" priority="569" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A706)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="586" priority="566" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="588" priority="570" operator="beginsWith" text="#">
       <formula>LEFT(A706,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="containsText" dxfId="585" priority="563" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="587" priority="567" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A26)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="584" priority="564" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="586" priority="568" operator="beginsWith" text="#">
       <formula>LEFT(A26,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="containsText" dxfId="583" priority="553" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="585" priority="557" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A29)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="582" priority="554" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="584" priority="558" operator="beginsWith" text="#">
       <formula>LEFT(A29,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A780">
-    <cfRule type="containsText" dxfId="581" priority="551" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="583" priority="555" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A780)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="580" priority="552" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="582" priority="556" operator="beginsWith" text="#">
       <formula>LEFT(A780,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114 A124:A126">
-    <cfRule type="containsText" dxfId="579" priority="361" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="581" priority="365" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="578" priority="362" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="580" priority="366" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136">
-    <cfRule type="containsText" dxfId="577" priority="365" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="579" priority="369" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="576" priority="366" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="578" priority="370" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A151 A137">
-    <cfRule type="containsText" dxfId="575" priority="367" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="577" priority="371" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="574" priority="368" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="576" priority="372" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A156:A157 A153">
-    <cfRule type="containsText" dxfId="573" priority="369" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="575" priority="373" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="572" priority="370" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="574" priority="374" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152">
-    <cfRule type="containsText" dxfId="571" priority="371" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="573" priority="375" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="570" priority="372" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="572" priority="376" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A155">
-    <cfRule type="containsText" dxfId="569" priority="373" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="571" priority="377" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="568" priority="374" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="570" priority="378" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A158">
-    <cfRule type="containsText" dxfId="567" priority="375" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="569" priority="379" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="566" priority="376" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="568" priority="380" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A154">
-    <cfRule type="containsText" dxfId="565" priority="377" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="567" priority="381" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="564" priority="378" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="566" priority="382" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A162">
-    <cfRule type="containsText" dxfId="563" priority="379" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="565" priority="383" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="562" priority="380" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="564" priority="384" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A161 A172">
-    <cfRule type="containsText" dxfId="561" priority="381" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="563" priority="385" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="560" priority="382" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="562" priority="386" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A174">
-    <cfRule type="containsText" dxfId="559" priority="383" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="561" priority="387" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="558" priority="384" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="560" priority="388" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A176">
-    <cfRule type="containsText" dxfId="557" priority="385" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="559" priority="389" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="556" priority="386" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="558" priority="390" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="containsText" dxfId="555" priority="307" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="557" priority="311" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A35)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="554" priority="308" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="556" priority="312" operator="beginsWith" text="#">
       <formula>LEFT(A35,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="containsText" dxfId="553" priority="305" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="555" priority="309" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A36)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="552" priority="306" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="554" priority="310" operator="beginsWith" text="#">
       <formula>LEFT(A36,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A546">
-    <cfRule type="containsText" dxfId="551" priority="303" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="553" priority="307" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A546)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="550" priority="304" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="552" priority="308" operator="beginsWith" text="#">
       <formula>LEFT(A546,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A799">
-    <cfRule type="containsText" dxfId="549" priority="301" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="551" priority="305" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A799)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="548" priority="302" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="550" priority="306" operator="beginsWith" text="#">
       <formula>LEFT(A799,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:A110">
-    <cfRule type="containsText" dxfId="547" priority="1493" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="549" priority="1497" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="546" priority="1494" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="548" priority="1498" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A819">
-    <cfRule type="containsText" dxfId="545" priority="293" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="547" priority="297" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A819)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="544" priority="294" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="546" priority="298" operator="beginsWith" text="#">
       <formula>LEFT(A819,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A821">
-    <cfRule type="containsText" dxfId="543" priority="289" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="545" priority="293" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A821)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="542" priority="290" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="544" priority="294" operator="beginsWith" text="#">
       <formula>LEFT(A821,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A820">
-    <cfRule type="containsText" dxfId="541" priority="291" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="543" priority="295" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A820)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="540" priority="292" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="542" priority="296" operator="beginsWith" text="#">
       <formula>LEFT(A820,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A823">
-    <cfRule type="containsText" dxfId="539" priority="287" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="541" priority="291" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A823)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="538" priority="288" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="540" priority="292" operator="beginsWith" text="#">
       <formula>LEFT(A823,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A824">
-    <cfRule type="containsText" dxfId="537" priority="271" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="539" priority="275" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A824)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="536" priority="272" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="538" priority="276" operator="beginsWith" text="#">
       <formula>LEFT(A824,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A694">
-    <cfRule type="containsText" dxfId="535" priority="267" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="537" priority="271" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A694)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="534" priority="268" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="536" priority="272" operator="beginsWith" text="#">
       <formula>LEFT(A694,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A364">
-    <cfRule type="containsText" dxfId="533" priority="257" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="535" priority="261" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A364)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="532" priority="258" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="534" priority="262" operator="beginsWith" text="#">
       <formula>LEFT(A364,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A362">
-    <cfRule type="containsText" dxfId="531" priority="261" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="533" priority="265" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A362)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="530" priority="262" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="532" priority="266" operator="beginsWith" text="#">
       <formula>LEFT(A362,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A363">
-    <cfRule type="containsText" dxfId="529" priority="259" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="531" priority="263" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A363)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="528" priority="260" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="530" priority="264" operator="beginsWith" text="#">
       <formula>LEFT(A363,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A365">
-    <cfRule type="containsText" dxfId="527" priority="255" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="529" priority="259" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A365)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="526" priority="256" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="528" priority="260" operator="beginsWith" text="#">
       <formula>LEFT(A365,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A366">
-    <cfRule type="containsText" dxfId="525" priority="253" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="527" priority="257" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A366)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="524" priority="254" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="526" priority="258" operator="beginsWith" text="#">
       <formula>LEFT(A366,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A367">
-    <cfRule type="containsText" dxfId="523" priority="251" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="525" priority="255" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A367)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="522" priority="252" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="524" priority="256" operator="beginsWith" text="#">
       <formula>LEFT(A367,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A368">
-    <cfRule type="containsText" dxfId="521" priority="249" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="523" priority="253" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A368)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="520" priority="250" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="522" priority="254" operator="beginsWith" text="#">
       <formula>LEFT(A368,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A369">
-    <cfRule type="containsText" dxfId="519" priority="247" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="521" priority="251" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A369)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="518" priority="248" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="520" priority="252" operator="beginsWith" text="#">
       <formula>LEFT(A369,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A370">
-    <cfRule type="containsText" dxfId="517" priority="245" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="519" priority="249" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A370)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="516" priority="246" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="518" priority="250" operator="beginsWith" text="#">
       <formula>LEFT(A370,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A373">
-    <cfRule type="containsText" dxfId="515" priority="241" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="517" priority="245" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A373)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="514" priority="242" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="516" priority="246" operator="beginsWith" text="#">
       <formula>LEFT(A373,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A374">
-    <cfRule type="containsText" dxfId="513" priority="239" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="515" priority="243" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A374)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="512" priority="240" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="514" priority="244" operator="beginsWith" text="#">
       <formula>LEFT(A374,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A375">
-    <cfRule type="containsText" dxfId="511" priority="237" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="513" priority="241" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A375)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="510" priority="238" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="512" priority="242" operator="beginsWith" text="#">
       <formula>LEFT(A375,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A376">
-    <cfRule type="containsText" dxfId="509" priority="235" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="511" priority="239" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A376)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="508" priority="236" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="510" priority="240" operator="beginsWith" text="#">
       <formula>LEFT(A376,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A377">
-    <cfRule type="containsText" dxfId="507" priority="233" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="509" priority="237" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A377)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="506" priority="234" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="508" priority="238" operator="beginsWith" text="#">
       <formula>LEFT(A377,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A378">
-    <cfRule type="containsText" dxfId="505" priority="231" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="507" priority="235" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A378)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="504" priority="232" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="506" priority="236" operator="beginsWith" text="#">
       <formula>LEFT(A378,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A379">
-    <cfRule type="containsText" dxfId="503" priority="229" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="505" priority="233" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A379)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="502" priority="230" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="504" priority="234" operator="beginsWith" text="#">
       <formula>LEFT(A379,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A387:A393">
-    <cfRule type="containsText" dxfId="501" priority="227" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="503" priority="231" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A387)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="500" priority="228" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="502" priority="232" operator="beginsWith" text="#">
       <formula>LEFT(A387,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A385">
-    <cfRule type="containsText" dxfId="499" priority="225" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="501" priority="229" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A385)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="498" priority="226" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="500" priority="230" operator="beginsWith" text="#">
       <formula>LEFT(A385,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A394 A398:A401">
-    <cfRule type="containsText" dxfId="497" priority="223" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="499" priority="227" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A394)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="496" priority="224" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="498" priority="228" operator="beginsWith" text="#">
       <formula>LEFT(A394,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A406">
-    <cfRule type="containsText" dxfId="495" priority="221" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="497" priority="225" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A406)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="494" priority="222" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="496" priority="226" operator="beginsWith" text="#">
       <formula>LEFT(A406,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A417">
-    <cfRule type="containsText" dxfId="493" priority="219" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="495" priority="223" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A417)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="492" priority="220" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="494" priority="224" operator="beginsWith" text="#">
       <formula>LEFT(A417,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A380">
-    <cfRule type="containsText" dxfId="491" priority="217" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="493" priority="221" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A380)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="490" priority="218" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="492" priority="222" operator="beginsWith" text="#">
       <formula>LEFT(A380,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A412">
-    <cfRule type="containsText" dxfId="489" priority="215" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="491" priority="219" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A412)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="488" priority="216" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="490" priority="220" operator="beginsWith" text="#">
       <formula>LEFT(A412,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A413">
-    <cfRule type="containsText" dxfId="487" priority="213" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="489" priority="217" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A413)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="486" priority="214" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="488" priority="218" operator="beginsWith" text="#">
       <formula>LEFT(A413,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A414">
-    <cfRule type="containsText" dxfId="485" priority="211" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="487" priority="215" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A414)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="484" priority="212" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="486" priority="216" operator="beginsWith" text="#">
       <formula>LEFT(A414,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A416">
-    <cfRule type="containsText" dxfId="483" priority="207" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="485" priority="211" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A416)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="482" priority="208" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="484" priority="212" operator="beginsWith" text="#">
       <formula>LEFT(A416,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A418">
-    <cfRule type="containsText" dxfId="481" priority="205" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="483" priority="209" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A418)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="480" priority="206" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="482" priority="210" operator="beginsWith" text="#">
       <formula>LEFT(A418,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A419">
-    <cfRule type="containsText" dxfId="479" priority="203" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="481" priority="207" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A419)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="478" priority="204" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="480" priority="208" operator="beginsWith" text="#">
       <formula>LEFT(A419,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A461">
-    <cfRule type="containsText" dxfId="477" priority="201" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="479" priority="205" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A461)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="476" priority="202" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="478" priority="206" operator="beginsWith" text="#">
       <formula>LEFT(A461,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A420">
-    <cfRule type="containsText" dxfId="475" priority="199" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="477" priority="203" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A420)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="474" priority="200" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="476" priority="204" operator="beginsWith" text="#">
       <formula>LEFT(A420,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A421 A425 A428">
-    <cfRule type="containsText" dxfId="473" priority="197" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="475" priority="201" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A421)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="472" priority="198" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="474" priority="202" operator="beginsWith" text="#">
       <formula>LEFT(A421,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A430">
-    <cfRule type="containsText" dxfId="471" priority="193" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="473" priority="197" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A430)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="470" priority="194" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="472" priority="198" operator="beginsWith" text="#">
       <formula>LEFT(A430,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A781">
-    <cfRule type="containsText" dxfId="469" priority="179" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="471" priority="183" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A781)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="468" priority="180" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="470" priority="184" operator="beginsWith" text="#">
       <formula>LEFT(A781,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A782">
-    <cfRule type="containsText" dxfId="467" priority="177" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="469" priority="181" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A782)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="466" priority="178" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="468" priority="182" operator="beginsWith" text="#">
       <formula>LEFT(A782,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A371">
-    <cfRule type="containsText" dxfId="465" priority="175" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="467" priority="179" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A371)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="464" priority="176" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="466" priority="180" operator="beginsWith" text="#">
       <formula>LEFT(A371,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A505">
-    <cfRule type="containsText" dxfId="463" priority="173" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="465" priority="177" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A505)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="462" priority="174" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="464" priority="178" operator="beginsWith" text="#">
       <formula>LEFT(A505,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A506">
-    <cfRule type="containsText" dxfId="461" priority="171" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="463" priority="175" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A506)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="460" priority="172" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="462" priority="176" operator="beginsWith" text="#">
       <formula>LEFT(A506,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A507">
-    <cfRule type="containsText" dxfId="459" priority="169" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="461" priority="173" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A507)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="458" priority="170" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="460" priority="174" operator="beginsWith" text="#">
       <formula>LEFT(A507,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A530">
-    <cfRule type="containsText" dxfId="457" priority="167" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="459" priority="171" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A530)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="456" priority="168" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="458" priority="172" operator="beginsWith" text="#">
       <formula>LEFT(A530,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A526">
-    <cfRule type="containsText" dxfId="455" priority="165" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="457" priority="169" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A526)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="454" priority="166" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="456" priority="170" operator="beginsWith" text="#">
       <formula>LEFT(A526,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A825">
-    <cfRule type="containsText" dxfId="453" priority="161" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="455" priority="165" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A825)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="452" priority="162" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="454" priority="166" operator="beginsWith" text="#">
       <formula>LEFT(A825,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A783">
-    <cfRule type="containsText" dxfId="451" priority="157" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="453" priority="161" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A783)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="450" priority="158" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="452" priority="162" operator="beginsWith" text="#">
       <formula>LEFT(A783,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A261">
-    <cfRule type="containsText" dxfId="449" priority="155" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="451" priority="159" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A261)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="448" priority="156" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="450" priority="160" operator="beginsWith" text="#">
       <formula>LEFT(A261,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A826">
-    <cfRule type="containsText" dxfId="447" priority="145" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="449" priority="149" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A826)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="446" priority="146" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="448" priority="150" operator="beginsWith" text="#">
       <formula>LEFT(A826,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A179:A187 A189:A260">
-    <cfRule type="containsText" dxfId="445" priority="471" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="447" priority="475" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="444" priority="472" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="446" priority="476" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A173 A175 A165 A167:A171 A85 A87:A88 A91:A99 A101:A102 A106:A108 A78 A80:A83">
-    <cfRule type="containsText" dxfId="443" priority="359" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="445" priority="363" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="442" priority="360" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="444" priority="364" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A120">
-    <cfRule type="containsText" dxfId="441" priority="1507" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="443" priority="1511" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="440" priority="1508" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="442" priority="1512" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A159:A160 A163 A138:A147 A121:A122 A113 A111 A115:A119 A149:A150">
-    <cfRule type="containsText" dxfId="439" priority="1789" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="441" priority="1793" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="438" priority="1790" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="440" priority="1794" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A133 A127:A128 A130:A131">
-    <cfRule type="containsText" dxfId="437" priority="1849" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="439" priority="1853" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="436" priority="1850" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="438" priority="1854" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A123">
-    <cfRule type="containsText" dxfId="435" priority="1911" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="437" priority="1915" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="434" priority="1912" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="436" priority="1916" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135">
-    <cfRule type="containsText" dxfId="433" priority="153" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="435" priority="157" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="432" priority="154" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="434" priority="158" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A134">
-    <cfRule type="containsText" dxfId="431" priority="151" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="433" priority="155" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="430" priority="152" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="432" priority="156" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A784">
-    <cfRule type="containsText" dxfId="429" priority="149" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="431" priority="153" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="428" priority="150" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="430" priority="154" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A785">
-    <cfRule type="containsText" dxfId="427" priority="147" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="429" priority="151" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="426" priority="148" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="428" priority="152" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A827">
-    <cfRule type="containsText" dxfId="425" priority="143" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="427" priority="147" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A827)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="424" priority="144" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="426" priority="148" operator="beginsWith" text="#">
       <formula>LEFT(A827,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A828">
-    <cfRule type="containsText" dxfId="423" priority="141" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="425" priority="145" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A826)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="422" priority="142" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="424" priority="146" operator="beginsWith" text="#">
       <formula>LEFT(A826,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B833:B840">
-    <cfRule type="containsText" dxfId="421" priority="117" operator="containsText" text="......">
+  <conditionalFormatting sqref="B833 B840">
+    <cfRule type="containsText" dxfId="423" priority="121" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",B827)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="420" priority="118" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="422" priority="122" operator="beginsWith" text="#">
       <formula>LEFT(B827,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B829 B832">
-    <cfRule type="containsText" dxfId="419" priority="135" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="421" priority="139" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="418" priority="136" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="420" priority="140" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A829">
-    <cfRule type="containsText" dxfId="417" priority="129" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="419" priority="133" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A829)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="416" priority="130" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="418" priority="134" operator="beginsWith" text="#">
       <formula>LEFT(A829,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A830">
-    <cfRule type="containsText" dxfId="415" priority="127" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="417" priority="131" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A830)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="414" priority="128" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="416" priority="132" operator="beginsWith" text="#">
       <formula>LEFT(A830,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B830">
-    <cfRule type="containsText" dxfId="413" priority="125" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="415" priority="129" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="412" priority="126" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="414" priority="130" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A831">
-    <cfRule type="containsText" dxfId="411" priority="123" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="413" priority="127" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A831)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="410" priority="124" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="412" priority="128" operator="beginsWith" text="#">
       <formula>LEFT(A831,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B831">
-    <cfRule type="containsText" dxfId="409" priority="121" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="411" priority="125" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="408" priority="122" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="410" priority="126" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A832:A840">
-    <cfRule type="containsText" dxfId="407" priority="119" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="409" priority="123" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A832)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="406" priority="120" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="408" priority="124" operator="beginsWith" text="#">
       <formula>LEFT(A832,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B841">
-    <cfRule type="containsText" dxfId="405" priority="113" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="407" priority="117" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="404" priority="114" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="406" priority="118" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A841">
-    <cfRule type="containsText" dxfId="403" priority="115" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="405" priority="119" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A817)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="402" priority="116" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="404" priority="120" operator="beginsWith" text="#">
       <formula>LEFT(A817,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A807:A808 A816">
-    <cfRule type="containsText" dxfId="401" priority="109" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="403" priority="113" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A807)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="400" priority="110" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="402" priority="114" operator="beginsWith" text="#">
       <formula>LEFT(A807,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A792">
-    <cfRule type="containsText" dxfId="399" priority="107" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="401" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A792)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="398" priority="108" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="400" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(A792,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A793">
-    <cfRule type="containsText" dxfId="397" priority="105" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="399" priority="109" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A793)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="396" priority="106" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="398" priority="110" operator="beginsWith" text="#">
       <formula>LEFT(A793,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132">
+    <cfRule type="containsText" dxfId="397" priority="105" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="396" priority="106" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A639">
     <cfRule type="containsText" dxfId="395" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -50591,252 +50548,252 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A639">
-    <cfRule type="containsText" dxfId="393" priority="97" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="392" priority="98" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A791">
-    <cfRule type="containsText" dxfId="391" priority="89" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="393" priority="93" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A791)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="390" priority="90" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="392" priority="94" operator="beginsWith" text="#">
       <formula>LEFT(A791,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A806">
-    <cfRule type="containsText" dxfId="389" priority="87" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="391" priority="91" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A806)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="388" priority="88" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="390" priority="92" operator="beginsWith" text="#">
       <formula>LEFT(A806,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A509">
-    <cfRule type="containsText" dxfId="387" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="389" priority="89" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A509)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="386" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="388" priority="90" operator="beginsWith" text="#">
       <formula>LEFT(A509,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A809">
-    <cfRule type="containsText" dxfId="385" priority="83" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="387" priority="87" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A809)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="384" priority="84" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="386" priority="88" operator="beginsWith" text="#">
       <formula>LEFT(A809,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A811">
-    <cfRule type="containsText" dxfId="383" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="385" priority="83" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A811)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="382" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="384" priority="84" operator="beginsWith" text="#">
       <formula>LEFT(A811,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A813">
-    <cfRule type="containsText" dxfId="381" priority="75" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="383" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A813)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="380" priority="76" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="382" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A813,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A814">
-    <cfRule type="containsText" dxfId="379" priority="73" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="381" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A814)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="378" priority="74" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="380" priority="78" operator="beginsWith" text="#">
       <formula>LEFT(A814,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A815">
-    <cfRule type="containsText" dxfId="377" priority="71" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="379" priority="75" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A815)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="376" priority="72" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="378" priority="76" operator="beginsWith" text="#">
       <formula>LEFT(A815,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="375" priority="69" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="377" priority="73" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="374" priority="70" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="376" priority="74" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="373" priority="67" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="375" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="372" priority="68" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="374" priority="72" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A460">
-    <cfRule type="containsText" dxfId="371" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="373" priority="69" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A460)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="370" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="372" priority="70" operator="beginsWith" text="#">
       <formula>LEFT(A460,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A534">
-    <cfRule type="containsText" dxfId="369" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="371" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A534)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="368" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="370" priority="68" operator="beginsWith" text="#">
       <formula>LEFT(A534,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A786">
-    <cfRule type="containsText" dxfId="367" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="369" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A786)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="366" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="368" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A786,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A788">
-    <cfRule type="containsText" dxfId="365" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="367" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A788)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="364" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="366" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(A788,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A498:A499">
-    <cfRule type="containsText" dxfId="363" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="365" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A498)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="362" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="364" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A498,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A415">
-    <cfRule type="containsText" dxfId="361" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="363" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A415)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="360" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="362" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(A415,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A422:A424">
-    <cfRule type="containsText" dxfId="359" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="361" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A422)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="358" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="360" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(A422,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A426:A427">
-    <cfRule type="containsText" dxfId="357" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="359" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A426)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="356" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="358" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(A426,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A431:A433">
-    <cfRule type="containsText" dxfId="355" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="357" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A431)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="354" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="356" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A431,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A429">
-    <cfRule type="containsText" dxfId="353" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="355" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A429)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="352" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="354" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(A429,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="containsText" dxfId="351" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="353" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A27)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="350" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="352" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(A27,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A795">
-    <cfRule type="containsText" dxfId="349" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="351" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A795)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="348" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="350" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A795,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A372">
-    <cfRule type="containsText" dxfId="347" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="349" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A372)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="346" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="348" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A372,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A536">
-    <cfRule type="containsText" dxfId="345" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="347" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A536)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="344" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="346" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A536,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A812">
-    <cfRule type="containsText" dxfId="343" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="345" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A812)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="342" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="344" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A812,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A794">
-    <cfRule type="containsText" dxfId="341" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="343" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A794)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="340" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="342" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A794,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A810">
-    <cfRule type="containsText" dxfId="339" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="341" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A810)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="338" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="340" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A810,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A148">
-    <cfRule type="containsText" dxfId="337" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="339" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="336" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="338" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A787">
-    <cfRule type="containsText" dxfId="309" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="311" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A787)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="308" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="310" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A787,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A434">
-    <cfRule type="containsText" dxfId="307" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="309" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A434)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="306" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="308" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A434,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B834:B839">
+    <cfRule type="containsText" dxfId="307" priority="3019" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",B828)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="306" priority="3020" operator="beginsWith" text="#">
+      <formula>LEFT(B828,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50845,7 +50802,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="621" operator="containsText" text="......" id="{465F9812-1C00-47A7-97E2-89B77398E1B1}">
+          <x14:cfRule type="containsText" priority="625" operator="containsText" text="......" id="{465F9812-1C00-47A7-97E2-89B77398E1B1}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A824)))</xm:f>
             <x14:dxf>
               <font>
@@ -50854,7 +50811,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="622" operator="beginsWith" text="#" id="{900241AA-A787-44C0-BE12-6FDEB9E0011A}">
+          <x14:cfRule type="beginsWith" priority="626" operator="beginsWith" text="#" id="{900241AA-A787-44C0-BE12-6FDEB9E0011A}">
             <xm:f>LEFT(ServoDyn!A824,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -50871,7 +50828,7 @@
           <xm:sqref>A801:A802</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="345" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
+          <x14:cfRule type="containsText" priority="349" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A636)))</xm:f>
             <x14:dxf>
               <font>
@@ -50880,7 +50837,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="346" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
+          <x14:cfRule type="beginsWith" priority="350" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
             <xm:f>LEFT(ServoDyn!A636,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -50897,7 +50854,7 @@
           <xm:sqref>A529</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="269" operator="containsText" text="......" id="{5A5F5B76-44F7-40B2-B037-173F2905189B}">
+          <x14:cfRule type="containsText" priority="273" operator="containsText" text="......" id="{5A5F5B76-44F7-40B2-B037-173F2905189B}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A830)))</xm:f>
             <x14:dxf>
               <font>
@@ -50906,7 +50863,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="270" operator="beginsWith" text="#" id="{804DB11F-C4AE-4232-8FBE-AF82706C5D95}">
+          <x14:cfRule type="beginsWith" priority="274" operator="beginsWith" text="#" id="{804DB11F-C4AE-4232-8FBE-AF82706C5D95}">
             <xm:f>LEFT(ServoDyn!A830,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -50923,7 +50880,7 @@
           <xm:sqref>A822</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2393" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
+          <x14:cfRule type="containsText" priority="2397" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A614)))</xm:f>
             <x14:dxf>
               <font>
@@ -50932,7 +50889,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2394" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
+          <x14:cfRule type="beginsWith" priority="2398" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
             <xm:f>LEFT(ServoDyn!A614,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -50949,7 +50906,7 @@
           <xm:sqref>A37:A39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2427" operator="containsText" text="......" id="{5FD4013B-8363-458B-8AA3-B485798DA1C8}">
+          <x14:cfRule type="containsText" priority="2431" operator="containsText" text="......" id="{5FD4013B-8363-458B-8AA3-B485798DA1C8}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A820)))</xm:f>
             <x14:dxf>
               <font>
@@ -50958,7 +50915,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2428" operator="beginsWith" text="#" id="{5826827B-E3D9-4440-94B4-857DA3C7325E}">
+          <x14:cfRule type="beginsWith" priority="2432" operator="beginsWith" text="#" id="{5826827B-E3D9-4440-94B4-857DA3C7325E}">
             <xm:f>LEFT(ServoDyn!A820,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -50975,7 +50932,7 @@
           <xm:sqref>A800 A798</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2533" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
+          <x14:cfRule type="containsText" priority="2537" operator="containsText" text="......" id="{507E48B0-3CAC-4D71-99A1-A3F8378DB61A}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A193)))</xm:f>
             <x14:dxf>
               <font>
@@ -50984,7 +50941,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2534" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
+          <x14:cfRule type="beginsWith" priority="2538" operator="beginsWith" text="#" id="{898B5379-FC2A-4981-81A9-DB0DC745BCC7}">
             <xm:f>LEFT(ServoDyn!A193,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -51001,7 +50958,7 @@
           <xm:sqref>A100</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="43" operator="containsText" text="......" id="{B3A918C4-B2BC-4D04-A73A-60F23908D5E8}">
+          <x14:cfRule type="containsText" priority="47" operator="containsText" text="......" id="{B3A918C4-B2BC-4D04-A73A-60F23908D5E8}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A638)))</xm:f>
             <x14:dxf>
               <font>
@@ -51010,7 +50967,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="44" operator="beginsWith" text="#" id="{E63D196D-453F-4F6E-A440-3FD5E7A3CCA1}">
+          <x14:cfRule type="beginsWith" priority="48" operator="beginsWith" text="#" id="{E63D196D-453F-4F6E-A440-3FD5E7A3CCA1}">
             <xm:f>LEFT(ServoDyn!A638,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -51027,7 +50984,7 @@
           <xm:sqref>A533</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="41" operator="containsText" text="......" id="{BB3E001D-F2D7-48B8-95E8-E1B214CD528B}">
+          <x14:cfRule type="containsText" priority="45" operator="containsText" text="......" id="{BB3E001D-F2D7-48B8-95E8-E1B214CD528B}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A637)))</xm:f>
             <x14:dxf>
               <font>
@@ -51036,7 +50993,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="42" operator="beginsWith" text="#" id="{70E198F9-0134-498B-8B1B-EE4125788FE9}">
+          <x14:cfRule type="beginsWith" priority="46" operator="beginsWith" text="#" id="{70E198F9-0134-498B-8B1B-EE4125788FE9}">
             <xm:f>LEFT(ServoDyn!A637,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -51053,7 +51010,7 @@
           <xm:sqref>A531:A532</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="27" operator="containsText" text="......" id="{32A27F28-545A-4E1E-B13D-93ECD43750E8}">
+          <x14:cfRule type="containsText" priority="31" operator="containsText" text="......" id="{32A27F28-545A-4E1E-B13D-93ECD43750E8}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A616)))</xm:f>
             <x14:dxf>
               <font>
@@ -51062,7 +51019,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="28" operator="beginsWith" text="#" id="{F7DF63A2-938F-49A3-8D27-034E574DF050}">
+          <x14:cfRule type="beginsWith" priority="32" operator="beginsWith" text="#" id="{F7DF63A2-938F-49A3-8D27-034E574DF050}">
             <xm:f>LEFT(ServoDyn!A616,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -51079,7 +51036,7 @@
           <xm:sqref>A40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="21" operator="containsText" text="......" id="{3A0C7239-4C98-47AB-BB18-55087549381B}">
+          <x14:cfRule type="containsText" priority="25" operator="containsText" text="......" id="{3A0C7239-4C98-47AB-BB18-55087549381B}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A533)))</xm:f>
             <x14:dxf>
               <font>
@@ -51088,7 +51045,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="22" operator="beginsWith" text="#" id="{06E994C0-33A1-42DB-9E68-8282F1C763B6}">
+          <x14:cfRule type="beginsWith" priority="26" operator="beginsWith" text="#" id="{06E994C0-33A1-42DB-9E68-8282F1C763B6}">
             <xm:f>LEFT(ServoDyn!A533,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -51105,7 +51062,7 @@
           <xm:sqref>A538:A540</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="19" operator="containsText" text="......" id="{79FAC2E2-D276-4CB2-82C4-E53DC38EA0CF}">
+          <x14:cfRule type="containsText" priority="23" operator="containsText" text="......" id="{79FAC2E2-D276-4CB2-82C4-E53DC38EA0CF}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A826)))</xm:f>
             <x14:dxf>
               <font>
@@ -51114,7 +51071,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="20" operator="beginsWith" text="#" id="{2FBF85B0-5FE9-42D7-B0FB-8C2117306214}">
+          <x14:cfRule type="beginsWith" priority="24" operator="beginsWith" text="#" id="{2FBF85B0-5FE9-42D7-B0FB-8C2117306214}">
             <xm:f>LEFT(ServoDyn!A826,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -51131,7 +51088,7 @@
           <xm:sqref>A537</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2691" operator="containsText" text="......" id="{3A0C7239-4C98-47AB-BB18-55087549381B}">
+          <x14:cfRule type="containsText" priority="2695" operator="containsText" text="......" id="{3A0C7239-4C98-47AB-BB18-55087549381B}">
             <xm:f>NOT(ISERROR(SEARCH("......",ServoDyn!A535)))</xm:f>
             <x14:dxf>
               <font>
@@ -51140,7 +51097,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="2692" operator="beginsWith" text="#" id="{06E994C0-33A1-42DB-9E68-8282F1C763B6}">
+          <x14:cfRule type="beginsWith" priority="2696" operator="beginsWith" text="#" id="{06E994C0-33A1-42DB-9E68-8282F1C763B6}">
             <xm:f>LEFT(ServoDyn!A535,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -51157,7 +51114,7 @@
           <xm:sqref>A541</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="13" operator="containsText" text="......" id="{6407D79D-0F09-420F-8E90-54150C698CB1}">
+          <x14:cfRule type="containsText" priority="17" operator="containsText" text="......" id="{6407D79D-0F09-420F-8E90-54150C698CB1}">
             <xm:f>NOT(ISERROR(SEARCH("......",FAST!A21)))</xm:f>
             <x14:dxf>
               <font>
@@ -51166,7 +51123,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="beginsWith" priority="14" operator="beginsWith" text="#" id="{3580DF1B-A708-493B-B1F0-861A00779670}">
+          <x14:cfRule type="beginsWith" priority="18" operator="beginsWith" text="#" id="{3580DF1B-A708-493B-B1F0-861A00779670}">
             <xm:f>LEFT(FAST!A21,LEN("#"))="#"</xm:f>
             <x14:dxf>
               <font>
@@ -61454,8 +61411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D109" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="E145" sqref="E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changed MoorDyn location to master instead of matt_current branch; updated dependencies; added mapping between ED and BD hub location for pitch actuator in BD (haven't updated with BD code that contains the implementation, yet).
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1133 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: a505a155a55bbfd14e82a0e62502058dff8fbaeb
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1200" windowWidth="11568" windowHeight="4524" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="1200" windowWidth="11568" windowHeight="4524" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14750" uniqueCount="2654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14759" uniqueCount="2656">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -8195,6 +8195,12 @@
   </si>
   <si>
     <t>BPCutoff</t>
+  </si>
+  <si>
+    <t>ED_P_2_BD_P_Hub</t>
+  </si>
+  <si>
+    <t>"ElastoDyn hub to BeamDyn for hub orientation necessary for pitch actuator"</t>
   </si>
 </sst>
 </file>
@@ -8418,7 +8424,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="882">
+  <dxfs count="872">
     <dxf>
       <font>
         <u val="none"/>
@@ -15815,91 +15821,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -16843,11 +16764,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J418"/>
+  <dimension ref="A1:J419"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A305" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E313" sqref="E313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24034,47 +23955,47 @@
         <v>2504</v>
       </c>
     </row>
-    <row r="313" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A313" s="3" t="s">
+    <row r="313" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A313" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B313" s="27" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C313" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D313" s="27" t="s">
+        <v>1874</v>
+      </c>
+      <c r="E313" s="27" t="s">
+        <v>2654</v>
+      </c>
+      <c r="F313" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G313" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H313" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I313" s="28" t="s">
+        <v>2655</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A314" s="3" t="s">
         <v>1900</v>
       </c>
-      <c r="I313" s="12"/>
-    </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A314" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B314" s="27" t="s">
+      <c r="I314" s="12"/>
+    </row>
+    <row r="315" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A315" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B315" s="27" t="s">
         <v>1757</v>
-      </c>
-      <c r="C314" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D314" s="27" t="s">
-        <v>1874</v>
-      </c>
-      <c r="E314" s="27" t="s">
-        <v>1878</v>
-      </c>
-      <c r="F314" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G314" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H314" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I314" s="28" t="s">
-        <v>1912</v>
-      </c>
-    </row>
-    <row r="315" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A315" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B315" s="27" t="s">
-        <v>27</v>
       </c>
       <c r="C315" s="27" t="s">
         <v>1877</v>
@@ -24083,7 +24004,7 @@
         <v>1874</v>
       </c>
       <c r="E315" s="27" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="F315" s="27" t="s">
         <v>26</v>
@@ -24095,10 +24016,10 @@
         <v>26</v>
       </c>
       <c r="I315" s="28" t="s">
-        <v>1913</v>
-      </c>
-    </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A316" s="27" t="s">
         <v>22</v>
       </c>
@@ -24112,7 +24033,7 @@
         <v>1874</v>
       </c>
       <c r="E316" s="27" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="F316" s="27" t="s">
         <v>26</v>
@@ -24124,7 +24045,7 @@
         <v>26</v>
       </c>
       <c r="I316" s="28" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.3">
@@ -24141,7 +24062,7 @@
         <v>1874</v>
       </c>
       <c r="E317" s="27" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="F317" s="27" t="s">
         <v>26</v>
@@ -24153,7 +24074,7 @@
         <v>26</v>
       </c>
       <c r="I317" s="28" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.3">
@@ -24170,7 +24091,7 @@
         <v>1874</v>
       </c>
       <c r="E318" s="27" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="F318" s="27" t="s">
         <v>26</v>
@@ -24182,7 +24103,7 @@
         <v>26</v>
       </c>
       <c r="I318" s="28" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.3">
@@ -24199,55 +24120,55 @@
         <v>1874</v>
       </c>
       <c r="E319" s="27" t="s">
+        <v>1882</v>
+      </c>
+      <c r="F319" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G319" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H319" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I319" s="28" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="320" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A320" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B320" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C320" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D320" s="27" t="s">
+        <v>1874</v>
+      </c>
+      <c r="E320" s="27" t="s">
         <v>1883</v>
       </c>
-      <c r="F319" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G319" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H319" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I319" s="28" t="s">
+      <c r="F320" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G320" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H320" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I320" s="28" t="s">
         <v>1917</v>
       </c>
     </row>
-    <row r="320" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A320" s="3" t="s">
+    <row r="321" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A321" s="3" t="s">
         <v>2632</v>
       </c>
-      <c r="I320" s="12"/>
-    </row>
-    <row r="321" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A321" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B321" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C321" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D321" s="27" t="s">
-        <v>1874</v>
-      </c>
-      <c r="E321" s="27" t="s">
-        <v>2230</v>
-      </c>
-      <c r="F321" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G321" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H321" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I321" s="28" t="s">
-        <v>2633</v>
-      </c>
+      <c r="I321" s="12"/>
     </row>
     <row r="322" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A322" s="27" t="s">
@@ -24263,55 +24184,55 @@
         <v>1874</v>
       </c>
       <c r="E322" s="27" t="s">
+        <v>2230</v>
+      </c>
+      <c r="F322" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G322" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H322" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I322" s="28" t="s">
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="323" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A323" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B323" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C323" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D323" s="27" t="s">
+        <v>1874</v>
+      </c>
+      <c r="E323" s="27" t="s">
         <v>2231</v>
       </c>
-      <c r="F322" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G322" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H322" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I322" s="28" t="s">
+      <c r="F323" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G323" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H323" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I323" s="28" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="323" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A323" s="3" t="s">
+    <row r="324" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A324" s="3" t="s">
         <v>1899</v>
       </c>
-      <c r="I323" s="12"/>
-    </row>
-    <row r="324" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A324" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B324" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C324" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D324" s="27" t="s">
-        <v>1874</v>
-      </c>
-      <c r="E324" s="27" t="s">
-        <v>1884</v>
-      </c>
-      <c r="F324" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G324" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H324" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I324" s="28" t="s">
-        <v>1918</v>
-      </c>
+      <c r="I324" s="12"/>
     </row>
     <row r="325" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A325" s="27" t="s">
@@ -24327,55 +24248,55 @@
         <v>1874</v>
       </c>
       <c r="E325" s="27" t="s">
+        <v>1884</v>
+      </c>
+      <c r="F325" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G325" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H325" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I325" s="28" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="326" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A326" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B326" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C326" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D326" s="27" t="s">
+        <v>1874</v>
+      </c>
+      <c r="E326" s="27" t="s">
         <v>1885</v>
       </c>
-      <c r="F325" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G325" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H325" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I325" s="28" t="s">
+      <c r="F326" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G326" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H326" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I326" s="28" t="s">
         <v>1919</v>
       </c>
     </row>
-    <row r="326" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A326" s="3" t="s">
+    <row r="327" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A327" s="3" t="s">
         <v>1898</v>
       </c>
-      <c r="I326" s="12"/>
-    </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A327" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B327" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C327" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D327" s="27" t="s">
-        <v>1874</v>
-      </c>
-      <c r="E327" s="27" t="s">
-        <v>1886</v>
-      </c>
-      <c r="F327" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G327" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H327" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I327" s="28" t="s">
-        <v>1920</v>
-      </c>
+      <c r="I327" s="12"/>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A328" s="27" t="s">
@@ -24391,7 +24312,7 @@
         <v>1874</v>
       </c>
       <c r="E328" s="27" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="F328" s="27" t="s">
         <v>26</v>
@@ -24403,7 +24324,7 @@
         <v>26</v>
       </c>
       <c r="I328" s="28" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
@@ -24420,7 +24341,7 @@
         <v>1874</v>
       </c>
       <c r="E329" s="27" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="F329" s="27" t="s">
         <v>26</v>
@@ -24432,7 +24353,7 @@
         <v>26</v>
       </c>
       <c r="I329" s="28" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
@@ -24449,55 +24370,55 @@
         <v>1874</v>
       </c>
       <c r="E330" s="27" t="s">
+        <v>1888</v>
+      </c>
+      <c r="F330" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G330" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H330" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I330" s="28" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A331" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B331" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C331" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D331" s="27" t="s">
+        <v>1874</v>
+      </c>
+      <c r="E331" s="27" t="s">
         <v>1889</v>
       </c>
-      <c r="F330" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G330" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H330" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I330" s="28" t="s">
+      <c r="F331" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G331" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H331" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I331" s="28" t="s">
         <v>1923</v>
       </c>
     </row>
-    <row r="331" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A331" s="3" t="s">
+    <row r="332" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A332" s="3" t="s">
         <v>2201</v>
       </c>
-      <c r="I331" s="12"/>
-    </row>
-    <row r="332" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A332" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B332" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C332" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D332" s="27" t="s">
-        <v>1874</v>
-      </c>
-      <c r="E332" s="27" t="s">
-        <v>2202</v>
-      </c>
-      <c r="F332" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G332" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H332" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I332" s="28" t="s">
-        <v>2203</v>
-      </c>
+      <c r="I332" s="12"/>
     </row>
     <row r="333" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A333" s="27" t="s">
@@ -24513,55 +24434,55 @@
         <v>1874</v>
       </c>
       <c r="E333" s="27" t="s">
+        <v>2202</v>
+      </c>
+      <c r="F333" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G333" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H333" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I333" s="28" t="s">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="334" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A334" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B334" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C334" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D334" s="27" t="s">
+        <v>1874</v>
+      </c>
+      <c r="E334" s="27" t="s">
         <v>2204</v>
       </c>
-      <c r="F333" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G333" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H333" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I333" s="28" t="s">
+      <c r="F334" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G334" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H334" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I334" s="28" t="s">
         <v>2205</v>
       </c>
     </row>
-    <row r="334" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A334" s="3" t="s">
+    <row r="335" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A335" s="3" t="s">
         <v>2540</v>
       </c>
-      <c r="I334" s="12"/>
-    </row>
-    <row r="335" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A335" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B335" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C335" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D335" s="27" t="s">
-        <v>1874</v>
-      </c>
-      <c r="E335" s="27" t="s">
-        <v>2541</v>
-      </c>
-      <c r="F335" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G335" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H335" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I335" s="28" t="s">
-        <v>2546</v>
-      </c>
+      <c r="I335" s="12"/>
     </row>
     <row r="336" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A336" s="27" t="s">
@@ -24577,7 +24498,7 @@
         <v>1874</v>
       </c>
       <c r="E336" s="27" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="F336" s="27" t="s">
         <v>31</v>
@@ -24589,10 +24510,10 @@
         <v>26</v>
       </c>
       <c r="I336" s="28" t="s">
-        <v>2547</v>
-      </c>
-    </row>
-    <row r="337" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>2546</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A337" s="27" t="s">
         <v>22</v>
       </c>
@@ -24606,7 +24527,7 @@
         <v>1874</v>
       </c>
       <c r="E337" s="27" t="s">
-        <v>2545</v>
+        <v>2542</v>
       </c>
       <c r="F337" s="27" t="s">
         <v>31</v>
@@ -24618,43 +24539,43 @@
         <v>26</v>
       </c>
       <c r="I337" s="28" t="s">
+        <v>2547</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A338" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B338" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C338" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D338" s="27" t="s">
+        <v>1874</v>
+      </c>
+      <c r="E338" s="27" t="s">
+        <v>2545</v>
+      </c>
+      <c r="F338" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G338" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H338" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I338" s="28" t="s">
         <v>2548</v>
       </c>
     </row>
-    <row r="338" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A338" s="3" t="s">
+    <row r="339" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A339" s="3" t="s">
         <v>2539</v>
       </c>
-      <c r="I338" s="12"/>
-    </row>
-    <row r="339" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A339" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B339" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C339" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D339" s="27" t="s">
-        <v>1874</v>
-      </c>
-      <c r="E339" s="27" t="s">
-        <v>1890</v>
-      </c>
-      <c r="F339" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G339" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H339" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I339" s="28" t="s">
-        <v>2468</v>
-      </c>
+      <c r="I339" s="12"/>
     </row>
     <row r="340" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A340" s="27" t="s">
@@ -24670,7 +24591,7 @@
         <v>1874</v>
       </c>
       <c r="E340" s="27" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="F340" s="27" t="s">
         <v>26</v>
@@ -24682,7 +24603,7 @@
         <v>26</v>
       </c>
       <c r="I340" s="28" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="341" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -24699,10 +24620,10 @@
         <v>1874</v>
       </c>
       <c r="E341" s="27" t="s">
-        <v>2470</v>
+        <v>1891</v>
       </c>
       <c r="F341" s="27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G341" s="27" t="s">
         <v>26</v>
@@ -24711,7 +24632,7 @@
         <v>26</v>
       </c>
       <c r="I341" s="28" t="s">
-        <v>2471</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="342" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -24728,55 +24649,55 @@
         <v>1874</v>
       </c>
       <c r="E342" s="27" t="s">
+        <v>2470</v>
+      </c>
+      <c r="F342" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G342" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H342" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I342" s="28" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A343" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B343" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C343" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D343" s="27" t="s">
+        <v>1874</v>
+      </c>
+      <c r="E343" s="27" t="s">
         <v>2472</v>
       </c>
-      <c r="F342" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G342" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H342" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I342" s="28" t="s">
+      <c r="F343" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G343" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H343" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I343" s="28" t="s">
         <v>2476</v>
       </c>
     </row>
-    <row r="343" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A343" s="3" t="s">
+    <row r="344" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A344" s="3" t="s">
         <v>1897</v>
       </c>
-      <c r="I343" s="12"/>
-    </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A344" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B344" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C344" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D344" s="27" t="s">
-        <v>1874</v>
-      </c>
-      <c r="E344" s="27" t="s">
-        <v>1892</v>
-      </c>
-      <c r="F344" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G344" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H344" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I344" s="28" t="s">
-        <v>1924</v>
-      </c>
+      <c r="I344" s="12"/>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A345" s="27" t="s">
@@ -24792,55 +24713,55 @@
         <v>1874</v>
       </c>
       <c r="E345" s="27" t="s">
+        <v>1892</v>
+      </c>
+      <c r="F345" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G345" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H345" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I345" s="28" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="346" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A346" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B346" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C346" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D346" s="27" t="s">
+        <v>1874</v>
+      </c>
+      <c r="E346" s="27" t="s">
         <v>1893</v>
       </c>
-      <c r="F345" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G345" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H345" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I345" s="28" t="s">
+      <c r="F346" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G346" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H346" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I346" s="28" t="s">
         <v>1925</v>
       </c>
     </row>
-    <row r="346" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A346" s="3" t="s">
+    <row r="347" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A347" s="3" t="s">
         <v>1896</v>
       </c>
-      <c r="I346" s="12"/>
-    </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A347" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B347" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C347" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D347" s="27" t="s">
-        <v>1874</v>
-      </c>
-      <c r="E347" s="27" t="s">
-        <v>1894</v>
-      </c>
-      <c r="F347" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G347" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H347" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I347" s="28" t="s">
-        <v>1926</v>
-      </c>
+      <c r="I347" s="12"/>
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A348" s="27" t="s">
@@ -24856,7 +24777,7 @@
         <v>1874</v>
       </c>
       <c r="E348" s="27" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="F348" s="27" t="s">
         <v>31</v>
@@ -24868,43 +24789,43 @@
         <v>26</v>
       </c>
       <c r="I348" s="28" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="349" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A349" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B349" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C349" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D349" s="27" t="s">
+        <v>1874</v>
+      </c>
+      <c r="E349" s="27" t="s">
+        <v>1895</v>
+      </c>
+      <c r="F349" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G349" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H349" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I349" s="28" t="s">
         <v>1927</v>
       </c>
     </row>
-    <row r="349" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A349" s="3" t="s">
+    <row r="350" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A350" s="3" t="s">
         <v>1934</v>
       </c>
-      <c r="I349" s="12"/>
-    </row>
-    <row r="350" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A350" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B350" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C350" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D350" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E350" s="27" t="s">
-        <v>2508</v>
-      </c>
-      <c r="F350" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="G350" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H350" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I350" s="28" t="s">
-        <v>2507</v>
-      </c>
+      <c r="I350" s="12"/>
     </row>
     <row r="351" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A351" s="27" t="s">
@@ -24917,13 +24838,13 @@
         <v>1877</v>
       </c>
       <c r="D351" s="27" t="s">
-        <v>1903</v>
+        <v>34</v>
       </c>
       <c r="E351" s="27" t="s">
-        <v>1901</v>
+        <v>2508</v>
       </c>
       <c r="F351" s="27" t="s">
-        <v>31</v>
+        <v>195</v>
       </c>
       <c r="G351" s="27" t="s">
         <v>26</v>
@@ -24932,7 +24853,7 @@
         <v>26</v>
       </c>
       <c r="I351" s="28" t="s">
-        <v>2509</v>
+        <v>2507</v>
       </c>
     </row>
     <row r="352" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -24949,55 +24870,55 @@
         <v>1903</v>
       </c>
       <c r="E352" s="27" t="s">
+        <v>1901</v>
+      </c>
+      <c r="F352" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G352" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H352" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I352" s="28" t="s">
+        <v>2509</v>
+      </c>
+    </row>
+    <row r="353" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A353" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B353" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C353" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D353" s="27" t="s">
+        <v>1903</v>
+      </c>
+      <c r="E353" s="27" t="s">
         <v>1902</v>
       </c>
-      <c r="F352" s="27" t="s">
+      <c r="F353" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="G352" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H352" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I352" s="28" t="s">
+      <c r="G353" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H353" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I353" s="28" t="s">
         <v>1928</v>
       </c>
     </row>
-    <row r="353" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A353" s="3" t="s">
+    <row r="354" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A354" s="3" t="s">
         <v>1935</v>
       </c>
-      <c r="I353" s="12"/>
-    </row>
-    <row r="354" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A354" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B354" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C354" s="27" t="s">
-        <v>1877</v>
-      </c>
-      <c r="D354" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="E354" s="27" t="s">
-        <v>1904</v>
-      </c>
-      <c r="F354" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G354" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H354" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I354" s="28" t="s">
-        <v>1929</v>
-      </c>
+      <c r="I354" s="12"/>
     </row>
     <row r="355" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A355" s="27" t="s">
@@ -25013,7 +24934,7 @@
         <v>56</v>
       </c>
       <c r="E355" s="27" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="F355" s="27" t="s">
         <v>26</v>
@@ -25025,7 +24946,7 @@
         <v>26</v>
       </c>
       <c r="I355" s="28" t="s">
-        <v>1932</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="356" spans="1:9" x14ac:dyDescent="0.3">
@@ -25042,7 +24963,7 @@
         <v>56</v>
       </c>
       <c r="E356" s="27" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="F356" s="27" t="s">
         <v>26</v>
@@ -25054,7 +24975,7 @@
         <v>26</v>
       </c>
       <c r="I356" s="28" t="s">
-        <v>1930</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.3">
@@ -25071,7 +24992,7 @@
         <v>56</v>
       </c>
       <c r="E357" s="27" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="F357" s="27" t="s">
         <v>26</v>
@@ -25100,7 +25021,7 @@
         <v>56</v>
       </c>
       <c r="E358" s="27" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="F358" s="27" t="s">
         <v>26</v>
@@ -25112,7 +25033,7 @@
         <v>26</v>
       </c>
       <c r="I358" s="28" t="s">
-        <v>1933</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.3">
@@ -25129,7 +25050,7 @@
         <v>56</v>
       </c>
       <c r="E359" s="27" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="F359" s="27" t="s">
         <v>26</v>
@@ -25141,7 +25062,7 @@
         <v>26</v>
       </c>
       <c r="I359" s="28" t="s">
-        <v>1931</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.3">
@@ -25158,7 +25079,7 @@
         <v>56</v>
       </c>
       <c r="E360" s="27" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="F360" s="27" t="s">
         <v>26</v>
@@ -25187,7 +25108,7 @@
         <v>56</v>
       </c>
       <c r="E361" s="27" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="F361" s="27" t="s">
         <v>26</v>
@@ -25216,7 +25137,7 @@
         <v>56</v>
       </c>
       <c r="E362" s="27" t="s">
-        <v>2512</v>
+        <v>1911</v>
       </c>
       <c r="F362" s="27" t="s">
         <v>26</v>
@@ -25228,7 +25149,7 @@
         <v>26</v>
       </c>
       <c r="I362" s="28" t="s">
-        <v>2505</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.3">
@@ -25245,7 +25166,7 @@
         <v>56</v>
       </c>
       <c r="E363" s="27" t="s">
-        <v>2511</v>
+        <v>2512</v>
       </c>
       <c r="F363" s="27" t="s">
         <v>26</v>
@@ -25274,10 +25195,10 @@
         <v>56</v>
       </c>
       <c r="E364" s="27" t="s">
-        <v>2510</v>
+        <v>2511</v>
       </c>
       <c r="F364" s="27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G364" s="27" t="s">
         <v>26</v>
@@ -25286,10 +25207,10 @@
         <v>26</v>
       </c>
       <c r="I364" s="28" t="s">
-        <v>2506</v>
-      </c>
-    </row>
-    <row r="365" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="365" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A365" s="27" t="s">
         <v>22</v>
       </c>
@@ -25303,7 +25224,7 @@
         <v>56</v>
       </c>
       <c r="E365" s="27" t="s">
-        <v>2543</v>
+        <v>2510</v>
       </c>
       <c r="F365" s="27" t="s">
         <v>31</v>
@@ -25315,10 +25236,10 @@
         <v>26</v>
       </c>
       <c r="I365" s="28" t="s">
-        <v>2544</v>
-      </c>
-    </row>
-    <row r="366" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="366" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A366" s="27" t="s">
         <v>22</v>
       </c>
@@ -25332,62 +25253,62 @@
         <v>56</v>
       </c>
       <c r="E366" s="27" t="s">
+        <v>2543</v>
+      </c>
+      <c r="F366" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G366" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H366" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I366" s="28" t="s">
+        <v>2544</v>
+      </c>
+    </row>
+    <row r="367" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A367" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B367" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C367" s="27" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D367" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E367" s="27" t="s">
         <v>2637</v>
       </c>
-      <c r="F366" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G366" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H366" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I366" s="28" t="s">
+      <c r="F367" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G367" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H367" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I367" s="28" t="s">
         <v>2638</v>
       </c>
     </row>
-    <row r="367" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A367" s="3" t="s">
+    <row r="368" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A368" s="3" t="s">
         <v>2182</v>
       </c>
-      <c r="I367" s="12"/>
-    </row>
-    <row r="368" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A368" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B368" s="27" t="s">
-        <v>1757</v>
-      </c>
-      <c r="C368" s="27" t="s">
-        <v>2206</v>
-      </c>
-      <c r="D368" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E368" s="27" t="s">
-        <v>959</v>
-      </c>
-      <c r="F368" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G368" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H368" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I368" s="28" t="s">
-        <v>2210</v>
-      </c>
+      <c r="I368" s="12"/>
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A369" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B369" s="27" t="s">
-        <v>27</v>
+        <v>1757</v>
       </c>
       <c r="C369" s="27" t="s">
         <v>2206</v>
@@ -25396,7 +25317,7 @@
         <v>34</v>
       </c>
       <c r="E369" s="27" t="s">
-        <v>955</v>
+        <v>959</v>
       </c>
       <c r="F369" s="27" t="s">
         <v>26</v>
@@ -25408,7 +25329,7 @@
         <v>26</v>
       </c>
       <c r="I369" s="28" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="370" spans="1:10" x14ac:dyDescent="0.3">
@@ -25425,7 +25346,7 @@
         <v>34</v>
       </c>
       <c r="E370" s="27" t="s">
-        <v>1066</v>
+        <v>955</v>
       </c>
       <c r="F370" s="27" t="s">
         <v>26</v>
@@ -25437,7 +25358,7 @@
         <v>26</v>
       </c>
       <c r="I370" s="28" t="s">
-        <v>2213</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="371" spans="1:10" x14ac:dyDescent="0.3">
@@ -25454,7 +25375,7 @@
         <v>34</v>
       </c>
       <c r="E371" s="27" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="F371" s="27" t="s">
         <v>26</v>
@@ -25466,7 +25387,7 @@
         <v>26</v>
       </c>
       <c r="I371" s="28" t="s">
-        <v>2212</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="372" spans="1:10" x14ac:dyDescent="0.3">
@@ -25483,10 +25404,10 @@
         <v>34</v>
       </c>
       <c r="E372" s="27" t="s">
-        <v>1040</v>
-      </c>
-      <c r="F372" s="27">
-        <v>3</v>
+        <v>1067</v>
+      </c>
+      <c r="F372" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="G372" s="27" t="s">
         <v>26</v>
@@ -25495,13 +25416,10 @@
         <v>26</v>
       </c>
       <c r="I372" s="28" t="s">
-        <v>2214</v>
-      </c>
-      <c r="J372" s="27" t="s">
-        <v>2217</v>
-      </c>
-    </row>
-    <row r="373" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="373" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A373" s="27" t="s">
         <v>22</v>
       </c>
@@ -25515,10 +25433,10 @@
         <v>34</v>
       </c>
       <c r="E373" s="27" t="s">
-        <v>961</v>
-      </c>
-      <c r="F373" s="27" t="s">
-        <v>26</v>
+        <v>1040</v>
+      </c>
+      <c r="F373" s="27">
+        <v>3</v>
       </c>
       <c r="G373" s="27" t="s">
         <v>26</v>
@@ -25527,10 +25445,13 @@
         <v>26</v>
       </c>
       <c r="I373" s="28" t="s">
-        <v>2233</v>
-      </c>
-    </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.3">
+        <v>2214</v>
+      </c>
+      <c r="J373" s="27" t="s">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="374" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A374" s="27" t="s">
         <v>22</v>
       </c>
@@ -25544,68 +25465,65 @@
         <v>34</v>
       </c>
       <c r="E374" s="27" t="s">
+        <v>961</v>
+      </c>
+      <c r="F374" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G374" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H374" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I374" s="28" t="s">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="375" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A375" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B375" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C375" s="27" t="s">
+        <v>2206</v>
+      </c>
+      <c r="D375" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E375" s="27" t="s">
         <v>2208</v>
       </c>
-      <c r="F374" s="27">
+      <c r="F375" s="27">
         <v>3</v>
       </c>
-      <c r="G374" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H374" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I374" s="28" t="s">
+      <c r="G375" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H375" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I375" s="28" t="s">
         <v>2209</v>
       </c>
-      <c r="J374" s="27" t="s">
+      <c r="J375" s="27" t="s">
         <v>1426</v>
       </c>
     </row>
-    <row r="376" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A376" s="3" t="s">
+    <row r="377" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A377" s="3" t="s">
         <v>1961</v>
       </c>
-      <c r="I376" s="12"/>
-    </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A377" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B377" s="27" t="s">
-        <v>1757</v>
-      </c>
-      <c r="C377" s="27" t="s">
-        <v>1962</v>
-      </c>
-      <c r="D377" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E377" s="27" t="s">
-        <v>1936</v>
-      </c>
-      <c r="F377" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G377" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H377" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I377" s="28" t="s">
-        <v>1937</v>
-      </c>
-      <c r="J377" s="27" t="s">
-        <v>1938</v>
-      </c>
+      <c r="I377" s="12"/>
     </row>
     <row r="378" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A378" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B378" s="27" t="s">
-        <v>27</v>
+        <v>1757</v>
       </c>
       <c r="C378" s="27" t="s">
         <v>1962</v>
@@ -25614,7 +25532,7 @@
         <v>44</v>
       </c>
       <c r="E378" s="27" t="s">
-        <v>1939</v>
+        <v>1936</v>
       </c>
       <c r="F378" s="27" t="s">
         <v>26</v>
@@ -25626,13 +25544,13 @@
         <v>26</v>
       </c>
       <c r="I378" s="28" t="s">
-        <v>1940</v>
+        <v>1937</v>
       </c>
       <c r="J378" s="27" t="s">
         <v>1938</v>
       </c>
     </row>
-    <row r="379" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A379" s="27" t="s">
         <v>22</v>
       </c>
@@ -25646,7 +25564,7 @@
         <v>44</v>
       </c>
       <c r="E379" s="27" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="F379" s="27" t="s">
         <v>26</v>
@@ -25658,13 +25576,13 @@
         <v>26</v>
       </c>
       <c r="I379" s="28" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="J379" s="27" t="s">
         <v>1938</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A380" s="27" t="s">
         <v>22</v>
       </c>
@@ -25675,10 +25593,10 @@
         <v>1962</v>
       </c>
       <c r="D380" s="27" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E380" s="27" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="F380" s="27" t="s">
         <v>26</v>
@@ -25690,7 +25608,7 @@
         <v>26</v>
       </c>
       <c r="I380" s="28" t="s">
-        <v>1951</v>
+        <v>1942</v>
       </c>
       <c r="J380" s="27" t="s">
         <v>1938</v>
@@ -25710,7 +25628,7 @@
         <v>34</v>
       </c>
       <c r="E381" s="27" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="F381" s="27" t="s">
         <v>26</v>
@@ -25722,7 +25640,7 @@
         <v>26</v>
       </c>
       <c r="I381" s="28" t="s">
-        <v>1949</v>
+        <v>1951</v>
       </c>
       <c r="J381" s="27" t="s">
         <v>1938</v>
@@ -25742,7 +25660,7 @@
         <v>34</v>
       </c>
       <c r="E382" s="27" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="F382" s="27" t="s">
         <v>26</v>
@@ -25754,7 +25672,7 @@
         <v>26</v>
       </c>
       <c r="I382" s="28" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="J382" s="27" t="s">
         <v>1938</v>
@@ -25771,13 +25689,13 @@
         <v>1962</v>
       </c>
       <c r="D383" s="27" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E383" s="27" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="F383" s="27" t="s">
-        <v>1948</v>
+        <v>26</v>
       </c>
       <c r="G383" s="27" t="s">
         <v>26</v>
@@ -25786,7 +25704,10 @@
         <v>26</v>
       </c>
       <c r="I383" s="28" t="s">
-        <v>1952</v>
+        <v>1950</v>
+      </c>
+      <c r="J383" s="27" t="s">
+        <v>1938</v>
       </c>
     </row>
     <row r="384" spans="1:10" x14ac:dyDescent="0.3">
@@ -25803,7 +25724,7 @@
         <v>41</v>
       </c>
       <c r="E384" s="27" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="F384" s="27" t="s">
         <v>1948</v>
@@ -25815,12 +25736,12 @@
         <v>26</v>
       </c>
       <c r="I384" s="28" t="s">
-        <v>1953</v>
-      </c>
-    </row>
-    <row r="385" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="385" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A385" s="27" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B385" s="27" t="s">
         <v>27</v>
@@ -25829,13 +25750,13 @@
         <v>1962</v>
       </c>
       <c r="D385" s="27" t="s">
-        <v>197</v>
+        <v>41</v>
       </c>
       <c r="E385" s="27" t="s">
-        <v>1963</v>
+        <v>1947</v>
       </c>
       <c r="F385" s="27" t="s">
-        <v>26</v>
+        <v>1948</v>
       </c>
       <c r="G385" s="27" t="s">
         <v>26</v>
@@ -25844,15 +25765,12 @@
         <v>26</v>
       </c>
       <c r="I385" s="28" t="s">
-        <v>1964</v>
-      </c>
-      <c r="J385" s="27" t="s">
-        <v>1938</v>
-      </c>
-    </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="386" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A386" s="27" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B386" s="27" t="s">
         <v>27</v>
@@ -25861,10 +25779,10 @@
         <v>1962</v>
       </c>
       <c r="D386" s="27" t="s">
-        <v>1956</v>
+        <v>197</v>
       </c>
       <c r="E386" s="27" t="s">
-        <v>1955</v>
+        <v>1963</v>
       </c>
       <c r="F386" s="27" t="s">
         <v>26</v>
@@ -25876,10 +25794,10 @@
         <v>26</v>
       </c>
       <c r="I386" s="28" t="s">
-        <v>1957</v>
+        <v>1964</v>
       </c>
       <c r="J386" s="27" t="s">
-        <v>1958</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="387" spans="1:10" x14ac:dyDescent="0.3">
@@ -25893,66 +25811,66 @@
         <v>1962</v>
       </c>
       <c r="D387" s="27" t="s">
+        <v>1956</v>
+      </c>
+      <c r="E387" s="27" t="s">
+        <v>1955</v>
+      </c>
+      <c r="F387" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G387" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H387" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I387" s="28" t="s">
+        <v>1957</v>
+      </c>
+      <c r="J387" s="27" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="388" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A388" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B388" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C388" s="27" t="s">
+        <v>1962</v>
+      </c>
+      <c r="D388" s="27" t="s">
         <v>2206</v>
       </c>
-      <c r="E387" s="27" t="s">
+      <c r="E388" s="27" t="s">
         <v>2215</v>
       </c>
-      <c r="F387" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G387" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H387" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I387" s="28" t="s">
+      <c r="F388" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G388" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H388" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I388" s="28" t="s">
         <v>2216</v>
       </c>
-      <c r="J387" s="27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="389" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A389" s="3" t="s">
+      <c r="J388" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="390" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A390" s="3" t="s">
         <v>2207</v>
       </c>
-      <c r="I389" s="12"/>
-    </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A390" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B390" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C390" s="27" t="s">
-        <v>2183</v>
-      </c>
-      <c r="D390" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E390" s="27" t="s">
-        <v>2130</v>
-      </c>
-      <c r="F390" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G390" s="27">
-        <v>-1</v>
-      </c>
-      <c r="H390" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I390" s="28" t="s">
-        <v>2184</v>
-      </c>
-      <c r="J390" s="27" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="391" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I390" s="12"/>
+    </row>
+    <row r="391" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A391" s="27" t="s">
         <v>22</v>
       </c>
@@ -25963,28 +25881,28 @@
         <v>2183</v>
       </c>
       <c r="D391" s="27" t="s">
-        <v>197</v>
+        <v>44</v>
       </c>
       <c r="E391" s="27" t="s">
-        <v>2167</v>
+        <v>2130</v>
       </c>
       <c r="F391" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G391" s="27" t="s">
-        <v>2159</v>
+      <c r="G391" s="27">
+        <v>-1</v>
       </c>
       <c r="H391" s="27" t="s">
         <v>26</v>
       </c>
       <c r="I391" s="28" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="J391" s="27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="392" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="392" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A392" s="27" t="s">
         <v>22</v>
       </c>
@@ -25995,22 +25913,22 @@
         <v>2183</v>
       </c>
       <c r="D392" s="27" t="s">
-        <v>235</v>
+        <v>197</v>
       </c>
       <c r="E392" s="27" t="s">
-        <v>2127</v>
+        <v>2167</v>
       </c>
       <c r="F392" s="27" t="s">
         <v>26</v>
       </c>
       <c r="G392" s="27" t="s">
-        <v>26</v>
+        <v>2159</v>
       </c>
       <c r="H392" s="27" t="s">
         <v>26</v>
       </c>
       <c r="I392" s="28" t="s">
-        <v>2152</v>
+        <v>2185</v>
       </c>
       <c r="J392" s="27" t="s">
         <v>26</v>
@@ -26027,10 +25945,10 @@
         <v>2183</v>
       </c>
       <c r="D393" s="27" t="s">
-        <v>197</v>
+        <v>235</v>
       </c>
       <c r="E393" s="27" t="s">
-        <v>2605</v>
+        <v>2127</v>
       </c>
       <c r="F393" s="27" t="s">
         <v>26</v>
@@ -26042,7 +25960,7 @@
         <v>26</v>
       </c>
       <c r="I393" s="28" t="s">
-        <v>2606</v>
+        <v>2152</v>
       </c>
       <c r="J393" s="27" t="s">
         <v>26</v>
@@ -26059,13 +25977,13 @@
         <v>2183</v>
       </c>
       <c r="D394" s="27" t="s">
-        <v>34</v>
+        <v>197</v>
       </c>
       <c r="E394" s="27" t="s">
-        <v>2607</v>
+        <v>2605</v>
       </c>
       <c r="F394" s="27" t="s">
-        <v>2007</v>
+        <v>26</v>
       </c>
       <c r="G394" s="27" t="s">
         <v>26</v>
@@ -26074,13 +25992,13 @@
         <v>26</v>
       </c>
       <c r="I394" s="28" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
       <c r="J394" s="27" t="s">
-        <v>1426</v>
-      </c>
-    </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="395" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A395" s="27" t="s">
         <v>22</v>
       </c>
@@ -26091,32 +26009,32 @@
         <v>2183</v>
       </c>
       <c r="D395" s="27" t="s">
-        <v>197</v>
+        <v>34</v>
       </c>
       <c r="E395" s="27" t="s">
-        <v>2609</v>
-      </c>
-      <c r="F395" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G395" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H395" s="5" t="s">
+        <v>2607</v>
+      </c>
+      <c r="F395" s="27" t="s">
+        <v>2007</v>
+      </c>
+      <c r="G395" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H395" s="27" t="s">
         <v>26</v>
       </c>
       <c r="I395" s="28" t="s">
-        <v>2611</v>
+        <v>2608</v>
       </c>
       <c r="J395" s="27" t="s">
-        <v>26</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="396" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A396" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B396" s="5" t="s">
+      <c r="B396" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C396" s="27" t="s">
@@ -26126,61 +26044,61 @@
         <v>197</v>
       </c>
       <c r="E396" s="27" t="s">
+        <v>2609</v>
+      </c>
+      <c r="F396" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G396" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H396" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I396" s="28" t="s">
+        <v>2611</v>
+      </c>
+      <c r="J396" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="397" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A397" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B397" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C397" s="27" t="s">
+        <v>2183</v>
+      </c>
+      <c r="D397" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E397" s="27" t="s">
         <v>2610</v>
       </c>
-      <c r="F396" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G396" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H396" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I396" s="28" t="s">
+      <c r="F397" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G397" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H397" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I397" s="28" t="s">
         <v>2612</v>
       </c>
-      <c r="J396" s="27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="398" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A398" s="3" t="s">
+      <c r="J397" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="399" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A399" s="3" t="s">
         <v>2250</v>
       </c>
-      <c r="I398" s="12"/>
-    </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A399" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B399" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C399" s="27" t="s">
-        <v>2252</v>
-      </c>
-      <c r="D399" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="E399" s="27" t="s">
-        <v>2282</v>
-      </c>
-      <c r="F399" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G399" s="27">
-        <v>1</v>
-      </c>
-      <c r="H399" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I399" s="28" t="s">
-        <v>2283</v>
-      </c>
-      <c r="J399" s="27" t="s">
-        <v>26</v>
-      </c>
+      <c r="I399" s="12"/>
     </row>
     <row r="400" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A400" s="27" t="s">
@@ -26193,22 +26111,22 @@
         <v>2252</v>
       </c>
       <c r="D400" s="27" t="s">
-        <v>1965</v>
+        <v>197</v>
       </c>
       <c r="E400" s="27" t="s">
-        <v>2251</v>
+        <v>2282</v>
       </c>
       <c r="F400" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G400" s="27" t="s">
-        <v>26</v>
+      <c r="G400" s="27">
+        <v>1</v>
       </c>
       <c r="H400" s="27" t="s">
         <v>26</v>
       </c>
       <c r="I400" s="28" t="s">
-        <v>2266</v>
+        <v>2283</v>
       </c>
       <c r="J400" s="27" t="s">
         <v>26</v>
@@ -26225,10 +26143,10 @@
         <v>2252</v>
       </c>
       <c r="D401" s="27" t="s">
-        <v>1995</v>
+        <v>1965</v>
       </c>
       <c r="E401" s="27" t="s">
-        <v>2253</v>
+        <v>2251</v>
       </c>
       <c r="F401" s="27" t="s">
         <v>26</v>
@@ -26240,7 +26158,7 @@
         <v>26</v>
       </c>
       <c r="I401" s="28" t="s">
-        <v>2267</v>
+        <v>2266</v>
       </c>
       <c r="J401" s="27" t="s">
         <v>26</v>
@@ -26257,10 +26175,10 @@
         <v>2252</v>
       </c>
       <c r="D402" s="27" t="s">
-        <v>1962</v>
+        <v>1995</v>
       </c>
       <c r="E402" s="27" t="s">
-        <v>2254</v>
+        <v>2253</v>
       </c>
       <c r="F402" s="27" t="s">
         <v>26</v>
@@ -26272,7 +26190,7 @@
         <v>26</v>
       </c>
       <c r="I402" s="28" t="s">
-        <v>2268</v>
+        <v>2267</v>
       </c>
       <c r="J402" s="27" t="s">
         <v>26</v>
@@ -26289,10 +26207,10 @@
         <v>2252</v>
       </c>
       <c r="D403" s="27" t="s">
-        <v>1877</v>
+        <v>1962</v>
       </c>
       <c r="E403" s="27" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
       <c r="F403" s="27" t="s">
         <v>26</v>
@@ -26304,7 +26222,7 @@
         <v>26</v>
       </c>
       <c r="I403" s="28" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="J403" s="27" t="s">
         <v>26</v>
@@ -26321,10 +26239,10 @@
         <v>2252</v>
       </c>
       <c r="D404" s="27" t="s">
-        <v>1792</v>
+        <v>1877</v>
       </c>
       <c r="E404" s="27" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="F404" s="27" t="s">
         <v>26</v>
@@ -26336,7 +26254,7 @@
         <v>26</v>
       </c>
       <c r="I404" s="28" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="J404" s="27" t="s">
         <v>26</v>
@@ -26353,10 +26271,10 @@
         <v>2252</v>
       </c>
       <c r="D405" s="27" t="s">
-        <v>2483</v>
+        <v>1792</v>
       </c>
       <c r="E405" s="27" t="s">
-        <v>2491</v>
+        <v>2256</v>
       </c>
       <c r="F405" s="27" t="s">
         <v>26</v>
@@ -26368,7 +26286,7 @@
         <v>26</v>
       </c>
       <c r="I405" s="28" t="s">
-        <v>2492</v>
+        <v>2270</v>
       </c>
       <c r="J405" s="27" t="s">
         <v>26</v>
@@ -26385,10 +26303,10 @@
         <v>2252</v>
       </c>
       <c r="D406" s="27" t="s">
-        <v>1794</v>
+        <v>2483</v>
       </c>
       <c r="E406" s="27" t="s">
-        <v>2257</v>
+        <v>2491</v>
       </c>
       <c r="F406" s="27" t="s">
         <v>26</v>
@@ -26400,7 +26318,7 @@
         <v>26</v>
       </c>
       <c r="I406" s="28" t="s">
-        <v>2271</v>
+        <v>2492</v>
       </c>
       <c r="J406" s="27" t="s">
         <v>26</v>
@@ -26417,10 +26335,10 @@
         <v>2252</v>
       </c>
       <c r="D407" s="27" t="s">
-        <v>1821</v>
+        <v>1794</v>
       </c>
       <c r="E407" s="27" t="s">
-        <v>2258</v>
+        <v>2257</v>
       </c>
       <c r="F407" s="27" t="s">
         <v>26</v>
@@ -26432,7 +26350,7 @@
         <v>26</v>
       </c>
       <c r="I407" s="28" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
       <c r="J407" s="27" t="s">
         <v>26</v>
@@ -26449,10 +26367,10 @@
         <v>2252</v>
       </c>
       <c r="D408" s="27" t="s">
-        <v>2417</v>
+        <v>1821</v>
       </c>
       <c r="E408" s="27" t="s">
-        <v>2427</v>
+        <v>2258</v>
       </c>
       <c r="F408" s="27" t="s">
         <v>26</v>
@@ -26464,7 +26382,7 @@
         <v>26</v>
       </c>
       <c r="I408" s="28" t="s">
-        <v>2428</v>
+        <v>2272</v>
       </c>
       <c r="J408" s="27" t="s">
         <v>26</v>
@@ -26481,10 +26399,10 @@
         <v>2252</v>
       </c>
       <c r="D409" s="27" t="s">
-        <v>1870</v>
+        <v>2417</v>
       </c>
       <c r="E409" s="27" t="s">
-        <v>2281</v>
+        <v>2427</v>
       </c>
       <c r="F409" s="27" t="s">
         <v>26</v>
@@ -26496,7 +26414,7 @@
         <v>26</v>
       </c>
       <c r="I409" s="28" t="s">
-        <v>2273</v>
+        <v>2428</v>
       </c>
       <c r="J409" s="27" t="s">
         <v>26</v>
@@ -26513,10 +26431,10 @@
         <v>2252</v>
       </c>
       <c r="D410" s="27" t="s">
-        <v>2575</v>
+        <v>1870</v>
       </c>
       <c r="E410" s="27" t="s">
-        <v>2585</v>
+        <v>2281</v>
       </c>
       <c r="F410" s="27" t="s">
         <v>26</v>
@@ -26528,7 +26446,7 @@
         <v>26</v>
       </c>
       <c r="I410" s="28" t="s">
-        <v>2586</v>
+        <v>2273</v>
       </c>
       <c r="J410" s="27" t="s">
         <v>26</v>
@@ -26545,10 +26463,10 @@
         <v>2252</v>
       </c>
       <c r="D411" s="27" t="s">
-        <v>1830</v>
+        <v>2575</v>
       </c>
       <c r="E411" s="27" t="s">
-        <v>2259</v>
+        <v>2585</v>
       </c>
       <c r="F411" s="27" t="s">
         <v>26</v>
@@ -26560,7 +26478,7 @@
         <v>26</v>
       </c>
       <c r="I411" s="28" t="s">
-        <v>2274</v>
+        <v>2586</v>
       </c>
       <c r="J411" s="27" t="s">
         <v>26</v>
@@ -26577,10 +26495,10 @@
         <v>2252</v>
       </c>
       <c r="D412" s="27" t="s">
-        <v>1807</v>
+        <v>1830</v>
       </c>
       <c r="E412" s="27" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="F412" s="27" t="s">
         <v>26</v>
@@ -26592,7 +26510,7 @@
         <v>26</v>
       </c>
       <c r="I412" s="28" t="s">
-        <v>2275</v>
+        <v>2274</v>
       </c>
       <c r="J412" s="27" t="s">
         <v>26</v>
@@ -26609,10 +26527,10 @@
         <v>2252</v>
       </c>
       <c r="D413" s="27" t="s">
-        <v>1867</v>
+        <v>1807</v>
       </c>
       <c r="E413" s="27" t="s">
-        <v>2261</v>
+        <v>2260</v>
       </c>
       <c r="F413" s="27" t="s">
         <v>26</v>
@@ -26624,7 +26542,7 @@
         <v>26</v>
       </c>
       <c r="I413" s="28" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
       <c r="J413" s="27" t="s">
         <v>26</v>
@@ -26641,10 +26559,10 @@
         <v>2252</v>
       </c>
       <c r="D414" s="27" t="s">
-        <v>1849</v>
+        <v>1867</v>
       </c>
       <c r="E414" s="27" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="F414" s="27" t="s">
         <v>26</v>
@@ -26656,7 +26574,7 @@
         <v>26</v>
       </c>
       <c r="I414" s="28" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
       <c r="J414" s="27" t="s">
         <v>26</v>
@@ -26673,10 +26591,10 @@
         <v>2252</v>
       </c>
       <c r="D415" s="27" t="s">
-        <v>2219</v>
+        <v>1849</v>
       </c>
       <c r="E415" s="27" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="F415" s="27" t="s">
         <v>26</v>
@@ -26688,7 +26606,7 @@
         <v>26</v>
       </c>
       <c r="I415" s="28" t="s">
-        <v>2278</v>
+        <v>2277</v>
       </c>
       <c r="J415" s="27" t="s">
         <v>26</v>
@@ -26705,10 +26623,10 @@
         <v>2252</v>
       </c>
       <c r="D416" s="27" t="s">
-        <v>2624</v>
+        <v>2219</v>
       </c>
       <c r="E416" s="27" t="s">
-        <v>2635</v>
+        <v>2263</v>
       </c>
       <c r="F416" s="27" t="s">
         <v>26</v>
@@ -26720,7 +26638,7 @@
         <v>26</v>
       </c>
       <c r="I416" s="28" t="s">
-        <v>2636</v>
+        <v>2278</v>
       </c>
       <c r="J416" s="27" t="s">
         <v>26</v>
@@ -26737,10 +26655,10 @@
         <v>2252</v>
       </c>
       <c r="D417" s="27" t="s">
-        <v>1839</v>
+        <v>2624</v>
       </c>
       <c r="E417" s="27" t="s">
-        <v>2264</v>
+        <v>2635</v>
       </c>
       <c r="F417" s="27" t="s">
         <v>26</v>
@@ -26752,7 +26670,7 @@
         <v>26</v>
       </c>
       <c r="I417" s="28" t="s">
-        <v>2279</v>
+        <v>2636</v>
       </c>
       <c r="J417" s="27" t="s">
         <v>26</v>
@@ -26769,24 +26687,56 @@
         <v>2252</v>
       </c>
       <c r="D418" s="27" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E418" s="27" t="s">
+        <v>2264</v>
+      </c>
+      <c r="F418" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G418" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H418" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I418" s="28" t="s">
+        <v>2279</v>
+      </c>
+      <c r="J418" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="419" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A419" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B419" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C419" s="27" t="s">
+        <v>2252</v>
+      </c>
+      <c r="D419" s="27" t="s">
         <v>1758</v>
       </c>
-      <c r="E418" s="27" t="s">
+      <c r="E419" s="27" t="s">
         <v>2265</v>
       </c>
-      <c r="F418" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G418" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H418" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="I418" s="28" t="s">
+      <c r="F419" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G419" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H419" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I419" s="28" t="s">
         <v>2280</v>
       </c>
-      <c r="J418" s="27" t="s">
+      <c r="J419" s="27" t="s">
         <v>26</v>
       </c>
     </row>
@@ -26935,7 +26885,7 @@
       <formula>LEFT(A206,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A308:A309 A313">
+  <conditionalFormatting sqref="A308:A309 A314">
     <cfRule type="containsText" dxfId="833" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A308)))</formula>
     </cfRule>
@@ -26943,76 +26893,76 @@
       <formula>LEFT(A308,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A320">
+  <conditionalFormatting sqref="A321">
     <cfRule type="containsText" dxfId="831" priority="61" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A320)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A321)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="830" priority="62" operator="beginsWith" text="#">
-      <formula>LEFT(A320,LEN("#"))="#"</formula>
+      <formula>LEFT(A321,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A323">
+  <conditionalFormatting sqref="A324">
     <cfRule type="containsText" dxfId="829" priority="59" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A323)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A324)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="828" priority="60" operator="beginsWith" text="#">
-      <formula>LEFT(A323,LEN("#"))="#"</formula>
+      <formula>LEFT(A324,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A326">
+  <conditionalFormatting sqref="A327">
     <cfRule type="containsText" dxfId="827" priority="57" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A326)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A327)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="826" priority="58" operator="beginsWith" text="#">
-      <formula>LEFT(A326,LEN("#"))="#"</formula>
+      <formula>LEFT(A327,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A334">
+  <conditionalFormatting sqref="A335">
     <cfRule type="containsText" dxfId="825" priority="55" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A334)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A335)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="824" priority="56" operator="beginsWith" text="#">
-      <formula>LEFT(A334,LEN("#"))="#"</formula>
+      <formula>LEFT(A335,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A343">
+  <conditionalFormatting sqref="A344">
     <cfRule type="containsText" dxfId="823" priority="53" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A343)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A344)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="822" priority="54" operator="beginsWith" text="#">
-      <formula>LEFT(A343,LEN("#"))="#"</formula>
+      <formula>LEFT(A344,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A346">
+  <conditionalFormatting sqref="A347">
     <cfRule type="containsText" dxfId="821" priority="51" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A346)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A347)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="820" priority="52" operator="beginsWith" text="#">
-      <formula>LEFT(A346,LEN("#"))="#"</formula>
+      <formula>LEFT(A347,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A349">
+  <conditionalFormatting sqref="A350">
     <cfRule type="containsText" dxfId="819" priority="49" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A349)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A350)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="818" priority="50" operator="beginsWith" text="#">
-      <formula>LEFT(A349,LEN("#"))="#"</formula>
+      <formula>LEFT(A350,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A353">
+  <conditionalFormatting sqref="A354">
     <cfRule type="containsText" dxfId="817" priority="47" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A353)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A354)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="816" priority="48" operator="beginsWith" text="#">
-      <formula>LEFT(A353,LEN("#"))="#"</formula>
+      <formula>LEFT(A354,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A376">
+  <conditionalFormatting sqref="A377">
     <cfRule type="containsText" dxfId="815" priority="45" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A376)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A377)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="814" priority="46" operator="beginsWith" text="#">
-      <formula>LEFT(A376,LEN("#"))="#"</formula>
+      <formula>LEFT(A377,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:A62">
@@ -27079,28 +27029,28 @@
       <formula>LEFT(A98,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A389">
+  <conditionalFormatting sqref="A390">
     <cfRule type="containsText" dxfId="797" priority="27" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A389)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A390)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="796" priority="28" operator="beginsWith" text="#">
-      <formula>LEFT(A389,LEN("#"))="#"</formula>
+      <formula>LEFT(A390,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A331">
+  <conditionalFormatting sqref="A332">
     <cfRule type="containsText" dxfId="795" priority="25" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A331)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A332)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="794" priority="26" operator="beginsWith" text="#">
-      <formula>LEFT(A331,LEN("#"))="#"</formula>
+      <formula>LEFT(A332,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A367">
+  <conditionalFormatting sqref="A368">
     <cfRule type="containsText" dxfId="793" priority="23" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A367)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A368)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="792" priority="24" operator="beginsWith" text="#">
-      <formula>LEFT(A367,LEN("#"))="#"</formula>
+      <formula>LEFT(A368,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A284">
@@ -27111,12 +27061,12 @@
       <formula>LEFT(A284,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A398">
+  <conditionalFormatting sqref="A399">
     <cfRule type="containsText" dxfId="789" priority="19" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A398)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A399)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="788" priority="20" operator="beginsWith" text="#">
-      <formula>LEFT(A398,LEN("#"))="#"</formula>
+      <formula>LEFT(A399,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A182">
@@ -27159,12 +27109,12 @@
       <formula>LEFT(A310,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A338">
+  <conditionalFormatting sqref="A339">
     <cfRule type="containsText" dxfId="777" priority="5" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A338)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A339)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="776" priority="6" operator="beginsWith" text="#">
-      <formula>LEFT(A338,LEN("#"))="#"</formula>
+      <formula>LEFT(A339,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A218">
@@ -52605,7 +52555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
@@ -61756,34 +61706,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130">
-    <cfRule type="containsText" dxfId="185" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="209" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A130)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="184" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="208" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A130,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A164">
-    <cfRule type="containsText" dxfId="183" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="207" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A164)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="182" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="206" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A164,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A195">
-    <cfRule type="containsText" dxfId="181" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="205" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A195)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="180" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="204" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A195,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A163">
-    <cfRule type="containsText" dxfId="179" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="203" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="178" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="202" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
made translation displacements double precision for BD coupling in single precision; updated dependencies;
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1140 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: e65fcab4008e57fcd37d9553f75f8c613abebf66
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -27120,8 +27120,8 @@
   <dimension ref="A1:J841"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A520" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E531" sqref="A1:XFD1048576"/>
+      <pane ySplit="11" topLeftCell="A539" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E549" sqref="E549"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36784,7 +36784,7 @@
         <v>1398</v>
       </c>
       <c r="D351" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E351" s="5" t="s">
         <v>718</v>
@@ -36816,7 +36816,7 @@
         <v>1398</v>
       </c>
       <c r="D352" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E352" s="5" t="s">
         <v>719</v>
@@ -36848,7 +36848,7 @@
         <v>1398</v>
       </c>
       <c r="D353" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E353" s="5" t="s">
         <v>720</v>
@@ -36880,7 +36880,7 @@
         <v>1398</v>
       </c>
       <c r="D354" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E354" s="5" t="s">
         <v>721</v>
@@ -36912,7 +36912,7 @@
         <v>1398</v>
       </c>
       <c r="D355" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E355" s="5" t="s">
         <v>722</v>
@@ -36944,7 +36944,7 @@
         <v>1398</v>
       </c>
       <c r="D356" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E356" s="5" t="s">
         <v>723</v>
@@ -36976,7 +36976,7 @@
         <v>1398</v>
       </c>
       <c r="D357" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E357" s="5" t="s">
         <v>724</v>
@@ -37008,7 +37008,7 @@
         <v>1398</v>
       </c>
       <c r="D358" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E358" s="5" t="s">
         <v>725</v>
@@ -37040,7 +37040,7 @@
         <v>1398</v>
       </c>
       <c r="D359" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E359" s="5" t="s">
         <v>726</v>
@@ -37072,7 +37072,7 @@
         <v>1398</v>
       </c>
       <c r="D360" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E360" s="5" t="s">
         <v>727</v>
@@ -37104,7 +37104,7 @@
         <v>1398</v>
       </c>
       <c r="D361" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E361" s="5" t="s">
         <v>1451</v>
@@ -37136,7 +37136,7 @@
         <v>1398</v>
       </c>
       <c r="D362" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E362" s="5" t="s">
         <v>1453</v>
@@ -37168,7 +37168,7 @@
         <v>1398</v>
       </c>
       <c r="D363" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E363" s="5" t="s">
         <v>1454</v>
@@ -37200,7 +37200,7 @@
         <v>1398</v>
       </c>
       <c r="D364" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E364" s="5" t="s">
         <v>1458</v>
@@ -37232,7 +37232,7 @@
         <v>1398</v>
       </c>
       <c r="D365" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E365" s="5" t="s">
         <v>1460</v>
@@ -37264,7 +37264,7 @@
         <v>1398</v>
       </c>
       <c r="D366" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E366" s="5" t="s">
         <v>1461</v>
@@ -37296,7 +37296,7 @@
         <v>1398</v>
       </c>
       <c r="D367" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E367" s="5" t="s">
         <v>1463</v>
@@ -37328,7 +37328,7 @@
         <v>1398</v>
       </c>
       <c r="D368" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E368" s="5" t="s">
         <v>1465</v>
@@ -37360,7 +37360,7 @@
         <v>1398</v>
       </c>
       <c r="D369" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E369" s="5" t="s">
         <v>1467</v>
@@ -37392,7 +37392,7 @@
         <v>1398</v>
       </c>
       <c r="D370" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E370" s="5" t="s">
         <v>1469</v>
@@ -37424,7 +37424,7 @@
         <v>1398</v>
       </c>
       <c r="D371" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E371" s="5" t="s">
         <v>2171</v>
@@ -37456,7 +37456,7 @@
         <v>1398</v>
       </c>
       <c r="D372" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E372" s="5" t="s">
         <v>1471</v>
@@ -37488,7 +37488,7 @@
         <v>1398</v>
       </c>
       <c r="D373" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E373" s="5" t="s">
         <v>1473</v>
@@ -37520,7 +37520,7 @@
         <v>1398</v>
       </c>
       <c r="D374" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E374" s="5" t="s">
         <v>1475</v>
@@ -37552,7 +37552,7 @@
         <v>1398</v>
       </c>
       <c r="D375" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E375" s="5" t="s">
         <v>1477</v>
@@ -37584,7 +37584,7 @@
         <v>1398</v>
       </c>
       <c r="D376" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E376" s="5" t="s">
         <v>1479</v>
@@ -37616,7 +37616,7 @@
         <v>1398</v>
       </c>
       <c r="D377" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E377" s="5" t="s">
         <v>1481</v>
@@ -37648,7 +37648,7 @@
         <v>1398</v>
       </c>
       <c r="D378" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E378" s="5" t="s">
         <v>1483</v>
@@ -38359,7 +38359,7 @@
         <v>1398</v>
       </c>
       <c r="D404" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E404" s="5" t="s">
         <v>729</v>
@@ -40842,7 +40842,7 @@
         <v>1398</v>
       </c>
       <c r="D493" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E493" s="5" t="s">
         <v>728</v>
@@ -42185,7 +42185,7 @@
         <v>43</v>
       </c>
       <c r="D549" s="5" t="s">
-        <v>34</v>
+        <v>2653</v>
       </c>
       <c r="E549" s="5" t="s">
         <v>246</v>

</xml_diff>

<commit_message>
updated dependencies and modified FAST version date added check that OrcaFlex can't be used with restart capabilities
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1153 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: b3874115b934a278c2935d4cb38e945527dd3b1a
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1200" windowWidth="11568" windowHeight="4524" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="1200" windowWidth="11568" windowHeight="4524" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="2" r:id="rId1"/>
@@ -16743,9 +16743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J419"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A305" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E313" sqref="E313"/>
+      <selection pane="bottomLeft" activeCell="I312" sqref="I312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27119,9 +27119,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J841"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="11" topLeftCell="A539" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E549" sqref="E549"/>
+      <selection pane="bottomLeft" activeCell="D551" sqref="D551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
renamed NumSCin and NumSCout to NumCtrl2SC and NumSC2Ctrl for a little more clarity. Fixed copy-paste error that used u instead of y in the supercontroller data arrays
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1164 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: b144e48c2069d36811b771b012435ab56a6788e5
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -8053,12 +8053,6 @@
     <t>"Initial position of turbine base (origin used in future for graphics)"</t>
   </si>
   <si>
-    <t>NumSCin</t>
-  </si>
-  <si>
-    <t>NumSCout</t>
-  </si>
-  <si>
     <t>"number of controller inputs [from supercontroller]"</t>
   </si>
   <si>
@@ -8195,6 +8189,12 @@
   </si>
   <si>
     <t>R8Ki</t>
+  </si>
+  <si>
+    <t>NumSC2Ctrl</t>
+  </si>
+  <si>
+    <t>NumCtrl2SC</t>
   </si>
 </sst>
 </file>
@@ -16743,9 +16743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J419"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A305" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I312" sqref="I312"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17011,7 +17011,7 @@
         <v>1752</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -17497,7 +17497,7 @@
         <v>41</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>2615</v>
+        <v>2613</v>
       </c>
       <c r="F53" s="27" t="s">
         <v>26</v>
@@ -17506,7 +17506,7 @@
         <v>13</v>
       </c>
       <c r="I53" s="28" t="s">
-        <v>2616</v>
+        <v>2614</v>
       </c>
       <c r="J53" s="27" t="e">
         <f>-A53</f>
@@ -18126,7 +18126,7 @@
         <v>197</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>2636</v>
+        <v>2634</v>
       </c>
       <c r="F77" s="27" t="s">
         <v>1945</v>
@@ -18138,7 +18138,7 @@
         <v>26</v>
       </c>
       <c r="I77" s="28" t="s">
-        <v>2637</v>
+        <v>2635</v>
       </c>
       <c r="J77" s="27" t="s">
         <v>26</v>
@@ -18207,7 +18207,7 @@
         <v>26</v>
       </c>
       <c r="I80" s="28" t="s">
-        <v>2619</v>
+        <v>2617</v>
       </c>
       <c r="J80" s="27" t="s">
         <v>26</v>
@@ -18239,7 +18239,7 @@
         <v>26</v>
       </c>
       <c r="I81" s="28" t="s">
-        <v>2618</v>
+        <v>2616</v>
       </c>
       <c r="J81" s="27" t="s">
         <v>26</v>
@@ -18367,7 +18367,7 @@
         <v>26</v>
       </c>
       <c r="I85" s="28" t="s">
-        <v>2617</v>
+        <v>2615</v>
       </c>
       <c r="J85" s="27" t="s">
         <v>26</v>
@@ -23562,7 +23562,7 @@
     </row>
     <row r="296" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A296" s="3" t="s">
-        <v>2620</v>
+        <v>2618</v>
       </c>
       <c r="I296" s="12"/>
     </row>
@@ -23574,10 +23574,10 @@
         <v>1754</v>
       </c>
       <c r="C297" s="27" t="s">
-        <v>2621</v>
+        <v>2619</v>
       </c>
       <c r="D297" s="27" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="E297" s="27" t="s">
         <v>1763</v>
@@ -23606,7 +23606,7 @@
         <v>27</v>
       </c>
       <c r="D298" s="27" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="E298" s="27" t="s">
         <v>1764</v>
@@ -23635,7 +23635,7 @@
         <v>27</v>
       </c>
       <c r="D299" s="27" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
       <c r="E299" s="27" t="s">
         <v>1765</v>
@@ -23664,7 +23664,7 @@
         <v>27</v>
       </c>
       <c r="D300" s="27" t="s">
-        <v>2625</v>
+        <v>2623</v>
       </c>
       <c r="E300" s="27" t="s">
         <v>1766</v>
@@ -23693,7 +23693,7 @@
         <v>27</v>
       </c>
       <c r="D301" s="27" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
       <c r="E301" s="27" t="s">
         <v>1767</v>
@@ -23722,7 +23722,7 @@
         <v>27</v>
       </c>
       <c r="D302" s="27" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
       <c r="E302" s="27" t="s">
         <v>1768</v>
@@ -23751,7 +23751,7 @@
         <v>27</v>
       </c>
       <c r="D303" s="27" t="s">
-        <v>2628</v>
+        <v>2626</v>
       </c>
       <c r="E303" s="27" t="s">
         <v>1769</v>
@@ -23780,7 +23780,7 @@
         <v>27</v>
       </c>
       <c r="D304" s="27" t="s">
-        <v>2625</v>
+        <v>2623</v>
       </c>
       <c r="E304" s="27" t="s">
         <v>1770</v>
@@ -23809,7 +23809,7 @@
         <v>27</v>
       </c>
       <c r="D305" s="27" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
       <c r="E305" s="27" t="s">
         <v>1771</v>
@@ -23946,7 +23946,7 @@
         <v>1871</v>
       </c>
       <c r="E313" s="27" t="s">
-        <v>2651</v>
+        <v>2649</v>
       </c>
       <c r="F313" s="27" t="s">
         <v>31</v>
@@ -23958,7 +23958,7 @@
         <v>26</v>
       </c>
       <c r="I313" s="28" t="s">
-        <v>2652</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="314" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -24143,7 +24143,7 @@
     </row>
     <row r="321" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A321" s="3" t="s">
-        <v>2629</v>
+        <v>2627</v>
       </c>
       <c r="I321" s="12"/>
     </row>
@@ -24173,7 +24173,7 @@
         <v>26</v>
       </c>
       <c r="I322" s="28" t="s">
-        <v>2630</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="323" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -24202,7 +24202,7 @@
         <v>26</v>
       </c>
       <c r="I323" s="28" t="s">
-        <v>2631</v>
+        <v>2629</v>
       </c>
     </row>
     <row r="324" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -25259,7 +25259,7 @@
         <v>56</v>
       </c>
       <c r="E367" s="27" t="s">
-        <v>2634</v>
+        <v>2632</v>
       </c>
       <c r="F367" s="27" t="s">
         <v>26</v>
@@ -25271,7 +25271,7 @@
         <v>26</v>
       </c>
       <c r="I367" s="28" t="s">
-        <v>2635</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="368" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -26021,19 +26021,19 @@
         <v>197</v>
       </c>
       <c r="E396" s="27" t="s">
+        <v>2652</v>
+      </c>
+      <c r="F396" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G396" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H396" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I396" s="28" t="s">
         <v>2606</v>
-      </c>
-      <c r="F396" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G396" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H396" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I396" s="28" t="s">
-        <v>2608</v>
       </c>
       <c r="J396" s="27" t="s">
         <v>26</v>
@@ -26053,19 +26053,19 @@
         <v>197</v>
       </c>
       <c r="E397" s="27" t="s">
+        <v>2653</v>
+      </c>
+      <c r="F397" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G397" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H397" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I397" s="28" t="s">
         <v>2607</v>
-      </c>
-      <c r="F397" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G397" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H397" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I397" s="28" t="s">
-        <v>2609</v>
       </c>
       <c r="J397" s="27" t="s">
         <v>26</v>
@@ -26632,10 +26632,10 @@
         <v>2249</v>
       </c>
       <c r="D417" s="27" t="s">
-        <v>2621</v>
+        <v>2619</v>
       </c>
       <c r="E417" s="27" t="s">
-        <v>2632</v>
+        <v>2630</v>
       </c>
       <c r="F417" s="27" t="s">
         <v>26</v>
@@ -26647,7 +26647,7 @@
         <v>26</v>
       </c>
       <c r="I417" s="28" t="s">
-        <v>2633</v>
+        <v>2631</v>
       </c>
       <c r="J417" s="27" t="s">
         <v>26</v>
@@ -34377,7 +34377,7 @@
         <v>1249</v>
       </c>
       <c r="D268" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E268" s="7" t="s">
         <v>89</v>
@@ -34409,7 +34409,7 @@
         <v>1249</v>
       </c>
       <c r="D269" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E269" s="7" t="s">
         <v>90</v>
@@ -34441,7 +34441,7 @@
         <v>1249</v>
       </c>
       <c r="D270" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E270" s="7" t="s">
         <v>91</v>
@@ -34473,7 +34473,7 @@
         <v>1249</v>
       </c>
       <c r="D271" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E271" s="7" t="s">
         <v>92</v>
@@ -34505,7 +34505,7 @@
         <v>1249</v>
       </c>
       <c r="D272" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E272" s="7" t="s">
         <v>93</v>
@@ -34537,7 +34537,7 @@
         <v>1249</v>
       </c>
       <c r="D273" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E273" s="7" t="s">
         <v>94</v>
@@ -34569,7 +34569,7 @@
         <v>1249</v>
       </c>
       <c r="D274" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E274" s="7" t="s">
         <v>95</v>
@@ -34601,7 +34601,7 @@
         <v>1249</v>
       </c>
       <c r="D275" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E275" s="7" t="s">
         <v>96</v>
@@ -34633,7 +34633,7 @@
         <v>1249</v>
       </c>
       <c r="D276" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E276" s="7" t="s">
         <v>97</v>
@@ -34665,7 +34665,7 @@
         <v>1249</v>
       </c>
       <c r="D277" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E277" s="9" t="s">
         <v>98</v>
@@ -34697,7 +34697,7 @@
         <v>1249</v>
       </c>
       <c r="D278" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E278" s="9" t="s">
         <v>99</v>
@@ -34729,7 +34729,7 @@
         <v>1249</v>
       </c>
       <c r="D279" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E279" s="9" t="s">
         <v>100</v>
@@ -34761,7 +34761,7 @@
         <v>1249</v>
       </c>
       <c r="D280" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E280" s="9" t="s">
         <v>101</v>
@@ -34793,7 +34793,7 @@
         <v>1249</v>
       </c>
       <c r="D281" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E281" s="9" t="s">
         <v>102</v>
@@ -34825,7 +34825,7 @@
         <v>1249</v>
       </c>
       <c r="D282" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E282" s="9" t="s">
         <v>103</v>
@@ -34857,7 +34857,7 @@
         <v>1249</v>
       </c>
       <c r="D283" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E283" s="9" t="s">
         <v>104</v>
@@ -34889,7 +34889,7 @@
         <v>1249</v>
       </c>
       <c r="D284" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E284" s="9" t="s">
         <v>105</v>
@@ -34921,7 +34921,7 @@
         <v>1249</v>
       </c>
       <c r="D285" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E285" s="9" t="s">
         <v>106</v>
@@ -34953,7 +34953,7 @@
         <v>1249</v>
       </c>
       <c r="D286" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E286" s="9" t="s">
         <v>107</v>
@@ -34985,7 +34985,7 @@
         <v>1249</v>
       </c>
       <c r="D287" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E287" s="9" t="s">
         <v>108</v>
@@ -35017,7 +35017,7 @@
         <v>1249</v>
       </c>
       <c r="D288" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E288" s="9" t="s">
         <v>109</v>
@@ -35049,7 +35049,7 @@
         <v>1249</v>
       </c>
       <c r="D289" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E289" s="10" t="s">
         <v>110</v>
@@ -35081,7 +35081,7 @@
         <v>1249</v>
       </c>
       <c r="D290" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E290" s="10" t="s">
         <v>111</v>
@@ -35113,7 +35113,7 @@
         <v>1249</v>
       </c>
       <c r="D291" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E291" s="10" t="s">
         <v>112</v>
@@ -35145,7 +35145,7 @@
         <v>1249</v>
       </c>
       <c r="D292" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E292" s="10" t="s">
         <v>113</v>
@@ -35177,7 +35177,7 @@
         <v>1249</v>
       </c>
       <c r="D293" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E293" s="10" t="s">
         <v>114</v>
@@ -35209,7 +35209,7 @@
         <v>1249</v>
       </c>
       <c r="D294" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E294" s="10" t="s">
         <v>115</v>
@@ -35241,7 +35241,7 @@
         <v>1249</v>
       </c>
       <c r="D295" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E295" s="10" t="s">
         <v>116</v>
@@ -35273,7 +35273,7 @@
         <v>1249</v>
       </c>
       <c r="D296" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E296" s="10" t="s">
         <v>117</v>
@@ -35305,7 +35305,7 @@
         <v>1249</v>
       </c>
       <c r="D297" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E297" s="10" t="s">
         <v>118</v>
@@ -35337,7 +35337,7 @@
         <v>1249</v>
       </c>
       <c r="D298" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E298" s="10" t="s">
         <v>119</v>
@@ -35369,7 +35369,7 @@
         <v>1249</v>
       </c>
       <c r="D299" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E299" s="10" t="s">
         <v>120</v>
@@ -35401,7 +35401,7 @@
         <v>1249</v>
       </c>
       <c r="D300" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E300" s="10" t="s">
         <v>121</v>
@@ -35433,7 +35433,7 @@
         <v>1249</v>
       </c>
       <c r="D301" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E301" s="10" t="s">
         <v>122</v>
@@ -35465,7 +35465,7 @@
         <v>1249</v>
       </c>
       <c r="D302" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E302" s="10" t="s">
         <v>123</v>
@@ -35497,7 +35497,7 @@
         <v>1249</v>
       </c>
       <c r="D303" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E303" s="10" t="s">
         <v>124</v>
@@ -35529,7 +35529,7 @@
         <v>1249</v>
       </c>
       <c r="D304" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E304" s="10" t="s">
         <v>125</v>
@@ -35561,7 +35561,7 @@
         <v>1249</v>
       </c>
       <c r="D305" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E305" s="10" t="s">
         <v>126</v>
@@ -35593,7 +35593,7 @@
         <v>1249</v>
       </c>
       <c r="D306" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E306" s="10" t="s">
         <v>127</v>
@@ -35625,7 +35625,7 @@
         <v>1249</v>
       </c>
       <c r="D307" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E307" s="10" t="s">
         <v>128</v>
@@ -35657,7 +35657,7 @@
         <v>1249</v>
       </c>
       <c r="D308" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E308" s="10" t="s">
         <v>129</v>
@@ -35689,7 +35689,7 @@
         <v>1249</v>
       </c>
       <c r="D309" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E309" s="10" t="s">
         <v>130</v>
@@ -35721,7 +35721,7 @@
         <v>1249</v>
       </c>
       <c r="D310" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E310" s="10" t="s">
         <v>131</v>
@@ -35753,7 +35753,7 @@
         <v>1249</v>
       </c>
       <c r="D311" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E311" s="10" t="s">
         <v>132</v>
@@ -35785,7 +35785,7 @@
         <v>1249</v>
       </c>
       <c r="D312" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E312" s="10" t="s">
         <v>133</v>
@@ -35817,7 +35817,7 @@
         <v>1249</v>
       </c>
       <c r="D313" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E313" s="10" t="s">
         <v>134</v>
@@ -35849,7 +35849,7 @@
         <v>1249</v>
       </c>
       <c r="D314" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E314" s="10" t="s">
         <v>135</v>
@@ -35881,7 +35881,7 @@
         <v>1249</v>
       </c>
       <c r="D315" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E315" s="10" t="s">
         <v>136</v>
@@ -35913,7 +35913,7 @@
         <v>1249</v>
       </c>
       <c r="D316" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E316" s="10" t="s">
         <v>137</v>
@@ -35945,7 +35945,7 @@
         <v>1249</v>
       </c>
       <c r="D317" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E317" s="10" t="s">
         <v>138</v>
@@ -35977,7 +35977,7 @@
         <v>1249</v>
       </c>
       <c r="D318" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E318" s="10" t="s">
         <v>139</v>
@@ -36009,7 +36009,7 @@
         <v>1249</v>
       </c>
       <c r="D319" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E319" s="10" t="s">
         <v>140</v>
@@ -36041,7 +36041,7 @@
         <v>1249</v>
       </c>
       <c r="D320" s="6" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E320" s="10" t="s">
         <v>141</v>
@@ -36784,7 +36784,7 @@
         <v>1398</v>
       </c>
       <c r="D351" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E351" s="5" t="s">
         <v>718</v>
@@ -36816,7 +36816,7 @@
         <v>1398</v>
       </c>
       <c r="D352" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E352" s="5" t="s">
         <v>719</v>
@@ -36848,7 +36848,7 @@
         <v>1398</v>
       </c>
       <c r="D353" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E353" s="5" t="s">
         <v>720</v>
@@ -36880,7 +36880,7 @@
         <v>1398</v>
       </c>
       <c r="D354" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E354" s="5" t="s">
         <v>721</v>
@@ -36912,7 +36912,7 @@
         <v>1398</v>
       </c>
       <c r="D355" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E355" s="5" t="s">
         <v>722</v>
@@ -36944,7 +36944,7 @@
         <v>1398</v>
       </c>
       <c r="D356" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E356" s="5" t="s">
         <v>723</v>
@@ -36976,7 +36976,7 @@
         <v>1398</v>
       </c>
       <c r="D357" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E357" s="5" t="s">
         <v>724</v>
@@ -37008,7 +37008,7 @@
         <v>1398</v>
       </c>
       <c r="D358" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E358" s="5" t="s">
         <v>725</v>
@@ -37040,7 +37040,7 @@
         <v>1398</v>
       </c>
       <c r="D359" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E359" s="5" t="s">
         <v>726</v>
@@ -37072,7 +37072,7 @@
         <v>1398</v>
       </c>
       <c r="D360" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E360" s="5" t="s">
         <v>727</v>
@@ -37104,7 +37104,7 @@
         <v>1398</v>
       </c>
       <c r="D361" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E361" s="5" t="s">
         <v>1451</v>
@@ -37136,7 +37136,7 @@
         <v>1398</v>
       </c>
       <c r="D362" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E362" s="5" t="s">
         <v>1453</v>
@@ -37168,7 +37168,7 @@
         <v>1398</v>
       </c>
       <c r="D363" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E363" s="5" t="s">
         <v>1454</v>
@@ -37200,7 +37200,7 @@
         <v>1398</v>
       </c>
       <c r="D364" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E364" s="5" t="s">
         <v>1458</v>
@@ -37232,7 +37232,7 @@
         <v>1398</v>
       </c>
       <c r="D365" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E365" s="5" t="s">
         <v>1460</v>
@@ -37264,7 +37264,7 @@
         <v>1398</v>
       </c>
       <c r="D366" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E366" s="5" t="s">
         <v>1461</v>
@@ -37296,7 +37296,7 @@
         <v>1398</v>
       </c>
       <c r="D367" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E367" s="5" t="s">
         <v>1463</v>
@@ -37328,7 +37328,7 @@
         <v>1398</v>
       </c>
       <c r="D368" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E368" s="5" t="s">
         <v>1465</v>
@@ -37360,7 +37360,7 @@
         <v>1398</v>
       </c>
       <c r="D369" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E369" s="5" t="s">
         <v>1467</v>
@@ -37392,7 +37392,7 @@
         <v>1398</v>
       </c>
       <c r="D370" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E370" s="5" t="s">
         <v>1469</v>
@@ -37424,7 +37424,7 @@
         <v>1398</v>
       </c>
       <c r="D371" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E371" s="5" t="s">
         <v>2171</v>
@@ -37456,7 +37456,7 @@
         <v>1398</v>
       </c>
       <c r="D372" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E372" s="5" t="s">
         <v>1471</v>
@@ -37488,7 +37488,7 @@
         <v>1398</v>
       </c>
       <c r="D373" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E373" s="5" t="s">
         <v>1473</v>
@@ -37520,7 +37520,7 @@
         <v>1398</v>
       </c>
       <c r="D374" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E374" s="5" t="s">
         <v>1475</v>
@@ -37552,7 +37552,7 @@
         <v>1398</v>
       </c>
       <c r="D375" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E375" s="5" t="s">
         <v>1477</v>
@@ -37584,7 +37584,7 @@
         <v>1398</v>
       </c>
       <c r="D376" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E376" s="5" t="s">
         <v>1479</v>
@@ -37616,7 +37616,7 @@
         <v>1398</v>
       </c>
       <c r="D377" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E377" s="5" t="s">
         <v>1481</v>
@@ -37648,7 +37648,7 @@
         <v>1398</v>
       </c>
       <c r="D378" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E378" s="5" t="s">
         <v>1483</v>
@@ -38359,7 +38359,7 @@
         <v>1398</v>
       </c>
       <c r="D404" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E404" s="5" t="s">
         <v>729</v>
@@ -40842,7 +40842,7 @@
         <v>1398</v>
       </c>
       <c r="D493" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E493" s="5" t="s">
         <v>728</v>
@@ -41318,7 +41318,7 @@
         <v>33</v>
       </c>
       <c r="D512" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E512" s="5" t="s">
         <v>211</v>
@@ -41609,7 +41609,7 @@
         <v>40</v>
       </c>
       <c r="D527" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E527" s="5" t="s">
         <v>717</v>
@@ -41670,7 +41670,7 @@
         <v>40</v>
       </c>
       <c r="D529" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E529" s="5" t="s">
         <v>639</v>
@@ -41699,7 +41699,7 @@
         <v>40</v>
       </c>
       <c r="D530" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E530" s="5" t="s">
         <v>1746</v>
@@ -41728,7 +41728,7 @@
         <v>40</v>
       </c>
       <c r="D531" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E531" s="5" t="s">
         <v>1748</v>
@@ -42185,7 +42185,7 @@
         <v>43</v>
       </c>
       <c r="D549" s="5" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="E549" s="5" t="s">
         <v>246</v>
@@ -52489,9 +52489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J316"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52961,19 +52961,19 @@
         <v>197</v>
       </c>
       <c r="E33" s="27" t="s">
+        <v>2652</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" s="28" t="s">
         <v>2606</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I33" s="28" t="s">
-        <v>2608</v>
       </c>
       <c r="J33" s="27" t="s">
         <v>26</v>
@@ -52993,19 +52993,19 @@
         <v>197</v>
       </c>
       <c r="E34" s="27" t="s">
+        <v>2653</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I34" s="28" t="s">
         <v>2607</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I34" s="28" t="s">
-        <v>2609</v>
       </c>
       <c r="J34" s="27" t="s">
         <v>26</v>
@@ -54949,19 +54949,19 @@
         <v>235</v>
       </c>
       <c r="E101" s="5" t="s">
+        <v>2644</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I101" s="10" t="s">
         <v>2646</v>
-      </c>
-      <c r="F101" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G101" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H101" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I101" s="10" t="s">
-        <v>2648</v>
       </c>
       <c r="J101" s="5" t="s">
         <v>26</v>
@@ -54981,7 +54981,7 @@
         <v>34</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>2650</v>
+        <v>2648</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>26</v>
@@ -54993,7 +54993,7 @@
         <v>26</v>
       </c>
       <c r="I102" s="10" t="s">
-        <v>2649</v>
+        <v>2647</v>
       </c>
       <c r="J102" s="5" t="s">
         <v>1346</v>
@@ -55831,7 +55831,7 @@
         <v>34</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>2639</v>
+        <v>2637</v>
       </c>
       <c r="F130" s="5" t="s">
         <v>730</v>
@@ -55843,7 +55843,7 @@
         <v>26</v>
       </c>
       <c r="I130" s="10" t="s">
-        <v>2638</v>
+        <v>2636</v>
       </c>
       <c r="J130" s="5" t="s">
         <v>248</v>
@@ -55863,7 +55863,7 @@
         <v>1590</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
       <c r="F131" s="5" t="s">
         <v>31</v>
@@ -55875,7 +55875,7 @@
         <v>26</v>
       </c>
       <c r="I131" s="10" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
       <c r="J131" s="5" t="s">
         <v>26</v>
@@ -55977,7 +55977,7 @@
         <v>34</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>2642</v>
+        <v>2640</v>
       </c>
       <c r="F139" s="5" t="s">
         <v>31</v>
@@ -55989,7 +55989,7 @@
         <v>26</v>
       </c>
       <c r="I139" s="10" t="s">
-        <v>2640</v>
+        <v>2638</v>
       </c>
       <c r="J139" s="5" t="s">
         <v>26</v>
@@ -56629,7 +56629,7 @@
         <v>44</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>2644</v>
+        <v>2642</v>
       </c>
       <c r="F163" s="5" t="s">
         <v>26</v>
@@ -56641,7 +56641,7 @@
         <v>26</v>
       </c>
       <c r="I163" s="10" t="s">
-        <v>2645</v>
+        <v>2643</v>
       </c>
       <c r="J163" s="5" t="s">
         <v>1111</v>
@@ -56661,7 +56661,7 @@
         <v>34</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>2643</v>
+        <v>2641</v>
       </c>
       <c r="F164" s="5" t="s">
         <v>31</v>
@@ -56673,7 +56673,7 @@
         <v>26</v>
       </c>
       <c r="I164" s="10" t="s">
-        <v>2640</v>
+        <v>2638</v>
       </c>
       <c r="J164" s="5" t="s">
         <v>26</v>
@@ -57489,7 +57489,7 @@
         <v>34</v>
       </c>
       <c r="E195" s="5" t="s">
-        <v>2641</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.3">
@@ -58771,7 +58771,7 @@
         <v>235</v>
       </c>
       <c r="E238" s="5" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="F238" s="5" t="s">
         <v>26</v>
@@ -58783,7 +58783,7 @@
         <v>26</v>
       </c>
       <c r="I238" s="10" t="s">
-        <v>2647</v>
+        <v>2645</v>
       </c>
       <c r="J238" s="5" t="s">
         <v>26</v>
@@ -60721,7 +60721,7 @@
         <v>26</v>
       </c>
       <c r="I302" s="5" t="s">
-        <v>2611</v>
+        <v>2609</v>
       </c>
       <c r="J302" s="5" t="s">
         <v>26</v>
@@ -61056,7 +61056,7 @@
         <v>26</v>
       </c>
       <c r="I316" s="5" t="s">
-        <v>2610</v>
+        <v>2608</v>
       </c>
       <c r="J316" s="5" t="s">
         <v>26</v>
@@ -68090,7 +68090,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD19"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68240,19 +68240,19 @@
         <v>197</v>
       </c>
       <c r="E18" s="27" t="s">
+        <v>2652</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="28" t="s">
         <v>2606</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>2608</v>
       </c>
       <c r="J18" s="27" t="s">
         <v>26</v>
@@ -68272,19 +68272,19 @@
         <v>197</v>
       </c>
       <c r="E19" s="27" t="s">
+        <v>2653</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="28" t="s">
         <v>2607</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="28" t="s">
-        <v>2609</v>
       </c>
       <c r="J19" s="27" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
updated ElastoDyn blade input meshes to receive point loads instead of distributed because previous mesh ignored any values input on the blade tip and blade root
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1172 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: f3a7f06778f75cec86e84ea2550231f4875b4767
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14886" uniqueCount="2672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14886" uniqueCount="2673">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -7810,9 +7810,6 @@
     <t>BDED_L_2_AD_L_B</t>
   </si>
   <si>
-    <t>AD_L_2_BDED_L_B</t>
-  </si>
-  <si>
     <t>y_BD_BldMotion_4Loads</t>
   </si>
   <si>
@@ -7820,12 +7817,6 @@
   </si>
   <si>
     <t>BD_L_2_BD_L</t>
-  </si>
-  <si>
-    <t>"Map ElastoDyn BladeLn2Mesh line2 meshes OR BeamDyn BldMotion line2 meshes to AeroDyn14 InputMarkers OR AeroDyn BladeMotion line2 meshes"</t>
-  </si>
-  <si>
-    <t>"Map AeroDyn14 InputMarkers or AeroDyn BladeLoad line2 meshes to ElastoDyn BladeLn2Mesh line2 meshes or BeamDyn BldMotion line2 meshes"</t>
   </si>
   <si>
     <t>"Map BeamDyn BldMotion output meshes to locations on the BD input DistrLoad mesh stored in MeshMapType%y_BD_BldMotion_4Loads (BD input and output meshes are not siblings and in fact have nodes at different locations"</t>
@@ -8249,6 +8240,18 @@
   </si>
   <si>
     <t>"Map ServoDyn tower point mesh to ElastoDyn point load mesh on the tower"</t>
+  </si>
+  <si>
+    <t>BladePtLoads</t>
+  </si>
+  <si>
+    <t>"Map ElastoDyn BladeLn2Mesh point meshes OR BeamDyn BldMotion line2 meshes to AeroDyn14 InputMarkers OR AeroDyn BladeMotion line2 meshes"</t>
+  </si>
+  <si>
+    <t>"Map AeroDyn14 InputMarkers or AeroDyn BladeLoad line2 meshes to ElastoDyn BladePtLoad point meshes or BeamDyn BldMotion line2 meshes"</t>
+  </si>
+  <si>
+    <t>AD_L_2_BDED_B</t>
   </si>
 </sst>
 </file>
@@ -16951,8 +16954,8 @@
   <dimension ref="A1:J421"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17178,7 +17181,7 @@
         <v>1752</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>2572</v>
+        <v>2569</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -17218,7 +17221,7 @@
         <v>1752</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>2605</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -17358,7 +17361,7 @@
         <v>41</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>2539</v>
+        <v>2536</v>
       </c>
       <c r="F42" s="27" t="s">
         <v>26</v>
@@ -17367,7 +17370,7 @@
         <v>2</v>
       </c>
       <c r="I42" s="28" t="s">
-        <v>2540</v>
+        <v>2537</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -17704,7 +17707,7 @@
         <v>41</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>2606</v>
+        <v>2603</v>
       </c>
       <c r="F53" s="27" t="s">
         <v>26</v>
@@ -17713,7 +17716,7 @@
         <v>13</v>
       </c>
       <c r="I53" s="28" t="s">
-        <v>2607</v>
+        <v>2604</v>
       </c>
       <c r="J53" s="27" t="e">
         <f>-A53</f>
@@ -18333,7 +18336,7 @@
         <v>197</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>2627</v>
+        <v>2624</v>
       </c>
       <c r="F77" s="27" t="s">
         <v>1944</v>
@@ -18345,7 +18348,7 @@
         <v>26</v>
       </c>
       <c r="I77" s="28" t="s">
-        <v>2628</v>
+        <v>2625</v>
       </c>
       <c r="J77" s="27" t="s">
         <v>26</v>
@@ -18414,7 +18417,7 @@
         <v>26</v>
       </c>
       <c r="I80" s="28" t="s">
-        <v>2610</v>
+        <v>2607</v>
       </c>
       <c r="J80" s="27" t="s">
         <v>26</v>
@@ -18446,7 +18449,7 @@
         <v>26</v>
       </c>
       <c r="I81" s="28" t="s">
-        <v>2609</v>
+        <v>2606</v>
       </c>
       <c r="J81" s="27" t="s">
         <v>26</v>
@@ -18574,7 +18577,7 @@
         <v>26</v>
       </c>
       <c r="I85" s="28" t="s">
-        <v>2608</v>
+        <v>2605</v>
       </c>
       <c r="J85" s="27" t="s">
         <v>26</v>
@@ -21871,7 +21874,7 @@
     </row>
     <row r="218" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="3" t="s">
-        <v>2574</v>
+        <v>2571</v>
       </c>
       <c r="I218" s="12"/>
     </row>
@@ -21883,10 +21886,10 @@
         <v>1754</v>
       </c>
       <c r="C219" s="27" t="s">
-        <v>2565</v>
+        <v>2562</v>
       </c>
       <c r="D219" s="27" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="E219" s="27" t="s">
         <v>1768</v>
@@ -21915,7 +21918,7 @@
         <v>27</v>
       </c>
       <c r="D220" s="27" t="s">
-        <v>2546</v>
+        <v>2543</v>
       </c>
       <c r="E220" s="27" t="s">
         <v>1769</v>
@@ -21944,7 +21947,7 @@
         <v>27</v>
       </c>
       <c r="D221" s="27" t="s">
-        <v>2573</v>
+        <v>2570</v>
       </c>
       <c r="E221" s="27" t="s">
         <v>1767</v>
@@ -21973,7 +21976,7 @@
         <v>27</v>
       </c>
       <c r="D222" s="27" t="s">
-        <v>2582</v>
+        <v>2579</v>
       </c>
       <c r="E222" s="27" t="s">
         <v>1423</v>
@@ -23769,7 +23772,7 @@
     </row>
     <row r="296" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A296" s="3" t="s">
-        <v>2611</v>
+        <v>2608</v>
       </c>
       <c r="I296" s="12"/>
     </row>
@@ -23781,10 +23784,10 @@
         <v>1754</v>
       </c>
       <c r="C297" s="27" t="s">
-        <v>2612</v>
+        <v>2609</v>
       </c>
       <c r="D297" s="27" t="s">
-        <v>2613</v>
+        <v>2610</v>
       </c>
       <c r="E297" s="27" t="s">
         <v>1763</v>
@@ -23813,7 +23816,7 @@
         <v>27</v>
       </c>
       <c r="D298" s="27" t="s">
-        <v>2614</v>
+        <v>2611</v>
       </c>
       <c r="E298" s="27" t="s">
         <v>1764</v>
@@ -23842,7 +23845,7 @@
         <v>27</v>
       </c>
       <c r="D299" s="27" t="s">
-        <v>2615</v>
+        <v>2612</v>
       </c>
       <c r="E299" s="27" t="s">
         <v>1765</v>
@@ -23871,7 +23874,7 @@
         <v>27</v>
       </c>
       <c r="D300" s="27" t="s">
-        <v>2616</v>
+        <v>2613</v>
       </c>
       <c r="E300" s="27" t="s">
         <v>1766</v>
@@ -23900,7 +23903,7 @@
         <v>27</v>
       </c>
       <c r="D301" s="27" t="s">
-        <v>2617</v>
+        <v>2614</v>
       </c>
       <c r="E301" s="27" t="s">
         <v>1767</v>
@@ -23929,7 +23932,7 @@
         <v>27</v>
       </c>
       <c r="D302" s="27" t="s">
-        <v>2618</v>
+        <v>2615</v>
       </c>
       <c r="E302" s="27" t="s">
         <v>1768</v>
@@ -23958,7 +23961,7 @@
         <v>27</v>
       </c>
       <c r="D303" s="27" t="s">
-        <v>2619</v>
+        <v>2616</v>
       </c>
       <c r="E303" s="27" t="s">
         <v>1769</v>
@@ -23987,7 +23990,7 @@
         <v>27</v>
       </c>
       <c r="D304" s="27" t="s">
-        <v>2616</v>
+        <v>2613</v>
       </c>
       <c r="E304" s="27" t="s">
         <v>1770</v>
@@ -24016,7 +24019,7 @@
         <v>27</v>
       </c>
       <c r="D305" s="27" t="s">
-        <v>2618</v>
+        <v>2615</v>
       </c>
       <c r="E305" s="27" t="s">
         <v>1771</v>
@@ -24153,7 +24156,7 @@
         <v>1871</v>
       </c>
       <c r="E313" s="27" t="s">
-        <v>2642</v>
+        <v>2639</v>
       </c>
       <c r="F313" s="27" t="s">
         <v>31</v>
@@ -24165,7 +24168,7 @@
         <v>26</v>
       </c>
       <c r="I313" s="28" t="s">
-        <v>2643</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="314" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -24350,7 +24353,7 @@
     </row>
     <row r="321" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A321" s="3" t="s">
-        <v>2620</v>
+        <v>2617</v>
       </c>
       <c r="I321" s="12"/>
     </row>
@@ -24380,7 +24383,7 @@
         <v>26</v>
       </c>
       <c r="I322" s="28" t="s">
-        <v>2621</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="323" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -24409,7 +24412,7 @@
         <v>26</v>
       </c>
       <c r="I323" s="28" t="s">
-        <v>2622</v>
+        <v>2619</v>
       </c>
     </row>
     <row r="324" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -24600,7 +24603,7 @@
     </row>
     <row r="332" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A332" s="3" t="s">
-        <v>2666</v>
+        <v>2663</v>
       </c>
       <c r="I332" s="12"/>
     </row>
@@ -24676,7 +24679,7 @@
         <v>1871</v>
       </c>
       <c r="E335" s="27" t="s">
-        <v>2663</v>
+        <v>2660</v>
       </c>
       <c r="F335" s="27" t="s">
         <v>26</v>
@@ -24688,7 +24691,7 @@
         <v>26</v>
       </c>
       <c r="I335" s="28" t="s">
-        <v>2662</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="336" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -24705,7 +24708,7 @@
         <v>1871</v>
       </c>
       <c r="E336" s="27" t="s">
-        <v>2670</v>
+        <v>2667</v>
       </c>
       <c r="F336" s="27" t="s">
         <v>26</v>
@@ -24717,7 +24720,7 @@
         <v>26</v>
       </c>
       <c r="I336" s="28" t="s">
-        <v>2671</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="337" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -24752,7 +24755,7 @@
         <v>26</v>
       </c>
       <c r="I338" s="28" t="s">
-        <v>2536</v>
+        <v>2670</v>
       </c>
     </row>
     <row r="339" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -24769,7 +24772,7 @@
         <v>1871</v>
       </c>
       <c r="E339" s="27" t="s">
-        <v>2532</v>
+        <v>2672</v>
       </c>
       <c r="F339" s="27" t="s">
         <v>31</v>
@@ -24781,7 +24784,7 @@
         <v>26</v>
       </c>
       <c r="I339" s="28" t="s">
-        <v>2537</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="340" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -24798,7 +24801,7 @@
         <v>1871</v>
       </c>
       <c r="E340" s="27" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="F340" s="27" t="s">
         <v>31</v>
@@ -24810,7 +24813,7 @@
         <v>26</v>
       </c>
       <c r="I340" s="28" t="s">
-        <v>2538</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="341" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -24862,7 +24865,7 @@
         <v>1871</v>
       </c>
       <c r="E343" s="27" t="s">
-        <v>2668</v>
+        <v>2665</v>
       </c>
       <c r="F343" s="27" t="s">
         <v>26</v>
@@ -24874,7 +24877,7 @@
         <v>26</v>
       </c>
       <c r="I343" s="28" t="s">
-        <v>2669</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="344" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -25495,7 +25498,7 @@
         <v>56</v>
       </c>
       <c r="E368" s="27" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="F368" s="27" t="s">
         <v>31</v>
@@ -25507,7 +25510,7 @@
         <v>26</v>
       </c>
       <c r="I368" s="28" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.3">
@@ -25524,7 +25527,7 @@
         <v>56</v>
       </c>
       <c r="E369" s="27" t="s">
-        <v>2625</v>
+        <v>2622</v>
       </c>
       <c r="F369" s="27" t="s">
         <v>26</v>
@@ -25536,7 +25539,7 @@
         <v>26</v>
       </c>
       <c r="I369" s="28" t="s">
-        <v>2626</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="370" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -26222,7 +26225,7 @@
         <v>197</v>
       </c>
       <c r="E396" s="27" t="s">
-        <v>2595</v>
+        <v>2592</v>
       </c>
       <c r="F396" s="27" t="s">
         <v>26</v>
@@ -26234,7 +26237,7 @@
         <v>26</v>
       </c>
       <c r="I396" s="28" t="s">
-        <v>2596</v>
+        <v>2593</v>
       </c>
       <c r="J396" s="27" t="s">
         <v>26</v>
@@ -26254,7 +26257,7 @@
         <v>34</v>
       </c>
       <c r="E397" s="27" t="s">
-        <v>2597</v>
+        <v>2594</v>
       </c>
       <c r="F397" s="27" t="s">
         <v>2003</v>
@@ -26266,7 +26269,7 @@
         <v>26</v>
       </c>
       <c r="I397" s="28" t="s">
-        <v>2598</v>
+        <v>2595</v>
       </c>
       <c r="J397" s="27" t="s">
         <v>1423</v>
@@ -26286,7 +26289,7 @@
         <v>197</v>
       </c>
       <c r="E398" s="27" t="s">
-        <v>2645</v>
+        <v>2642</v>
       </c>
       <c r="F398" s="5" t="s">
         <v>26</v>
@@ -26298,7 +26301,7 @@
         <v>26</v>
       </c>
       <c r="I398" s="28" t="s">
-        <v>2599</v>
+        <v>2596</v>
       </c>
       <c r="J398" s="27" t="s">
         <v>26</v>
@@ -26318,7 +26321,7 @@
         <v>197</v>
       </c>
       <c r="E399" s="27" t="s">
-        <v>2646</v>
+        <v>2643</v>
       </c>
       <c r="F399" s="5" t="s">
         <v>26</v>
@@ -26330,7 +26333,7 @@
         <v>26</v>
       </c>
       <c r="I399" s="28" t="s">
-        <v>2600</v>
+        <v>2597</v>
       </c>
       <c r="J399" s="27" t="s">
         <v>26</v>
@@ -26705,10 +26708,10 @@
         <v>2243</v>
       </c>
       <c r="D413" s="27" t="s">
-        <v>2565</v>
+        <v>2562</v>
       </c>
       <c r="E413" s="27" t="s">
-        <v>2575</v>
+        <v>2572</v>
       </c>
       <c r="F413" s="27" t="s">
         <v>26</v>
@@ -26720,7 +26723,7 @@
         <v>26</v>
       </c>
       <c r="I413" s="28" t="s">
-        <v>2576</v>
+        <v>2573</v>
       </c>
       <c r="J413" s="27" t="s">
         <v>26</v>
@@ -26897,10 +26900,10 @@
         <v>2243</v>
       </c>
       <c r="D419" s="27" t="s">
-        <v>2612</v>
+        <v>2609</v>
       </c>
       <c r="E419" s="27" t="s">
-        <v>2623</v>
+        <v>2620</v>
       </c>
       <c r="F419" s="27" t="s">
         <v>26</v>
@@ -26912,7 +26915,7 @@
         <v>26</v>
       </c>
       <c r="I419" s="28" t="s">
-        <v>2624</v>
+        <v>2621</v>
       </c>
       <c r="J419" s="27" t="s">
         <v>26</v>
@@ -27384,9 +27387,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J842"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A634" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E646" sqref="E646"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A695" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C709" sqref="C709"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28014,7 +28017,7 @@
         <v>34</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>2664</v>
+        <v>2661</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>2003</v>
@@ -28026,7 +28029,7 @@
         <v>26</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>2665</v>
+        <v>2662</v>
       </c>
       <c r="J40" s="5" t="s">
         <v>1423</v>
@@ -34674,7 +34677,7 @@
         <v>1249</v>
       </c>
       <c r="D269" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E269" s="7" t="s">
         <v>89</v>
@@ -34706,7 +34709,7 @@
         <v>1249</v>
       </c>
       <c r="D270" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E270" s="7" t="s">
         <v>90</v>
@@ -34738,7 +34741,7 @@
         <v>1249</v>
       </c>
       <c r="D271" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E271" s="7" t="s">
         <v>91</v>
@@ -34770,7 +34773,7 @@
         <v>1249</v>
       </c>
       <c r="D272" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E272" s="7" t="s">
         <v>92</v>
@@ -34802,7 +34805,7 @@
         <v>1249</v>
       </c>
       <c r="D273" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E273" s="7" t="s">
         <v>93</v>
@@ -34834,7 +34837,7 @@
         <v>1249</v>
       </c>
       <c r="D274" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E274" s="7" t="s">
         <v>94</v>
@@ -34866,7 +34869,7 @@
         <v>1249</v>
       </c>
       <c r="D275" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E275" s="7" t="s">
         <v>95</v>
@@ -34898,7 +34901,7 @@
         <v>1249</v>
       </c>
       <c r="D276" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E276" s="7" t="s">
         <v>96</v>
@@ -34930,7 +34933,7 @@
         <v>1249</v>
       </c>
       <c r="D277" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E277" s="7" t="s">
         <v>97</v>
@@ -34962,7 +34965,7 @@
         <v>1249</v>
       </c>
       <c r="D278" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E278" s="9" t="s">
         <v>98</v>
@@ -34994,7 +34997,7 @@
         <v>1249</v>
       </c>
       <c r="D279" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E279" s="9" t="s">
         <v>99</v>
@@ -35026,7 +35029,7 @@
         <v>1249</v>
       </c>
       <c r="D280" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E280" s="9" t="s">
         <v>100</v>
@@ -35058,7 +35061,7 @@
         <v>1249</v>
       </c>
       <c r="D281" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E281" s="9" t="s">
         <v>101</v>
@@ -35090,7 +35093,7 @@
         <v>1249</v>
       </c>
       <c r="D282" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E282" s="9" t="s">
         <v>102</v>
@@ -35122,7 +35125,7 @@
         <v>1249</v>
       </c>
       <c r="D283" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E283" s="9" t="s">
         <v>103</v>
@@ -35154,7 +35157,7 @@
         <v>1249</v>
       </c>
       <c r="D284" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E284" s="9" t="s">
         <v>104</v>
@@ -35186,7 +35189,7 @@
         <v>1249</v>
       </c>
       <c r="D285" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E285" s="9" t="s">
         <v>105</v>
@@ -35218,7 +35221,7 @@
         <v>1249</v>
       </c>
       <c r="D286" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E286" s="9" t="s">
         <v>106</v>
@@ -35250,7 +35253,7 @@
         <v>1249</v>
       </c>
       <c r="D287" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E287" s="9" t="s">
         <v>107</v>
@@ -35282,7 +35285,7 @@
         <v>1249</v>
       </c>
       <c r="D288" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E288" s="9" t="s">
         <v>108</v>
@@ -35314,7 +35317,7 @@
         <v>1249</v>
       </c>
       <c r="D289" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E289" s="9" t="s">
         <v>109</v>
@@ -35346,7 +35349,7 @@
         <v>1249</v>
       </c>
       <c r="D290" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E290" s="10" t="s">
         <v>110</v>
@@ -35378,7 +35381,7 @@
         <v>1249</v>
       </c>
       <c r="D291" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E291" s="10" t="s">
         <v>111</v>
@@ -35410,7 +35413,7 @@
         <v>1249</v>
       </c>
       <c r="D292" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E292" s="10" t="s">
         <v>112</v>
@@ -35442,7 +35445,7 @@
         <v>1249</v>
       </c>
       <c r="D293" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E293" s="10" t="s">
         <v>113</v>
@@ -35474,7 +35477,7 @@
         <v>1249</v>
       </c>
       <c r="D294" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E294" s="10" t="s">
         <v>114</v>
@@ -35506,7 +35509,7 @@
         <v>1249</v>
       </c>
       <c r="D295" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E295" s="10" t="s">
         <v>115</v>
@@ -35538,7 +35541,7 @@
         <v>1249</v>
       </c>
       <c r="D296" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E296" s="10" t="s">
         <v>116</v>
@@ -35570,7 +35573,7 @@
         <v>1249</v>
       </c>
       <c r="D297" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E297" s="10" t="s">
         <v>117</v>
@@ -35602,7 +35605,7 @@
         <v>1249</v>
       </c>
       <c r="D298" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E298" s="10" t="s">
         <v>118</v>
@@ -35634,7 +35637,7 @@
         <v>1249</v>
       </c>
       <c r="D299" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E299" s="10" t="s">
         <v>119</v>
@@ -35666,7 +35669,7 @@
         <v>1249</v>
       </c>
       <c r="D300" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E300" s="10" t="s">
         <v>120</v>
@@ -35698,7 +35701,7 @@
         <v>1249</v>
       </c>
       <c r="D301" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E301" s="10" t="s">
         <v>121</v>
@@ -35730,7 +35733,7 @@
         <v>1249</v>
       </c>
       <c r="D302" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E302" s="10" t="s">
         <v>122</v>
@@ -35762,7 +35765,7 @@
         <v>1249</v>
       </c>
       <c r="D303" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E303" s="10" t="s">
         <v>123</v>
@@ -35794,7 +35797,7 @@
         <v>1249</v>
       </c>
       <c r="D304" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E304" s="10" t="s">
         <v>124</v>
@@ -35826,7 +35829,7 @@
         <v>1249</v>
       </c>
       <c r="D305" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E305" s="10" t="s">
         <v>125</v>
@@ -35858,7 +35861,7 @@
         <v>1249</v>
       </c>
       <c r="D306" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E306" s="10" t="s">
         <v>126</v>
@@ -35890,7 +35893,7 @@
         <v>1249</v>
       </c>
       <c r="D307" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E307" s="10" t="s">
         <v>127</v>
@@ -35922,7 +35925,7 @@
         <v>1249</v>
       </c>
       <c r="D308" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E308" s="10" t="s">
         <v>128</v>
@@ -35954,7 +35957,7 @@
         <v>1249</v>
       </c>
       <c r="D309" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E309" s="10" t="s">
         <v>129</v>
@@ -35986,7 +35989,7 @@
         <v>1249</v>
       </c>
       <c r="D310" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E310" s="10" t="s">
         <v>130</v>
@@ -36018,7 +36021,7 @@
         <v>1249</v>
       </c>
       <c r="D311" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E311" s="10" t="s">
         <v>131</v>
@@ -36050,7 +36053,7 @@
         <v>1249</v>
       </c>
       <c r="D312" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E312" s="10" t="s">
         <v>132</v>
@@ -36082,7 +36085,7 @@
         <v>1249</v>
       </c>
       <c r="D313" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E313" s="10" t="s">
         <v>133</v>
@@ -36114,7 +36117,7 @@
         <v>1249</v>
       </c>
       <c r="D314" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E314" s="10" t="s">
         <v>134</v>
@@ -36146,7 +36149,7 @@
         <v>1249</v>
       </c>
       <c r="D315" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E315" s="10" t="s">
         <v>135</v>
@@ -36178,7 +36181,7 @@
         <v>1249</v>
       </c>
       <c r="D316" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E316" s="10" t="s">
         <v>136</v>
@@ -36210,7 +36213,7 @@
         <v>1249</v>
       </c>
       <c r="D317" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E317" s="10" t="s">
         <v>137</v>
@@ -36242,7 +36245,7 @@
         <v>1249</v>
       </c>
       <c r="D318" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E318" s="10" t="s">
         <v>138</v>
@@ -36274,7 +36277,7 @@
         <v>1249</v>
       </c>
       <c r="D319" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E319" s="10" t="s">
         <v>139</v>
@@ -36306,7 +36309,7 @@
         <v>1249</v>
       </c>
       <c r="D320" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E320" s="10" t="s">
         <v>140</v>
@@ -36338,7 +36341,7 @@
         <v>1249</v>
       </c>
       <c r="D321" s="6" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E321" s="10" t="s">
         <v>141</v>
@@ -37081,7 +37084,7 @@
         <v>1398</v>
       </c>
       <c r="D352" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E352" s="5" t="s">
         <v>718</v>
@@ -37113,7 +37116,7 @@
         <v>1398</v>
       </c>
       <c r="D353" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E353" s="5" t="s">
         <v>719</v>
@@ -37145,7 +37148,7 @@
         <v>1398</v>
       </c>
       <c r="D354" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E354" s="5" t="s">
         <v>720</v>
@@ -37177,7 +37180,7 @@
         <v>1398</v>
       </c>
       <c r="D355" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E355" s="5" t="s">
         <v>721</v>
@@ -37209,7 +37212,7 @@
         <v>1398</v>
       </c>
       <c r="D356" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E356" s="5" t="s">
         <v>722</v>
@@ -37241,7 +37244,7 @@
         <v>1398</v>
       </c>
       <c r="D357" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E357" s="5" t="s">
         <v>723</v>
@@ -37273,7 +37276,7 @@
         <v>1398</v>
       </c>
       <c r="D358" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E358" s="5" t="s">
         <v>724</v>
@@ -37305,7 +37308,7 @@
         <v>1398</v>
       </c>
       <c r="D359" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E359" s="5" t="s">
         <v>725</v>
@@ -37337,7 +37340,7 @@
         <v>1398</v>
       </c>
       <c r="D360" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E360" s="5" t="s">
         <v>726</v>
@@ -37369,7 +37372,7 @@
         <v>1398</v>
       </c>
       <c r="D361" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E361" s="5" t="s">
         <v>727</v>
@@ -37401,7 +37404,7 @@
         <v>1398</v>
       </c>
       <c r="D362" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E362" s="5" t="s">
         <v>1451</v>
@@ -37433,7 +37436,7 @@
         <v>1398</v>
       </c>
       <c r="D363" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E363" s="5" t="s">
         <v>1453</v>
@@ -37465,7 +37468,7 @@
         <v>1398</v>
       </c>
       <c r="D364" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E364" s="5" t="s">
         <v>1454</v>
@@ -37497,7 +37500,7 @@
         <v>1398</v>
       </c>
       <c r="D365" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E365" s="5" t="s">
         <v>1458</v>
@@ -37529,7 +37532,7 @@
         <v>1398</v>
       </c>
       <c r="D366" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E366" s="5" t="s">
         <v>1460</v>
@@ -37561,7 +37564,7 @@
         <v>1398</v>
       </c>
       <c r="D367" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E367" s="5" t="s">
         <v>1461</v>
@@ -37593,7 +37596,7 @@
         <v>1398</v>
       </c>
       <c r="D368" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E368" s="5" t="s">
         <v>1463</v>
@@ -37625,7 +37628,7 @@
         <v>1398</v>
       </c>
       <c r="D369" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E369" s="5" t="s">
         <v>1465</v>
@@ -37657,7 +37660,7 @@
         <v>1398</v>
       </c>
       <c r="D370" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E370" s="5" t="s">
         <v>1467</v>
@@ -37689,7 +37692,7 @@
         <v>1398</v>
       </c>
       <c r="D371" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E371" s="5" t="s">
         <v>1469</v>
@@ -37721,7 +37724,7 @@
         <v>1398</v>
       </c>
       <c r="D372" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E372" s="5" t="s">
         <v>2170</v>
@@ -37753,7 +37756,7 @@
         <v>1398</v>
       </c>
       <c r="D373" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E373" s="5" t="s">
         <v>1471</v>
@@ -37785,7 +37788,7 @@
         <v>1398</v>
       </c>
       <c r="D374" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E374" s="5" t="s">
         <v>1473</v>
@@ -37817,7 +37820,7 @@
         <v>1398</v>
       </c>
       <c r="D375" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E375" s="5" t="s">
         <v>1475</v>
@@ -37849,7 +37852,7 @@
         <v>1398</v>
       </c>
       <c r="D376" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E376" s="5" t="s">
         <v>1477</v>
@@ -37881,7 +37884,7 @@
         <v>1398</v>
       </c>
       <c r="D377" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E377" s="5" t="s">
         <v>1479</v>
@@ -37913,7 +37916,7 @@
         <v>1398</v>
       </c>
       <c r="D378" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E378" s="5" t="s">
         <v>1481</v>
@@ -37945,7 +37948,7 @@
         <v>1398</v>
       </c>
       <c r="D379" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E379" s="5" t="s">
         <v>1483</v>
@@ -38656,7 +38659,7 @@
         <v>1398</v>
       </c>
       <c r="D405" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E405" s="5" t="s">
         <v>729</v>
@@ -41139,7 +41142,7 @@
         <v>1398</v>
       </c>
       <c r="D494" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E494" s="5" t="s">
         <v>728</v>
@@ -41615,7 +41618,7 @@
         <v>33</v>
       </c>
       <c r="D513" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E513" s="5" t="s">
         <v>211</v>
@@ -41906,7 +41909,7 @@
         <v>40</v>
       </c>
       <c r="D528" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E528" s="5" t="s">
         <v>717</v>
@@ -41967,7 +41970,7 @@
         <v>40</v>
       </c>
       <c r="D530" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E530" s="5" t="s">
         <v>639</v>
@@ -41996,7 +41999,7 @@
         <v>40</v>
       </c>
       <c r="D531" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E531" s="5" t="s">
         <v>1746</v>
@@ -42025,7 +42028,7 @@
         <v>40</v>
       </c>
       <c r="D532" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E532" s="5" t="s">
         <v>1748</v>
@@ -42482,7 +42485,7 @@
         <v>43</v>
       </c>
       <c r="D550" s="5" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="E550" s="5" t="s">
         <v>246</v>
@@ -49439,7 +49442,7 @@
         <v>56</v>
       </c>
       <c r="E791" s="5" t="s">
-        <v>1711</v>
+        <v>2669</v>
       </c>
       <c r="F791" s="5" t="s">
         <v>31</v>
@@ -49501,7 +49504,7 @@
         <v>56</v>
       </c>
       <c r="E793" s="5" t="s">
-        <v>2667</v>
+        <v>2664</v>
       </c>
       <c r="F793" s="5" t="s">
         <v>26</v>
@@ -50552,7 +50555,7 @@
         <v>34</v>
       </c>
       <c r="E832" s="5" t="s">
-        <v>2591</v>
+        <v>2588</v>
       </c>
       <c r="F832" s="5" t="s">
         <v>26</v>
@@ -53188,7 +53191,7 @@
         <v>34</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>2647</v>
+        <v>2644</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>2003</v>
@@ -53200,7 +53203,7 @@
         <v>26</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>1423</v>
@@ -53252,7 +53255,7 @@
         <v>34</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>2592</v>
+        <v>2589</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>26</v>
@@ -53264,7 +53267,7 @@
         <v>26</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>2593</v>
+        <v>2590</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>1660</v>
@@ -53296,7 +53299,7 @@
         <v>26</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>2594</v>
+        <v>2591</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>2321</v>
@@ -53316,7 +53319,7 @@
         <v>197</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>2645</v>
+        <v>2642</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>26</v>
@@ -53328,7 +53331,7 @@
         <v>26</v>
       </c>
       <c r="I34" s="28" t="s">
-        <v>2599</v>
+        <v>2596</v>
       </c>
       <c r="J34" s="27" t="s">
         <v>26</v>
@@ -53348,7 +53351,7 @@
         <v>197</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>2646</v>
+        <v>2643</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>26</v>
@@ -53360,7 +53363,7 @@
         <v>26</v>
       </c>
       <c r="I35" s="28" t="s">
-        <v>2600</v>
+        <v>2597</v>
       </c>
       <c r="J35" s="27" t="s">
         <v>26</v>
@@ -55272,7 +55275,7 @@
         <v>44</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>2585</v>
+        <v>2582</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>26</v>
@@ -55284,7 +55287,7 @@
         <v>26</v>
       </c>
       <c r="I101" s="10" t="s">
-        <v>2586</v>
+        <v>2583</v>
       </c>
       <c r="J101" s="5" t="s">
         <v>1111</v>
@@ -55304,7 +55307,7 @@
         <v>235</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>2637</v>
+        <v>2634</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>26</v>
@@ -55316,7 +55319,7 @@
         <v>26</v>
       </c>
       <c r="I102" s="10" t="s">
-        <v>2639</v>
+        <v>2636</v>
       </c>
       <c r="J102" s="5" t="s">
         <v>26</v>
@@ -55336,7 +55339,7 @@
         <v>34</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>2641</v>
+        <v>2638</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>26</v>
@@ -55348,7 +55351,7 @@
         <v>26</v>
       </c>
       <c r="I103" s="10" t="s">
-        <v>2640</v>
+        <v>2637</v>
       </c>
       <c r="J103" s="5" t="s">
         <v>1346</v>
@@ -55944,7 +55947,7 @@
         <v>235</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>2649</v>
+        <v>2646</v>
       </c>
       <c r="F122" s="5" t="s">
         <v>26</v>
@@ -55956,7 +55959,7 @@
         <v>26</v>
       </c>
       <c r="I122" s="5" t="s">
-        <v>2651</v>
+        <v>2648</v>
       </c>
       <c r="J122" s="5" t="s">
         <v>26</v>
@@ -55976,7 +55979,7 @@
         <v>24</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>2650</v>
+        <v>2647</v>
       </c>
       <c r="F123" s="5" t="s">
         <v>26</v>
@@ -55988,7 +55991,7 @@
         <v>26</v>
       </c>
       <c r="I123" s="5" t="s">
-        <v>2652</v>
+        <v>2649</v>
       </c>
       <c r="J123" s="5" t="s">
         <v>26</v>
@@ -56250,7 +56253,7 @@
         <v>34</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>2630</v>
+        <v>2627</v>
       </c>
       <c r="F133" s="5" t="s">
         <v>730</v>
@@ -56262,7 +56265,7 @@
         <v>26</v>
       </c>
       <c r="I133" s="10" t="s">
-        <v>2629</v>
+        <v>2626</v>
       </c>
       <c r="J133" s="5" t="s">
         <v>248</v>
@@ -56282,7 +56285,7 @@
         <v>1590</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>2603</v>
+        <v>2600</v>
       </c>
       <c r="F134" s="5" t="s">
         <v>31</v>
@@ -56294,7 +56297,7 @@
         <v>26</v>
       </c>
       <c r="I134" s="10" t="s">
-        <v>2604</v>
+        <v>2601</v>
       </c>
       <c r="J134" s="5" t="s">
         <v>26</v>
@@ -56370,7 +56373,7 @@
         <v>26</v>
       </c>
       <c r="I139" s="10" t="s">
-        <v>2654</v>
+        <v>2651</v>
       </c>
       <c r="J139" s="5" t="s">
         <v>26</v>
@@ -56390,7 +56393,7 @@
         <v>2186</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>2653</v>
+        <v>2650</v>
       </c>
       <c r="F140" s="5" t="s">
         <v>26</v>
@@ -56402,7 +56405,7 @@
         <v>26</v>
       </c>
       <c r="I140" s="10" t="s">
-        <v>2655</v>
+        <v>2652</v>
       </c>
       <c r="J140" s="5" t="s">
         <v>26</v>
@@ -56428,7 +56431,7 @@
         <v>34</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>2633</v>
+        <v>2630</v>
       </c>
       <c r="F143" s="5" t="s">
         <v>31</v>
@@ -56440,7 +56443,7 @@
         <v>26</v>
       </c>
       <c r="I143" s="10" t="s">
-        <v>2631</v>
+        <v>2628</v>
       </c>
       <c r="J143" s="5" t="s">
         <v>26</v>
@@ -56472,7 +56475,7 @@
         <v>26</v>
       </c>
       <c r="I144" s="10" t="s">
-        <v>2654</v>
+        <v>2651</v>
       </c>
       <c r="J144" s="5" t="s">
         <v>26</v>
@@ -56492,7 +56495,7 @@
         <v>2185</v>
       </c>
       <c r="E145" s="5" t="s">
-        <v>2653</v>
+        <v>2650</v>
       </c>
       <c r="F145" s="5" t="s">
         <v>26</v>
@@ -56504,7 +56507,7 @@
         <v>26</v>
       </c>
       <c r="I145" s="10" t="s">
-        <v>2655</v>
+        <v>2652</v>
       </c>
       <c r="J145" s="5" t="s">
         <v>26</v>
@@ -56574,7 +56577,7 @@
         <v>26</v>
       </c>
       <c r="I149" s="10" t="s">
-        <v>2654</v>
+        <v>2651</v>
       </c>
       <c r="J149" s="5" t="s">
         <v>26</v>
@@ -56594,7 +56597,7 @@
         <v>2184</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>2653</v>
+        <v>2650</v>
       </c>
       <c r="F150" s="5" t="s">
         <v>26</v>
@@ -56606,7 +56609,7 @@
         <v>26</v>
       </c>
       <c r="I150" s="10" t="s">
-        <v>2655</v>
+        <v>2652</v>
       </c>
       <c r="J150" s="5" t="s">
         <v>26</v>
@@ -57124,7 +57127,7 @@
         <v>26</v>
       </c>
       <c r="I168" s="10" t="s">
-        <v>2654</v>
+        <v>2651</v>
       </c>
       <c r="J168" s="5" t="s">
         <v>26</v>
@@ -57144,7 +57147,7 @@
         <v>2183</v>
       </c>
       <c r="E169" s="5" t="s">
-        <v>2653</v>
+        <v>2650</v>
       </c>
       <c r="F169" s="5" t="s">
         <v>26</v>
@@ -57156,7 +57159,7 @@
         <v>26</v>
       </c>
       <c r="I169" s="10" t="s">
-        <v>2655</v>
+        <v>2652</v>
       </c>
       <c r="J169" s="5" t="s">
         <v>26</v>
@@ -57176,7 +57179,7 @@
         <v>44</v>
       </c>
       <c r="E170" s="5" t="s">
-        <v>2635</v>
+        <v>2632</v>
       </c>
       <c r="F170" s="5" t="s">
         <v>26</v>
@@ -57188,7 +57191,7 @@
         <v>26</v>
       </c>
       <c r="I170" s="10" t="s">
-        <v>2636</v>
+        <v>2633</v>
       </c>
       <c r="J170" s="5" t="s">
         <v>1111</v>
@@ -57208,7 +57211,7 @@
         <v>34</v>
       </c>
       <c r="E171" s="5" t="s">
-        <v>2634</v>
+        <v>2631</v>
       </c>
       <c r="F171" s="5" t="s">
         <v>31</v>
@@ -57220,7 +57223,7 @@
         <v>26</v>
       </c>
       <c r="I171" s="10" t="s">
-        <v>2631</v>
+        <v>2628</v>
       </c>
       <c r="J171" s="5" t="s">
         <v>26</v>
@@ -58036,7 +58039,7 @@
         <v>34</v>
       </c>
       <c r="E202" s="5" t="s">
-        <v>2632</v>
+        <v>2629</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.3">
@@ -59146,7 +59149,7 @@
         <v>235</v>
       </c>
       <c r="E238" s="5" t="s">
-        <v>2649</v>
+        <v>2646</v>
       </c>
       <c r="F238" s="5" t="s">
         <v>26</v>
@@ -59158,7 +59161,7 @@
         <v>26</v>
       </c>
       <c r="I238" s="5" t="s">
-        <v>2651</v>
+        <v>2648</v>
       </c>
       <c r="J238" s="5" t="s">
         <v>26</v>
@@ -59350,7 +59353,7 @@
         <v>235</v>
       </c>
       <c r="E246" s="5" t="s">
-        <v>2637</v>
+        <v>2634</v>
       </c>
       <c r="F246" s="5" t="s">
         <v>26</v>
@@ -59362,7 +59365,7 @@
         <v>26</v>
       </c>
       <c r="I246" s="10" t="s">
-        <v>2638</v>
+        <v>2635</v>
       </c>
       <c r="J246" s="5" t="s">
         <v>26</v>
@@ -59382,7 +59385,7 @@
         <v>44</v>
       </c>
       <c r="E247" s="5" t="s">
-        <v>2585</v>
+        <v>2582</v>
       </c>
       <c r="F247" s="6" t="s">
         <v>26</v>
@@ -59394,7 +59397,7 @@
         <v>26</v>
       </c>
       <c r="I247" s="10" t="s">
-        <v>2587</v>
+        <v>2584</v>
       </c>
       <c r="J247" s="5" t="s">
         <v>1111</v>
@@ -60002,7 +60005,7 @@
         <v>26</v>
       </c>
       <c r="I266" s="10" t="s">
-        <v>2661</v>
+        <v>2658</v>
       </c>
       <c r="J266" s="5" t="s">
         <v>26</v>
@@ -60022,7 +60025,7 @@
         <v>2187</v>
       </c>
       <c r="E267" s="5" t="s">
-        <v>2653</v>
+        <v>2650</v>
       </c>
       <c r="F267" s="5" t="s">
         <v>26</v>
@@ -60034,7 +60037,7 @@
         <v>26</v>
       </c>
       <c r="I267" s="10" t="s">
-        <v>2660</v>
+        <v>2657</v>
       </c>
       <c r="J267" s="5" t="s">
         <v>26</v>
@@ -60054,7 +60057,7 @@
         <v>34</v>
       </c>
       <c r="E268" s="5" t="s">
-        <v>2592</v>
+        <v>2589</v>
       </c>
       <c r="F268" s="5" t="s">
         <v>26</v>
@@ -60066,7 +60069,7 @@
         <v>26</v>
       </c>
       <c r="I268" s="5" t="s">
-        <v>2593</v>
+        <v>2590</v>
       </c>
       <c r="J268" s="5" t="s">
         <v>1660</v>
@@ -60098,7 +60101,7 @@
         <v>26</v>
       </c>
       <c r="I269" s="5" t="s">
-        <v>2594</v>
+        <v>2591</v>
       </c>
       <c r="J269" s="5" t="s">
         <v>2321</v>
@@ -60808,7 +60811,7 @@
         <v>34</v>
       </c>
       <c r="E295" s="5" t="s">
-        <v>2591</v>
+        <v>2588</v>
       </c>
       <c r="F295" s="5" t="s">
         <v>26</v>
@@ -61300,7 +61303,7 @@
         <v>26</v>
       </c>
       <c r="I310" s="10" t="s">
-        <v>2656</v>
+        <v>2653</v>
       </c>
       <c r="J310" s="5" t="s">
         <v>26</v>
@@ -61320,7 +61323,7 @@
         <v>2189</v>
       </c>
       <c r="E311" s="5" t="s">
-        <v>2653</v>
+        <v>2650</v>
       </c>
       <c r="F311" s="5" t="s">
         <v>26</v>
@@ -61332,7 +61335,7 @@
         <v>26</v>
       </c>
       <c r="I311" s="10" t="s">
-        <v>2657</v>
+        <v>2654</v>
       </c>
       <c r="J311" s="5" t="s">
         <v>26</v>
@@ -61352,7 +61355,7 @@
         <v>1590</v>
       </c>
       <c r="E312" s="5" t="s">
-        <v>2588</v>
+        <v>2585</v>
       </c>
       <c r="F312" s="5" t="s">
         <v>31</v>
@@ -61364,7 +61367,7 @@
         <v>26</v>
       </c>
       <c r="I312" s="5" t="s">
-        <v>2602</v>
+        <v>2599</v>
       </c>
       <c r="J312" s="5" t="s">
         <v>26</v>
@@ -61667,7 +61670,7 @@
         <v>26</v>
       </c>
       <c r="I325" s="10" t="s">
-        <v>2658</v>
+        <v>2655</v>
       </c>
       <c r="J325" s="5" t="s">
         <v>26</v>
@@ -61687,7 +61690,7 @@
         <v>2188</v>
       </c>
       <c r="E326" s="5" t="s">
-        <v>2653</v>
+        <v>2650</v>
       </c>
       <c r="F326" s="5" t="s">
         <v>26</v>
@@ -61699,7 +61702,7 @@
         <v>26</v>
       </c>
       <c r="I326" s="10" t="s">
-        <v>2659</v>
+        <v>2656</v>
       </c>
       <c r="J326" s="5" t="s">
         <v>26</v>
@@ -61719,7 +61722,7 @@
         <v>1590</v>
       </c>
       <c r="E327" s="5" t="s">
-        <v>2588</v>
+        <v>2585</v>
       </c>
       <c r="F327" s="5" t="s">
         <v>31</v>
@@ -61731,7 +61734,7 @@
         <v>26</v>
       </c>
       <c r="I327" s="5" t="s">
-        <v>2601</v>
+        <v>2598</v>
       </c>
       <c r="J327" s="5" t="s">
         <v>26</v>
@@ -68872,7 +68875,7 @@
     </row>
     <row r="2" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>2564</v>
+        <v>2561</v>
       </c>
       <c r="I2" s="22"/>
     </row>
@@ -68979,7 +68982,7 @@
     </row>
     <row r="17" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
-        <v>2542</v>
+        <v>2539</v>
       </c>
       <c r="I17" s="22"/>
     </row>
@@ -68988,7 +68991,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>2543</v>
+        <v>2540</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>23</v>
@@ -68997,7 +69000,7 @@
         <v>197</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>2645</v>
+        <v>2642</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>26</v>
@@ -69009,7 +69012,7 @@
         <v>26</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>2599</v>
+        <v>2596</v>
       </c>
       <c r="J18" s="27" t="s">
         <v>26</v>
@@ -69029,7 +69032,7 @@
         <v>197</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>2646</v>
+        <v>2643</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>26</v>
@@ -69041,7 +69044,7 @@
         <v>26</v>
       </c>
       <c r="I19" s="28" t="s">
-        <v>2600</v>
+        <v>2597</v>
       </c>
       <c r="J19" s="27" t="s">
         <v>26</v>
@@ -69052,7 +69055,7 @@
     </row>
     <row r="21" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
-        <v>2561</v>
+        <v>2558</v>
       </c>
       <c r="I21" s="22"/>
     </row>
@@ -69067,7 +69070,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>2543</v>
+        <v>2540</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>28</v>
@@ -69163,7 +69166,7 @@
     </row>
     <row r="27" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
-        <v>2580</v>
+        <v>2577</v>
       </c>
       <c r="I27" s="22"/>
     </row>
@@ -69172,16 +69175,16 @@
         <v>22</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>2543</v>
+        <v>2540</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>2582</v>
+        <v>2579</v>
       </c>
       <c r="D28" s="27" t="s">
         <v>56</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>2566</v>
+        <v>2563</v>
       </c>
       <c r="F28" s="27" t="s">
         <v>31</v>
@@ -69193,7 +69196,7 @@
         <v>26</v>
       </c>
       <c r="I28" s="28" t="s">
-        <v>2568</v>
+        <v>2565</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>26</v>
@@ -69213,7 +69216,7 @@
         <v>56</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>2569</v>
+        <v>2566</v>
       </c>
       <c r="F29" s="27" t="s">
         <v>31</v>
@@ -69225,7 +69228,7 @@
         <v>26</v>
       </c>
       <c r="I29" s="28" t="s">
-        <v>2570</v>
+        <v>2567</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>26</v>
@@ -69245,7 +69248,7 @@
         <v>1871</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>2583</v>
+        <v>2580</v>
       </c>
       <c r="F30" s="27" t="s">
         <v>31</v>
@@ -69257,7 +69260,7 @@
         <v>26</v>
       </c>
       <c r="I30" s="28" t="s">
-        <v>2581</v>
+        <v>2578</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>26</v>
@@ -69277,7 +69280,7 @@
         <v>1871</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>2584</v>
+        <v>2581</v>
       </c>
       <c r="F31" s="27" t="s">
         <v>31</v>
@@ -69289,7 +69292,7 @@
         <v>26</v>
       </c>
       <c r="I31" s="28" t="s">
-        <v>2581</v>
+        <v>2578</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>26</v>
@@ -69309,7 +69312,7 @@
         <v>22</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>2543</v>
+        <v>2540</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>43</v>
@@ -69330,7 +69333,7 @@
         <v>26</v>
       </c>
       <c r="I34" s="28" t="s">
-        <v>2571</v>
+        <v>2568</v>
       </c>
       <c r="J34" s="27" t="s">
         <v>2321</v>
@@ -69341,7 +69344,7 @@
         <v>22</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>2543</v>
+        <v>2540</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>43</v>
@@ -69350,7 +69353,7 @@
         <v>197</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>2562</v>
+        <v>2559</v>
       </c>
       <c r="F35" s="27" t="s">
         <v>26</v>
@@ -69362,7 +69365,7 @@
         <v>26</v>
       </c>
       <c r="I35" s="28" t="s">
-        <v>2563</v>
+        <v>2560</v>
       </c>
       <c r="J35" s="27" t="s">
         <v>26</v>
@@ -69373,7 +69376,7 @@
     </row>
     <row r="37" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
       <c r="I37" s="22"/>
     </row>
@@ -69391,7 +69394,7 @@
         <v>34</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>2550</v>
+        <v>2547</v>
       </c>
       <c r="F38" s="27" t="s">
         <v>31</v>
@@ -69403,7 +69406,7 @@
         <v>26</v>
       </c>
       <c r="I38" s="28" t="s">
-        <v>2547</v>
+        <v>2544</v>
       </c>
       <c r="J38" s="27" t="s">
         <v>2136</v>
@@ -69423,7 +69426,7 @@
         <v>34</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>2551</v>
+        <v>2548</v>
       </c>
       <c r="F39" s="27" t="s">
         <v>31</v>
@@ -69435,7 +69438,7 @@
         <v>26</v>
       </c>
       <c r="I39" s="28" t="s">
-        <v>2548</v>
+        <v>2545</v>
       </c>
       <c r="J39" s="27" t="s">
         <v>2136</v>
@@ -69455,7 +69458,7 @@
         <v>34</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>2552</v>
+        <v>2549</v>
       </c>
       <c r="F40" s="27" t="s">
         <v>31</v>
@@ -69467,7 +69470,7 @@
         <v>26</v>
       </c>
       <c r="I40" s="28" t="s">
-        <v>2549</v>
+        <v>2546</v>
       </c>
       <c r="J40" s="27" t="s">
         <v>2136</v>
@@ -69487,7 +69490,7 @@
         <v>34</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>2553</v>
+        <v>2550</v>
       </c>
       <c r="F41" s="27" t="s">
         <v>31</v>
@@ -69499,10 +69502,10 @@
         <v>26</v>
       </c>
       <c r="I41" s="28" t="s">
-        <v>2577</v>
+        <v>2574</v>
       </c>
       <c r="J41" s="27" t="s">
-        <v>2567</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -69519,7 +69522,7 @@
         <v>34</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>2554</v>
+        <v>2551</v>
       </c>
       <c r="F42" s="27" t="s">
         <v>31</v>
@@ -69531,10 +69534,10 @@
         <v>26</v>
       </c>
       <c r="I42" s="28" t="s">
-        <v>2578</v>
+        <v>2575</v>
       </c>
       <c r="J42" s="27" t="s">
-        <v>2567</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -69551,7 +69554,7 @@
         <v>34</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>2555</v>
+        <v>2552</v>
       </c>
       <c r="F43" s="27" t="s">
         <v>31</v>
@@ -69563,10 +69566,10 @@
         <v>26</v>
       </c>
       <c r="I43" s="28" t="s">
-        <v>2579</v>
+        <v>2576</v>
       </c>
       <c r="J43" s="27" t="s">
-        <v>2567</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -69583,7 +69586,7 @@
         <v>34</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>2588</v>
+        <v>2585</v>
       </c>
       <c r="F44" s="27" t="s">
         <v>31</v>
@@ -69595,7 +69598,7 @@
         <v>26</v>
       </c>
       <c r="I44" s="28" t="s">
-        <v>2590</v>
+        <v>2587</v>
       </c>
       <c r="J44" s="27" t="s">
         <v>26</v>
@@ -69606,7 +69609,7 @@
     </row>
     <row r="46" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
-        <v>2545</v>
+        <v>2542</v>
       </c>
       <c r="I46" s="22"/>
     </row>
@@ -69615,7 +69618,7 @@
         <v>22</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>2543</v>
+        <v>2540</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>50</v>
@@ -69636,7 +69639,7 @@
         <v>26</v>
       </c>
       <c r="I47" s="28" t="s">
-        <v>2558</v>
+        <v>2555</v>
       </c>
       <c r="J47" s="27" t="s">
         <v>1660</v>
@@ -69656,7 +69659,7 @@
         <v>34</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>2556</v>
+        <v>2553</v>
       </c>
       <c r="F48" s="27" t="s">
         <v>31</v>
@@ -69668,7 +69671,7 @@
         <v>26</v>
       </c>
       <c r="I48" s="28" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="J48" s="27" t="s">
         <v>1660</v>
@@ -69688,7 +69691,7 @@
         <v>34</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="F49" s="27" t="s">
         <v>31</v>
@@ -69700,7 +69703,7 @@
         <v>26</v>
       </c>
       <c r="I49" s="28" t="s">
-        <v>2559</v>
+        <v>2556</v>
       </c>
       <c r="J49" s="27" t="s">
         <v>1660</v>
@@ -69720,7 +69723,7 @@
         <v>34</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>2588</v>
+        <v>2585</v>
       </c>
       <c r="F50" s="27" t="s">
         <v>31</v>
@@ -69732,7 +69735,7 @@
         <v>26</v>
       </c>
       <c r="I50" s="28" t="s">
-        <v>2589</v>
+        <v>2586</v>
       </c>
       <c r="J50" s="27" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
updated InflowWind with MiscVar type; required change to DWM as well. updated dependencies (note the BD has gauss quadrature without -1 again)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1187 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 81e49f13a1fcda4085f9f656e5791cad8f85bd7a
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14895" uniqueCount="2690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14895" uniqueCount="2692">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -8303,6 +8303,12 @@
   </si>
   <si>
     <t># ..... Misc Variables ................................................................................................................</t>
+  </si>
+  <si>
+    <t>InflowWind_MiscVarType</t>
+  </si>
+  <si>
+    <t>"Misc/optimization variables"</t>
   </si>
 </sst>
 </file>
@@ -8526,7 +8532,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="920">
+  <dxfs count="892">
     <dxf>
       <font>
         <u val="none"/>
@@ -16093,244 +16099,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -17261,10 +17029,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="895" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="891" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="894" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="890" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17277,8 +17045,8 @@
   <dimension ref="A1:J421"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D180" sqref="D180"/>
+      <pane ySplit="11" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G213" sqref="G213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22009,7 +21777,7 @@
         <v>1756</v>
       </c>
       <c r="F210" s="27" t="s">
-        <v>26</v>
+        <v>1858</v>
       </c>
       <c r="G210" s="27" t="s">
         <v>26</v>
@@ -22018,7 +21786,7 @@
         <v>26</v>
       </c>
       <c r="I210" s="28" t="s">
-        <v>1766</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
@@ -22108,7 +21876,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" s="27" t="s">
         <v>22</v>
       </c>
@@ -22119,10 +21887,10 @@
         <v>27</v>
       </c>
       <c r="D214" s="27" t="s">
-        <v>2271</v>
+        <v>2690</v>
       </c>
       <c r="E214" s="27" t="s">
-        <v>1760</v>
+        <v>1421</v>
       </c>
       <c r="F214" s="27" t="s">
         <v>26</v>
@@ -22134,7 +21902,7 @@
         <v>26</v>
       </c>
       <c r="I214" s="28" t="s">
-        <v>1770</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
@@ -27310,394 +27078,394 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A11">
-    <cfRule type="containsText" dxfId="893" priority="101" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="889" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="892" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="888" priority="102" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A14">
-    <cfRule type="containsText" dxfId="891" priority="99" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="887" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A13)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="890" priority="100" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="886" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(A13,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="889" priority="97" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="885" priority="97" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="888" priority="98" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="884" priority="98" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="887" priority="95" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="883" priority="95" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="886" priority="96" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="882" priority="96" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="885" priority="93" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="881" priority="93" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="884" priority="94" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="880" priority="94" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="883" priority="91" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="879" priority="91" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="882" priority="92" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="878" priority="92" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128">
-    <cfRule type="containsText" dxfId="881" priority="89" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="877" priority="89" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A128)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="880" priority="90" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="876" priority="90" operator="beginsWith" text="#">
       <formula>LEFT(A128,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A155">
-    <cfRule type="containsText" dxfId="879" priority="87" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="875" priority="87" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A155)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="878" priority="88" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="874" priority="88" operator="beginsWith" text="#">
       <formula>LEFT(A155,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A169">
-    <cfRule type="containsText" dxfId="877" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="873" priority="85" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A169)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="876" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="872" priority="86" operator="beginsWith" text="#">
       <formula>LEFT(A169,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A224">
-    <cfRule type="containsText" dxfId="875" priority="83" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="871" priority="83" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A224)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="874" priority="84" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="870" priority="84" operator="beginsWith" text="#">
       <formula>LEFT(A224,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A129">
-    <cfRule type="containsText" dxfId="873" priority="81" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="869" priority="81" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A129)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="872" priority="82" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="868" priority="82" operator="beginsWith" text="#">
       <formula>LEFT(A129,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130">
-    <cfRule type="containsText" dxfId="871" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="867" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A130)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="870" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="866" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A130,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A194">
-    <cfRule type="containsText" dxfId="869" priority="77" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="865" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A194)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="868" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="864" priority="78" operator="beginsWith" text="#">
       <formula>LEFT(A194,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A236">
-    <cfRule type="containsText" dxfId="867" priority="75" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="863" priority="75" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A236)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="866" priority="76" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="862" priority="76" operator="beginsWith" text="#">
       <formula>LEFT(A236,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A248">
-    <cfRule type="containsText" dxfId="865" priority="73" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="861" priority="73" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A248)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="864" priority="74" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="860" priority="74" operator="beginsWith" text="#">
       <formula>LEFT(A248,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A260">
-    <cfRule type="containsText" dxfId="863" priority="71" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="859" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A260)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="862" priority="72" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="858" priority="72" operator="beginsWith" text="#">
       <formula>LEFT(A260,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272">
-    <cfRule type="containsText" dxfId="861" priority="69" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="857" priority="69" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A272)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="860" priority="70" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="856" priority="70" operator="beginsWith" text="#">
       <formula>LEFT(A272,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A206">
-    <cfRule type="containsText" dxfId="859" priority="67" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="855" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A206)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="858" priority="68" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="854" priority="68" operator="beginsWith" text="#">
       <formula>LEFT(A206,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A308:A309 A314">
-    <cfRule type="containsText" dxfId="857" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="853" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A308)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="856" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="852" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A308,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A321">
-    <cfRule type="containsText" dxfId="855" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="851" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A321)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="854" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="850" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A321,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A324">
-    <cfRule type="containsText" dxfId="853" priority="59" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="849" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A324)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="852" priority="60" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="848" priority="60" operator="beginsWith" text="#">
       <formula>LEFT(A324,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A327">
-    <cfRule type="containsText" dxfId="851" priority="57" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="847" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A327)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="850" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="846" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(A327,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A337">
-    <cfRule type="containsText" dxfId="849" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="845" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A337)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="848" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="844" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(A337,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A346">
-    <cfRule type="containsText" dxfId="847" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="843" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A346)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="846" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="842" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(A346,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A349">
-    <cfRule type="containsText" dxfId="845" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="841" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A349)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="844" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="840" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(A349,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A352">
-    <cfRule type="containsText" dxfId="843" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="839" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A352)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="842" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="838" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(A352,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A356">
-    <cfRule type="containsText" dxfId="841" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="837" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A356)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="840" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="836" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A356,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A379">
-    <cfRule type="containsText" dxfId="839" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="835" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A379)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="838" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="834" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A379,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:A62">
-    <cfRule type="containsText" dxfId="837" priority="43" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="833" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A61)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="836" priority="44" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="832" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A61,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:A38">
-    <cfRule type="containsText" dxfId="835" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="831" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A34)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="834" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="830" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(A34,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="containsText" dxfId="833" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="829" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A57)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="832" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="828" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A57,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114">
-    <cfRule type="containsText" dxfId="831" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="827" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A114)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="830" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="826" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A114,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74">
-    <cfRule type="containsText" dxfId="829" priority="35" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="825" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A74)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="828" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="824" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A74,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
-    <cfRule type="containsText" dxfId="827" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="823" priority="33" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A78)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="826" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="822" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(A78,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="containsText" dxfId="825" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="821" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A88)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="824" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="820" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(A88,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="containsText" dxfId="823" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="819" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A98)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="822" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="818" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A98,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A392">
-    <cfRule type="containsText" dxfId="821" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="817" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A392)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="820" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="816" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A392,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A332">
-    <cfRule type="containsText" dxfId="819" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="815" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A332)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="818" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="814" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A332,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A370">
-    <cfRule type="containsText" dxfId="817" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="813" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A370)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="816" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="812" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A370,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A284">
-    <cfRule type="containsText" dxfId="815" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="811" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A284)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="814" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="810" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A284,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A401">
-    <cfRule type="containsText" dxfId="813" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="809" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A401)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="812" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="808" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A401,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A182">
-    <cfRule type="containsText" dxfId="811" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="807" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A182)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="810" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="806" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A182,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142">
-    <cfRule type="containsText" dxfId="809" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="805" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A142)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="808" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="804" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A142,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A143">
-    <cfRule type="containsText" dxfId="807" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="803" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A143)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="806" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="802" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A143,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="containsText" dxfId="805" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="801" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A144)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="804" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="800" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A144,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A310">
-    <cfRule type="containsText" dxfId="803" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="799" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A310)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="802" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="798" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A310,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A341">
-    <cfRule type="containsText" dxfId="801" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="797" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A341)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="800" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="796" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A341,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A218">
-    <cfRule type="containsText" dxfId="799" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="795" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A218)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="798" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="794" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A218,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A296">
-    <cfRule type="containsText" dxfId="797" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="793" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A296)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="796" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="792" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A296,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51136,1538 +50904,1538 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A262:A318 A334 A325 A548:A549 A654:A687 A536 A71 A40:A59 A703:A718 A698:A701 A720:A726 A692:A696 A23 A25:A29 A258:A260 A543 A839:A1048576 A785:A786 A348:A357 A377:A380 A391:A393 A404:A407 A563:A634 A431:A455 A458:A465 A504 A467:A493 A398:A401 A792:A793 A636:A652 A799:A801 A813:A814 A1:A11 A506:A509 A18:A21 A496:A500 A538:A541 A511:A519 A528:A530">
-    <cfRule type="containsText" dxfId="795" priority="923" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="791" priority="923" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="794" priority="924" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="790" priority="924" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A261">
-    <cfRule type="containsText" dxfId="793" priority="911" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="789" priority="911" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A261)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="792" priority="912" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="788" priority="912" operator="beginsWith" text="#">
       <formula>LEFT(A261,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A14 A37 A17">
-    <cfRule type="containsText" dxfId="791" priority="905" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="787" priority="905" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A13)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="790" priority="906" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="786" priority="906" operator="beginsWith" text="#">
       <formula>LEFT(A13,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:A73">
-    <cfRule type="containsText" dxfId="789" priority="901" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="785" priority="901" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A72)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="788" priority="902" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="784" priority="902" operator="beginsWith" text="#">
       <formula>LEFT(A72,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="787" priority="899" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="783" priority="899" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="786" priority="900" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="782" priority="900" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A545">
-    <cfRule type="containsText" dxfId="785" priority="895" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="781" priority="895" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A545)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="784" priority="896" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="780" priority="896" operator="beginsWith" text="#">
       <formula>LEFT(A545,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A544">
-    <cfRule type="containsText" dxfId="783" priority="897" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="779" priority="897" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A544)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="782" priority="898" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="778" priority="898" operator="beginsWith" text="#">
       <formula>LEFT(A544,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A557">
-    <cfRule type="containsText" dxfId="781" priority="893" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="777" priority="893" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A557)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="780" priority="894" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="776" priority="894" operator="beginsWith" text="#">
       <formula>LEFT(A557,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A558">
-    <cfRule type="containsText" dxfId="779" priority="891" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="775" priority="891" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A558)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="778" priority="892" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="774" priority="892" operator="beginsWith" text="#">
       <formula>LEFT(A558,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A555">
-    <cfRule type="containsText" dxfId="777" priority="889" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="773" priority="889" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A555)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="776" priority="890" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="772" priority="890" operator="beginsWith" text="#">
       <formula>LEFT(A555,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A556">
-    <cfRule type="containsText" dxfId="775" priority="887" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="771" priority="887" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A556)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="774" priority="888" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="770" priority="888" operator="beginsWith" text="#">
       <formula>LEFT(A556,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A559">
-    <cfRule type="containsText" dxfId="773" priority="883" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="769" priority="883" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A559)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="772" priority="884" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="768" priority="884" operator="beginsWith" text="#">
       <formula>LEFT(A559,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A510">
-    <cfRule type="containsText" dxfId="771" priority="879" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="767" priority="879" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A510)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="770" priority="880" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="766" priority="880" operator="beginsWith" text="#">
       <formula>LEFT(A510,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A546">
-    <cfRule type="containsText" dxfId="769" priority="877" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="765" priority="877" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A546)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="768" priority="878" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="764" priority="878" operator="beginsWith" text="#">
       <formula>LEFT(A546,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A560">
-    <cfRule type="containsText" dxfId="767" priority="875" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="763" priority="875" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A560)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="766" priority="876" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="762" priority="876" operator="beginsWith" text="#">
       <formula>LEFT(A560,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A653">
-    <cfRule type="containsText" dxfId="765" priority="873" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="761" priority="873" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A653)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="764" priority="874" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="760" priority="874" operator="beginsWith" text="#">
       <formula>LEFT(A653,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A547">
-    <cfRule type="containsText" dxfId="763" priority="867" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="759" priority="867" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A547)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="762" priority="868" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="758" priority="868" operator="beginsWith" text="#">
       <formula>LEFT(A547,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A319:A321">
-    <cfRule type="containsText" dxfId="761" priority="865" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="757" priority="865" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A319)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="760" priority="866" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="756" priority="866" operator="beginsWith" text="#">
       <formula>LEFT(A319,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A322">
-    <cfRule type="containsText" dxfId="759" priority="861" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="755" priority="861" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A322)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="758" priority="862" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="754" priority="862" operator="beginsWith" text="#">
       <formula>LEFT(A322,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A323:A324 A326:A331">
-    <cfRule type="containsText" dxfId="757" priority="859" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="753" priority="859" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A323)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="756" priority="860" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="752" priority="860" operator="beginsWith" text="#">
       <formula>LEFT(A323,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A332:A333 A335:A341 A551">
-    <cfRule type="containsText" dxfId="755" priority="857" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="751" priority="857" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A332)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="754" priority="858" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="750" priority="858" operator="beginsWith" text="#">
       <formula>LEFT(A332,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A550">
-    <cfRule type="containsText" dxfId="753" priority="813" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="749" priority="813" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A550)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="752" priority="814" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="748" priority="814" operator="beginsWith" text="#">
       <formula>LEFT(A550,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A343">
-    <cfRule type="containsText" dxfId="751" priority="801" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="747" priority="801" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A343)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="750" priority="802" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="746" priority="802" operator="beginsWith" text="#">
       <formula>LEFT(A343,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A342">
-    <cfRule type="containsText" dxfId="749" priority="803" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="745" priority="803" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A342)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="748" priority="804" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="744" priority="804" operator="beginsWith" text="#">
       <formula>LEFT(A342,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A552">
-    <cfRule type="containsText" dxfId="747" priority="799" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="743" priority="799" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A552)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="746" priority="800" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="742" priority="800" operator="beginsWith" text="#">
       <formula>LEFT(A552,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A553">
-    <cfRule type="containsText" dxfId="745" priority="797" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="741" priority="797" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A553)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="744" priority="798" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="740" priority="798" operator="beginsWith" text="#">
       <formula>LEFT(A553,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A344:A345">
-    <cfRule type="containsText" dxfId="743" priority="795" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="739" priority="795" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A344)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="742" priority="796" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="738" priority="796" operator="beginsWith" text="#">
       <formula>LEFT(A344,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A562">
-    <cfRule type="containsText" dxfId="741" priority="787" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="737" priority="787" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A562)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="740" priority="788" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="736" priority="788" operator="beginsWith" text="#">
       <formula>LEFT(A562,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A561">
-    <cfRule type="containsText" dxfId="739" priority="789" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="735" priority="789" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A561)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="738" priority="790" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="734" priority="790" operator="beginsWith" text="#">
       <formula>LEFT(A561,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A689">
-    <cfRule type="containsText" dxfId="737" priority="757" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="733" priority="757" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A689)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="736" priority="758" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="732" priority="758" operator="beginsWith" text="#">
       <formula>LEFT(A689,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A346:A347 A382">
-    <cfRule type="containsText" dxfId="735" priority="753" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="731" priority="753" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A346)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="734" priority="754" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="730" priority="754" operator="beginsWith" text="#">
       <formula>LEFT(A346,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A403">
-    <cfRule type="containsText" dxfId="733" priority="751" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="729" priority="751" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A403)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="732" priority="752" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="728" priority="752" operator="beginsWith" text="#">
       <formula>LEFT(A403,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A521">
-    <cfRule type="containsText" dxfId="731" priority="745" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="727" priority="745" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A521)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="730" priority="746" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="726" priority="746" operator="beginsWith" text="#">
       <formula>LEFT(A521,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="containsText" dxfId="729" priority="719" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="725" priority="719" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A38)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="728" priority="720" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="724" priority="720" operator="beginsWith" text="#">
       <formula>LEFT(A38,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="containsText" dxfId="727" priority="717" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="723" priority="717" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A39)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="726" priority="718" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="722" priority="718" operator="beginsWith" text="#">
       <formula>LEFT(A39,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="containsText" dxfId="725" priority="709" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="721" priority="709" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A60)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="724" priority="710" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="720" priority="710" operator="beginsWith" text="#">
       <formula>LEFT(A60,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="containsText" dxfId="723" priority="707" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="719" priority="707" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A61)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="722" priority="708" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="718" priority="708" operator="beginsWith" text="#">
       <formula>LEFT(A61,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="containsText" dxfId="721" priority="705" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="717" priority="705" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A62)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="720" priority="706" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="716" priority="706" operator="beginsWith" text="#">
       <formula>LEFT(A62,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63">
-    <cfRule type="containsText" dxfId="719" priority="703" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="715" priority="703" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A63)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="718" priority="704" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="714" priority="704" operator="beginsWith" text="#">
       <formula>LEFT(A63,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A727">
-    <cfRule type="containsText" dxfId="717" priority="701" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="713" priority="701" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A727)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="716" priority="702" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="712" priority="702" operator="beginsWith" text="#">
       <formula>LEFT(A727,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A728">
-    <cfRule type="containsText" dxfId="715" priority="699" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="711" priority="699" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A728)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="714" priority="700" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="710" priority="700" operator="beginsWith" text="#">
       <formula>LEFT(A728,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A729">
-    <cfRule type="containsText" dxfId="713" priority="697" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="709" priority="697" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A729)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="712" priority="698" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="708" priority="698" operator="beginsWith" text="#">
       <formula>LEFT(A729,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A731:A734">
-    <cfRule type="containsText" dxfId="711" priority="691" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="707" priority="691" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A731)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="710" priority="692" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="706" priority="692" operator="beginsWith" text="#">
       <formula>LEFT(A731,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A730">
-    <cfRule type="containsText" dxfId="709" priority="687" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="705" priority="687" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A730)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="708" priority="688" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="704" priority="688" operator="beginsWith" text="#">
       <formula>LEFT(A730,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A735:A742">
-    <cfRule type="containsText" dxfId="707" priority="681" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="703" priority="681" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A735)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="706" priority="682" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="702" priority="682" operator="beginsWith" text="#">
       <formula>LEFT(A735,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A743:A753">
-    <cfRule type="containsText" dxfId="705" priority="675" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="701" priority="675" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A743)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="704" priority="676" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="700" priority="676" operator="beginsWith" text="#">
       <formula>LEFT(A743,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A754">
-    <cfRule type="containsText" dxfId="703" priority="677" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="699" priority="677" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A754)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="702" priority="678" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="698" priority="678" operator="beginsWith" text="#">
       <formula>LEFT(A754,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A755:A765">
-    <cfRule type="containsText" dxfId="701" priority="669" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="697" priority="669" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A755)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="700" priority="670" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="696" priority="670" operator="beginsWith" text="#">
       <formula>LEFT(A755,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A766">
-    <cfRule type="containsText" dxfId="699" priority="671" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="695" priority="671" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A766)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="698" priority="672" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="694" priority="672" operator="beginsWith" text="#">
       <formula>LEFT(A766,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A767">
-    <cfRule type="containsText" dxfId="697" priority="665" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="693" priority="665" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A767)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="696" priority="666" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="692" priority="666" operator="beginsWith" text="#">
       <formula>LEFT(A767,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A771:A772">
-    <cfRule type="containsText" dxfId="695" priority="655" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="691" priority="655" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A771)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="694" priority="656" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="690" priority="656" operator="beginsWith" text="#">
       <formula>LEFT(A771,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A768">
-    <cfRule type="containsText" dxfId="693" priority="661" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="689" priority="661" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A768)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="692" priority="662" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="688" priority="662" operator="beginsWith" text="#">
       <formula>LEFT(A768,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A769">
-    <cfRule type="containsText" dxfId="691" priority="659" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="687" priority="659" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A769)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="690" priority="660" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="686" priority="660" operator="beginsWith" text="#">
       <formula>LEFT(A769,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A770">
-    <cfRule type="containsText" dxfId="689" priority="657" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="685" priority="657" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A770)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="688" priority="658" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="684" priority="658" operator="beginsWith" text="#">
       <formula>LEFT(A770,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A773:A774">
-    <cfRule type="containsText" dxfId="687" priority="651" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="683" priority="651" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A773)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="686" priority="652" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="682" priority="652" operator="beginsWith" text="#">
       <formula>LEFT(A773,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A775">
-    <cfRule type="containsText" dxfId="685" priority="641" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="681" priority="641" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A775)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="684" priority="642" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="680" priority="642" operator="beginsWith" text="#">
       <formula>LEFT(A775,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A554">
-    <cfRule type="containsText" dxfId="683" priority="637" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="679" priority="637" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A554)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="682" priority="638" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="678" priority="638" operator="beginsWith" text="#">
       <formula>LEFT(A554,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A688">
-    <cfRule type="containsText" dxfId="681" priority="607" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="677" priority="607" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A688)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="680" priority="608" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="676" priority="608" operator="beginsWith" text="#">
       <formula>LEFT(A688,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="containsText" dxfId="679" priority="605" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="675" priority="605" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A65)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="678" priority="606" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="674" priority="606" operator="beginsWith" text="#">
       <formula>LEFT(A65,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="containsText" dxfId="677" priority="603" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="673" priority="603" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A66)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="676" priority="604" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="672" priority="604" operator="beginsWith" text="#">
       <formula>LEFT(A66,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67:A69">
-    <cfRule type="containsText" dxfId="675" priority="601" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="671" priority="601" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A67)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="674" priority="602" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="670" priority="602" operator="beginsWith" text="#">
       <formula>LEFT(A67,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A719">
-    <cfRule type="containsText" dxfId="673" priority="581" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="669" priority="581" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A719)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="672" priority="582" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="668" priority="582" operator="beginsWith" text="#">
       <formula>LEFT(A719,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A691">
-    <cfRule type="containsText" dxfId="671" priority="587" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="667" priority="587" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A691)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="670" priority="588" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="666" priority="588" operator="beginsWith" text="#">
       <formula>LEFT(A691,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A697">
-    <cfRule type="containsText" dxfId="669" priority="583" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="665" priority="583" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A697)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="668" priority="584" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="664" priority="584" operator="beginsWith" text="#">
       <formula>LEFT(A697,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A702">
-    <cfRule type="containsText" dxfId="667" priority="579" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="663" priority="579" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A702)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="666" priority="580" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="662" priority="580" operator="beginsWith" text="#">
       <formula>LEFT(A702,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="containsText" dxfId="665" priority="577" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="661" priority="577" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A22)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="664" priority="578" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="660" priority="578" operator="beginsWith" text="#">
       <formula>LEFT(A22,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="containsText" dxfId="663" priority="567" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="659" priority="567" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A24)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="662" priority="568" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="658" priority="568" operator="beginsWith" text="#">
       <formula>LEFT(A24,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A776">
-    <cfRule type="containsText" dxfId="661" priority="565" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="657" priority="565" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A776)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="660" priority="566" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="656" priority="566" operator="beginsWith" text="#">
       <formula>LEFT(A776,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110 A120:A122">
-    <cfRule type="containsText" dxfId="659" priority="375" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="655" priority="375" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="658" priority="376" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="654" priority="376" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A132">
-    <cfRule type="containsText" dxfId="657" priority="379" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="653" priority="379" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="656" priority="380" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="652" priority="380" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A147 A133">
-    <cfRule type="containsText" dxfId="655" priority="381" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="651" priority="381" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="654" priority="382" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="650" priority="382" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152:A153 A149">
-    <cfRule type="containsText" dxfId="653" priority="383" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="649" priority="383" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="652" priority="384" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="648" priority="384" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A148">
-    <cfRule type="containsText" dxfId="651" priority="385" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="647" priority="385" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="650" priority="386" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="646" priority="386" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A151">
-    <cfRule type="containsText" dxfId="649" priority="387" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="645" priority="387" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="648" priority="388" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="644" priority="388" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A154">
-    <cfRule type="containsText" dxfId="647" priority="389" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="643" priority="389" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="646" priority="390" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="642" priority="390" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A150">
-    <cfRule type="containsText" dxfId="645" priority="391" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="641" priority="391" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="644" priority="392" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="640" priority="392" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A158">
-    <cfRule type="containsText" dxfId="643" priority="393" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="639" priority="393" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="642" priority="394" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="638" priority="394" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A157 A168">
-    <cfRule type="containsText" dxfId="641" priority="395" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="637" priority="395" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="640" priority="396" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="636" priority="396" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A170">
-    <cfRule type="containsText" dxfId="639" priority="397" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="635" priority="397" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="638" priority="398" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="634" priority="398" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A172">
-    <cfRule type="containsText" dxfId="637" priority="399" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="633" priority="399" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="636" priority="400" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="632" priority="400" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="containsText" dxfId="635" priority="321" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="631" priority="321" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A30)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="634" priority="322" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="630" priority="322" operator="beginsWith" text="#">
       <formula>LEFT(A30,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="containsText" dxfId="633" priority="319" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="629" priority="319" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A31)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="632" priority="320" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="628" priority="320" operator="beginsWith" text="#">
       <formula>LEFT(A31,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A542">
-    <cfRule type="containsText" dxfId="631" priority="317" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="627" priority="317" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A542)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="630" priority="318" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="626" priority="318" operator="beginsWith" text="#">
       <formula>LEFT(A542,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A795">
-    <cfRule type="containsText" dxfId="629" priority="315" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="625" priority="315" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A795)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="628" priority="316" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="624" priority="316" operator="beginsWith" text="#">
       <formula>LEFT(A795,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:A106">
-    <cfRule type="containsText" dxfId="627" priority="1507" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="623" priority="1507" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="626" priority="1508" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="622" priority="1508" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A815">
-    <cfRule type="containsText" dxfId="625" priority="307" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="621" priority="307" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A815)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="624" priority="308" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="620" priority="308" operator="beginsWith" text="#">
       <formula>LEFT(A815,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A817">
-    <cfRule type="containsText" dxfId="623" priority="303" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="619" priority="303" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A817)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="622" priority="304" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="618" priority="304" operator="beginsWith" text="#">
       <formula>LEFT(A817,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A816">
-    <cfRule type="containsText" dxfId="621" priority="305" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="617" priority="305" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A816)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="620" priority="306" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="616" priority="306" operator="beginsWith" text="#">
       <formula>LEFT(A816,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A819">
-    <cfRule type="containsText" dxfId="619" priority="301" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="615" priority="301" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A819)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="618" priority="302" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="614" priority="302" operator="beginsWith" text="#">
       <formula>LEFT(A819,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A820">
-    <cfRule type="containsText" dxfId="617" priority="285" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="613" priority="285" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A820)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="616" priority="286" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="612" priority="286" operator="beginsWith" text="#">
       <formula>LEFT(A820,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A690">
-    <cfRule type="containsText" dxfId="615" priority="281" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="611" priority="281" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A690)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="614" priority="282" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="610" priority="282" operator="beginsWith" text="#">
       <formula>LEFT(A690,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A360">
-    <cfRule type="containsText" dxfId="613" priority="271" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="609" priority="271" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A360)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="612" priority="272" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="608" priority="272" operator="beginsWith" text="#">
       <formula>LEFT(A360,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A358">
-    <cfRule type="containsText" dxfId="611" priority="275" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="607" priority="275" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A358)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="610" priority="276" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="606" priority="276" operator="beginsWith" text="#">
       <formula>LEFT(A358,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A359">
-    <cfRule type="containsText" dxfId="609" priority="273" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="605" priority="273" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A359)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="608" priority="274" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="604" priority="274" operator="beginsWith" text="#">
       <formula>LEFT(A359,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A361">
-    <cfRule type="containsText" dxfId="607" priority="269" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="603" priority="269" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A361)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="606" priority="270" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="602" priority="270" operator="beginsWith" text="#">
       <formula>LEFT(A361,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A362">
-    <cfRule type="containsText" dxfId="605" priority="267" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="601" priority="267" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A362)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="604" priority="268" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="600" priority="268" operator="beginsWith" text="#">
       <formula>LEFT(A362,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A363">
-    <cfRule type="containsText" dxfId="603" priority="265" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="599" priority="265" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A363)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="602" priority="266" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="598" priority="266" operator="beginsWith" text="#">
       <formula>LEFT(A363,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A364">
-    <cfRule type="containsText" dxfId="601" priority="263" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="597" priority="263" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A364)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="600" priority="264" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="596" priority="264" operator="beginsWith" text="#">
       <formula>LEFT(A364,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A365">
-    <cfRule type="containsText" dxfId="599" priority="261" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="595" priority="261" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A365)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="598" priority="262" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="594" priority="262" operator="beginsWith" text="#">
       <formula>LEFT(A365,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A366">
-    <cfRule type="containsText" dxfId="597" priority="259" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="593" priority="259" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A366)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="596" priority="260" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="592" priority="260" operator="beginsWith" text="#">
       <formula>LEFT(A366,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A369">
-    <cfRule type="containsText" dxfId="595" priority="255" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="591" priority="255" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A369)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="594" priority="256" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="590" priority="256" operator="beginsWith" text="#">
       <formula>LEFT(A369,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A370">
-    <cfRule type="containsText" dxfId="593" priority="253" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="589" priority="253" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A370)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="592" priority="254" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="588" priority="254" operator="beginsWith" text="#">
       <formula>LEFT(A370,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A371">
-    <cfRule type="containsText" dxfId="591" priority="251" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="587" priority="251" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A371)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="590" priority="252" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="586" priority="252" operator="beginsWith" text="#">
       <formula>LEFT(A371,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A372">
-    <cfRule type="containsText" dxfId="589" priority="249" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="585" priority="249" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A372)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="588" priority="250" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="584" priority="250" operator="beginsWith" text="#">
       <formula>LEFT(A372,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A373">
-    <cfRule type="containsText" dxfId="587" priority="247" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="583" priority="247" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A373)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="586" priority="248" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="582" priority="248" operator="beginsWith" text="#">
       <formula>LEFT(A373,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A374">
-    <cfRule type="containsText" dxfId="585" priority="245" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="581" priority="245" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A374)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="584" priority="246" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="580" priority="246" operator="beginsWith" text="#">
       <formula>LEFT(A374,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A375">
-    <cfRule type="containsText" dxfId="583" priority="243" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="579" priority="243" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A375)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="582" priority="244" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="578" priority="244" operator="beginsWith" text="#">
       <formula>LEFT(A375,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A383:A389">
-    <cfRule type="containsText" dxfId="581" priority="241" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="577" priority="241" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A383)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="580" priority="242" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="576" priority="242" operator="beginsWith" text="#">
       <formula>LEFT(A383,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A381">
-    <cfRule type="containsText" dxfId="579" priority="239" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="575" priority="239" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A381)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="578" priority="240" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="574" priority="240" operator="beginsWith" text="#">
       <formula>LEFT(A381,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A390 A394:A397">
-    <cfRule type="containsText" dxfId="577" priority="237" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="573" priority="237" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A390)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="576" priority="238" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="572" priority="238" operator="beginsWith" text="#">
       <formula>LEFT(A390,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A402">
-    <cfRule type="containsText" dxfId="575" priority="235" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="571" priority="235" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A402)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="574" priority="236" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="570" priority="236" operator="beginsWith" text="#">
       <formula>LEFT(A402,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A413">
-    <cfRule type="containsText" dxfId="573" priority="233" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="569" priority="233" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A413)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="572" priority="234" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="568" priority="234" operator="beginsWith" text="#">
       <formula>LEFT(A413,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A376">
-    <cfRule type="containsText" dxfId="571" priority="231" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="567" priority="231" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A376)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="570" priority="232" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="566" priority="232" operator="beginsWith" text="#">
       <formula>LEFT(A376,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A408">
-    <cfRule type="containsText" dxfId="569" priority="229" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="565" priority="229" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A408)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="568" priority="230" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="564" priority="230" operator="beginsWith" text="#">
       <formula>LEFT(A408,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A409">
-    <cfRule type="containsText" dxfId="567" priority="227" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="563" priority="227" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A409)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="566" priority="228" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="562" priority="228" operator="beginsWith" text="#">
       <formula>LEFT(A409,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A410">
-    <cfRule type="containsText" dxfId="565" priority="225" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="561" priority="225" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A410)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="564" priority="226" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="560" priority="226" operator="beginsWith" text="#">
       <formula>LEFT(A410,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A412">
-    <cfRule type="containsText" dxfId="563" priority="221" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="559" priority="221" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A412)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="562" priority="222" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="558" priority="222" operator="beginsWith" text="#">
       <formula>LEFT(A412,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A414">
-    <cfRule type="containsText" dxfId="561" priority="219" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="557" priority="219" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A414)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="560" priority="220" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="556" priority="220" operator="beginsWith" text="#">
       <formula>LEFT(A414,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A415">
-    <cfRule type="containsText" dxfId="559" priority="217" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="555" priority="217" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A415)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="558" priority="218" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="554" priority="218" operator="beginsWith" text="#">
       <formula>LEFT(A415,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A457">
-    <cfRule type="containsText" dxfId="557" priority="215" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="553" priority="215" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A457)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="556" priority="216" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="552" priority="216" operator="beginsWith" text="#">
       <formula>LEFT(A457,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A416">
-    <cfRule type="containsText" dxfId="555" priority="213" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="551" priority="213" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A416)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="554" priority="214" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="550" priority="214" operator="beginsWith" text="#">
       <formula>LEFT(A416,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A417 A421 A424">
-    <cfRule type="containsText" dxfId="553" priority="211" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="549" priority="211" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A417)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="552" priority="212" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="548" priority="212" operator="beginsWith" text="#">
       <formula>LEFT(A417,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A426">
-    <cfRule type="containsText" dxfId="551" priority="207" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="547" priority="207" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A426)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="550" priority="208" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="546" priority="208" operator="beginsWith" text="#">
       <formula>LEFT(A426,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A777">
-    <cfRule type="containsText" dxfId="549" priority="193" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="545" priority="193" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A777)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="548" priority="194" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="544" priority="194" operator="beginsWith" text="#">
       <formula>LEFT(A777,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A778">
-    <cfRule type="containsText" dxfId="547" priority="191" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="543" priority="191" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A778)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="546" priority="192" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="542" priority="192" operator="beginsWith" text="#">
       <formula>LEFT(A778,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A367">
-    <cfRule type="containsText" dxfId="545" priority="189" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="541" priority="189" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A367)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="544" priority="190" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="540" priority="190" operator="beginsWith" text="#">
       <formula>LEFT(A367,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A501">
-    <cfRule type="containsText" dxfId="543" priority="187" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="539" priority="187" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A501)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="542" priority="188" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="538" priority="188" operator="beginsWith" text="#">
       <formula>LEFT(A501,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A502">
-    <cfRule type="containsText" dxfId="541" priority="185" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="537" priority="185" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A502)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="540" priority="186" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="536" priority="186" operator="beginsWith" text="#">
       <formula>LEFT(A502,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A503">
-    <cfRule type="containsText" dxfId="539" priority="183" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="535" priority="183" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A503)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="538" priority="184" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="534" priority="184" operator="beginsWith" text="#">
       <formula>LEFT(A503,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A531">
-    <cfRule type="containsText" dxfId="537" priority="181" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="533" priority="181" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A531)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="536" priority="182" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="532" priority="182" operator="beginsWith" text="#">
       <formula>LEFT(A531,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A520">
-    <cfRule type="containsText" dxfId="535" priority="179" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="531" priority="179" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A520)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="534" priority="180" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="530" priority="180" operator="beginsWith" text="#">
       <formula>LEFT(A520,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A821">
-    <cfRule type="containsText" dxfId="533" priority="175" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="529" priority="175" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A821)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="532" priority="176" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="528" priority="176" operator="beginsWith" text="#">
       <formula>LEFT(A821,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A779">
-    <cfRule type="containsText" dxfId="531" priority="171" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="527" priority="171" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A779)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="530" priority="172" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="526" priority="172" operator="beginsWith" text="#">
       <formula>LEFT(A779,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A257">
-    <cfRule type="containsText" dxfId="529" priority="169" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="525" priority="169" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A257)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="528" priority="170" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="524" priority="170" operator="beginsWith" text="#">
       <formula>LEFT(A257,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A822">
-    <cfRule type="containsText" dxfId="527" priority="159" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="523" priority="159" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A822)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="526" priority="160" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="522" priority="160" operator="beginsWith" text="#">
       <formula>LEFT(A822,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A175:A183 A185:A256">
-    <cfRule type="containsText" dxfId="525" priority="485" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="521" priority="485" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="524" priority="486" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="520" priority="486" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A169 A171 A161 A163:A167 A81 A83:A84 A87:A95 A97:A98 A102:A104 A74 A76:A79">
-    <cfRule type="containsText" dxfId="523" priority="373" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="519" priority="373" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="522" priority="374" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="518" priority="374" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116">
-    <cfRule type="containsText" dxfId="521" priority="1521" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="517" priority="1521" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="520" priority="1522" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="516" priority="1522" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A155:A156 A159 A134:A143 A117:A118 A109 A107 A111:A115 A145:A146">
-    <cfRule type="containsText" dxfId="519" priority="1803" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="515" priority="1803" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="518" priority="1804" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="514" priority="1804" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A129 A123:A124 A126:A127">
-    <cfRule type="containsText" dxfId="517" priority="1863" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="513" priority="1863" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="516" priority="1864" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="512" priority="1864" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A119">
-    <cfRule type="containsText" dxfId="515" priority="1925" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="511" priority="1925" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="514" priority="1926" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="510" priority="1926" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A131">
-    <cfRule type="containsText" dxfId="513" priority="167" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="509" priority="167" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="512" priority="168" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="508" priority="168" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130">
-    <cfRule type="containsText" dxfId="511" priority="165" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="507" priority="165" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="510" priority="166" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="506" priority="166" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A780">
-    <cfRule type="containsText" dxfId="509" priority="163" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="505" priority="163" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="508" priority="164" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="504" priority="164" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A781">
-    <cfRule type="containsText" dxfId="507" priority="161" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="503" priority="161" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="506" priority="162" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="502" priority="162" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A823">
-    <cfRule type="containsText" dxfId="505" priority="157" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="501" priority="157" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A823)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="504" priority="158" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="500" priority="158" operator="beginsWith" text="#">
       <formula>LEFT(A823,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A824">
-    <cfRule type="containsText" dxfId="503" priority="155" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="499" priority="155" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A822)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="502" priority="156" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="498" priority="156" operator="beginsWith" text="#">
       <formula>LEFT(A822,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B835:B837">
-    <cfRule type="containsText" dxfId="501" priority="131" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="497" priority="131" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",B829)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="500" priority="132" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="496" priority="132" operator="beginsWith" text="#">
       <formula>LEFT(B829,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B825 B829">
-    <cfRule type="containsText" dxfId="499" priority="149" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="495" priority="149" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="498" priority="150" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="494" priority="150" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A825">
-    <cfRule type="containsText" dxfId="497" priority="143" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="493" priority="143" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A825)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="496" priority="144" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="492" priority="144" operator="beginsWith" text="#">
       <formula>LEFT(A825,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A826">
-    <cfRule type="containsText" dxfId="495" priority="141" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="491" priority="141" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A826)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="494" priority="142" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="490" priority="142" operator="beginsWith" text="#">
       <formula>LEFT(A826,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B826">
-    <cfRule type="containsText" dxfId="493" priority="139" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="489" priority="139" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="492" priority="140" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="488" priority="140" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A827">
-    <cfRule type="containsText" dxfId="491" priority="137" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="487" priority="137" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A827)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="490" priority="138" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="486" priority="138" operator="beginsWith" text="#">
       <formula>LEFT(A827,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B827">
-    <cfRule type="containsText" dxfId="489" priority="135" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="485" priority="135" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="488" priority="136" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="484" priority="136" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A829:A837">
-    <cfRule type="containsText" dxfId="487" priority="133" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="483" priority="133" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A829)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="486" priority="134" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="482" priority="134" operator="beginsWith" text="#">
       <formula>LEFT(A829,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B838">
-    <cfRule type="containsText" dxfId="485" priority="127" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="481" priority="127" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="484" priority="128" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="480" priority="128" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A838">
-    <cfRule type="containsText" dxfId="483" priority="129" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="479" priority="129" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A813)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="482" priority="130" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="478" priority="130" operator="beginsWith" text="#">
       <formula>LEFT(A813,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A803:A804 A812">
-    <cfRule type="containsText" dxfId="481" priority="123" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="477" priority="123" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A803)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="480" priority="124" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="476" priority="124" operator="beginsWith" text="#">
       <formula>LEFT(A803,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A788">
-    <cfRule type="containsText" dxfId="479" priority="121" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="475" priority="121" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A788)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="478" priority="122" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="474" priority="122" operator="beginsWith" text="#">
       <formula>LEFT(A788,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A789">
-    <cfRule type="containsText" dxfId="477" priority="119" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="473" priority="119" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A789)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="476" priority="120" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="472" priority="120" operator="beginsWith" text="#">
       <formula>LEFT(A789,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128">
-    <cfRule type="containsText" dxfId="475" priority="115" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="471" priority="115" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="474" priority="116" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="470" priority="116" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A635">
-    <cfRule type="containsText" dxfId="473" priority="111" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="469" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="472" priority="112" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="468" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A787">
-    <cfRule type="containsText" dxfId="471" priority="103" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="467" priority="103" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A787)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="470" priority="104" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="466" priority="104" operator="beginsWith" text="#">
       <formula>LEFT(A787,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A802">
-    <cfRule type="containsText" dxfId="469" priority="101" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="465" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A802)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="468" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="464" priority="102" operator="beginsWith" text="#">
       <formula>LEFT(A802,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A505">
-    <cfRule type="containsText" dxfId="467" priority="99" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="463" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A505)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="466" priority="100" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="462" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(A505,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A805">
-    <cfRule type="containsText" dxfId="465" priority="97" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="461" priority="97" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A805)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="464" priority="98" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="460" priority="98" operator="beginsWith" text="#">
       <formula>LEFT(A805,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A807">
-    <cfRule type="containsText" dxfId="463" priority="93" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="459" priority="93" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A807)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="462" priority="94" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="458" priority="94" operator="beginsWith" text="#">
       <formula>LEFT(A807,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A809">
-    <cfRule type="containsText" dxfId="461" priority="89" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="457" priority="89" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A809)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="460" priority="90" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="456" priority="90" operator="beginsWith" text="#">
       <formula>LEFT(A809,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A810">
-    <cfRule type="containsText" dxfId="459" priority="87" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="455" priority="87" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A810)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="458" priority="88" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="454" priority="88" operator="beginsWith" text="#">
       <formula>LEFT(A810,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A811">
-    <cfRule type="containsText" dxfId="457" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="453" priority="85" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A811)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="456" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="452" priority="86" operator="beginsWith" text="#">
       <formula>LEFT(A811,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A456">
-    <cfRule type="containsText" dxfId="455" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="451" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A456)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="454" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="450" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A456,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A782">
-    <cfRule type="containsText" dxfId="453" priority="75" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="449" priority="75" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A782)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="452" priority="76" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="448" priority="76" operator="beginsWith" text="#">
       <formula>LEFT(A782,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A784">
-    <cfRule type="containsText" dxfId="451" priority="73" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="447" priority="73" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A784)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="450" priority="74" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="446" priority="74" operator="beginsWith" text="#">
       <formula>LEFT(A784,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A494:A495">
-    <cfRule type="containsText" dxfId="449" priority="71" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="445" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A494)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="448" priority="72" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="444" priority="72" operator="beginsWith" text="#">
       <formula>LEFT(A494,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A411">
-    <cfRule type="containsText" dxfId="447" priority="69" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="443" priority="69" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A411)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="446" priority="70" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="442" priority="70" operator="beginsWith" text="#">
       <formula>LEFT(A411,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A418:A420">
-    <cfRule type="containsText" dxfId="445" priority="67" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="441" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A418)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="444" priority="68" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="440" priority="68" operator="beginsWith" text="#">
       <formula>LEFT(A418,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A422:A423">
-    <cfRule type="containsText" dxfId="443" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="439" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A422)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="442" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="438" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A422,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A427:A429">
-    <cfRule type="containsText" dxfId="441" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="437" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A427)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="440" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="436" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(A427,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A425">
-    <cfRule type="containsText" dxfId="439" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="435" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A425)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="438" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="434" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A425,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A791">
-    <cfRule type="containsText" dxfId="437" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="433" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A791)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="436" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="432" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A791,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A368">
-    <cfRule type="containsText" dxfId="435" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="431" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A368)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="434" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="430" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A368,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A522">
-    <cfRule type="containsText" dxfId="433" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="429" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A522)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="432" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="428" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A522,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A808">
-    <cfRule type="containsText" dxfId="431" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="427" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A808)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="430" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="426" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A808,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A790">
-    <cfRule type="containsText" dxfId="429" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="425" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A790)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="428" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="424" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A790,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A806">
-    <cfRule type="containsText" dxfId="427" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="423" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A806)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="426" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="422" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A806,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="containsText" dxfId="425" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="421" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="424" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="420" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A783">
-    <cfRule type="containsText" dxfId="423" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="419" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A783)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="422" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="418" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A783,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A430">
-    <cfRule type="containsText" dxfId="421" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="417" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A430)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="420" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="416" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A430,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B830:B834">
-    <cfRule type="containsText" dxfId="419" priority="3057" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="415" priority="3057" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",B823)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="418" priority="3058" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="414" priority="3058" operator="beginsWith" text="#">
       <formula>LEFT(B823,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B828">
-    <cfRule type="containsText" dxfId="417" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="413" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="416" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="412" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A828">
-    <cfRule type="containsText" dxfId="415" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="411" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A828)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="414" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="410" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A828,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A527">
-    <cfRule type="containsText" dxfId="389" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="409" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A527)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="388" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="408" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A527,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -62030,730 +61798,730 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A276:A280 A319:A324 A31:A35 A175:A201 A326:A328 A334:A1048576 A204 A1:A11 A136:A138 A141:A143 A16:A19 A130:A133 A38 A208:A232 A238 A146:A151 A155 A158:A159">
-    <cfRule type="containsText" dxfId="387" priority="399" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="383" priority="399" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="386" priority="400" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="382" priority="400" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A15">
-    <cfRule type="containsText" dxfId="385" priority="391" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="381" priority="391" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A14)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="384" priority="392" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="380" priority="392" operator="beginsWith" text="#">
       <formula>LEFT(A14,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="383" priority="389" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="379" priority="389" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="382" priority="390" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="378" priority="390" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:A40">
-    <cfRule type="containsText" dxfId="381" priority="387" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="377" priority="387" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A39)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="380" priority="388" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="376" priority="388" operator="beginsWith" text="#">
       <formula>LEFT(A39,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="containsText" dxfId="379" priority="385" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="375" priority="385" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A13)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="378" priority="386" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="374" priority="386" operator="beginsWith" text="#">
       <formula>LEFT(A13,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A241">
-    <cfRule type="containsText" dxfId="377" priority="313" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="373" priority="313" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A241)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="376" priority="314" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="372" priority="314" operator="beginsWith" text="#">
       <formula>LEFT(A241,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A203">
-    <cfRule type="containsText" dxfId="375" priority="303" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="371" priority="303" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A203)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="374" priority="304" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="370" priority="304" operator="beginsWith" text="#">
       <formula>LEFT(A203,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="containsText" dxfId="373" priority="293" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="369" priority="293" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A20)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="372" priority="294" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="368" priority="294" operator="beginsWith" text="#">
       <formula>LEFT(A20,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A244">
-    <cfRule type="containsText" dxfId="371" priority="271" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="367" priority="271" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A244)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="370" priority="272" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="366" priority="272" operator="beginsWith" text="#">
       <formula>LEFT(A244,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A275">
-    <cfRule type="containsText" dxfId="369" priority="255" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="365" priority="255" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A275)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="368" priority="256" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="364" priority="256" operator="beginsWith" text="#">
       <formula>LEFT(A275,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="containsText" dxfId="367" priority="291" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="363" priority="291" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="366" priority="292" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="362" priority="292" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:A78">
-    <cfRule type="containsText" dxfId="365" priority="1199" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="361" priority="1199" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="364" priority="1200" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="360" priority="1200" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:A63">
-    <cfRule type="containsText" dxfId="363" priority="1249" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="359" priority="1249" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="362" priority="1250" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="358" priority="1250" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64:A67">
-    <cfRule type="containsText" dxfId="361" priority="1419" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="357" priority="1419" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="360" priority="1420" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="356" priority="1420" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:A83">
-    <cfRule type="containsText" dxfId="359" priority="1589" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="355" priority="1589" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="358" priority="1590" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="354" priority="1590" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A233">
-    <cfRule type="containsText" dxfId="357" priority="257" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="353" priority="257" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="356" priority="258" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="352" priority="258" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A325">
-    <cfRule type="containsText" dxfId="355" priority="249" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="351" priority="249" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A325)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="354" priority="250" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="350" priority="250" operator="beginsWith" text="#">
       <formula>LEFT(A325,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A282">
-    <cfRule type="containsText" dxfId="353" priority="239" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="349" priority="239" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A282)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="352" priority="240" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="348" priority="240" operator="beginsWith" text="#">
       <formula>LEFT(A282,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A312">
-    <cfRule type="containsText" dxfId="351" priority="241" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="347" priority="241" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A312)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="350" priority="242" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="346" priority="242" operator="beginsWith" text="#">
       <formula>LEFT(A312,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
-    <cfRule type="containsText" dxfId="349" priority="237" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="345" priority="237" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A153)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="348" priority="238" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="344" priority="238" operator="beginsWith" text="#">
       <formula>LEFT(A153,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A154">
-    <cfRule type="containsText" dxfId="347" priority="235" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="343" priority="235" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A154)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="346" priority="236" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="342" priority="236" operator="beginsWith" text="#">
       <formula>LEFT(A154,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A286:A287">
-    <cfRule type="containsText" dxfId="345" priority="231" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="341" priority="231" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A286)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="344" priority="232" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="340" priority="232" operator="beginsWith" text="#">
       <formula>LEFT(A286,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A234">
-    <cfRule type="containsText" dxfId="343" priority="229" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="339" priority="229" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="342" priority="230" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="338" priority="230" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A205">
-    <cfRule type="containsText" dxfId="341" priority="223" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="337" priority="223" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="340" priority="224" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="336" priority="224" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A288">
-    <cfRule type="containsText" dxfId="339" priority="221" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="335" priority="221" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A288)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="338" priority="222" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="334" priority="222" operator="beginsWith" text="#">
       <formula>LEFT(A288,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A284">
-    <cfRule type="containsText" dxfId="337" priority="217" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="333" priority="217" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A284)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="336" priority="218" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="332" priority="218" operator="beginsWith" text="#">
       <formula>LEFT(A284,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A291">
-    <cfRule type="containsText" dxfId="335" priority="215" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="331" priority="215" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A291)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="334" priority="216" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="330" priority="216" operator="beginsWith" text="#">
       <formula>LEFT(A291,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A289">
-    <cfRule type="containsText" dxfId="333" priority="211" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="329" priority="211" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A289)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="332" priority="212" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="328" priority="212" operator="beginsWith" text="#">
       <formula>LEFT(A289,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A290">
-    <cfRule type="containsText" dxfId="331" priority="209" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="327" priority="209" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A290)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="330" priority="210" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="326" priority="210" operator="beginsWith" text="#">
       <formula>LEFT(A290,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A285">
-    <cfRule type="containsText" dxfId="329" priority="207" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="325" priority="207" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A285)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="328" priority="208" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="324" priority="208" operator="beginsWith" text="#">
       <formula>LEFT(A285,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A329">
-    <cfRule type="containsText" dxfId="327" priority="205" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="323" priority="205" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A329)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="326" priority="206" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="322" priority="206" operator="beginsWith" text="#">
       <formula>LEFT(A329,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A239">
-    <cfRule type="containsText" dxfId="325" priority="203" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="321" priority="203" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A239)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="324" priority="204" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="320" priority="204" operator="beginsWith" text="#">
       <formula>LEFT(A239,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A240">
-    <cfRule type="containsText" dxfId="323" priority="201" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="319" priority="201" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A240)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="322" priority="202" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="318" priority="202" operator="beginsWith" text="#">
       <formula>LEFT(A240,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A161">
-    <cfRule type="containsText" dxfId="321" priority="199" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="317" priority="199" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="320" priority="200" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="316" priority="200" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A162">
-    <cfRule type="containsText" dxfId="319" priority="197" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="315" priority="197" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="318" priority="198" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="314" priority="198" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A283">
-    <cfRule type="containsText" dxfId="317" priority="193" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="313" priority="193" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A283)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="316" priority="194" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="312" priority="194" operator="beginsWith" text="#">
       <formula>LEFT(A283,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A292">
-    <cfRule type="containsText" dxfId="315" priority="191" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="311" priority="191" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A292)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="314" priority="192" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="310" priority="192" operator="beginsWith" text="#">
       <formula>LEFT(A292,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A293">
-    <cfRule type="containsText" dxfId="313" priority="189" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="309" priority="189" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A293)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="312" priority="190" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="308" priority="190" operator="beginsWith" text="#">
       <formula>LEFT(A293,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A294">
-    <cfRule type="containsText" dxfId="311" priority="187" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="307" priority="187" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A294)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="310" priority="188" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="306" priority="188" operator="beginsWith" text="#">
       <formula>LEFT(A294,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A235:A237 A86:A87 A89">
-    <cfRule type="containsText" dxfId="309" priority="285" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="305" priority="285" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="308" priority="286" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="304" priority="286" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79:A80">
-    <cfRule type="containsText" dxfId="307" priority="2213" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="303" priority="2213" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="306" priority="2214" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="302" priority="2214" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="containsText" dxfId="305" priority="2325" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="301" priority="2325" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="304" priority="2326" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="300" priority="2326" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="containsText" dxfId="303" priority="185" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="299" priority="185" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A88)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="302" priority="186" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="298" priority="186" operator="beginsWith" text="#">
       <formula>LEFT(A88,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A121">
-    <cfRule type="containsText" dxfId="301" priority="175" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="297" priority="175" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="300" priority="176" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="296" priority="176" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A120">
-    <cfRule type="containsText" dxfId="299" priority="171" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="295" priority="171" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A120)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="298" priority="172" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="294" priority="172" operator="beginsWith" text="#">
       <formula>LEFT(A120,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A169">
-    <cfRule type="containsText" dxfId="297" priority="169" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="293" priority="169" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="296" priority="170" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="292" priority="170" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A249">
-    <cfRule type="containsText" dxfId="295" priority="137" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="291" priority="137" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A249)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="294" priority="138" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="290" priority="138" operator="beginsWith" text="#">
       <formula>LEFT(A249,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A122">
-    <cfRule type="containsText" dxfId="293" priority="127" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="289" priority="127" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A122)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="292" priority="128" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="288" priority="128" operator="beginsWith" text="#">
       <formula>LEFT(A122,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A281">
-    <cfRule type="containsText" dxfId="291" priority="121" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="287" priority="121" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A281)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="290" priority="122" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="286" priority="122" operator="beginsWith" text="#">
       <formula>LEFT(A281,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A123">
-    <cfRule type="containsText" dxfId="289" priority="119" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="285" priority="119" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A123)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="288" priority="120" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="284" priority="120" operator="beginsWith" text="#">
       <formula>LEFT(A123,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A124">
-    <cfRule type="containsText" dxfId="287" priority="117" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="283" priority="117" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A124)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="286" priority="118" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="282" priority="118" operator="beginsWith" text="#">
       <formula>LEFT(A124,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A125">
-    <cfRule type="containsText" dxfId="285" priority="115" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="281" priority="115" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A125)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="284" priority="116" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="280" priority="116" operator="beginsWith" text="#">
       <formula>LEFT(A125,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A126">
-    <cfRule type="containsText" dxfId="283" priority="113" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="279" priority="113" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A126)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="282" priority="114" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="278" priority="114" operator="beginsWith" text="#">
       <formula>LEFT(A126,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A127">
-    <cfRule type="containsText" dxfId="281" priority="111" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="277" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A127)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="280" priority="112" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="276" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(A127,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A313">
-    <cfRule type="containsText" dxfId="279" priority="107" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="275" priority="107" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A313)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="278" priority="108" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="274" priority="108" operator="beginsWith" text="#">
       <formula>LEFT(A313,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A314 A318">
-    <cfRule type="containsText" dxfId="277" priority="103" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="273" priority="103" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A314)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="276" priority="104" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="272" priority="104" operator="beginsWith" text="#">
       <formula>LEFT(A314,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="containsText" dxfId="275" priority="101" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="271" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A36)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="274" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="270" priority="102" operator="beginsWith" text="#">
       <formula>LEFT(A36,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A168">
-    <cfRule type="containsText" dxfId="273" priority="99" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="269" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="272" priority="100" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="268" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A170">
-    <cfRule type="containsText" dxfId="271" priority="91" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="267" priority="91" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="270" priority="92" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="266" priority="92" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A134">
-    <cfRule type="containsText" dxfId="269" priority="89" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="265" priority="89" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A134)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="268" priority="90" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="264" priority="90" operator="beginsWith" text="#">
       <formula>LEFT(A134,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A139">
-    <cfRule type="containsText" dxfId="267" priority="87" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="263" priority="87" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A139)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="266" priority="88" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="262" priority="88" operator="beginsWith" text="#">
       <formula>LEFT(A139,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="containsText" dxfId="265" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="261" priority="85" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A144)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="264" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="260" priority="86" operator="beginsWith" text="#">
       <formula>LEFT(A144,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A164">
-    <cfRule type="containsText" dxfId="263" priority="83" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="259" priority="83" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A164)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="262" priority="84" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="258" priority="84" operator="beginsWith" text="#">
       <formula>LEFT(A164,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A271">
-    <cfRule type="containsText" dxfId="261" priority="81" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="257" priority="81" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A271)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="260" priority="82" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="256" priority="82" operator="beginsWith" text="#">
       <formula>LEFT(A271,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A330">
-    <cfRule type="containsText" dxfId="259" priority="79" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="255" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A330)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="258" priority="80" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="254" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(A330,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A315">
-    <cfRule type="containsText" dxfId="257" priority="77" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="253" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A315)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="256" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="252" priority="78" operator="beginsWith" text="#">
       <formula>LEFT(A315,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="containsText" dxfId="255" priority="69" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="251" priority="69" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A37)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="254" priority="70" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="250" priority="70" operator="beginsWith" text="#">
       <formula>LEFT(A37,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A273:A274">
-    <cfRule type="containsText" dxfId="253" priority="55" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="249" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A273)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="252" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="248" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(A273,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A332">
-    <cfRule type="containsText" dxfId="251" priority="53" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="247" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="250" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="246" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A317">
-    <cfRule type="containsText" dxfId="249" priority="51" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="245" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="248" priority="52" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="244" priority="52" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A129">
-    <cfRule type="containsText" dxfId="247" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="243" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="246" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="242" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128">
-    <cfRule type="containsText" dxfId="245" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="241" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A128)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="244" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="240" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A128,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A172">
-    <cfRule type="containsText" dxfId="243" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="239" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A172)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="242" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="238" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(A172,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A206">
-    <cfRule type="containsText" dxfId="241" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="237" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A206)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="240" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="236" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A206,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A171">
-    <cfRule type="containsText" dxfId="239" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="235" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="238" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="234" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135">
-    <cfRule type="containsText" dxfId="237" priority="35" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="233" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A135)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="236" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="232" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A135,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A140">
-    <cfRule type="containsText" dxfId="235" priority="33" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="231" priority="33" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A140)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="234" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="230" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(A140,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145">
-    <cfRule type="containsText" dxfId="233" priority="31" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="229" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A145)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="232" priority="32" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="228" priority="32" operator="beginsWith" text="#">
       <formula>LEFT(A145,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A165:A166">
-    <cfRule type="containsText" dxfId="231" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="227" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A165)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="230" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="226" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A165,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A316">
-    <cfRule type="containsText" dxfId="229" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="225" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A316)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="228" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="224" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A316,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A331">
-    <cfRule type="containsText" dxfId="227" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="223" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A331)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="226" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="222" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A331,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272">
-    <cfRule type="containsText" dxfId="225" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="221" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A272)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="224" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="220" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A272,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A173">
-    <cfRule type="containsText" dxfId="197" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="219" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A173)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="196" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="218" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A173,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A174">
-    <cfRule type="containsText" dxfId="195" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="217" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A174)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="194" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="216" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A174,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A207">
-    <cfRule type="containsText" dxfId="193" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="215" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A207)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="192" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="214" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A207,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A157">
-    <cfRule type="containsText" dxfId="191" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="213" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A157)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="190" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="212" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A157,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152">
-    <cfRule type="containsText" dxfId="189" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="211" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A152)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="188" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="210" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A152,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A156">
-    <cfRule type="containsText" dxfId="187" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="209" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A156)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="186" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="208" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A156,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A160">
-    <cfRule type="containsText" dxfId="185" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="207" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A160)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="184" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="206" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A160,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A163">
-    <cfRule type="containsText" dxfId="183" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="205" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A163)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="182" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="204" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A163,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A167">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="203" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A167)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="202" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A167,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -64298,106 +64066,106 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A7">
-    <cfRule type="containsText" dxfId="181" priority="29" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="177" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="180" priority="30" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="176" priority="30" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A10">
-    <cfRule type="containsText" dxfId="179" priority="27" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="175" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A9)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="178" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="174" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(A9,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="containsText" dxfId="177" priority="25" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="173" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A13)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="176" priority="26" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="172" priority="26" operator="beginsWith" text="#">
       <formula>LEFT(A13,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="175" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="171" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="174" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="170" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="containsText" dxfId="173" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="169" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A11)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="172" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="168" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A11,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="containsText" dxfId="171" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="167" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A8)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="170" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="166" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A8,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="containsText" dxfId="169" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="165" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A32)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="168" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="164" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A32,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="containsText" dxfId="167" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="163" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A21)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="166" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="162" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A21,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55">
-    <cfRule type="containsText" dxfId="165" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="161" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A55)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="164" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="160" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A55,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="containsText" dxfId="163" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="159" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A62)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="162" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="158" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A62,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="containsText" dxfId="161" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="157" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A53)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="160" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="156" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A53,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="containsText" dxfId="159" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="155" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A29)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="158" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="154" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A29,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="containsText" dxfId="157" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="153" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A66)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="156" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="152" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A66,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -68346,298 +68114,298 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A11">
-    <cfRule type="containsText" dxfId="145" priority="175" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="141" priority="175" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="144" priority="176" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="140" priority="176" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A14">
-    <cfRule type="containsText" dxfId="143" priority="173" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="139" priority="173" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A13)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="142" priority="174" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="138" priority="174" operator="beginsWith" text="#">
       <formula>LEFT(A13,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:A20">
-    <cfRule type="containsText" dxfId="141" priority="171" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="137" priority="171" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="140" priority="172" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="136" priority="172" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="139" priority="169" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="135" priority="169" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="138" priority="170" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="134" priority="170" operator="beginsWith" text="#">
       <formula>LEFT(A16,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="137" priority="167" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="133" priority="167" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A15)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="136" priority="168" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="132" priority="168" operator="beginsWith" text="#">
       <formula>LEFT(A15,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="135" priority="165" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="131" priority="165" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="134" priority="166" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="130" priority="166" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:A39">
-    <cfRule type="containsText" dxfId="133" priority="163" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="129" priority="163" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A38)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="132" priority="164" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="128" priority="164" operator="beginsWith" text="#">
       <formula>LEFT(A38,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="containsText" dxfId="131" priority="161" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="127" priority="161" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="130" priority="162" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="126" priority="162" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50">
-    <cfRule type="containsText" dxfId="129" priority="155" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="125" priority="155" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="128" priority="156" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="124" priority="156" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="containsText" dxfId="127" priority="145" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="123" priority="145" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A22)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="126" priority="146" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="122" priority="146" operator="beginsWith" text="#">
       <formula>LEFT(A22,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="containsText" dxfId="125" priority="143" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="121" priority="143" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A32)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="124" priority="144" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="120" priority="144" operator="beginsWith" text="#">
       <formula>LEFT(A32,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:A102">
-    <cfRule type="containsText" dxfId="123" priority="129" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="119" priority="129" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A92)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="122" priority="130" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="118" priority="130" operator="beginsWith" text="#">
       <formula>LEFT(A92,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103:A105">
-    <cfRule type="containsText" dxfId="121" priority="121" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="117" priority="121" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A103)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="120" priority="122" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="116" priority="122" operator="beginsWith" text="#">
       <formula>LEFT(A103,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A121:A124">
-    <cfRule type="containsText" dxfId="119" priority="119" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="115" priority="119" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A121)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="118" priority="120" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="114" priority="120" operator="beginsWith" text="#">
       <formula>LEFT(A121,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A139">
-    <cfRule type="containsText" dxfId="117" priority="111" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="113" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A139)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="116" priority="112" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="112" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(A139,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A150 A155">
-    <cfRule type="containsText" dxfId="115" priority="109" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="111" priority="109" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A150)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="114" priority="110" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="110" priority="110" operator="beginsWith" text="#">
       <formula>LEFT(A150,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A160 A163:A164">
-    <cfRule type="containsText" dxfId="113" priority="105" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="109" priority="105" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A160)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="112" priority="106" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="108" priority="106" operator="beginsWith" text="#">
       <formula>LEFT(A160,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137">
-    <cfRule type="containsText" dxfId="111" priority="101" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="107" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A137)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="110" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="106" priority="102" operator="beginsWith" text="#">
       <formula>LEFT(A137,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A129">
-    <cfRule type="containsText" dxfId="109" priority="99" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="105" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A129)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="108" priority="100" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="104" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(A129,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138">
-    <cfRule type="containsText" dxfId="107" priority="97" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="103" priority="97" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A138)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="106" priority="98" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="102" priority="98" operator="beginsWith" text="#">
       <formula>LEFT(A138,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A149">
-    <cfRule type="containsText" dxfId="105" priority="67" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="101" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A149)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="104" priority="68" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="100" priority="68" operator="beginsWith" text="#">
       <formula>LEFT(A149,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A159">
-    <cfRule type="containsText" dxfId="103" priority="65" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="99" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A159)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="102" priority="66" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="98" priority="66" operator="beginsWith" text="#">
       <formula>LEFT(A159,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130">
-    <cfRule type="containsText" dxfId="101" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="97" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A130)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="100" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="96" priority="64" operator="beginsWith" text="#">
       <formula>LEFT(A130,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A131">
-    <cfRule type="containsText" dxfId="99" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="95" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A131)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="98" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="94" priority="62" operator="beginsWith" text="#">
       <formula>LEFT(A131,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107:A108">
-    <cfRule type="containsText" dxfId="97" priority="43" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="93" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A107)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="44" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="92" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A107,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106">
-    <cfRule type="containsText" dxfId="95" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="91" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A106)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="94" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="90" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(A106,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109">
-    <cfRule type="containsText" dxfId="93" priority="23" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="89" priority="23" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A109)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="92" priority="24" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="88" priority="24" operator="beginsWith" text="#">
       <formula>LEFT(A109,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110">
-    <cfRule type="containsText" dxfId="91" priority="21" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="87" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A110)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="90" priority="22" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="86" priority="22" operator="beginsWith" text="#">
       <formula>LEFT(A110,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111">
-    <cfRule type="containsText" dxfId="89" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="85" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A111)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="84" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A111,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A112">
-    <cfRule type="containsText" dxfId="87" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="83" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A112)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="86" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="82" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A112,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A113">
-    <cfRule type="containsText" dxfId="85" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="81" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A113)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="84" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="80" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A113,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114">
-    <cfRule type="containsText" dxfId="83" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="79" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A114)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="82" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="78" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A114,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A115">
-    <cfRule type="containsText" dxfId="81" priority="11" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="77" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A115)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="80" priority="12" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="76" priority="12" operator="beginsWith" text="#">
       <formula>LEFT(A115,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A118">
-    <cfRule type="containsText" dxfId="79" priority="9" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A118)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="78" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="74" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(A118,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A119">
-    <cfRule type="containsText" dxfId="77" priority="7" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="73" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A119)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="76" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="72" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(A119,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A117">
-    <cfRule type="containsText" dxfId="75" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A117)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="74" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="70" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A117,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116">
-    <cfRule type="containsText" dxfId="73" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A116)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="72" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="68" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A116,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -70101,98 +69869,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A7">
-    <cfRule type="containsText" dxfId="31" priority="49" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="27" priority="49" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="26" priority="50" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A10">
-    <cfRule type="containsText" dxfId="29" priority="47" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="25" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A9)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="24" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(A9,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="containsText" dxfId="27" priority="45" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="23" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A13)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="46" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="22" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(A13,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="25" priority="43" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="21" priority="43" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A12)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="44" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="20" priority="44" operator="beginsWith" text="#">
       <formula>LEFT(A12,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="containsText" dxfId="23" priority="41" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="19" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A11)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="18" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(A11,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="containsText" dxfId="21" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="17" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A8)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="16" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(A8,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A37)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="14" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(A37,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A46)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="12" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(A46,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="11" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="10" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(A17,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A21)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="8" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(A21,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A33)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="6" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A33,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A27)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="4" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A27,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated OrcaFlexInterface with MiscVars
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1190 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: f04b65d460510afafd612b89c4bff32724390ced
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2694">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -8312,6 +8312,9 @@
   </si>
   <si>
     <t>BD_MiscVarType</t>
+  </si>
+  <si>
+    <t>Orca_MiscVarType</t>
   </si>
 </sst>
 </file>
@@ -17047,9 +17050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J422"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D201" sqref="D201"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I301" sqref="I301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24003,7 +24006,7 @@
         <v>1756</v>
       </c>
       <c r="F301" s="27" t="s">
-        <v>26</v>
+        <v>1858</v>
       </c>
       <c r="G301" s="27" t="s">
         <v>26</v>
@@ -24012,7 +24015,7 @@
         <v>26</v>
       </c>
       <c r="I301" s="28" t="s">
-        <v>1766</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
@@ -24102,7 +24105,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="305" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A305" s="27" t="s">
         <v>22</v>
       </c>
@@ -24113,10 +24116,10 @@
         <v>27</v>
       </c>
       <c r="D305" s="27" t="s">
-        <v>2603</v>
+        <v>2693</v>
       </c>
       <c r="E305" s="27" t="s">
-        <v>1760</v>
+        <v>1421</v>
       </c>
       <c r="F305" s="27" t="s">
         <v>26</v>
@@ -24128,7 +24131,7 @@
         <v>26</v>
       </c>
       <c r="I305" s="28" t="s">
-        <v>1770</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated HydroDyn with MiscVars
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1191 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: d4980849abf105d8cb7484c21e7f93c0b99899cb
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2695">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -8315,6 +8315,9 @@
   </si>
   <si>
     <t>Orca_MiscVarType</t>
+  </si>
+  <si>
+    <t>HydroDyn_MiscVarType</t>
   </si>
 </sst>
 </file>
@@ -17050,9 +17053,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I301" sqref="I301"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D248" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22526,7 +22529,7 @@
         <v>1756</v>
       </c>
       <c r="F241" s="27" t="s">
-        <v>26</v>
+        <v>1858</v>
       </c>
       <c r="G241" s="27" t="s">
         <v>26</v>
@@ -22535,7 +22538,7 @@
         <v>26</v>
       </c>
       <c r="I241" s="28" t="s">
-        <v>1766</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.3">
@@ -22625,7 +22628,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="245" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245" s="27" t="s">
         <v>22</v>
       </c>
@@ -22636,10 +22639,10 @@
         <v>27</v>
       </c>
       <c r="D245" s="27" t="s">
-        <v>1821</v>
+        <v>2694</v>
       </c>
       <c r="E245" s="27" t="s">
-        <v>1760</v>
+        <v>1421</v>
       </c>
       <c r="F245" s="27" t="s">
         <v>26</v>
@@ -22651,7 +22654,7 @@
         <v>26</v>
       </c>
       <c r="I245" s="28" t="s">
-        <v>1770</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- updated AD14/DWM with MiscVars - fixed IVF compilation of discon DLLs for preprocessor directives
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1194 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: df036eca346f13086d8b2623b83b579325918350
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2696">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -8318,6 +8318,9 @@
   </si>
   <si>
     <t>HydroDyn_MiscVarType</t>
+  </si>
+  <si>
+    <t>AD14_MiscVarType</t>
   </si>
 </sst>
 </file>
@@ -17053,9 +17056,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J422"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D248" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21223,7 +21226,7 @@
         <v>1756</v>
       </c>
       <c r="F187" s="27" t="s">
-        <v>26</v>
+        <v>1858</v>
       </c>
       <c r="G187" s="27" t="s">
         <v>26</v>
@@ -21232,7 +21235,7 @@
         <v>26</v>
       </c>
       <c r="I187" s="28" t="s">
-        <v>1766</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
@@ -21322,7 +21325,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="191" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" s="27" t="s">
         <v>22</v>
       </c>
@@ -21333,10 +21336,10 @@
         <v>27</v>
       </c>
       <c r="D191" s="27" t="s">
-        <v>2402</v>
+        <v>2695</v>
       </c>
       <c r="E191" s="27" t="s">
-        <v>1760</v>
+        <v>1421</v>
       </c>
       <c r="F191" s="27" t="s">
         <v>26</v>
@@ -21348,7 +21351,7 @@
         <v>26</v>
       </c>
       <c r="I191" s="28" t="s">
-        <v>1770</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- updated SubDyn with MiscVars
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1195 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 92ab5548b42d88c3d546feaced44bf2040172f55
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2697">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -8321,6 +8321,9 @@
   </si>
   <si>
     <t>AD14_MiscVarType</t>
+  </si>
+  <si>
+    <t>SD_MiscVarType</t>
   </si>
 </sst>
 </file>
@@ -17056,9 +17059,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22236,7 +22239,7 @@
         <v>1756</v>
       </c>
       <c r="F229" s="27" t="s">
-        <v>26</v>
+        <v>1858</v>
       </c>
       <c r="G229" s="27" t="s">
         <v>26</v>
@@ -22245,7 +22248,7 @@
         <v>26</v>
       </c>
       <c r="I229" s="28" t="s">
-        <v>1766</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
@@ -22335,7 +22338,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" s="27" t="s">
         <v>22</v>
       </c>
@@ -22346,10 +22349,10 @@
         <v>27</v>
       </c>
       <c r="D233" s="27" t="s">
-        <v>1785</v>
+        <v>2696</v>
       </c>
       <c r="E233" s="27" t="s">
-        <v>1760</v>
+        <v>1421</v>
       </c>
       <c r="F233" s="27" t="s">
         <v>26</v>
@@ -22361,7 +22364,7 @@
         <v>26</v>
       </c>
       <c r="I233" s="28" t="s">
-        <v>1770</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- updated FEAM with MiscVars - fixed copy of OtherStates in Orca, which we wouldn't notice because it doesn't use other states.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1199 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 426626b9e534acabda8a164681e6b438075ab131
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2698">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -8324,6 +8324,9 @@
   </si>
   <si>
     <t>SD_MiscVarType</t>
+  </si>
+  <si>
+    <t>FEAM_MiscVarType</t>
   </si>
 </sst>
 </file>
@@ -17059,9 +17062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J422"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I278" sqref="I278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23423,7 +23426,7 @@
         <v>1756</v>
       </c>
       <c r="F277" s="27" t="s">
-        <v>26</v>
+        <v>1858</v>
       </c>
       <c r="G277" s="27" t="s">
         <v>26</v>
@@ -23432,7 +23435,7 @@
         <v>26</v>
       </c>
       <c r="I277" s="28" t="s">
-        <v>1766</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
@@ -23522,7 +23525,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="281" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A281" s="27" t="s">
         <v>22</v>
       </c>
@@ -23533,10 +23536,10 @@
         <v>27</v>
       </c>
       <c r="D281" s="27" t="s">
-        <v>1840</v>
+        <v>2697</v>
       </c>
       <c r="E281" s="27" t="s">
-        <v>1760</v>
+        <v>1421</v>
       </c>
       <c r="F281" s="27" t="s">
         <v>26</v>
@@ -23548,7 +23551,7 @@
         <v>26</v>
       </c>
       <c r="I281" s="28" t="s">
-        <v>1770</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- updated IceDyn with MiscVars - updated ReadFASTtext.m so PlotFASToutput.m can read files without units (like IceDyn's driver output)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1202 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 01c68c11b7ad968df6c54a913a7c7e2f733f205f
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2699">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -8327,6 +8327,9 @@
   </si>
   <si>
     <t>FEAM_MiscVarType</t>
+  </si>
+  <si>
+    <t>IceD_MiscVarType</t>
   </si>
 </sst>
 </file>
@@ -17062,9 +17065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I278" sqref="I278"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19978,7 +19981,7 @@
         <v>1756</v>
       </c>
       <c r="F134" s="27" t="s">
-        <v>31</v>
+        <v>195</v>
       </c>
       <c r="G134" s="27" t="s">
         <v>26</v>
@@ -19987,7 +19990,7 @@
         <v>26</v>
       </c>
       <c r="I134" s="28" t="s">
-        <v>1766</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
@@ -20077,7 +20080,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="27" t="s">
         <v>22</v>
       </c>
@@ -20088,10 +20091,10 @@
         <v>27</v>
       </c>
       <c r="D138" s="27" t="s">
-        <v>1749</v>
+        <v>2698</v>
       </c>
       <c r="E138" s="27" t="s">
-        <v>1760</v>
+        <v>1421</v>
       </c>
       <c r="F138" s="27" t="s">
         <v>31</v>
@@ -20103,7 +20106,7 @@
         <v>26</v>
       </c>
       <c r="I138" s="28" t="s">
-        <v>1770</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated IceFloe with MiscVar type also update TMD dependencies with updated code from UMass
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1204 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 63dd1b9c7e7c21b69d50ad6ca3a297d6c6d4d78e
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2700">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -8330,6 +8330,9 @@
   </si>
   <si>
     <t>IceD_MiscVarType</t>
+  </si>
+  <si>
+    <t>IceFloe_MiscVarType</t>
   </si>
 </sst>
 </file>
@@ -17065,9 +17068,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J422"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A139" sqref="A139"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E258" sqref="E258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22837,7 +22840,7 @@
         <v>1756</v>
       </c>
       <c r="F253" s="27" t="s">
-        <v>26</v>
+        <v>1858</v>
       </c>
       <c r="G253" s="27" t="s">
         <v>26</v>
@@ -22846,7 +22849,7 @@
         <v>26</v>
       </c>
       <c r="I253" s="28" t="s">
-        <v>1766</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.3">
@@ -22936,7 +22939,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="257" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A257" s="27" t="s">
         <v>22</v>
       </c>
@@ -22947,10 +22950,10 @@
         <v>27</v>
       </c>
       <c r="D257" s="27" t="s">
-        <v>1850</v>
+        <v>2699</v>
       </c>
       <c r="E257" s="27" t="s">
-        <v>1760</v>
+        <v>1421</v>
       </c>
       <c r="F257" s="27" t="s">
         <v>26</v>
@@ -22962,7 +22965,7 @@
         <v>26</v>
       </c>
       <c r="I257" s="28" t="s">
-        <v>1770</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated MoorDyn with MiscVar type
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1206 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 800094f18c47cbb4718648625d078575ec350473
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14904" uniqueCount="2701">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -8333,6 +8333,9 @@
   </si>
   <si>
     <t>IceFloe_MiscVarType</t>
+  </si>
+  <si>
+    <t>MD_MiscVarType</t>
   </si>
 </sst>
 </file>
@@ -17068,9 +17071,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E258" sqref="E258"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C280" sqref="C280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23728,7 +23731,7 @@
         <v>1756</v>
       </c>
       <c r="F289" s="27" t="s">
-        <v>26</v>
+        <v>1858</v>
       </c>
       <c r="G289" s="27" t="s">
         <v>26</v>
@@ -23737,7 +23740,7 @@
         <v>26</v>
       </c>
       <c r="I289" s="28" t="s">
-        <v>1766</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.3">
@@ -23827,7 +23830,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="293" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A293" s="27" t="s">
         <v>22</v>
       </c>
@@ -23838,10 +23841,10 @@
         <v>27</v>
       </c>
       <c r="D293" s="27" t="s">
-        <v>2204</v>
+        <v>2700</v>
       </c>
       <c r="E293" s="27" t="s">
-        <v>1760</v>
+        <v>1421</v>
       </c>
       <c r="F293" s="27" t="s">
         <v>26</v>
@@ -23853,7 +23856,7 @@
         <v>26</v>
       </c>
       <c r="I293" s="28" t="s">
-        <v>1770</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- added "visualization" section to primary FAST input file and updates CertTests with this change - added SrvD input-file change from latest commit - added AD change so cm is steady solution with UA - added check that DT isn't zero when reading input file because we use it later in that routine (before checking in the ValidateInput routine) - combined sibling meshes into a single vtp output file when possible (reduce number of files being generated) - added option to output fields or not (including with surfaces) - changed version to 8.15 and updated templates
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1224 10acb478-4768-415a-8850-bacdb5912d4d

Former-commit-id: 9926a5ad5c39c24a554aa582b6f7adb23bf714a7
</commit_message>
<xml_diff>
--- a/modules-local/fast-library/src/RegistryEntries.xlsx
+++ b/modules-local/fast-library/src/RegistryEntries.xlsx
@@ -8679,7 +8679,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="908">
+  <dxfs count="902">
     <dxf>
       <font>
         <u val="none"/>
@@ -16331,57 +16331,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -17329,7 +17278,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J121" sqref="J121"/>
+      <selection pane="bottomLeft" activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19982,7 +19931,7 @@
         <v>27</v>
       </c>
       <c r="D121" s="27" t="s">
-        <v>41</v>
+        <v>235</v>
       </c>
       <c r="E121" s="27" t="s">
         <v>2739</v>
@@ -69399,26 +69348,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108">
-    <cfRule type="containsText" dxfId="33" priority="5" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A108)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="32" priority="6" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="72" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(A108,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107">
-    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="71" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A107)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="70" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(A107,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109">
-    <cfRule type="containsText" dxfId="29" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="69" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A109)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="68" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A109,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>